<commit_message>
data reupload by nikhil
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -35,7 +35,7 @@
     <t>Stock Group Summary</t>
   </si>
   <si>
-    <t>1-Jul-25 to 1-Nov-25</t>
+    <t>1-Jul-25 to 24-Oct-25</t>
   </si>
   <si>
     <t/>
@@ -569,10 +569,10 @@
     <t>4294 PATRIKA (5273)</t>
   </si>
   <si>
-    <t>4295 PATRIKA (ANE W H) (286-A)</t>
-  </si>
-  <si>
-    <t>4296 PATRIKA (ANE WALA) (1407)</t>
+    <t>4295 PATRIKA (286-A)</t>
+  </si>
+  <si>
+    <t>4296 PATRIKA (1407)</t>
   </si>
   <si>
     <t>4297 PATRIKA (306)</t>
@@ -632,7 +632,7 @@
     <t>5053 PATRIKA (5213)</t>
   </si>
   <si>
-    <t>5054 PATRIKA *-* (6000) (25/162)</t>
+    <t>5054 PATRIKA *-* (25/162)</t>
   </si>
   <si>
     <t>5055 PATRIKA (25/272)</t>
@@ -707,7 +707,7 @@
     <t>5078 PATRIKA (DCU) (2156 CREAM)</t>
   </si>
   <si>
-    <t>5079 PATRIKA (ANE WALA) (296-A (NEHA)</t>
+    <t>5079 PATRIKA (296-A (NEHA)</t>
   </si>
   <si>
     <t>5080 PATRIKA (2501 GE NEW)</t>
@@ -746,7 +746,7 @@
     <t>5092 PATRIKA (05 NAVIN BHAI)</t>
   </si>
   <si>
-    <t>5093 PATRIKA (5400) (5350)</t>
+    <t>5093 PATRIKA (5350)</t>
   </si>
   <si>
     <t>5094 PATRIKA (5251)</t>
@@ -782,7 +782,7 @@
     <t>5105 PATRIKA (JC) (5335)</t>
   </si>
   <si>
-    <t>5106 PATRIKA (AN WALA) (253-A / 257-A)</t>
+    <t>5106 PATRIKA (253-A / 257-A)</t>
   </si>
   <si>
     <t>5107 PATRIKA (5356 RJ)</t>
@@ -983,7 +983,7 @@
     <t>5555 PATRIKA (2903)</t>
   </si>
   <si>
-    <t>5556 PATRIKA *-* (ANE WALA) (2952)</t>
+    <t>5556 PATRIKA *-* (2952)</t>
   </si>
   <si>
     <t>5557 PATRIKA (2312 SBC)</t>
@@ -992,7 +992,7 @@
     <t>5558 PATRIKA *-* (121 NEHA)</t>
   </si>
   <si>
-    <t>5559 PATRIKA (1500) (2293)</t>
+    <t>5559 PATRIKA (2293)</t>
   </si>
   <si>
     <t>5560 PATRIKA (F/G) *-* (2915)</t>
@@ -1001,7 +1001,7 @@
     <t>5561 PATRIKA *-* (25358)</t>
   </si>
   <si>
-    <t>5562 PATRIKA *-* (ANE WALA) (114-B (NEHA))</t>
+    <t>5562 PATRIKA *-* (114-B (NEHA))</t>
   </si>
   <si>
     <t>5563 PATRIKA (5387)</t>
@@ -1130,7 +1130,7 @@
     <t>5605 PATRIKA (JC) (3102)</t>
   </si>
   <si>
-    <t>5606 PATRIKA *-* (ANE WALA) (221-A)</t>
+    <t>5606 PATRIKA *-* (221-A)</t>
   </si>
   <si>
     <t>5607 PATRIKA (25442)</t>
@@ -1202,7 +1202,7 @@
     <t>6604 PATRIKA *-* (5196)</t>
   </si>
   <si>
-    <t>6605 PATRIKA ANE WALA (5191)</t>
+    <t>6605 PATRIKA (5191)</t>
   </si>
   <si>
     <t>6606 PATRIKA (3023)</t>
@@ -1325,7 +1325,7 @@
     <t>6645 PATRIKA *-* (3031)</t>
   </si>
   <si>
-    <t>6646 PATRIKA *-* (700) (3034)</t>
+    <t>6646 PATRIKA *-* (3034)</t>
   </si>
   <si>
     <t>6647 PATRIKA *-* (25382)</t>
@@ -1346,7 +1346,7 @@
     <t>6652 PATRIKA *-* (2764 SBC)</t>
   </si>
   <si>
-    <t>6653 PATRIKA *-* (ANE WALA) (834 SBC NEW)</t>
+    <t>6653 PATRIKA *-* (834 SBC NEW)</t>
   </si>
   <si>
     <t>6654 PATRIKA *-* (3461)</t>
@@ -1379,7 +1379,7 @@
     <t>6663 PATRIKA (7103 (PADDING))</t>
   </si>
   <si>
-    <t>6664 PATRIKA *-* (3500) (5823)</t>
+    <t>6664 PATRIKA *-* (5823)</t>
   </si>
   <si>
     <t>6665 PATRIKA *-* (603 DHANESH)</t>
@@ -1412,7 +1412,7 @@
     <t>6674 PATRIKA (DCU) (1503)</t>
   </si>
   <si>
-    <t>6675 PATRIKA *-* (1800) (1282)</t>
+    <t>6675 PATRIKA *-* (1282)</t>
   </si>
   <si>
     <t>6676 PATRIKA (DCU) (533 KBC)</t>
@@ -1502,7 +1502,7 @@
     <t>7415 PATRIKA *-* (3162 SBC)</t>
   </si>
   <si>
-    <t>7416 PATRIKA (1800) (2234)</t>
+    <t>7416 PATRIKA (2234)</t>
   </si>
   <si>
     <t>7417 PATRIKA (S-201 INV)</t>
@@ -1541,7 +1541,7 @@
     <t>7428 PATRIKA (1223 SBC)</t>
   </si>
   <si>
-    <t>7429 PATRIKA (F/G) *-* (ANE WALA) (1851 MONARCH)</t>
+    <t>7429 PATRIKA (F/G) *-* (1851 MONARCH)</t>
   </si>
   <si>
     <t>7430 PATRIKA (6310 GE)</t>
@@ -1607,10 +1607,10 @@
     <t>7450 PATRIKA (DCU) (3753)</t>
   </si>
   <si>
-    <t>7451 PATRIKA (ANE WALA) (273 NEHA)</t>
-  </si>
-  <si>
-    <t>7452 PATRIKA (ANE WALA) (278-B)</t>
+    <t>7451 PATRIKA (273 NEHA)</t>
+  </si>
+  <si>
+    <t>7452 PATRIKA (278-B)</t>
   </si>
   <si>
     <t>9001 CARD (O.C.) (2498 Cream)</t>
@@ -1661,13 +1661,13 @@
     <t>9304 CARDS (5083 Blue)</t>
   </si>
   <si>
-    <t>9305 CARDS (9070) (1500) (4701 Nice)</t>
+    <t>9305 CARDS (9070) (4701 Nice)</t>
   </si>
   <si>
     <t>9306 CARDS (0543 Nice)</t>
   </si>
   <si>
-    <t>9307 CARDS *-* (600 (5243 Nice)</t>
+    <t>9307 CARDS *-* (5243 Nice)</t>
   </si>
   <si>
     <t>9308 CARDS (9852)</t>
@@ -2848,16 +2848,16 @@
         <v>27</v>
       </c>
       <c r="B24" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="25">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="D24" s="26">
         <v>1.65</v>
       </c>
       <c r="E24" s="27">
-        <v>15.68</v>
+        <v>12.38</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2880,16 +2880,16 @@
         <v>29</v>
       </c>
       <c r="B26" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26" s="25">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D26" s="26">
         <v>2</v>
       </c>
       <c r="E26" s="27">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3016,16 +3016,16 @@
         <v>37</v>
       </c>
       <c r="B34" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C34" s="25">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D34" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E34" s="27">
-        <v>400.2</v>
+        <v>388.7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3033,16 +3033,16 @@
         <v>38</v>
       </c>
       <c r="B35" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" s="25">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D35" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E35" s="27">
-        <v>395.6</v>
+        <v>384.1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3800,10 +3800,10 @@
         <v>89</v>
       </c>
       <c r="B86" s="24">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C86" s="25">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="D86" s="28"/>
       <c r="E86" s="29"/>
@@ -3813,10 +3813,10 @@
         <v>90</v>
       </c>
       <c r="B87" s="24">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C87" s="25">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="D87" s="28"/>
       <c r="E87" s="29"/>
@@ -3865,16 +3865,16 @@
         <v>94</v>
       </c>
       <c r="B91" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C91" s="25">
-        <v>14.5</v>
+        <v>9.5</v>
       </c>
       <c r="D91" s="26">
         <v>12.5</v>
       </c>
       <c r="E91" s="27">
-        <v>181.25</v>
+        <v>118.75</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,16 +3899,16 @@
         <v>96</v>
       </c>
       <c r="B93" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C93" s="25">
-        <v>15.5</v>
+        <v>13.5</v>
       </c>
       <c r="D93" s="26">
         <v>12.5</v>
       </c>
       <c r="E93" s="27">
-        <v>193.75</v>
+        <v>168.75</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -4561,16 +4561,16 @@
         <v>136</v>
       </c>
       <c r="B133" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C133" s="25">
-        <v>13.5</v>
+        <v>11.5</v>
       </c>
       <c r="D133" s="26">
         <v>3.25</v>
       </c>
       <c r="E133" s="27">
-        <v>43.88</v>
+        <v>37.380000000000003</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4806,16 +4806,16 @@
         <v>151</v>
       </c>
       <c r="B148" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C148" s="25">
-        <v>27.5</v>
+        <v>22.5</v>
       </c>
       <c r="D148" s="26">
         <v>2.65</v>
       </c>
       <c r="E148" s="27">
-        <v>72.88</v>
+        <v>59.63</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4953,16 +4953,16 @@
         <v>160</v>
       </c>
       <c r="B157" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C157" s="25">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D157" s="26">
         <v>4.5</v>
       </c>
       <c r="E157" s="27">
-        <v>184.5</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -5196,16 +5196,16 @@
         <v>175</v>
       </c>
       <c r="B172" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C172" s="25">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D172" s="26">
         <v>2.7</v>
       </c>
       <c r="E172" s="27">
-        <v>59.4</v>
+        <v>48.6</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -5213,16 +5213,16 @@
         <v>176</v>
       </c>
       <c r="B173" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C173" s="25">
-        <v>29.5</v>
+        <v>124.5</v>
       </c>
       <c r="D173" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E173" s="27">
-        <v>67.849999999999994</v>
+        <v>286.35000000000002</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5281,16 +5281,16 @@
         <v>180</v>
       </c>
       <c r="B177" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C177" s="25">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D177" s="26">
         <v>3.88</v>
       </c>
       <c r="E177" s="27">
-        <v>186</v>
+        <v>155</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5301,13 +5301,13 @@
         <v>7</v>
       </c>
       <c r="C178" s="25">
-        <v>0.5</v>
+        <v>99.5</v>
       </c>
       <c r="D178" s="26">
-        <v>3.26</v>
+        <v>3.25</v>
       </c>
       <c r="E178" s="27">
-        <v>1.63</v>
+        <v>323.38</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -5315,16 +5315,16 @@
         <v>182</v>
       </c>
       <c r="B179" s="24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C179" s="25">
-        <v>-1</v>
+        <v>60</v>
       </c>
       <c r="D179" s="26">
         <v>3.5</v>
       </c>
       <c r="E179" s="27">
-        <v>-3.5</v>
+        <v>210</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5466,16 +5466,16 @@
         <v>191</v>
       </c>
       <c r="B188" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C188" s="25">
-        <v>140.5</v>
+        <v>137.5</v>
       </c>
       <c r="D188" s="26">
         <v>3.5</v>
       </c>
       <c r="E188" s="27">
-        <v>491.75</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5628,16 +5628,16 @@
         <v>201</v>
       </c>
       <c r="B198" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C198" s="25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D198" s="26">
         <v>4.8</v>
       </c>
       <c r="E198" s="27">
-        <v>52.8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5645,16 +5645,16 @@
         <v>202</v>
       </c>
       <c r="B199" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C199" s="25">
-        <v>7.5</v>
+        <v>64.5</v>
       </c>
       <c r="D199" s="26">
         <v>6.3</v>
       </c>
       <c r="E199" s="27">
-        <v>47.25</v>
+        <v>406.35</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5662,16 +5662,16 @@
         <v>203</v>
       </c>
       <c r="B200" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C200" s="25">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D200" s="26">
         <v>3</v>
       </c>
       <c r="E200" s="27">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5713,16 +5713,16 @@
         <v>206</v>
       </c>
       <c r="B203" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C203" s="25">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D203" s="26">
         <v>3.9</v>
       </c>
       <c r="E203" s="27">
-        <v>46.8</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5956,16 +5956,16 @@
         <v>221</v>
       </c>
       <c r="B218" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C218" s="25">
-        <v>37.5</v>
+        <v>35.5</v>
       </c>
       <c r="D218" s="26">
         <v>4.28</v>
       </c>
       <c r="E218" s="27">
-        <v>160.5</v>
+        <v>151.94</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5973,16 +5973,16 @@
         <v>222</v>
       </c>
       <c r="B219" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C219" s="25">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D219" s="26">
         <v>6</v>
       </c>
       <c r="E219" s="27">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -6057,13 +6057,13 @@
         <v>3</v>
       </c>
       <c r="C224" s="25">
-        <v>8.5</v>
+        <v>18.5</v>
       </c>
       <c r="D224" s="26">
         <v>4.5</v>
       </c>
       <c r="E224" s="27">
-        <v>38.25</v>
+        <v>83.25</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6105,16 +6105,16 @@
         <v>230</v>
       </c>
       <c r="B227" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C227" s="25">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D227" s="26">
         <v>4.4000000000000004</v>
       </c>
       <c r="E227" s="27">
-        <v>145.1</v>
+        <v>131.9</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6122,16 +6122,16 @@
         <v>231</v>
       </c>
       <c r="B228" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C228" s="25">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D228" s="26">
         <v>4.3099999999999996</v>
       </c>
       <c r="E228" s="27">
-        <v>267.17</v>
+        <v>254.24</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6220,16 +6220,16 @@
         <v>237</v>
       </c>
       <c r="B234" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C234" s="25">
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
       <c r="D234" s="26">
         <v>4.7</v>
       </c>
       <c r="E234" s="27">
-        <v>96.35</v>
+        <v>91.65</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -6272,13 +6272,13 @@
         <v>9</v>
       </c>
       <c r="C237" s="25">
-        <v>-0.5</v>
+        <v>53.5</v>
       </c>
       <c r="D237" s="26">
         <v>6</v>
       </c>
       <c r="E237" s="27">
-        <v>-3</v>
+        <v>321</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6401,16 +6401,16 @@
         <v>248</v>
       </c>
       <c r="B245" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C245" s="25">
-        <v>66.5</v>
+        <v>63.5</v>
       </c>
       <c r="D245" s="26">
         <v>4.5</v>
       </c>
       <c r="E245" s="27">
-        <v>299.25</v>
+        <v>285.75</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6470,13 +6470,13 @@
         <v>3</v>
       </c>
       <c r="C249" s="25">
-        <v>18.5</v>
+        <v>67.5</v>
       </c>
       <c r="D249" s="26">
         <v>3.15</v>
       </c>
       <c r="E249" s="27">
-        <v>58.28</v>
+        <v>212.63</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -6518,16 +6518,16 @@
         <v>255</v>
       </c>
       <c r="B252" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C252" s="25">
-        <v>70.5</v>
+        <v>67.5</v>
       </c>
       <c r="D252" s="26">
         <v>4.16</v>
       </c>
       <c r="E252" s="27">
-        <v>293.27999999999997</v>
+        <v>280.8</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6754,13 +6754,13 @@
         <v>5</v>
       </c>
       <c r="C267" s="25">
-        <v>10.35</v>
+        <v>14.35</v>
       </c>
       <c r="D267" s="26">
         <v>9.4499999999999993</v>
       </c>
       <c r="E267" s="27">
-        <v>97.81</v>
+        <v>135.61000000000001</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -7024,16 +7024,16 @@
         <v>287</v>
       </c>
       <c r="B284" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C284" s="25">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D284" s="26">
         <v>4.28</v>
       </c>
       <c r="E284" s="27">
-        <v>115.56</v>
+        <v>94.16</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -7105,16 +7105,16 @@
         <v>292</v>
       </c>
       <c r="B289" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C289" s="25">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D289" s="26">
         <v>9</v>
       </c>
       <c r="E289" s="27">
-        <v>144</v>
+        <v>108</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7320,16 +7320,16 @@
         <v>305</v>
       </c>
       <c r="B302" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C302" s="25">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D302" s="26">
         <v>5.7</v>
       </c>
       <c r="E302" s="27">
-        <v>108.3</v>
+        <v>148.19999999999999</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7551,13 +7551,13 @@
         <v>3</v>
       </c>
       <c r="C316" s="25">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D316" s="26">
         <v>6.65</v>
       </c>
       <c r="E316" s="27">
-        <v>39.9</v>
+        <v>126.35</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
@@ -7596,13 +7596,13 @@
         <v>2</v>
       </c>
       <c r="C319" s="25">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D319" s="26">
         <v>6.18</v>
       </c>
       <c r="E319" s="27">
-        <v>105.06</v>
+        <v>197.76</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
@@ -7613,13 +7613,13 @@
         <v>12</v>
       </c>
       <c r="C320" s="25">
-        <v>6.5</v>
+        <v>54.5</v>
       </c>
       <c r="D320" s="26">
         <v>7.13</v>
       </c>
       <c r="E320" s="27">
-        <v>46.35</v>
+        <v>388.59</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -7644,16 +7644,16 @@
         <v>325</v>
       </c>
       <c r="B322" s="24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C322" s="25">
-        <v>-11.5</v>
+        <v>13.5</v>
       </c>
       <c r="D322" s="26">
         <v>6.6</v>
       </c>
       <c r="E322" s="27">
-        <v>-75.900000000000006</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
@@ -7695,16 +7695,16 @@
         <v>328</v>
       </c>
       <c r="B325" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C325" s="25">
-        <v>29</v>
+        <v>27.5</v>
       </c>
       <c r="D325" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E325" s="27">
-        <v>237.8</v>
+        <v>225.5</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -7829,16 +7829,16 @@
         <v>336</v>
       </c>
       <c r="B333" s="24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C333" s="25">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D333" s="26">
         <v>3.6</v>
       </c>
       <c r="E333" s="27">
-        <v>129.6</v>
+        <v>100.8</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7943,15 +7943,17 @@
       <c r="A340" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="B340" s="24"/>
+      <c r="B340" s="24">
+        <v>1</v>
+      </c>
       <c r="C340" s="25">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D340" s="26">
         <v>5.3</v>
       </c>
       <c r="E340" s="27">
-        <v>90.1</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
@@ -8088,13 +8090,13 @@
         <v>3</v>
       </c>
       <c r="C349" s="25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D349" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E349" s="27">
-        <v>68.400000000000006</v>
+        <v>128.25</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -8348,13 +8350,13 @@
         <v>10</v>
       </c>
       <c r="C365" s="25">
-        <v>-9.5</v>
+        <v>20.5</v>
       </c>
       <c r="D365" s="26">
         <v>5.2</v>
       </c>
       <c r="E365" s="27">
-        <v>-49.4</v>
+        <v>106.6</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -8394,16 +8396,16 @@
         <v>371</v>
       </c>
       <c r="B368" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C368" s="25">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D368" s="26">
         <v>5.3</v>
       </c>
       <c r="E368" s="27">
-        <v>318</v>
+        <v>302.10000000000002</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -8618,16 +8620,16 @@
         <v>385</v>
       </c>
       <c r="B382" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C382" s="25">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D382" s="26">
         <v>5</v>
       </c>
       <c r="E382" s="27">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
@@ -8696,15 +8698,17 @@
       <c r="A387" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="B387" s="24"/>
+      <c r="B387" s="24">
+        <v>1</v>
+      </c>
       <c r="C387" s="25">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="D387" s="26">
         <v>13</v>
       </c>
       <c r="E387" s="27">
-        <v>123.5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
@@ -8732,13 +8736,13 @@
         <v>2</v>
       </c>
       <c r="C389" s="25">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D389" s="26">
         <v>8.75</v>
       </c>
       <c r="E389" s="27">
-        <v>26.25</v>
+        <v>96.25</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
@@ -8811,15 +8815,17 @@
       <c r="A394" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="B394" s="24"/>
+      <c r="B394" s="24">
+        <v>1</v>
+      </c>
       <c r="C394" s="25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D394" s="26">
         <v>11</v>
       </c>
       <c r="E394" s="27">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
@@ -9000,16 +9006,16 @@
         <v>409</v>
       </c>
       <c r="B406" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C406" s="25">
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="D406" s="26">
         <v>22.5</v>
       </c>
       <c r="E406" s="27">
-        <v>258.75</v>
+        <v>213.75</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
@@ -9047,16 +9053,16 @@
         <v>412</v>
       </c>
       <c r="B409" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C409" s="25">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D409" s="26">
         <v>10.5</v>
       </c>
       <c r="E409" s="27">
-        <v>157.5</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
@@ -9171,16 +9177,16 @@
         <v>420</v>
       </c>
       <c r="B417" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C417" s="25">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="D417" s="26">
         <v>16</v>
       </c>
       <c r="E417" s="27">
-        <v>200</v>
+        <v>168</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.25">
@@ -9254,16 +9260,16 @@
         <v>425</v>
       </c>
       <c r="B422" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C422" s="25">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="D422" s="26">
         <v>9.5</v>
       </c>
       <c r="E422" s="27">
-        <v>118.75</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -9385,13 +9391,13 @@
         <v>1</v>
       </c>
       <c r="C430" s="25">
-        <v>4.5</v>
+        <v>11.5</v>
       </c>
       <c r="D430" s="26">
         <v>11.88</v>
       </c>
       <c r="E430" s="27">
-        <v>53.46</v>
+        <v>136.62</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
@@ -9483,13 +9489,13 @@
         <v>2</v>
       </c>
       <c r="C436" s="25">
-        <v>2.5</v>
+        <v>22.5</v>
       </c>
       <c r="D436" s="26">
         <v>9.26</v>
       </c>
       <c r="E436" s="27">
-        <v>23.15</v>
+        <v>208.35</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
@@ -9500,13 +9506,13 @@
         <v>3</v>
       </c>
       <c r="C437" s="25">
-        <v>11.5</v>
+        <v>21</v>
       </c>
       <c r="D437" s="26">
         <v>10.45</v>
       </c>
       <c r="E437" s="27">
-        <v>120.18</v>
+        <v>219.45</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -9675,13 +9681,13 @@
         <v>11</v>
       </c>
       <c r="C448" s="25">
-        <v>-7.5</v>
+        <v>27.5</v>
       </c>
       <c r="D448" s="26">
         <v>11.25</v>
       </c>
       <c r="E448" s="27">
-        <v>-84.38</v>
+        <v>309.38</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -9844,13 +9850,13 @@
       </c>
       <c r="B459" s="24"/>
       <c r="C459" s="25">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D459" s="26">
         <v>12.8</v>
       </c>
       <c r="E459" s="27">
-        <v>51.2</v>
+        <v>281.60000000000002</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
@@ -10336,13 +10342,13 @@
         <v>10</v>
       </c>
       <c r="C489" s="25">
-        <v>-1.5</v>
+        <v>36.5</v>
       </c>
       <c r="D489" s="26">
         <v>4.28</v>
       </c>
       <c r="E489" s="27">
-        <v>-6.42</v>
+        <v>156.22</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.25">
@@ -10500,13 +10506,13 @@
         <v>9</v>
       </c>
       <c r="C499" s="25">
-        <v>9.5</v>
+        <v>25.5</v>
       </c>
       <c r="D499" s="26">
         <v>9.5</v>
       </c>
       <c r="E499" s="27">
-        <v>90.25</v>
+        <v>242.25</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10551,13 +10557,13 @@
         <v>23</v>
       </c>
       <c r="C502" s="25">
-        <v>-6.5</v>
+        <v>41.5</v>
       </c>
       <c r="D502" s="26">
         <v>3.9</v>
       </c>
       <c r="E502" s="27">
-        <v>-25.35</v>
+        <v>161.85</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.25">
@@ -10912,16 +10918,16 @@
         <v>527</v>
       </c>
       <c r="B524" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C524" s="25">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="D524" s="26">
         <v>1.4</v>
       </c>
       <c r="E524" s="27">
-        <v>37.799999999999997</v>
+        <v>186.2</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
@@ -10929,16 +10935,16 @@
         <v>528</v>
       </c>
       <c r="B525" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C525" s="25">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="D525" s="26">
         <v>1.8</v>
       </c>
       <c r="E525" s="27">
-        <v>27</v>
+        <v>221.4</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
@@ -10976,10 +10982,10 @@
         <v>531</v>
       </c>
       <c r="B528" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C528" s="25">
-        <v>61</v>
+        <v>60.5</v>
       </c>
       <c r="D528" s="28"/>
       <c r="E528" s="29"/>
@@ -11015,10 +11021,10 @@
         <v>534</v>
       </c>
       <c r="B531" s="24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C531" s="25">
-        <v>97</v>
+        <v>85.5</v>
       </c>
       <c r="D531" s="28"/>
       <c r="E531" s="29"/>
@@ -11028,16 +11034,16 @@
         <v>535</v>
       </c>
       <c r="B532" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C532" s="25">
-        <v>508.5</v>
+        <v>498.5</v>
       </c>
       <c r="D532" s="26">
         <v>0.87</v>
       </c>
       <c r="E532" s="27">
-        <v>442.4</v>
+        <v>433.7</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -11045,10 +11051,10 @@
         <v>536</v>
       </c>
       <c r="B533" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C533" s="25">
-        <v>-9</v>
+        <v>-29</v>
       </c>
       <c r="D533" s="28"/>
       <c r="E533" s="29"/>
@@ -11075,16 +11081,16 @@
         <v>538</v>
       </c>
       <c r="B535" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C535" s="25">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D535" s="26">
         <v>0.85</v>
       </c>
       <c r="E535" s="27">
-        <v>14.45</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.25">
@@ -11112,7 +11118,7 @@
         <v>8</v>
       </c>
       <c r="C537" s="25">
-        <v>-310</v>
+        <v>-300</v>
       </c>
       <c r="D537" s="28"/>
       <c r="E537" s="29"/>
@@ -11187,13 +11193,13 @@
         <v>2</v>
       </c>
       <c r="C542" s="25">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D542" s="26">
         <v>10</v>
       </c>
       <c r="E542" s="27">
-        <v>20</v>
+        <v>170</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">
@@ -11221,13 +11227,13 @@
         <v>1</v>
       </c>
       <c r="C544" s="25">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D544" s="26">
         <v>5</v>
       </c>
       <c r="E544" s="27">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.25">
@@ -11253,13 +11259,13 @@
         <v>3</v>
       </c>
       <c r="C546" s="25">
-        <v>-1.5</v>
+        <v>8.5</v>
       </c>
       <c r="D546" s="26">
         <v>3.5</v>
       </c>
       <c r="E546" s="27">
-        <v>-5.25</v>
+        <v>29.75</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
@@ -11382,16 +11388,16 @@
         <v>557</v>
       </c>
       <c r="B554" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C554" s="25">
-        <v>14.5</v>
+        <v>9.5</v>
       </c>
       <c r="D554" s="26">
         <v>2.8</v>
       </c>
       <c r="E554" s="27">
-        <v>40.61</v>
+        <v>26.61</v>
       </c>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.25">
@@ -11433,16 +11439,16 @@
         <v>560</v>
       </c>
       <c r="B557" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C557" s="25">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D557" s="26">
         <v>1.5</v>
       </c>
       <c r="E557" s="27">
-        <v>112.5</v>
+        <v>109.5</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.25">
@@ -11482,16 +11488,16 @@
         <v>563</v>
       </c>
       <c r="B560" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C560" s="25">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D560" s="26">
         <v>2.2799999999999998</v>
       </c>
       <c r="E560" s="27">
-        <v>59.28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
@@ -11616,9 +11622,15 @@
       <c r="B568" s="24">
         <v>1</v>
       </c>
-      <c r="C568" s="29"/>
-      <c r="D568" s="28"/>
-      <c r="E568" s="29"/>
+      <c r="C568" s="25">
+        <v>12</v>
+      </c>
+      <c r="D568" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="E568" s="27">
+        <v>42</v>
+      </c>
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A569" s="23" t="s">
@@ -11657,16 +11669,16 @@
         <v>574</v>
       </c>
       <c r="B571" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C571" s="25">
-        <v>19</v>
+        <v>16.5</v>
       </c>
       <c r="D571" s="26">
         <v>3.1</v>
       </c>
       <c r="E571" s="27">
-        <v>58.9</v>
+        <v>51.15</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
@@ -12096,16 +12108,16 @@
         <v>601</v>
       </c>
       <c r="B598" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C598" s="25">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D598" s="26">
         <v>2.5</v>
       </c>
       <c r="E598" s="27">
-        <v>70</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -12181,16 +12193,16 @@
         <v>606</v>
       </c>
       <c r="B603" s="24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C603" s="25">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D603" s="26">
         <v>2.25</v>
       </c>
       <c r="E603" s="27">
-        <v>135</v>
+        <v>112.5</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
@@ -12230,16 +12242,16 @@
         <v>609</v>
       </c>
       <c r="B606" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C606" s="25">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D606" s="26">
         <v>2.75</v>
       </c>
       <c r="E606" s="27">
-        <v>126.5</v>
+        <v>112.75</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12446,10 +12458,10 @@
         <v>623</v>
       </c>
       <c r="B620" s="24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C620" s="25">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D620" s="28"/>
       <c r="E620" s="29"/>
@@ -12639,10 +12651,10 @@
         <v>638</v>
       </c>
       <c r="B635" s="24">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C635" s="25">
-        <v>-0.27</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D635" s="28"/>
       <c r="E635" s="29"/>
@@ -12849,11 +12861,11 @@
       </c>
       <c r="B648" s="31"/>
       <c r="C648" s="32">
-        <v>18034.259999999998</v>
+        <v>18861.23</v>
       </c>
       <c r="D648" s="33"/>
       <c r="E648" s="34">
-        <v>74360.22</v>
+        <v>78373.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil 14 nov 10
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="686">
   <si>
     <t>Order Estimate - (from 1-Jul-2023)</t>
   </si>
@@ -218,13 +218,13 @@
     <t>1117 PATRIKA (1155)</t>
   </si>
   <si>
-    <t>1118 PATRIKA - B</t>
+    <t>1118 PATRIKA - B (DCU)</t>
   </si>
   <si>
     <t>1118 PATRIKA (सवाश्री-57)</t>
   </si>
   <si>
-    <t>1119 PATRIKA - B</t>
+    <t>1119 PATRIKA - B (DCU)</t>
   </si>
   <si>
     <t>1119 PATRIKA(सवाश्री-55)</t>
@@ -260,7 +260,7 @@
     <t>1129 PATRIKA (Eco-56)</t>
   </si>
   <si>
-    <t>1130 PATRIKA - B (ECO-60)</t>
+    <t>1130 PATRIKA - B (ECO-60) (DCU)</t>
   </si>
   <si>
     <t>1130 PATRIKA (Eco-59)</t>
@@ -326,16 +326,16 @@
     <t>1151 PATRIKA (DCU)</t>
   </si>
   <si>
-    <t>1152 PATRIKA</t>
-  </si>
-  <si>
-    <t>1153 PATRIKA</t>
-  </si>
-  <si>
-    <t>1154 PATRIKA</t>
-  </si>
-  <si>
-    <t>1155 PATRIKA</t>
+    <t>1152 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1153 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1154 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1155 PATRIKA (DCU)</t>
   </si>
   <si>
     <t>1156 PATRIKA-YELLOW</t>
@@ -1103,7 +1103,7 @@
     <t>5566 PATRIKA *-* (M)</t>
   </si>
   <si>
-    <t>5567 PATRIKA (MONDAY)</t>
+    <t>5567 PATRIKA</t>
   </si>
   <si>
     <t>5568 PATRIKA *-* (M)</t>
@@ -1352,7 +1352,7 @@
     <t>6625 PATRIKA *-* (M)</t>
   </si>
   <si>
-    <t>6626 PATRIKA *-* (M) 1600 (MONDAY)</t>
+    <t>6626 PATRIKA *-* (M)</t>
   </si>
   <si>
     <t>6627 PATRIKA *-* (M)</t>
@@ -2016,6 +2016,9 @@
   </si>
   <si>
     <t>9390 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9391 CARDS</t>
   </si>
   <si>
     <t>9*4 ENVELOPE (SBC)</t>
@@ -2602,7 +2605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E681"/>
+  <dimension ref="A1:E682"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2747,16 +2750,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="25">
-        <v>51.5</v>
+        <v>50.5</v>
       </c>
       <c r="D12" s="26">
         <v>1.95</v>
       </c>
       <c r="E12" s="27">
-        <v>100.43</v>
+        <v>98.48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3121,16 +3124,16 @@
         <v>37</v>
       </c>
       <c r="B34" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C34" s="25">
-        <v>144.5</v>
+        <v>142.5</v>
       </c>
       <c r="D34" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E34" s="27">
-        <v>332.35</v>
+        <v>327.75</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3317,16 +3320,16 @@
         <v>49</v>
       </c>
       <c r="B46" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46" s="25">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D46" s="26">
         <v>1.25</v>
       </c>
       <c r="E46" s="27">
-        <v>143.75</v>
+        <v>131.25</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3337,13 +3340,13 @@
         <v>3</v>
       </c>
       <c r="C47" s="25">
-        <v>119.5</v>
+        <v>110.5</v>
       </c>
       <c r="D47" s="26">
         <v>1.26</v>
       </c>
       <c r="E47" s="27">
-        <v>150.6</v>
+        <v>139.26</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3402,16 +3405,16 @@
         <v>54</v>
       </c>
       <c r="B51" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C51" s="25">
-        <v>161.5</v>
+        <v>155.5</v>
       </c>
       <c r="D51" s="26">
         <v>2.5</v>
       </c>
       <c r="E51" s="27">
-        <v>403.75</v>
+        <v>388.75</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3453,16 +3456,16 @@
         <v>57</v>
       </c>
       <c r="B54" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C54" s="25">
-        <v>53.75</v>
+        <v>47.75</v>
       </c>
       <c r="D54" s="26">
         <v>2.75</v>
       </c>
       <c r="E54" s="27">
-        <v>147.81</v>
+        <v>131.31</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3487,16 +3490,16 @@
         <v>59</v>
       </c>
       <c r="B56" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" s="25">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D56" s="26">
         <v>1.9</v>
       </c>
       <c r="E56" s="27">
-        <v>146.30000000000001</v>
+        <v>127.3</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3587,16 +3590,16 @@
         <v>65</v>
       </c>
       <c r="B62" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62" s="25">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D62" s="26">
         <v>1.65</v>
       </c>
       <c r="E62" s="27">
-        <v>77.55</v>
+        <v>67.650000000000006</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3619,16 +3622,16 @@
         <v>67</v>
       </c>
       <c r="B64" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64" s="25">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D64" s="26">
         <v>1.65</v>
       </c>
       <c r="E64" s="27">
-        <v>49.5</v>
+        <v>39.6</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3636,16 +3639,16 @@
         <v>68</v>
       </c>
       <c r="B65" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" s="25">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D65" s="26">
         <v>1.65</v>
       </c>
       <c r="E65" s="27">
-        <v>49.5</v>
+        <v>39.6</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3653,16 +3656,16 @@
         <v>69</v>
       </c>
       <c r="B66" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C66" s="25">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D66" s="26">
         <v>1.65</v>
       </c>
       <c r="E66" s="27">
-        <v>51.15</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3685,16 +3688,16 @@
         <v>71</v>
       </c>
       <c r="B68" s="24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C68" s="25">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D68" s="26">
         <v>1.4</v>
       </c>
       <c r="E68" s="27">
-        <v>81.2</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3702,16 +3705,16 @@
         <v>72</v>
       </c>
       <c r="B69" s="24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C69" s="25">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D69" s="26">
         <v>1.4</v>
       </c>
       <c r="E69" s="27">
-        <v>117.6</v>
+        <v>89.6</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3719,16 +3722,16 @@
         <v>73</v>
       </c>
       <c r="B70" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C70" s="25">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D70" s="26">
         <v>1.4</v>
       </c>
       <c r="E70" s="27">
-        <v>124.6</v>
+        <v>110.6</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,16 +3739,16 @@
         <v>74</v>
       </c>
       <c r="B71" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C71" s="25">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D71" s="26">
         <v>1.4</v>
       </c>
       <c r="E71" s="27">
-        <v>123.2</v>
+        <v>109.2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3951,9 +3954,11 @@
       <c r="A85" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B85" s="24"/>
+      <c r="B85" s="24">
+        <v>1</v>
+      </c>
       <c r="C85" s="25">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D85" s="29"/>
       <c r="E85" s="28"/>
@@ -3974,10 +3979,10 @@
         <v>90</v>
       </c>
       <c r="B87" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C87" s="25">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="28"/>
@@ -3987,10 +3992,10 @@
         <v>91</v>
       </c>
       <c r="B88" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C88" s="25">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="28"/>
@@ -4013,10 +4018,10 @@
         <v>93</v>
       </c>
       <c r="B90" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C90" s="25">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="28"/>
@@ -4026,16 +4031,16 @@
         <v>94</v>
       </c>
       <c r="B91" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C91" s="25">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D91" s="26">
         <v>3.2</v>
       </c>
       <c r="E91" s="27">
-        <v>217.6</v>
+        <v>185.6</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4154,76 +4159,84 @@
         <v>104</v>
       </c>
       <c r="B101" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C101" s="25">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D101" s="26">
         <v>2.5</v>
       </c>
       <c r="E101" s="27">
-        <v>72.5</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B102" s="24"/>
+      <c r="B102" s="24">
+        <v>1</v>
+      </c>
       <c r="C102" s="25">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D102" s="26">
         <v>2.5</v>
       </c>
       <c r="E102" s="27">
-        <v>107.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B103" s="24"/>
+      <c r="B103" s="24">
+        <v>1</v>
+      </c>
       <c r="C103" s="25">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D103" s="26">
         <v>2.5</v>
       </c>
       <c r="E103" s="27">
-        <v>107.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B104" s="24"/>
+      <c r="B104" s="24">
+        <v>1</v>
+      </c>
       <c r="C104" s="25">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D104" s="26">
         <v>2.5</v>
       </c>
       <c r="E104" s="27">
-        <v>107.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B105" s="24"/>
+      <c r="B105" s="24">
+        <v>1</v>
+      </c>
       <c r="C105" s="25">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D105" s="26">
         <v>2.5</v>
       </c>
       <c r="E105" s="27">
-        <v>107.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,10 +4244,10 @@
         <v>109</v>
       </c>
       <c r="B106" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C106" s="25">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D106" s="29"/>
       <c r="E106" s="28"/>
@@ -4244,10 +4257,10 @@
         <v>110</v>
       </c>
       <c r="B107" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107" s="25">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="28"/>
@@ -4305,10 +4318,10 @@
         <v>115</v>
       </c>
       <c r="B112" s="24">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C112" s="25">
-        <v>-0.96</v>
+        <v>-0.99</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="28"/>
@@ -4318,10 +4331,10 @@
         <v>116</v>
       </c>
       <c r="B113" s="24">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C113" s="25">
-        <v>-0.98</v>
+        <v>-1.02</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="28"/>
@@ -4416,13 +4429,13 @@
         <v>19</v>
       </c>
       <c r="C120" s="25">
-        <v>19.5</v>
+        <v>21.5</v>
       </c>
       <c r="D120" s="26">
         <v>12.5</v>
       </c>
       <c r="E120" s="27">
-        <v>243.75</v>
+        <v>268.75</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4532,16 +4545,16 @@
         <v>130</v>
       </c>
       <c r="B127" s="24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C127" s="25">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="D127" s="26">
         <v>12.5</v>
       </c>
       <c r="E127" s="27">
-        <v>87.5</v>
+        <v>106.25</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4598,16 +4611,16 @@
         <v>134</v>
       </c>
       <c r="B131" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C131" s="25">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="D131" s="26">
         <v>18.5</v>
       </c>
       <c r="E131" s="27">
-        <v>74</v>
+        <v>46.25</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4652,13 +4665,13 @@
         <v>14</v>
       </c>
       <c r="C134" s="25">
-        <v>31.5</v>
+        <v>11.5</v>
       </c>
       <c r="D134" s="26">
         <v>18.5</v>
       </c>
       <c r="E134" s="27">
-        <v>582.75</v>
+        <v>212.75</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4680,13 +4693,13 @@
         <v>5</v>
       </c>
       <c r="C136" s="25">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D136" s="26">
         <v>18.5</v>
       </c>
       <c r="E136" s="27">
-        <v>481</v>
+        <v>351.5</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4714,13 +4727,13 @@
         <v>7</v>
       </c>
       <c r="C138" s="25">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D138" s="26">
         <v>18.5</v>
       </c>
       <c r="E138" s="27">
-        <v>592</v>
+        <v>314.5</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4731,13 +4744,13 @@
         <v>18</v>
       </c>
       <c r="C139" s="25">
-        <v>41.5</v>
+        <v>26.5</v>
       </c>
       <c r="D139" s="26">
         <v>18.5</v>
       </c>
       <c r="E139" s="27">
-        <v>767.75</v>
+        <v>490.25</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4745,16 +4758,16 @@
         <v>143</v>
       </c>
       <c r="B140" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C140" s="25">
-        <v>16.5</v>
+        <v>14</v>
       </c>
       <c r="D140" s="26">
         <v>18.5</v>
       </c>
       <c r="E140" s="27">
-        <v>305.25</v>
+        <v>259</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4901,13 +4914,13 @@
         <v>5</v>
       </c>
       <c r="C149" s="25">
-        <v>47.5</v>
+        <v>29.5</v>
       </c>
       <c r="D149" s="26">
         <v>11.5</v>
       </c>
       <c r="E149" s="27">
-        <v>546.25</v>
+        <v>339.25</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4952,13 +4965,13 @@
         <v>17</v>
       </c>
       <c r="C152" s="25">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D152" s="26">
         <v>11.5</v>
       </c>
       <c r="E152" s="27">
-        <v>575</v>
+        <v>402.5</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -5011,16 +5024,16 @@
         <v>159</v>
       </c>
       <c r="B156" s="24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C156" s="25">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="D156" s="26">
         <v>1</v>
       </c>
       <c r="E156" s="27">
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -5039,16 +5052,16 @@
         <v>161</v>
       </c>
       <c r="B158" s="24">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C158" s="25">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D158" s="26">
         <v>1.1499999999999999</v>
       </c>
       <c r="E158" s="27">
-        <v>60.95</v>
+        <v>43.7</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -5116,16 +5129,16 @@
         <v>166</v>
       </c>
       <c r="B163" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C163" s="25">
-        <v>90.5</v>
+        <v>89.5</v>
       </c>
       <c r="D163" s="26">
         <v>2.7</v>
       </c>
       <c r="E163" s="27">
-        <v>244.35</v>
+        <v>241.65</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5247,15 +5260,17 @@
       <c r="A171" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="B171" s="24"/>
+      <c r="B171" s="24">
+        <v>1</v>
+      </c>
       <c r="C171" s="25">
-        <v>16.5</v>
+        <v>10.5</v>
       </c>
       <c r="D171" s="26">
         <v>4.25</v>
       </c>
       <c r="E171" s="27">
-        <v>70.13</v>
+        <v>44.63</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5315,13 +5330,13 @@
         <v>4</v>
       </c>
       <c r="C175" s="25">
-        <v>28.5</v>
+        <v>30.5</v>
       </c>
       <c r="D175" s="26">
         <v>2.76</v>
       </c>
       <c r="E175" s="27">
-        <v>78.72</v>
+        <v>84.24</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -5346,16 +5361,16 @@
         <v>180</v>
       </c>
       <c r="B177" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C177" s="25">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D177" s="26">
         <v>3.45</v>
       </c>
       <c r="E177" s="27">
-        <v>117.3</v>
+        <v>96.6</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5480,16 +5495,16 @@
         <v>188</v>
       </c>
       <c r="B185" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C185" s="25">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D185" s="26">
         <v>4.5</v>
       </c>
       <c r="E185" s="27">
-        <v>229.5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5599,16 +5614,16 @@
         <v>195</v>
       </c>
       <c r="B192" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C192" s="25">
-        <v>52</v>
+        <v>51.5</v>
       </c>
       <c r="D192" s="26">
         <v>2.6</v>
       </c>
       <c r="E192" s="27">
-        <v>135.19999999999999</v>
+        <v>133.9</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5710,16 +5725,16 @@
         <v>202</v>
       </c>
       <c r="B199" s="24">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C199" s="25">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D199" s="26">
         <v>2.7</v>
       </c>
       <c r="E199" s="27">
-        <v>299.7</v>
+        <v>291.60000000000002</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5999,16 +6014,16 @@
         <v>219</v>
       </c>
       <c r="B216" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C216" s="25">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D216" s="26">
         <v>3.5</v>
       </c>
       <c r="E216" s="27">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -6144,16 +6159,16 @@
         <v>228</v>
       </c>
       <c r="B225" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C225" s="25">
-        <v>23.5</v>
+        <v>21.5</v>
       </c>
       <c r="D225" s="26">
         <v>5.75</v>
       </c>
       <c r="E225" s="27">
-        <v>135.13</v>
+        <v>123.63</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -6178,16 +6193,16 @@
         <v>230</v>
       </c>
       <c r="B227" s="24">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C227" s="25">
-        <v>58.5</v>
+        <v>58</v>
       </c>
       <c r="D227" s="26">
         <v>6.3</v>
       </c>
       <c r="E227" s="27">
-        <v>368.55</v>
+        <v>365.4</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6327,16 +6342,16 @@
         <v>239</v>
       </c>
       <c r="B236" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C236" s="25">
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
       <c r="D236" s="26">
         <v>3.5</v>
       </c>
       <c r="E236" s="27">
-        <v>75.25</v>
+        <v>71.75</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -6481,16 +6496,16 @@
         <v>249</v>
       </c>
       <c r="B246" s="24">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C246" s="25">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D246" s="26">
         <v>4.28</v>
       </c>
       <c r="E246" s="27">
-        <v>316.72000000000003</v>
+        <v>308.16000000000003</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6515,16 +6530,16 @@
         <v>251</v>
       </c>
       <c r="B248" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C248" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D248" s="26">
         <v>4.5</v>
       </c>
       <c r="E248" s="27">
-        <v>157.5</v>
+        <v>112.5</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6681,16 +6696,16 @@
         <v>261</v>
       </c>
       <c r="B258" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C258" s="25">
-        <v>16.5</v>
+        <v>10.5</v>
       </c>
       <c r="D258" s="26">
         <v>4.28</v>
       </c>
       <c r="E258" s="27">
-        <v>70.62</v>
+        <v>44.94</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6698,17 +6713,11 @@
         <v>262</v>
       </c>
       <c r="B259" s="24">
-        <v>3</v>
-      </c>
-      <c r="C259" s="25">
-        <v>2.5</v>
-      </c>
-      <c r="D259" s="26">
-        <v>6.25</v>
-      </c>
-      <c r="E259" s="27">
-        <v>15.63</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C259" s="28"/>
+      <c r="D259" s="29"/>
+      <c r="E259" s="28"/>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="23" t="s">
@@ -6755,10 +6764,10 @@
         <v>58</v>
       </c>
       <c r="D262" s="26">
-        <v>4.79</v>
+        <v>4.82</v>
       </c>
       <c r="E262" s="27">
-        <v>277.97000000000003</v>
+        <v>279.45999999999998</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -6766,16 +6775,16 @@
         <v>266</v>
       </c>
       <c r="B263" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C263" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D263" s="26">
         <v>4.0999999999999996</v>
       </c>
       <c r="E263" s="27">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6934,16 +6943,16 @@
         <v>276</v>
       </c>
       <c r="B273" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C273" s="25">
-        <v>48</v>
+        <v>47.5</v>
       </c>
       <c r="D273" s="26">
         <v>4.5</v>
       </c>
       <c r="E273" s="27">
-        <v>216</v>
+        <v>213.75</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6951,16 +6960,16 @@
         <v>277</v>
       </c>
       <c r="B274" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C274" s="25">
-        <v>35.5</v>
+        <v>32.5</v>
       </c>
       <c r="D274" s="26">
         <v>3.8</v>
       </c>
       <c r="E274" s="27">
-        <v>134.9</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -6968,16 +6977,16 @@
         <v>278</v>
       </c>
       <c r="B275" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C275" s="25">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D275" s="26">
         <v>4.9000000000000004</v>
       </c>
       <c r="E275" s="27">
-        <v>181.38</v>
+        <v>176.48</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -7026,7 +7035,7 @@
         <v>5.97</v>
       </c>
       <c r="E278" s="27">
-        <v>196.98</v>
+        <v>197.17</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -7068,16 +7077,16 @@
         <v>284</v>
       </c>
       <c r="B281" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C281" s="25">
-        <v>26.5</v>
+        <v>16.5</v>
       </c>
       <c r="D281" s="26">
         <v>5.7</v>
       </c>
       <c r="E281" s="27">
-        <v>151.05000000000001</v>
+        <v>94.05</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -7117,16 +7126,16 @@
         <v>287</v>
       </c>
       <c r="B284" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C284" s="25">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D284" s="26">
         <v>4.29</v>
       </c>
       <c r="E284" s="27">
-        <v>535.66</v>
+        <v>522.79999999999995</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -7229,13 +7238,13 @@
         <v>4</v>
       </c>
       <c r="C291" s="25">
-        <v>23.5</v>
+        <v>18.5</v>
       </c>
       <c r="D291" s="26">
         <v>11.5</v>
       </c>
       <c r="E291" s="27">
-        <v>270.25</v>
+        <v>212.75</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7370,15 +7379,17 @@
       <c r="A300" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="B300" s="24"/>
+      <c r="B300" s="24">
+        <v>1</v>
+      </c>
       <c r="C300" s="25">
-        <v>12.5</v>
+        <v>7.5</v>
       </c>
       <c r="D300" s="26">
         <v>6.5</v>
       </c>
       <c r="E300" s="27">
-        <v>81.25</v>
+        <v>48.75</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -7469,16 +7480,16 @@
         <v>309</v>
       </c>
       <c r="B306" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C306" s="25">
-        <v>47.5</v>
+        <v>46.5</v>
       </c>
       <c r="D306" s="26">
         <v>6.75</v>
       </c>
       <c r="E306" s="27">
-        <v>320.63</v>
+        <v>313.88</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -7653,13 +7664,13 @@
         <v>27</v>
       </c>
       <c r="C317" s="25">
-        <v>79</v>
+        <v>41.5</v>
       </c>
       <c r="D317" s="26">
         <v>9</v>
       </c>
       <c r="E317" s="27">
-        <v>711</v>
+        <v>373.5</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
@@ -7687,13 +7698,13 @@
         <v>16</v>
       </c>
       <c r="C319" s="25">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="D319" s="26">
         <v>9</v>
       </c>
       <c r="E319" s="27">
-        <v>873</v>
+        <v>603</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
@@ -7721,13 +7732,13 @@
         <v>18</v>
       </c>
       <c r="C321" s="25">
-        <v>64.5</v>
+        <v>34.5</v>
       </c>
       <c r="D321" s="26">
         <v>9</v>
       </c>
       <c r="E321" s="27">
-        <v>580.5</v>
+        <v>310.5</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
@@ -7768,15 +7779,17 @@
       <c r="A324" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="B324" s="24"/>
+      <c r="B324" s="24">
+        <v>1</v>
+      </c>
       <c r="C324" s="25">
-        <v>10.5</v>
+        <v>5.5</v>
       </c>
       <c r="D324" s="26">
         <v>7</v>
       </c>
       <c r="E324" s="27">
-        <v>73.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
@@ -7784,16 +7797,16 @@
         <v>328</v>
       </c>
       <c r="B325" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C325" s="25">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D325" s="26">
         <v>3.4</v>
       </c>
       <c r="E325" s="27">
-        <v>200.6</v>
+        <v>166.6</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -8108,16 +8121,16 @@
         <v>348</v>
       </c>
       <c r="B345" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C345" s="25">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="D345" s="26">
         <v>6.65</v>
       </c>
       <c r="E345" s="27">
-        <v>69.83</v>
+        <v>59.85</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
@@ -8567,16 +8580,16 @@
         <v>375</v>
       </c>
       <c r="B372" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C372" s="25">
-        <v>23.5</v>
+        <v>23</v>
       </c>
       <c r="D372" s="26">
         <v>5.7</v>
       </c>
       <c r="E372" s="27">
-        <v>133.94999999999999</v>
+        <v>131.1</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
@@ -8786,16 +8799,16 @@
         <v>388</v>
       </c>
       <c r="B385" s="24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C385" s="25">
-        <v>32.5</v>
+        <v>34</v>
       </c>
       <c r="D385" s="26">
         <v>7</v>
       </c>
       <c r="E385" s="27">
-        <v>227.5</v>
+        <v>238</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
@@ -9131,15 +9144,17 @@
       <c r="A407" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="B407" s="24"/>
+      <c r="B407" s="24">
+        <v>1</v>
+      </c>
       <c r="C407" s="25">
-        <v>13.5</v>
+        <v>7.5</v>
       </c>
       <c r="D407" s="26">
         <v>5.23</v>
       </c>
       <c r="E407" s="27">
-        <v>70.61</v>
+        <v>39.229999999999997</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
@@ -9326,16 +9341,16 @@
         <v>422</v>
       </c>
       <c r="B419" s="24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C419" s="25">
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="D419" s="26">
         <v>9.75</v>
       </c>
       <c r="E419" s="27">
-        <v>43.88</v>
+        <v>68.25</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
@@ -9654,16 +9669,16 @@
         <v>442</v>
       </c>
       <c r="B439" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C439" s="25">
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="D439" s="26">
         <v>10</v>
       </c>
       <c r="E439" s="27">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
@@ -9686,16 +9701,16 @@
         <v>444</v>
       </c>
       <c r="B441" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C441" s="25">
-        <v>16.5</v>
+        <v>13.5</v>
       </c>
       <c r="D441" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E441" s="27">
-        <v>141.08000000000001</v>
+        <v>115.43</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
@@ -9923,16 +9938,16 @@
         <v>459</v>
       </c>
       <c r="B456" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C456" s="25">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="D456" s="26">
         <v>10.17</v>
       </c>
       <c r="E456" s="27">
-        <v>81.38</v>
+        <v>66.12</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
@@ -9972,16 +9987,16 @@
         <v>462</v>
       </c>
       <c r="B459" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C459" s="25">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="D459" s="26">
         <v>11.4</v>
       </c>
       <c r="E459" s="27">
-        <v>108.3</v>
+        <v>96.9</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
@@ -10106,16 +10121,16 @@
         <v>470</v>
       </c>
       <c r="B467" s="24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C467" s="25">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D467" s="26">
-        <v>10.46</v>
+        <v>10.45</v>
       </c>
       <c r="E467" s="27">
-        <v>5.23</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.25">
@@ -10319,16 +10334,16 @@
         <v>483</v>
       </c>
       <c r="B480" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C480" s="25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D480" s="26">
         <v>13.8</v>
       </c>
       <c r="E480" s="27">
-        <v>55.2</v>
+        <v>82.8</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.25">
@@ -10764,16 +10779,16 @@
         <v>510</v>
       </c>
       <c r="B507" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C507" s="25">
-        <v>83</v>
+        <v>80.5</v>
       </c>
       <c r="D507" s="26">
         <v>2.1</v>
       </c>
       <c r="E507" s="27">
-        <v>174.3</v>
+        <v>169.05</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -10845,16 +10860,16 @@
         <v>515</v>
       </c>
       <c r="B512" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C512" s="25">
-        <v>22.5</v>
+        <v>20.5</v>
       </c>
       <c r="D512" s="26">
         <v>3.5</v>
       </c>
       <c r="E512" s="27">
-        <v>78.75</v>
+        <v>71.75</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -11024,16 +11039,16 @@
         <v>526</v>
       </c>
       <c r="B523" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C523" s="25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D523" s="26">
         <v>4.75</v>
       </c>
       <c r="E523" s="27">
-        <v>52.25</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
@@ -11109,16 +11124,16 @@
         <v>531</v>
       </c>
       <c r="B528" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C528" s="25">
-        <v>19.5</v>
+        <v>15.5</v>
       </c>
       <c r="D528" s="26">
         <v>3.1</v>
       </c>
       <c r="E528" s="27">
-        <v>60.45</v>
+        <v>48.05</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -11129,13 +11144,13 @@
         <v>21</v>
       </c>
       <c r="C529" s="25">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D529" s="26">
         <v>9.5</v>
       </c>
       <c r="E529" s="27">
-        <v>370.5</v>
+        <v>446.5</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -11143,16 +11158,16 @@
         <v>533</v>
       </c>
       <c r="B530" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C530" s="25">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D530" s="26">
         <v>2.8</v>
       </c>
       <c r="E530" s="27">
-        <v>42</v>
+        <v>39.200000000000003</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
@@ -11177,16 +11192,16 @@
         <v>535</v>
       </c>
       <c r="B532" s="24">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C532" s="25">
-        <v>17.5</v>
+        <v>17</v>
       </c>
       <c r="D532" s="26">
         <v>3.9</v>
       </c>
       <c r="E532" s="27">
-        <v>68.25</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -11364,16 +11379,16 @@
         <v>546</v>
       </c>
       <c r="B543" s="24">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C543" s="25">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D543" s="26">
         <v>3.5</v>
       </c>
       <c r="E543" s="27">
-        <v>143.5</v>
+        <v>150.5</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
@@ -11547,16 +11562,16 @@
         <v>557</v>
       </c>
       <c r="B554" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C554" s="25">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D554" s="26">
         <v>1.4</v>
       </c>
       <c r="E554" s="27">
-        <v>331.8</v>
+        <v>330.4</v>
       </c>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.25">
@@ -11613,16 +11628,16 @@
         <v>561</v>
       </c>
       <c r="B558" s="24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C558" s="25">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D558" s="26">
         <v>1.5</v>
       </c>
       <c r="E558" s="27">
-        <v>583.5</v>
+        <v>582</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
@@ -11656,10 +11671,10 @@
         <v>564</v>
       </c>
       <c r="B561" s="24">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C561" s="25">
-        <v>-164.5</v>
+        <v>-276.5</v>
       </c>
       <c r="D561" s="29"/>
       <c r="E561" s="28"/>
@@ -11685,7 +11700,7 @@
         <v>18</v>
       </c>
       <c r="C563" s="25">
-        <v>16</v>
+        <v>-4</v>
       </c>
       <c r="D563" s="29"/>
       <c r="E563" s="28"/>
@@ -11695,16 +11710,16 @@
         <v>567</v>
       </c>
       <c r="B564" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C564" s="25">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D564" s="26">
         <v>0.87</v>
       </c>
       <c r="E564" s="27">
-        <v>353.22</v>
+        <v>351.48</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
@@ -11808,16 +11823,16 @@
         <v>574</v>
       </c>
       <c r="B571" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C571" s="25">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="D571" s="26">
         <v>5.5</v>
       </c>
       <c r="E571" s="27">
-        <v>68.75</v>
+        <v>57.75</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
@@ -11859,16 +11874,16 @@
         <v>577</v>
       </c>
       <c r="B574" s="24">
+        <v>9</v>
+      </c>
+      <c r="C574" s="25">
         <v>8</v>
-      </c>
-      <c r="C574" s="25">
-        <v>11</v>
       </c>
       <c r="D574" s="26">
         <v>10</v>
       </c>
       <c r="E574" s="27">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.25">
@@ -12012,16 +12027,16 @@
         <v>586</v>
       </c>
       <c r="B583" s="24">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C583" s="25">
-        <v>34.5</v>
+        <v>30.5</v>
       </c>
       <c r="D583" s="26">
         <v>2.79</v>
       </c>
       <c r="E583" s="27">
-        <v>96.42</v>
+        <v>85.24</v>
       </c>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
@@ -12144,16 +12159,16 @@
         <v>594</v>
       </c>
       <c r="B591" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C591" s="25">
-        <v>12.75</v>
+        <v>11.75</v>
       </c>
       <c r="D591" s="26">
         <v>1.5</v>
       </c>
       <c r="E591" s="27">
-        <v>19.13</v>
+        <v>17.63</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
@@ -12240,16 +12255,16 @@
         <v>600</v>
       </c>
       <c r="B597" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C597" s="25">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D597" s="26">
         <v>4.6500000000000004</v>
       </c>
       <c r="E597" s="27">
-        <v>120.9</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -12393,16 +12408,16 @@
         <v>609</v>
       </c>
       <c r="B606" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C606" s="25">
-        <v>15.5</v>
+        <v>13.5</v>
       </c>
       <c r="D606" s="26">
         <v>3.5</v>
       </c>
       <c r="E606" s="27">
-        <v>54.25</v>
+        <v>47.25</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12478,16 +12493,16 @@
         <v>614</v>
       </c>
       <c r="B611" s="24">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C611" s="25">
-        <v>39.5</v>
+        <v>37.5</v>
       </c>
       <c r="D611" s="26">
         <v>2.85</v>
       </c>
       <c r="E611" s="27">
-        <v>112.58</v>
+        <v>106.88</v>
       </c>
     </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.25">
@@ -12729,16 +12744,16 @@
         <v>629</v>
       </c>
       <c r="B626" s="24">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C626" s="25">
-        <v>26.5</v>
+        <v>22</v>
       </c>
       <c r="D626" s="26">
         <v>3.1</v>
       </c>
       <c r="E626" s="27">
-        <v>82.15</v>
+        <v>68.2</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -13142,10 +13157,10 @@
         <v>654</v>
       </c>
       <c r="B651" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C651" s="25">
-        <v>62.19</v>
+        <v>57.19</v>
       </c>
       <c r="D651" s="29"/>
       <c r="E651" s="28"/>
@@ -13171,7 +13186,7 @@
         <v>17</v>
       </c>
       <c r="C653" s="25">
-        <v>-33</v>
+        <v>-13</v>
       </c>
       <c r="D653" s="29"/>
       <c r="E653" s="28"/>
@@ -13197,7 +13212,7 @@
         <v>27</v>
       </c>
       <c r="C655" s="25">
-        <v>-50</v>
+        <v>-20</v>
       </c>
       <c r="D655" s="29"/>
       <c r="E655" s="28"/>
@@ -13207,10 +13222,10 @@
         <v>659</v>
       </c>
       <c r="B656" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C656" s="25">
-        <v>-47</v>
+        <v>-22</v>
       </c>
       <c r="D656" s="29"/>
       <c r="E656" s="28"/>
@@ -13223,7 +13238,7 @@
         <v>13</v>
       </c>
       <c r="C657" s="25">
-        <v>-18</v>
+        <v>2</v>
       </c>
       <c r="D657" s="29"/>
       <c r="E657" s="28"/>
@@ -13242,16 +13257,16 @@
         <v>662</v>
       </c>
       <c r="B659" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C659" s="25">
-        <v>141.5</v>
+        <v>139.5</v>
       </c>
       <c r="D659" s="26">
         <v>2.83</v>
       </c>
       <c r="E659" s="27">
-        <v>400.47</v>
+        <v>394.81</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.25">
@@ -13275,14 +13290,10 @@
       </c>
       <c r="B661" s="24"/>
       <c r="C661" s="25">
-        <v>502</v>
-      </c>
-      <c r="D661" s="26">
-        <v>0.82</v>
-      </c>
-      <c r="E661" s="27">
-        <v>411.64</v>
-      </c>
+        <v>9.5</v>
+      </c>
+      <c r="D661" s="29"/>
+      <c r="E661" s="28"/>
     </row>
     <row r="662" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A662" s="23" t="s">
@@ -13290,27 +13301,29 @@
       </c>
       <c r="B662" s="24"/>
       <c r="C662" s="25">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D662" s="26">
-        <v>1.1499999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="E662" s="27">
-        <v>575</v>
+        <v>411.64</v>
       </c>
     </row>
     <row r="663" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A663" s="23" t="s">
         <v>666</v>
       </c>
-      <c r="B663" s="24">
-        <v>1</v>
-      </c>
+      <c r="B663" s="24"/>
       <c r="C663" s="25">
-        <v>-0.5</v>
-      </c>
-      <c r="D663" s="29"/>
-      <c r="E663" s="28"/>
+        <v>500</v>
+      </c>
+      <c r="D663" s="26">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E663" s="27">
+        <v>575</v>
+      </c>
     </row>
     <row r="664" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A664" s="23" t="s">
@@ -13319,7 +13332,9 @@
       <c r="B664" s="24">
         <v>1</v>
       </c>
-      <c r="C664" s="28"/>
+      <c r="C664" s="25">
+        <v>-0.5</v>
+      </c>
       <c r="D664" s="29"/>
       <c r="E664" s="28"/>
     </row>
@@ -13328,11 +13343,9 @@
         <v>668</v>
       </c>
       <c r="B665" s="24">
-        <v>2</v>
-      </c>
-      <c r="C665" s="25">
-        <v>-0.02</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C665" s="28"/>
       <c r="D665" s="29"/>
       <c r="E665" s="28"/>
     </row>
@@ -13340,8 +13353,12 @@
       <c r="A666" s="23" t="s">
         <v>669</v>
       </c>
-      <c r="B666" s="24"/>
-      <c r="C666" s="28"/>
+      <c r="B666" s="24">
+        <v>2</v>
+      </c>
+      <c r="C666" s="25">
+        <v>-0.02</v>
+      </c>
       <c r="D666" s="29"/>
       <c r="E666" s="28"/>
     </row>
@@ -13349,12 +13366,8 @@
       <c r="A667" s="23" t="s">
         <v>670</v>
       </c>
-      <c r="B667" s="24">
-        <v>38</v>
-      </c>
-      <c r="C667" s="25">
-        <v>-0.38</v>
-      </c>
+      <c r="B667" s="24"/>
+      <c r="C667" s="28"/>
       <c r="D667" s="29"/>
       <c r="E667" s="28"/>
     </row>
@@ -13363,10 +13376,10 @@
         <v>671</v>
       </c>
       <c r="B668" s="24">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C668" s="25">
-        <v>-0.41</v>
+        <v>-0.38</v>
       </c>
       <c r="D668" s="29"/>
       <c r="E668" s="28"/>
@@ -13376,33 +13389,29 @@
         <v>672</v>
       </c>
       <c r="B669" s="24">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C669" s="25">
-        <v>-90</v>
-      </c>
-      <c r="D669" s="26">
-        <v>1</v>
-      </c>
-      <c r="E669" s="27">
-        <v>-90</v>
-      </c>
+        <v>-0.42</v>
+      </c>
+      <c r="D669" s="29"/>
+      <c r="E669" s="28"/>
     </row>
     <row r="670" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A670" s="23" t="s">
         <v>673</v>
       </c>
       <c r="B670" s="24">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C670" s="25">
-        <v>32.5</v>
+        <v>-90</v>
       </c>
       <c r="D670" s="26">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E670" s="27">
-        <v>81.25</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="671" spans="1:5" x14ac:dyDescent="0.25">
@@ -13410,16 +13419,16 @@
         <v>674</v>
       </c>
       <c r="B671" s="24">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C671" s="25">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D671" s="26">
         <v>2.5</v>
       </c>
       <c r="E671" s="27">
-        <v>87.5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="672" spans="1:5" x14ac:dyDescent="0.25">
@@ -13427,16 +13436,16 @@
         <v>675</v>
       </c>
       <c r="B672" s="24">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C672" s="25">
-        <v>72.75</v>
+        <v>34.5</v>
       </c>
       <c r="D672" s="26">
         <v>2.5</v>
       </c>
       <c r="E672" s="27">
-        <v>181.88</v>
+        <v>86.25</v>
       </c>
     </row>
     <row r="673" spans="1:5" x14ac:dyDescent="0.25">
@@ -13444,16 +13453,16 @@
         <v>676</v>
       </c>
       <c r="B673" s="24">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C673" s="25">
-        <v>73.5</v>
+        <v>71.75</v>
       </c>
       <c r="D673" s="26">
         <v>2.5</v>
       </c>
       <c r="E673" s="27">
-        <v>183.75</v>
+        <v>179.38</v>
       </c>
     </row>
     <row r="674" spans="1:5" x14ac:dyDescent="0.25">
@@ -13461,16 +13470,16 @@
         <v>677</v>
       </c>
       <c r="B674" s="24">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C674" s="25">
-        <v>47</v>
+        <v>73.5</v>
       </c>
       <c r="D674" s="26">
         <v>2.5</v>
       </c>
       <c r="E674" s="27">
-        <v>117.5</v>
+        <v>183.75</v>
       </c>
     </row>
     <row r="675" spans="1:5" x14ac:dyDescent="0.25">
@@ -13478,16 +13487,16 @@
         <v>678</v>
       </c>
       <c r="B675" s="24">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C675" s="25">
-        <v>52.75</v>
+        <v>46.5</v>
       </c>
       <c r="D675" s="26">
         <v>2.5</v>
       </c>
       <c r="E675" s="27">
-        <v>131.88</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="676" spans="1:5" x14ac:dyDescent="0.25">
@@ -13495,16 +13504,16 @@
         <v>679</v>
       </c>
       <c r="B676" s="24">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C676" s="25">
-        <v>40</v>
+        <v>52.75</v>
       </c>
       <c r="D676" s="26">
         <v>2.5</v>
       </c>
       <c r="E676" s="27">
-        <v>100</v>
+        <v>131.88</v>
       </c>
     </row>
     <row r="677" spans="1:5" x14ac:dyDescent="0.25">
@@ -13512,16 +13521,16 @@
         <v>680</v>
       </c>
       <c r="B677" s="24">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C677" s="25">
-        <v>51.75</v>
+        <v>39.25</v>
       </c>
       <c r="D677" s="26">
         <v>2.5</v>
       </c>
       <c r="E677" s="27">
-        <v>129.38</v>
+        <v>98.13</v>
       </c>
     </row>
     <row r="678" spans="1:5" x14ac:dyDescent="0.25">
@@ -13529,16 +13538,16 @@
         <v>681</v>
       </c>
       <c r="B678" s="24">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C678" s="25">
-        <v>84.25</v>
+        <v>51.75</v>
       </c>
       <c r="D678" s="26">
         <v>2.5</v>
       </c>
       <c r="E678" s="27">
-        <v>210.63</v>
+        <v>129.38</v>
       </c>
     </row>
     <row r="679" spans="1:5" x14ac:dyDescent="0.25">
@@ -13546,38 +13555,55 @@
         <v>682</v>
       </c>
       <c r="B679" s="24">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C679" s="25">
-        <v>-26.5</v>
-      </c>
-      <c r="D679" s="29"/>
-      <c r="E679" s="28"/>
+        <v>83.5</v>
+      </c>
+      <c r="D679" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="E679" s="27">
+        <v>208.75</v>
+      </c>
     </row>
     <row r="680" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A680" s="23" t="s">
         <v>683</v>
       </c>
       <c r="B680" s="24">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="C680" s="25">
-        <v>-167.5</v>
+        <v>-26.5</v>
       </c>
       <c r="D680" s="29"/>
       <c r="E680" s="28"/>
     </row>
     <row r="681" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A681" s="30" t="s">
+      <c r="A681" s="23" t="s">
         <v>684</v>
       </c>
-      <c r="B681" s="31"/>
-      <c r="C681" s="32">
-        <v>22707.18</v>
-      </c>
-      <c r="D681" s="33"/>
-      <c r="E681" s="34">
-        <v>88542.74</v>
+      <c r="B681" s="24">
+        <v>61</v>
+      </c>
+      <c r="C681" s="25">
+        <v>-168</v>
+      </c>
+      <c r="D681" s="29"/>
+      <c r="E681" s="28"/>
+    </row>
+    <row r="682" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A682" s="30" t="s">
+        <v>685</v>
+      </c>
+      <c r="B682" s="31"/>
+      <c r="C682" s="32">
+        <v>22091.1</v>
+      </c>
+      <c r="D682" s="33"/>
+      <c r="E682" s="34">
+        <v>85309.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil 03 dec @8.23
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="707">
   <si>
     <t>Order Estimate - (from 1-Jul-2023)</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Stock Group Summary</t>
   </si>
   <si>
-    <t>1-Jul-25 to 1-Dec-25</t>
+    <t>1-Jul-25 to 3-Dec-25</t>
   </si>
   <si>
     <t/>
@@ -1796,6 +1796,12 @@
     <t>9236 CARDS (DCU)</t>
   </si>
   <si>
+    <t>9237 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9238 CARDS (DCU)</t>
+  </si>
+  <si>
     <t>9301 CARDS</t>
   </si>
   <si>
@@ -2093,7 +2099,7 @@
     <t>FANCY SAMPLE SET</t>
   </si>
   <si>
-    <t>Gift Envelope (Pocket) Sr.</t>
+    <t>Gift Envelope (Pocket) SR...</t>
   </si>
   <si>
     <t>INVITATION LOOSE SAMPLES (2025)</t>
@@ -2662,7 +2668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E701"/>
+  <dimension ref="A1:E703"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2994,16 +3000,16 @@
         <v>26</v>
       </c>
       <c r="B23" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="25">
-        <v>53.5</v>
+        <v>43.5</v>
       </c>
       <c r="D23" s="26">
         <v>1.8</v>
       </c>
       <c r="E23" s="27">
-        <v>96.3</v>
+        <v>78.3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3045,16 +3051,16 @@
         <v>29</v>
       </c>
       <c r="B26" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" s="25">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D26" s="26">
         <v>2</v>
       </c>
       <c r="E26" s="27">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3096,16 +3102,16 @@
         <v>32</v>
       </c>
       <c r="B29" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" s="25">
-        <v>50</v>
+        <v>47.5</v>
       </c>
       <c r="D29" s="26">
         <v>2.38</v>
       </c>
       <c r="E29" s="27">
-        <v>119</v>
+        <v>113.05</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3158,16 +3164,16 @@
         <v>36</v>
       </c>
       <c r="B33" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" s="25">
-        <v>16.5</v>
+        <v>11.5</v>
       </c>
       <c r="D33" s="26">
         <v>2.5</v>
       </c>
       <c r="E33" s="27">
-        <v>41.25</v>
+        <v>28.75</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3223,15 +3229,17 @@
       <c r="A37" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="24">
+        <v>1</v>
+      </c>
       <c r="C37" s="25">
-        <v>29.5</v>
+        <v>24.5</v>
       </c>
       <c r="D37" s="26">
         <v>2.76</v>
       </c>
       <c r="E37" s="27">
-        <v>81.42</v>
+        <v>67.62</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3305,16 +3313,16 @@
         <v>45</v>
       </c>
       <c r="B42" s="24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C42" s="25">
-        <v>67.5</v>
+        <v>62.5</v>
       </c>
       <c r="D42" s="26">
         <v>2.35</v>
       </c>
       <c r="E42" s="27">
-        <v>158.63</v>
+        <v>146.88</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3322,16 +3330,16 @@
         <v>46</v>
       </c>
       <c r="B43" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C43" s="25">
-        <v>63.5</v>
+        <v>57</v>
       </c>
       <c r="D43" s="26">
         <v>2.66</v>
       </c>
       <c r="E43" s="27">
-        <v>168.91</v>
+        <v>151.62</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,16 +3415,16 @@
         <v>51</v>
       </c>
       <c r="B48" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C48" s="25">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D48" s="26">
         <v>1.4</v>
       </c>
       <c r="E48" s="27">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,16 +3432,16 @@
         <v>52</v>
       </c>
       <c r="B49" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" s="25">
-        <v>187</v>
+        <v>183.5</v>
       </c>
       <c r="D49" s="26">
         <v>1.4</v>
       </c>
       <c r="E49" s="27">
-        <v>261.8</v>
+        <v>256.89999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3492,16 +3500,16 @@
         <v>56</v>
       </c>
       <c r="B53" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C53" s="25">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D53" s="26">
         <v>2.75</v>
       </c>
       <c r="E53" s="27">
-        <v>112.75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3611,16 +3619,16 @@
         <v>63</v>
       </c>
       <c r="B60" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C60" s="25">
-        <v>305.5</v>
+        <v>300.5</v>
       </c>
       <c r="D60" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E60" s="27">
-        <v>339.11</v>
+        <v>333.56</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3756,16 +3764,16 @@
         <v>72</v>
       </c>
       <c r="B69" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C69" s="25">
-        <v>299.5</v>
+        <v>293.5</v>
       </c>
       <c r="D69" s="26">
         <v>1.4</v>
       </c>
       <c r="E69" s="27">
-        <v>419.3</v>
+        <v>410.9</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3773,16 +3781,16 @@
         <v>73</v>
       </c>
       <c r="B70" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C70" s="25">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D70" s="26">
         <v>1.4</v>
       </c>
       <c r="E70" s="27">
-        <v>418.6</v>
+        <v>414.4</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3824,16 +3832,16 @@
         <v>76</v>
       </c>
       <c r="B73" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C73" s="25">
-        <v>642.5</v>
+        <v>641.5</v>
       </c>
       <c r="D73" s="26">
         <v>1.2</v>
       </c>
       <c r="E73" s="27">
-        <v>771</v>
+        <v>769.8</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3841,16 +3849,16 @@
         <v>77</v>
       </c>
       <c r="B74" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C74" s="25">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>806.4</v>
+        <v>794.4</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3992,16 +4000,16 @@
         <v>86</v>
       </c>
       <c r="B83" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C83" s="25">
-        <v>267</v>
+        <v>167</v>
       </c>
       <c r="D83" s="26">
         <v>1.3</v>
       </c>
       <c r="E83" s="27">
-        <v>347.1</v>
+        <v>217.1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4009,16 +4017,16 @@
         <v>87</v>
       </c>
       <c r="B84" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C84" s="25">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="D84" s="26">
         <v>1.3</v>
       </c>
       <c r="E84" s="27">
-        <v>429</v>
+        <v>364</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4043,16 +4051,16 @@
         <v>89</v>
       </c>
       <c r="B86" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C86" s="25">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D86" s="26">
         <v>1.7</v>
       </c>
       <c r="E86" s="27">
-        <v>30.6</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4077,16 +4085,16 @@
         <v>91</v>
       </c>
       <c r="B88" s="24">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C88" s="25">
-        <v>10</v>
+        <v>-85</v>
       </c>
       <c r="D88" s="26">
         <v>0.64</v>
       </c>
       <c r="E88" s="27">
-        <v>6.43</v>
+        <v>-54.68</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4094,16 +4102,16 @@
         <v>92</v>
       </c>
       <c r="B89" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C89" s="25">
-        <v>94.7</v>
+        <v>64.7</v>
       </c>
       <c r="D89" s="26">
         <v>0.52</v>
       </c>
       <c r="E89" s="27">
-        <v>49.08</v>
+        <v>33.53</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4165,7 +4173,7 @@
         <v>7</v>
       </c>
       <c r="C93" s="25">
-        <v>-25</v>
+        <v>447</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="28"/>
@@ -4178,7 +4186,7 @@
         <v>6</v>
       </c>
       <c r="C94" s="25">
-        <v>-38</v>
+        <v>902</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="28"/>
@@ -4191,7 +4199,7 @@
         <v>4</v>
       </c>
       <c r="C95" s="25">
-        <v>-9</v>
+        <v>461</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="28"/>
@@ -4275,16 +4283,16 @@
         <v>105</v>
       </c>
       <c r="B102" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C102" s="25">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D102" s="26">
         <v>2.5</v>
       </c>
       <c r="E102" s="27">
-        <v>127.5</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4309,16 +4317,16 @@
         <v>107</v>
       </c>
       <c r="B104" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C104" s="25">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D104" s="26">
         <v>2.5</v>
       </c>
       <c r="E104" s="27">
-        <v>220</v>
+        <v>195</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -4326,16 +4334,16 @@
         <v>108</v>
       </c>
       <c r="B105" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C105" s="25">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D105" s="26">
         <v>2.5</v>
       </c>
       <c r="E105" s="27">
-        <v>175</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4385,7 +4393,9 @@
       <c r="A109" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B109" s="24"/>
+      <c r="B109" s="24">
+        <v>5</v>
+      </c>
       <c r="C109" s="28"/>
       <c r="D109" s="29"/>
       <c r="E109" s="28"/>
@@ -4394,8 +4404,12 @@
       <c r="A110" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B110" s="24"/>
-      <c r="C110" s="28"/>
+      <c r="B110" s="24">
+        <v>2</v>
+      </c>
+      <c r="C110" s="25">
+        <v>26</v>
+      </c>
       <c r="D110" s="29"/>
       <c r="E110" s="28"/>
     </row>
@@ -4403,8 +4417,12 @@
       <c r="A111" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="28"/>
+      <c r="B111" s="24">
+        <v>2</v>
+      </c>
+      <c r="C111" s="25">
+        <v>26</v>
+      </c>
       <c r="D111" s="29"/>
       <c r="E111" s="28"/>
     </row>
@@ -4412,8 +4430,12 @@
       <c r="A112" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="B112" s="24"/>
-      <c r="C112" s="28"/>
+      <c r="B112" s="24">
+        <v>4</v>
+      </c>
+      <c r="C112" s="25">
+        <v>10</v>
+      </c>
       <c r="D112" s="29"/>
       <c r="E112" s="28"/>
     </row>
@@ -4422,16 +4444,16 @@
         <v>116</v>
       </c>
       <c r="B113" s="24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C113" s="25">
-        <v>391.5</v>
+        <v>366.5</v>
       </c>
       <c r="D113" s="26">
         <v>0.7</v>
       </c>
       <c r="E113" s="27">
-        <v>274.05</v>
+        <v>256.55</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4452,10 +4474,10 @@
         <v>118</v>
       </c>
       <c r="B115" s="24">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C115" s="25">
-        <v>-0.2</v>
+        <v>-0.23</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="28"/>
@@ -4465,10 +4487,10 @@
         <v>119</v>
       </c>
       <c r="B116" s="24">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C116" s="25">
-        <v>-0.39</v>
+        <v>-0.4</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="28"/>
@@ -4487,10 +4509,10 @@
         <v>121</v>
       </c>
       <c r="B118" s="24">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C118" s="25">
-        <v>-1.44</v>
+        <v>-1.51</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="28"/>
@@ -4500,10 +4522,10 @@
         <v>122</v>
       </c>
       <c r="B119" s="24">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C119" s="25">
-        <v>-2.09</v>
+        <v>-2.17</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="28"/>
@@ -4663,16 +4685,16 @@
         <v>133</v>
       </c>
       <c r="B130" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C130" s="25">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D130" s="26">
         <v>12.5</v>
       </c>
       <c r="E130" s="27">
-        <v>137.5</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4714,16 +4736,16 @@
         <v>136</v>
       </c>
       <c r="B133" s="24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C133" s="25">
-        <v>11</v>
+        <v>5.5</v>
       </c>
       <c r="D133" s="26">
         <v>13.07</v>
       </c>
       <c r="E133" s="27">
-        <v>143.79</v>
+        <v>71.89</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4865,16 +4887,16 @@
         <v>145</v>
       </c>
       <c r="B142" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C142" s="25">
-        <v>18.5</v>
+        <v>19</v>
       </c>
       <c r="D142" s="26">
         <v>18.5</v>
       </c>
       <c r="E142" s="27">
-        <v>342.25</v>
+        <v>351.5</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4933,16 +4955,16 @@
         <v>149</v>
       </c>
       <c r="B146" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C146" s="25">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="D146" s="26">
         <v>18.5</v>
       </c>
       <c r="E146" s="27">
-        <v>157.25</v>
+        <v>138.75</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4967,16 +4989,16 @@
         <v>151</v>
       </c>
       <c r="B148" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C148" s="25">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D148" s="26">
         <v>11.5</v>
       </c>
       <c r="E148" s="27">
-        <v>310.5</v>
+        <v>253</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -5580,13 +5602,13 @@
         <v>13</v>
       </c>
       <c r="C186" s="25">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D186" s="26">
         <v>5</v>
       </c>
       <c r="E186" s="27">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5662,16 +5684,16 @@
         <v>194</v>
       </c>
       <c r="B191" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C191" s="25">
-        <v>50</v>
+        <v>47.5</v>
       </c>
       <c r="D191" s="26">
         <v>4.5</v>
       </c>
       <c r="E191" s="27">
-        <v>225</v>
+        <v>213.75</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5792,16 +5814,16 @@
         <v>202</v>
       </c>
       <c r="B199" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C199" s="25">
-        <v>60.5</v>
+        <v>58</v>
       </c>
       <c r="D199" s="26">
         <v>2.6</v>
       </c>
       <c r="E199" s="27">
-        <v>157.30000000000001</v>
+        <v>150.80000000000001</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5820,16 +5842,16 @@
         <v>204</v>
       </c>
       <c r="B201" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C201" s="25">
-        <v>62.5</v>
+        <v>58.5</v>
       </c>
       <c r="D201" s="26">
         <v>3.5</v>
       </c>
       <c r="E201" s="27">
-        <v>218.75</v>
+        <v>204.75</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5854,16 +5876,16 @@
         <v>206</v>
       </c>
       <c r="B203" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C203" s="25">
-        <v>41.5</v>
+        <v>37.5</v>
       </c>
       <c r="D203" s="26">
         <v>3.89</v>
       </c>
       <c r="E203" s="27">
-        <v>161.46</v>
+        <v>145.88999999999999</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5888,16 +5910,16 @@
         <v>208</v>
       </c>
       <c r="B205" s="24">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C205" s="25">
-        <v>234</v>
+        <v>232.5</v>
       </c>
       <c r="D205" s="26">
         <v>2.7</v>
       </c>
       <c r="E205" s="27">
-        <v>631.79999999999995</v>
+        <v>627.75</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5905,16 +5927,16 @@
         <v>209</v>
       </c>
       <c r="B206" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C206" s="25">
-        <v>197.5</v>
+        <v>192.5</v>
       </c>
       <c r="D206" s="26">
         <v>2.7</v>
       </c>
       <c r="E206" s="27">
-        <v>533.25</v>
+        <v>519.75</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -6058,16 +6080,16 @@
         <v>218</v>
       </c>
       <c r="B215" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C215" s="25">
-        <v>59.72</v>
+        <v>58.72</v>
       </c>
       <c r="D215" s="26">
         <v>3.16</v>
       </c>
       <c r="E215" s="27">
-        <v>188.72</v>
+        <v>185.56</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -6075,16 +6097,16 @@
         <v>219</v>
       </c>
       <c r="B216" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C216" s="25">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D216" s="26">
         <v>2.66</v>
       </c>
       <c r="E216" s="27">
-        <v>289.94</v>
+        <v>287.27999999999997</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -6109,16 +6131,16 @@
         <v>221</v>
       </c>
       <c r="B218" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C218" s="25">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D218" s="26">
         <v>4</v>
       </c>
       <c r="E218" s="27">
-        <v>528</v>
+        <v>508</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -6205,16 +6227,16 @@
         <v>227</v>
       </c>
       <c r="B224" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C224" s="25">
-        <v>89.5</v>
+        <v>89</v>
       </c>
       <c r="D224" s="26">
         <v>3.25</v>
       </c>
       <c r="E224" s="27">
-        <v>290.88</v>
+        <v>289.25</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6314,7 +6336,9 @@
         <v>234</v>
       </c>
       <c r="B231" s="24"/>
-      <c r="C231" s="28"/>
+      <c r="C231" s="25">
+        <v>15</v>
+      </c>
       <c r="D231" s="29"/>
       <c r="E231" s="28"/>
     </row>
@@ -6323,7 +6347,9 @@
         <v>235</v>
       </c>
       <c r="B232" s="24"/>
-      <c r="C232" s="28"/>
+      <c r="C232" s="25">
+        <v>25</v>
+      </c>
       <c r="D232" s="29"/>
       <c r="E232" s="28"/>
     </row>
@@ -6332,7 +6358,9 @@
         <v>236</v>
       </c>
       <c r="B233" s="24"/>
-      <c r="C233" s="28"/>
+      <c r="C233" s="25">
+        <v>25</v>
+      </c>
       <c r="D233" s="29"/>
       <c r="E233" s="28"/>
     </row>
@@ -6341,16 +6369,16 @@
         <v>237</v>
       </c>
       <c r="B234" s="24">
+        <v>16</v>
+      </c>
+      <c r="C234" s="25">
         <v>14</v>
-      </c>
-      <c r="C234" s="25">
-        <v>20</v>
       </c>
       <c r="D234" s="26">
         <v>8.25</v>
       </c>
       <c r="E234" s="27">
-        <v>165</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -6375,16 +6403,16 @@
         <v>239</v>
       </c>
       <c r="B236" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C236" s="25">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D236" s="26">
         <v>4.8</v>
       </c>
       <c r="E236" s="27">
-        <v>240</v>
+        <v>230.4</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -6409,16 +6437,16 @@
         <v>241</v>
       </c>
       <c r="B238" s="24">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C238" s="25">
-        <v>42.5</v>
+        <v>37.5</v>
       </c>
       <c r="D238" s="26">
         <v>3</v>
       </c>
       <c r="E238" s="27">
-        <v>127.5</v>
+        <v>112.5</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -6460,16 +6488,16 @@
         <v>244</v>
       </c>
       <c r="B241" s="24">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C241" s="25">
-        <v>169.5</v>
+        <v>162.5</v>
       </c>
       <c r="D241" s="26">
         <v>3.9</v>
       </c>
       <c r="E241" s="27">
-        <v>661.05</v>
+        <v>633.75</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6477,16 +6505,16 @@
         <v>245</v>
       </c>
       <c r="B242" s="24">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C242" s="25">
-        <v>145</v>
+        <v>143.5</v>
       </c>
       <c r="D242" s="26">
         <v>3.9</v>
       </c>
       <c r="E242" s="27">
-        <v>565.5</v>
+        <v>559.65</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6575,16 +6603,16 @@
         <v>251</v>
       </c>
       <c r="B248" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C248" s="25">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D248" s="26">
         <v>3.5</v>
       </c>
       <c r="E248" s="27">
-        <v>164.5</v>
+        <v>154</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6767,16 +6795,16 @@
         <v>263</v>
       </c>
       <c r="B260" s="24">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C260" s="25">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D260" s="26">
         <v>3.1</v>
       </c>
       <c r="E260" s="27">
-        <v>145.69999999999999</v>
+        <v>120.9</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -7004,16 +7032,16 @@
         <v>278</v>
       </c>
       <c r="B275" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C275" s="25">
-        <v>65.5</v>
+        <v>63.5</v>
       </c>
       <c r="D275" s="26">
         <v>6.18</v>
       </c>
       <c r="E275" s="27">
-        <v>404.81</v>
+        <v>392.45</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -7055,16 +7083,16 @@
         <v>281</v>
       </c>
       <c r="B278" s="24">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C278" s="25">
-        <v>14.5</v>
+        <v>8.5</v>
       </c>
       <c r="D278" s="26">
         <v>5</v>
       </c>
       <c r="E278" s="27">
-        <v>72.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -7106,16 +7134,16 @@
         <v>284</v>
       </c>
       <c r="B281" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C281" s="25">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D281" s="26">
         <v>4.63</v>
       </c>
       <c r="E281" s="27">
-        <v>157.25</v>
+        <v>143.38</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -7223,16 +7251,16 @@
         <v>291</v>
       </c>
       <c r="B288" s="24">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C288" s="25">
-        <v>125.5</v>
+        <v>125</v>
       </c>
       <c r="D288" s="26">
         <v>6</v>
       </c>
       <c r="E288" s="27">
-        <v>752.94</v>
+        <v>749.94</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -7762,16 +7790,16 @@
         <v>324</v>
       </c>
       <c r="B321" s="24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C321" s="25">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D321" s="26">
         <v>4.28</v>
       </c>
       <c r="E321" s="27">
-        <v>475.08</v>
+        <v>449.4</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
@@ -7860,16 +7888,16 @@
         <v>330</v>
       </c>
       <c r="B327" s="24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C327" s="25">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D327" s="26">
         <v>9</v>
       </c>
       <c r="E327" s="27">
-        <v>342</v>
+        <v>252</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -7928,16 +7956,16 @@
         <v>334</v>
       </c>
       <c r="B331" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C331" s="25">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D331" s="26">
         <v>9</v>
       </c>
       <c r="E331" s="27">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -7945,16 +7973,16 @@
         <v>335</v>
       </c>
       <c r="B332" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C332" s="25">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D332" s="26">
         <v>9</v>
       </c>
       <c r="E332" s="27">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -8225,13 +8253,13 @@
         <v>15</v>
       </c>
       <c r="C349" s="25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D349" s="26">
         <v>7.82</v>
       </c>
       <c r="E349" s="27">
-        <v>70.34</v>
+        <v>54.71</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -8358,16 +8386,16 @@
         <v>360</v>
       </c>
       <c r="B357" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C357" s="25">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D357" s="26">
         <v>7.2</v>
       </c>
       <c r="E357" s="27">
-        <v>180</v>
+        <v>165.6</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -8429,13 +8457,13 @@
         <v>34</v>
       </c>
       <c r="C361" s="25">
-        <v>65.5</v>
+        <v>259</v>
       </c>
       <c r="D361" s="26">
         <v>6.6</v>
       </c>
       <c r="E361" s="27">
-        <v>432.3</v>
+        <v>1709.4</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -8766,16 +8794,16 @@
         <v>384</v>
       </c>
       <c r="B381" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C381" s="25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D381" s="26">
         <v>5.7</v>
       </c>
       <c r="E381" s="27">
-        <v>131.1</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
@@ -8973,16 +9001,16 @@
         <v>397</v>
       </c>
       <c r="B394" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C394" s="25">
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="D394" s="26">
         <v>6.65</v>
       </c>
       <c r="E394" s="27">
-        <v>136.33000000000001</v>
+        <v>116.38</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
@@ -9150,16 +9178,16 @@
         <v>408</v>
       </c>
       <c r="B405" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C405" s="25">
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="D405" s="26">
         <v>8</v>
       </c>
       <c r="E405" s="27">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
@@ -9257,16 +9285,16 @@
         <v>415</v>
       </c>
       <c r="B412" s="24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C412" s="25">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D412" s="26">
         <v>6.46</v>
       </c>
       <c r="E412" s="27">
-        <v>142.12</v>
+        <v>116.28</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
@@ -9515,16 +9543,16 @@
         <v>431</v>
       </c>
       <c r="B428" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C428" s="25">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D428" s="26">
         <v>8.75</v>
       </c>
       <c r="E428" s="27">
-        <v>192.5</v>
+        <v>183.75</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -9532,16 +9560,16 @@
         <v>432</v>
       </c>
       <c r="B429" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C429" s="25">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D429" s="26">
         <v>9.75</v>
       </c>
       <c r="E429" s="27">
-        <v>146.25</v>
+        <v>136.5</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -9549,16 +9577,16 @@
         <v>433</v>
       </c>
       <c r="B430" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C430" s="25">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="D430" s="26">
         <v>15.5</v>
       </c>
       <c r="E430" s="27">
-        <v>124</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
@@ -9651,7 +9679,7 @@
         <v>439</v>
       </c>
       <c r="B436" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C436" s="25">
         <v>-0.5</v>
@@ -9853,16 +9881,16 @@
         <v>451</v>
       </c>
       <c r="B448" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C448" s="25">
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
       <c r="D448" s="26">
         <v>10.5</v>
       </c>
       <c r="E448" s="27">
-        <v>215.25</v>
+        <v>204.75</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -9902,16 +9930,16 @@
         <v>454</v>
       </c>
       <c r="B451" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C451" s="25">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="D451" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E451" s="27">
-        <v>76.95</v>
+        <v>64.13</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
@@ -10017,16 +10045,16 @@
         <v>461</v>
       </c>
       <c r="B458" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C458" s="25">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D458" s="26">
         <v>11.2</v>
       </c>
       <c r="E458" s="27">
-        <v>190.4</v>
+        <v>179.2</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -10196,16 +10224,16 @@
         <v>472</v>
       </c>
       <c r="B469" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C469" s="25">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="D469" s="26">
         <v>11.4</v>
       </c>
       <c r="E469" s="27">
-        <v>74.099999999999994</v>
+        <v>91.2</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
@@ -10213,16 +10241,16 @@
         <v>473</v>
       </c>
       <c r="B470" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C470" s="25">
-        <v>11.5</v>
+        <v>8.5</v>
       </c>
       <c r="D470" s="26">
         <v>11.88</v>
       </c>
       <c r="E470" s="27">
-        <v>136.62</v>
+        <v>100.98</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
@@ -10464,16 +10492,16 @@
         <v>488</v>
       </c>
       <c r="B485" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C485" s="25">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D485" s="26">
         <v>13.39</v>
       </c>
       <c r="E485" s="27">
-        <v>308.01</v>
+        <v>281.22000000000003</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
@@ -10481,16 +10509,16 @@
         <v>489</v>
       </c>
       <c r="B486" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C486" s="25">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D486" s="26">
         <v>9</v>
       </c>
       <c r="E486" s="27">
-        <v>243</v>
+        <v>225</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
@@ -10643,16 +10671,16 @@
         <v>499</v>
       </c>
       <c r="B496" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C496" s="25">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="D496" s="26">
         <v>10.17</v>
       </c>
       <c r="E496" s="27">
-        <v>86.42</v>
+        <v>76.25</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -10690,16 +10718,16 @@
         <v>502</v>
       </c>
       <c r="B499" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C499" s="25">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="D499" s="26">
         <v>29</v>
       </c>
       <c r="E499" s="27">
-        <v>217.5</v>
+        <v>188.5</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10854,16 +10882,16 @@
         <v>512</v>
       </c>
       <c r="B509" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C509" s="25">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D509" s="26">
         <v>5.23</v>
       </c>
       <c r="E509" s="27">
-        <v>57.53</v>
+        <v>31.38</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10973,16 +11001,16 @@
         <v>519</v>
       </c>
       <c r="B516" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C516" s="25">
-        <v>64.5</v>
+        <v>63.5</v>
       </c>
       <c r="D516" s="26">
         <v>1.95</v>
       </c>
       <c r="E516" s="27">
-        <v>125.78</v>
+        <v>123.83</v>
       </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.25">
@@ -11007,16 +11035,16 @@
         <v>521</v>
       </c>
       <c r="B518" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C518" s="25">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D518" s="26">
         <v>2.1</v>
       </c>
       <c r="E518" s="27">
-        <v>161.69999999999999</v>
+        <v>147</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
@@ -11041,16 +11069,16 @@
         <v>523</v>
       </c>
       <c r="B520" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C520" s="25">
-        <v>66</v>
+        <v>63.5</v>
       </c>
       <c r="D520" s="26">
         <v>3.8</v>
       </c>
       <c r="E520" s="27">
-        <v>250.8</v>
+        <v>241.3</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
@@ -11150,16 +11178,16 @@
         <v>530</v>
       </c>
       <c r="B527" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C527" s="25">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="D527" s="26">
         <v>1.8</v>
       </c>
       <c r="E527" s="27">
-        <v>5.4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
@@ -11184,16 +11212,16 @@
         <v>532</v>
       </c>
       <c r="B529" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C529" s="25">
-        <v>43.5</v>
+        <v>40.5</v>
       </c>
       <c r="D529" s="26">
         <v>4.28</v>
       </c>
       <c r="E529" s="27">
-        <v>186.18</v>
+        <v>173.34</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -11201,16 +11229,16 @@
         <v>533</v>
       </c>
       <c r="B530" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C530" s="25">
-        <v>35.5</v>
+        <v>30.5</v>
       </c>
       <c r="D530" s="26">
         <v>4.28</v>
       </c>
       <c r="E530" s="27">
-        <v>151.94</v>
+        <v>130.54</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
@@ -11269,16 +11297,16 @@
         <v>537</v>
       </c>
       <c r="B534" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C534" s="25">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D534" s="26">
         <v>4.75</v>
       </c>
       <c r="E534" s="27">
-        <v>152</v>
+        <v>147.25</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -11320,16 +11348,16 @@
         <v>540</v>
       </c>
       <c r="B537" s="24">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C537" s="25">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D537" s="26">
         <v>4.75</v>
       </c>
       <c r="E537" s="27">
-        <v>61.75</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
@@ -11354,16 +11382,16 @@
         <v>542</v>
       </c>
       <c r="B539" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C539" s="25">
-        <v>26.5</v>
+        <v>24.5</v>
       </c>
       <c r="D539" s="26">
         <v>3.1</v>
       </c>
       <c r="E539" s="27">
-        <v>82.15</v>
+        <v>75.95</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.25">
@@ -11388,16 +11416,16 @@
         <v>544</v>
       </c>
       <c r="B541" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C541" s="25">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D541" s="26">
         <v>2.8</v>
       </c>
       <c r="E541" s="27">
-        <v>39.200000000000003</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
@@ -11405,16 +11433,16 @@
         <v>545</v>
       </c>
       <c r="B542" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C542" s="25">
-        <v>31.5</v>
+        <v>29.5</v>
       </c>
       <c r="D542" s="26">
         <v>2.38</v>
       </c>
       <c r="E542" s="27">
-        <v>74.97</v>
+        <v>70.209999999999994</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">
@@ -11422,16 +11450,16 @@
         <v>546</v>
       </c>
       <c r="B543" s="24">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C543" s="25">
-        <v>41.5</v>
+        <v>38.5</v>
       </c>
       <c r="D543" s="26">
         <v>3.9</v>
       </c>
       <c r="E543" s="27">
-        <v>161.85</v>
+        <v>150.15</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
@@ -11490,16 +11518,16 @@
         <v>550</v>
       </c>
       <c r="B547" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C547" s="25">
-        <v>27.5</v>
+        <v>26</v>
       </c>
       <c r="D547" s="26">
         <v>2.85</v>
       </c>
       <c r="E547" s="27">
-        <v>78.38</v>
+        <v>74.099999999999994</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
@@ -11660,16 +11688,16 @@
         <v>560</v>
       </c>
       <c r="B557" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C557" s="25">
-        <v>51.5</v>
+        <v>46.5</v>
       </c>
       <c r="D557" s="26">
         <v>2.14</v>
       </c>
       <c r="E557" s="27">
-        <v>110.21</v>
+        <v>99.51</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.25">
@@ -11694,16 +11722,16 @@
         <v>562</v>
       </c>
       <c r="B559" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C559" s="25">
-        <v>61.5</v>
+        <v>56.5</v>
       </c>
       <c r="D559" s="26">
         <v>2.66</v>
       </c>
       <c r="E559" s="27">
-        <v>163.59</v>
+        <v>150.29</v>
       </c>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.25">
@@ -11792,16 +11820,16 @@
         <v>568</v>
       </c>
       <c r="B565" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C565" s="25">
-        <v>215.5</v>
+        <v>211.5</v>
       </c>
       <c r="D565" s="26">
         <v>1.4</v>
       </c>
       <c r="E565" s="27">
-        <v>301.7</v>
+        <v>296.10000000000002</v>
       </c>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.25">
@@ -11878,7 +11906,7 @@
         <v>32</v>
       </c>
       <c r="C570" s="25">
-        <v>-132</v>
+        <v>357</v>
       </c>
       <c r="D570" s="29"/>
       <c r="E570" s="28"/>
@@ -11888,10 +11916,10 @@
         <v>574</v>
       </c>
       <c r="B571" s="24">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C571" s="25">
-        <v>493.5</v>
+        <v>476.5</v>
       </c>
       <c r="D571" s="29"/>
       <c r="E571" s="28"/>
@@ -11917,7 +11945,7 @@
         <v>10</v>
       </c>
       <c r="C573" s="25">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="D573" s="29"/>
       <c r="E573" s="28"/>
@@ -11930,7 +11958,7 @@
         <v>23</v>
       </c>
       <c r="C574" s="25">
-        <v>121.4</v>
+        <v>201.4</v>
       </c>
       <c r="D574" s="29"/>
       <c r="E574" s="28"/>
@@ -11974,16 +12002,16 @@
         <v>580</v>
       </c>
       <c r="B577" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C577" s="25">
-        <v>579.5</v>
+        <v>569.5</v>
       </c>
       <c r="D577" s="26">
         <v>0.85</v>
       </c>
       <c r="E577" s="27">
-        <v>492.58</v>
+        <v>484.08</v>
       </c>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
@@ -12008,16 +12036,16 @@
         <v>582</v>
       </c>
       <c r="B579" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C579" s="25">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="D579" s="26">
         <v>0.85</v>
       </c>
       <c r="E579" s="27">
-        <v>498.1</v>
+        <v>489.6</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -12041,8 +12069,12 @@
       <c r="A581" s="23" t="s">
         <v>584</v>
       </c>
-      <c r="B581" s="24"/>
-      <c r="C581" s="28"/>
+      <c r="B581" s="24">
+        <v>6</v>
+      </c>
+      <c r="C581" s="25">
+        <v>22</v>
+      </c>
       <c r="D581" s="29"/>
       <c r="E581" s="28"/>
     </row>
@@ -12050,8 +12082,12 @@
       <c r="A582" s="23" t="s">
         <v>585</v>
       </c>
-      <c r="B582" s="24"/>
-      <c r="C582" s="28"/>
+      <c r="B582" s="24">
+        <v>7</v>
+      </c>
+      <c r="C582" s="25">
+        <v>8</v>
+      </c>
       <c r="D582" s="29"/>
       <c r="E582" s="28"/>
     </row>
@@ -12059,8 +12095,12 @@
       <c r="A583" s="23" t="s">
         <v>586</v>
       </c>
-      <c r="B583" s="24"/>
-      <c r="C583" s="28"/>
+      <c r="B583" s="24">
+        <v>6</v>
+      </c>
+      <c r="C583" s="25">
+        <v>14</v>
+      </c>
       <c r="D583" s="29"/>
       <c r="E583" s="28"/>
     </row>
@@ -12068,8 +12108,12 @@
       <c r="A584" s="23" t="s">
         <v>587</v>
       </c>
-      <c r="B584" s="24"/>
-      <c r="C584" s="28"/>
+      <c r="B584" s="24">
+        <v>6</v>
+      </c>
+      <c r="C584" s="25">
+        <v>18</v>
+      </c>
       <c r="D584" s="29"/>
       <c r="E584" s="28"/>
     </row>
@@ -12077,8 +12121,12 @@
       <c r="A585" s="23" t="s">
         <v>588</v>
       </c>
-      <c r="B585" s="24"/>
-      <c r="C585" s="28"/>
+      <c r="B585" s="24">
+        <v>4</v>
+      </c>
+      <c r="C585" s="25">
+        <v>30</v>
+      </c>
       <c r="D585" s="29"/>
       <c r="E585" s="28"/>
     </row>
@@ -12086,8 +12134,12 @@
       <c r="A586" s="23" t="s">
         <v>589</v>
       </c>
-      <c r="B586" s="24"/>
-      <c r="C586" s="28"/>
+      <c r="B586" s="24">
+        <v>5</v>
+      </c>
+      <c r="C586" s="25">
+        <v>24</v>
+      </c>
       <c r="D586" s="29"/>
       <c r="E586" s="28"/>
     </row>
@@ -12095,49 +12147,39 @@
       <c r="A587" s="23" t="s">
         <v>590</v>
       </c>
-      <c r="B587" s="24"/>
+      <c r="B587" s="24">
+        <v>1</v>
+      </c>
       <c r="C587" s="25">
-        <v>13</v>
-      </c>
-      <c r="D587" s="26">
-        <v>5.25</v>
-      </c>
-      <c r="E587" s="27">
-        <v>68.25</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D587" s="29"/>
+      <c r="E587" s="28"/>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A588" s="23" t="s">
         <v>591</v>
       </c>
       <c r="B588" s="24">
-        <v>5</v>
-      </c>
-      <c r="C588" s="25">
-        <v>8</v>
-      </c>
-      <c r="D588" s="26">
-        <v>5.5</v>
-      </c>
-      <c r="E588" s="27">
-        <v>44</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C588" s="28"/>
+      <c r="D588" s="29"/>
+      <c r="E588" s="28"/>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A589" s="23" t="s">
         <v>592</v>
       </c>
-      <c r="B589" s="24">
-        <v>3</v>
-      </c>
+      <c r="B589" s="24"/>
       <c r="C589" s="25">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D589" s="26">
-        <v>8.25</v>
+        <v>5.25</v>
       </c>
       <c r="E589" s="27">
-        <v>41.25</v>
+        <v>68.25</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -12145,16 +12187,16 @@
         <v>593</v>
       </c>
       <c r="B590" s="24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C590" s="25">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="D590" s="26">
-        <v>8.25</v>
+        <v>5.5</v>
       </c>
       <c r="E590" s="27">
-        <v>61.88</v>
+        <v>44</v>
       </c>
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
@@ -12162,16 +12204,16 @@
         <v>594</v>
       </c>
       <c r="B591" s="24">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C591" s="25">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D591" s="26">
-        <v>10</v>
+        <v>8.25</v>
       </c>
       <c r="E591" s="27">
-        <v>240</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
@@ -12179,16 +12221,16 @@
         <v>595</v>
       </c>
       <c r="B592" s="24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C592" s="25">
-        <v>38</v>
+        <v>7.5</v>
       </c>
       <c r="D592" s="26">
-        <v>5.5</v>
+        <v>8.25</v>
       </c>
       <c r="E592" s="27">
-        <v>209</v>
+        <v>61.88</v>
       </c>
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.25">
@@ -12196,16 +12238,16 @@
         <v>596</v>
       </c>
       <c r="B593" s="24">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C593" s="25">
-        <v>12.5</v>
+        <v>24</v>
       </c>
       <c r="D593" s="26">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E593" s="27">
-        <v>62.5</v>
+        <v>240</v>
       </c>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
@@ -12213,16 +12255,16 @@
         <v>597</v>
       </c>
       <c r="B594" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C594" s="25">
-        <v>12.01</v>
+        <v>38</v>
       </c>
       <c r="D594" s="26">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="E594" s="27">
-        <v>54.05</v>
+        <v>209</v>
       </c>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
@@ -12230,16 +12272,16 @@
         <v>598</v>
       </c>
       <c r="B595" s="24">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C595" s="25">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="D595" s="26">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="E595" s="27">
-        <v>87.5</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
@@ -12247,16 +12289,16 @@
         <v>599</v>
       </c>
       <c r="B596" s="24">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C596" s="25">
-        <v>34</v>
+        <v>12.01</v>
       </c>
       <c r="D596" s="26">
-        <v>5.75</v>
+        <v>4.5</v>
       </c>
       <c r="E596" s="27">
-        <v>195.5</v>
+        <v>54.05</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
@@ -12264,16 +12306,16 @@
         <v>600</v>
       </c>
       <c r="B597" s="24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C597" s="25">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D597" s="26">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="E597" s="27">
-        <v>80</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -12281,16 +12323,16 @@
         <v>601</v>
       </c>
       <c r="B598" s="24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C598" s="25">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D598" s="26">
-        <v>6.5</v>
+        <v>5.75</v>
       </c>
       <c r="E598" s="27">
-        <v>6.5</v>
+        <v>195.5</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -12298,16 +12340,16 @@
         <v>602</v>
       </c>
       <c r="B599" s="24">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C599" s="25">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D599" s="26">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="E599" s="27">
-        <v>45.5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -12315,16 +12357,16 @@
         <v>603</v>
       </c>
       <c r="B600" s="24">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C600" s="25">
-        <v>67</v>
+        <v>-1.5</v>
       </c>
       <c r="D600" s="26">
-        <v>2.75</v>
+        <v>6.5</v>
       </c>
       <c r="E600" s="27">
-        <v>184.06</v>
+        <v>-9.75</v>
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
@@ -12335,13 +12377,13 @@
         <v>2</v>
       </c>
       <c r="C601" s="25">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="D601" s="26">
-        <v>2.66</v>
+        <v>6.5</v>
       </c>
       <c r="E601" s="27">
-        <v>6.65</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -12349,16 +12391,16 @@
         <v>605</v>
       </c>
       <c r="B602" s="24">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C602" s="25">
-        <v>4.5</v>
+        <v>67</v>
       </c>
       <c r="D602" s="26">
-        <v>2.66</v>
+        <v>2.75</v>
       </c>
       <c r="E602" s="27">
-        <v>11.97</v>
+        <v>184.06</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -12366,16 +12408,16 @@
         <v>606</v>
       </c>
       <c r="B603" s="24">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C603" s="25">
-        <v>75</v>
+        <v>2.5</v>
       </c>
       <c r="D603" s="26">
-        <v>2.71</v>
+        <v>2.66</v>
       </c>
       <c r="E603" s="27">
-        <v>203.16</v>
+        <v>6.65</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
@@ -12383,16 +12425,16 @@
         <v>607</v>
       </c>
       <c r="B604" s="24">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C604" s="25">
-        <v>54</v>
+        <v>4.5</v>
       </c>
       <c r="D604" s="26">
-        <v>4</v>
+        <v>2.66</v>
       </c>
       <c r="E604" s="27">
-        <v>216</v>
+        <v>11.97</v>
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
@@ -12400,16 +12442,16 @@
         <v>608</v>
       </c>
       <c r="B605" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C605" s="25">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="D605" s="26">
-        <v>4</v>
+        <v>2.71</v>
       </c>
       <c r="E605" s="27">
-        <v>4</v>
+        <v>203.16</v>
       </c>
     </row>
     <row r="606" spans="1:5" x14ac:dyDescent="0.25">
@@ -12420,13 +12462,13 @@
         <v>14</v>
       </c>
       <c r="C606" s="25">
-        <v>52.5</v>
+        <v>54</v>
       </c>
       <c r="D606" s="26">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="E606" s="27">
-        <v>78.75</v>
+        <v>216</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12434,16 +12476,16 @@
         <v>610</v>
       </c>
       <c r="B607" s="24">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C607" s="25">
-        <v>10.5</v>
+        <v>-1</v>
       </c>
       <c r="D607" s="26">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="E607" s="27">
-        <v>15.75</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
@@ -12451,16 +12493,16 @@
         <v>611</v>
       </c>
       <c r="B608" s="24">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C608" s="25">
-        <v>10.75</v>
+        <v>51.5</v>
       </c>
       <c r="D608" s="26">
         <v>1.5</v>
       </c>
       <c r="E608" s="27">
-        <v>16.13</v>
+        <v>77.25</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
@@ -12468,16 +12510,16 @@
         <v>612</v>
       </c>
       <c r="B609" s="24">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C609" s="25">
-        <v>22.5</v>
+        <v>10.5</v>
       </c>
       <c r="D609" s="26">
-        <v>2.2799999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="E609" s="27">
-        <v>51.3</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.25">
@@ -12485,16 +12527,16 @@
         <v>613</v>
       </c>
       <c r="B610" s="24">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C610" s="25">
-        <v>58</v>
+        <v>8.75</v>
       </c>
       <c r="D610" s="26">
-        <v>2.2799999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="E610" s="27">
-        <v>132.24</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.25">
@@ -12502,16 +12544,16 @@
         <v>614</v>
       </c>
       <c r="B611" s="24">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C611" s="25">
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="D611" s="26">
-        <v>5</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="E611" s="27">
-        <v>75</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.25">
@@ -12519,27 +12561,33 @@
         <v>615</v>
       </c>
       <c r="B612" s="24">
-        <v>2</v>
-      </c>
-      <c r="C612" s="28"/>
-      <c r="D612" s="29"/>
-      <c r="E612" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="C612" s="25">
+        <v>55.5</v>
+      </c>
+      <c r="D612" s="26">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E612" s="27">
+        <v>126.54</v>
+      </c>
     </row>
     <row r="613" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A613" s="23" t="s">
         <v>616</v>
       </c>
       <c r="B613" s="24">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C613" s="25">
-        <v>35.5</v>
+        <v>15</v>
       </c>
       <c r="D613" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E613" s="27">
-        <v>106.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
@@ -12547,16 +12595,16 @@
         <v>617</v>
       </c>
       <c r="B614" s="24">
+        <v>2</v>
+      </c>
+      <c r="C614" s="25">
         <v>10</v>
       </c>
-      <c r="C614" s="25">
-        <v>26</v>
-      </c>
       <c r="D614" s="26">
-        <v>4.6500000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="E614" s="27">
-        <v>120.9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12564,16 +12612,16 @@
         <v>618</v>
       </c>
       <c r="B615" s="24">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C615" s="25">
-        <v>17.5</v>
+        <v>35.5</v>
       </c>
       <c r="D615" s="26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E615" s="27">
-        <v>87.5</v>
+        <v>106.5</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12581,16 +12629,16 @@
         <v>619</v>
       </c>
       <c r="B616" s="24">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C616" s="25">
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="D616" s="26">
-        <v>3.5</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="E616" s="27">
-        <v>26.25</v>
+        <v>111.6</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12598,16 +12646,16 @@
         <v>620</v>
       </c>
       <c r="B617" s="24">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C617" s="25">
-        <v>26.5</v>
+        <v>17.5</v>
       </c>
       <c r="D617" s="26">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="E617" s="27">
-        <v>92.75</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12615,16 +12663,16 @@
         <v>621</v>
       </c>
       <c r="B618" s="24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C618" s="25">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="D618" s="26">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="E618" s="27">
-        <v>22.5</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12632,16 +12680,16 @@
         <v>622</v>
       </c>
       <c r="B619" s="24">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C619" s="25">
-        <v>11.5</v>
+        <v>26.5</v>
       </c>
       <c r="D619" s="26">
-        <v>5.45</v>
+        <v>3.5</v>
       </c>
       <c r="E619" s="27">
-        <v>62.68</v>
+        <v>92.75</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12649,16 +12697,16 @@
         <v>623</v>
       </c>
       <c r="B620" s="24">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C620" s="25">
-        <v>31.5</v>
+        <v>5</v>
       </c>
       <c r="D620" s="26">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="E620" s="27">
-        <v>97.65</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12666,16 +12714,16 @@
         <v>624</v>
       </c>
       <c r="B621" s="24">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="C621" s="25">
-        <v>26.5</v>
+        <v>11.5</v>
       </c>
       <c r="D621" s="26">
-        <v>1.7</v>
+        <v>5.45</v>
       </c>
       <c r="E621" s="27">
-        <v>45.05</v>
+        <v>62.68</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12683,16 +12731,16 @@
         <v>625</v>
       </c>
       <c r="B622" s="24">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C622" s="25">
-        <v>40.5</v>
+        <v>23.5</v>
       </c>
       <c r="D622" s="26">
-        <v>3.33</v>
+        <v>3.1</v>
       </c>
       <c r="E622" s="27">
-        <v>134.87</v>
+        <v>72.849999999999994</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12700,16 +12748,16 @@
         <v>626</v>
       </c>
       <c r="B623" s="24">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C623" s="25">
-        <v>10.5</v>
+        <v>21.5</v>
       </c>
       <c r="D623" s="26">
-        <v>3.5</v>
+        <v>1.7</v>
       </c>
       <c r="E623" s="27">
-        <v>36.75</v>
+        <v>36.549999999999997</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12717,16 +12765,16 @@
         <v>627</v>
       </c>
       <c r="B624" s="24">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C624" s="25">
-        <v>18.5</v>
+        <v>35.5</v>
       </c>
       <c r="D624" s="26">
-        <v>3.5</v>
+        <v>3.33</v>
       </c>
       <c r="E624" s="27">
-        <v>64.75</v>
+        <v>118.22</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12734,16 +12782,16 @@
         <v>628</v>
       </c>
       <c r="B625" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C625" s="25">
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="D625" s="26">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="E625" s="27">
-        <v>22.5</v>
+        <v>36.75</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12751,16 +12799,16 @@
         <v>629</v>
       </c>
       <c r="B626" s="24">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C626" s="25">
-        <v>10.5</v>
+        <v>16.5</v>
       </c>
       <c r="D626" s="26">
-        <v>8.75</v>
+        <v>3.5</v>
       </c>
       <c r="E626" s="27">
-        <v>91.88</v>
+        <v>57.75</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -12771,13 +12819,13 @@
         <v>4</v>
       </c>
       <c r="C627" s="25">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D627" s="26">
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="E627" s="27">
-        <v>37.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12785,16 +12833,16 @@
         <v>631</v>
       </c>
       <c r="B628" s="24">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C628" s="25">
-        <v>107.3</v>
+        <v>10.5</v>
       </c>
       <c r="D628" s="26">
-        <v>2.85</v>
+        <v>8.75</v>
       </c>
       <c r="E628" s="27">
-        <v>305.81</v>
+        <v>91.88</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12802,16 +12850,16 @@
         <v>632</v>
       </c>
       <c r="B629" s="24">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C629" s="25">
-        <v>60.99</v>
+        <v>6</v>
       </c>
       <c r="D629" s="26">
-        <v>2</v>
+        <v>6.25</v>
       </c>
       <c r="E629" s="27">
-        <v>121.98</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -12819,16 +12867,16 @@
         <v>633</v>
       </c>
       <c r="B630" s="24">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="C630" s="25">
-        <v>3.5</v>
+        <v>107.3</v>
       </c>
       <c r="D630" s="26">
-        <v>5.6</v>
+        <v>2.85</v>
       </c>
       <c r="E630" s="27">
-        <v>19.600000000000001</v>
+        <v>305.81</v>
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
@@ -12836,16 +12884,16 @@
         <v>634</v>
       </c>
       <c r="B631" s="24">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C631" s="25">
-        <v>14.5</v>
+        <v>60.99</v>
       </c>
       <c r="D631" s="26">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="E631" s="27">
-        <v>79.75</v>
+        <v>121.98</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
@@ -12853,16 +12901,16 @@
         <v>635</v>
       </c>
       <c r="B632" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C632" s="25">
-        <v>13</v>
+        <v>3.5</v>
       </c>
       <c r="D632" s="26">
-        <v>5.5</v>
+        <v>5.6</v>
       </c>
       <c r="E632" s="27">
-        <v>71.5</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
@@ -12870,16 +12918,16 @@
         <v>636</v>
       </c>
       <c r="B633" s="24">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C633" s="25">
-        <v>32</v>
+        <v>14.5</v>
       </c>
       <c r="D633" s="26">
-        <v>3.1</v>
+        <v>5.5</v>
       </c>
       <c r="E633" s="27">
-        <v>99.2</v>
+        <v>79.75</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
@@ -12887,16 +12935,16 @@
         <v>637</v>
       </c>
       <c r="B634" s="24">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C634" s="25">
-        <v>26.5</v>
+        <v>13</v>
       </c>
       <c r="D634" s="26">
-        <v>5.68</v>
+        <v>5.5</v>
       </c>
       <c r="E634" s="27">
-        <v>150.52000000000001</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.25">
@@ -12904,16 +12952,16 @@
         <v>638</v>
       </c>
       <c r="B635" s="24">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C635" s="25">
-        <v>64.5</v>
+        <v>32</v>
       </c>
       <c r="D635" s="26">
-        <v>3.97</v>
+        <v>3.1</v>
       </c>
       <c r="E635" s="27">
-        <v>255.96</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="636" spans="1:5" x14ac:dyDescent="0.25">
@@ -12921,31 +12969,33 @@
         <v>639</v>
       </c>
       <c r="B636" s="24">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C636" s="25">
-        <v>26</v>
+        <v>26.5</v>
       </c>
       <c r="D636" s="26">
-        <v>4.8</v>
+        <v>5.68</v>
       </c>
       <c r="E636" s="27">
-        <v>124.8</v>
+        <v>150.52000000000001</v>
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A637" s="23" t="s">
         <v>640</v>
       </c>
-      <c r="B637" s="24"/>
+      <c r="B637" s="24">
+        <v>7</v>
+      </c>
       <c r="C637" s="25">
-        <v>1</v>
+        <v>64.5</v>
       </c>
       <c r="D637" s="26">
-        <v>6.75</v>
+        <v>3.97</v>
       </c>
       <c r="E637" s="27">
-        <v>6.75</v>
+        <v>255.96</v>
       </c>
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.25">
@@ -12953,33 +13003,31 @@
         <v>641</v>
       </c>
       <c r="B638" s="24">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C638" s="25">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D638" s="26">
-        <v>6.75</v>
+        <v>4.8</v>
       </c>
       <c r="E638" s="27">
-        <v>40.5</v>
+        <v>124.8</v>
       </c>
     </row>
     <row r="639" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A639" s="23" t="s">
         <v>642</v>
       </c>
-      <c r="B639" s="24">
+      <c r="B639" s="24"/>
+      <c r="C639" s="25">
         <v>1</v>
-      </c>
-      <c r="C639" s="25">
-        <v>8</v>
       </c>
       <c r="D639" s="26">
         <v>6.75</v>
       </c>
       <c r="E639" s="27">
-        <v>54</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="640" spans="1:5" x14ac:dyDescent="0.25">
@@ -12987,23 +13035,25 @@
         <v>643</v>
       </c>
       <c r="B640" s="24">
+        <v>8</v>
+      </c>
+      <c r="C640" s="25">
         <v>6</v>
-      </c>
-      <c r="C640" s="25">
-        <v>3</v>
       </c>
       <c r="D640" s="26">
         <v>6.75</v>
       </c>
       <c r="E640" s="27">
-        <v>20.25</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="641" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A641" s="23" t="s">
         <v>644</v>
       </c>
-      <c r="B641" s="24"/>
+      <c r="B641" s="24">
+        <v>1</v>
+      </c>
       <c r="C641" s="25">
         <v>8</v>
       </c>
@@ -13019,33 +13069,31 @@
         <v>645</v>
       </c>
       <c r="B642" s="24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C642" s="25">
-        <v>8.5</v>
+        <v>3</v>
       </c>
       <c r="D642" s="26">
-        <v>5.5</v>
+        <v>6.75</v>
       </c>
       <c r="E642" s="27">
-        <v>46.75</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="643" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A643" s="23" t="s">
         <v>646</v>
       </c>
-      <c r="B643" s="24">
-        <v>59</v>
-      </c>
+      <c r="B643" s="24"/>
       <c r="C643" s="25">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="D643" s="26">
-        <v>3.1</v>
+        <v>6.75</v>
       </c>
       <c r="E643" s="27">
-        <v>226.3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="644" spans="1:5" x14ac:dyDescent="0.25">
@@ -13053,16 +13101,16 @@
         <v>647</v>
       </c>
       <c r="B644" s="24">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C644" s="25">
-        <v>45.5</v>
+        <v>8.5</v>
       </c>
       <c r="D644" s="26">
-        <v>3.6</v>
+        <v>5.5</v>
       </c>
       <c r="E644" s="27">
-        <v>163.80000000000001</v>
+        <v>46.75</v>
       </c>
     </row>
     <row r="645" spans="1:5" x14ac:dyDescent="0.25">
@@ -13070,16 +13118,16 @@
         <v>648</v>
       </c>
       <c r="B645" s="24">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C645" s="25">
-        <v>6.5</v>
+        <v>72</v>
       </c>
       <c r="D645" s="26">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="E645" s="27">
-        <v>22.75</v>
+        <v>223.2</v>
       </c>
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.25">
@@ -13087,16 +13135,16 @@
         <v>649</v>
       </c>
       <c r="B646" s="24">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C646" s="25">
-        <v>6</v>
+        <v>44.5</v>
       </c>
       <c r="D646" s="26">
-        <v>4.25</v>
+        <v>3.6</v>
       </c>
       <c r="E646" s="27">
-        <v>25.5</v>
+        <v>160.19999999999999</v>
       </c>
     </row>
     <row r="647" spans="1:5" x14ac:dyDescent="0.25">
@@ -13104,16 +13152,16 @@
         <v>650</v>
       </c>
       <c r="B647" s="24">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C647" s="25">
-        <v>66.5</v>
+        <v>6.5</v>
       </c>
       <c r="D647" s="26">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="E647" s="27">
-        <v>249.38</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="648" spans="1:5" x14ac:dyDescent="0.25">
@@ -13121,16 +13169,16 @@
         <v>651</v>
       </c>
       <c r="B648" s="24">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C648" s="25">
-        <v>30.5</v>
+        <v>6</v>
       </c>
       <c r="D648" s="26">
-        <v>2.5</v>
+        <v>4.25</v>
       </c>
       <c r="E648" s="27">
-        <v>76.25</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="649" spans="1:5" x14ac:dyDescent="0.25">
@@ -13138,16 +13186,16 @@
         <v>652</v>
       </c>
       <c r="B649" s="24">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C649" s="25">
-        <v>15.5</v>
+        <v>65</v>
       </c>
       <c r="D649" s="26">
-        <v>7.31</v>
+        <v>3.75</v>
       </c>
       <c r="E649" s="27">
-        <v>113.34</v>
+        <v>243.75</v>
       </c>
     </row>
     <row r="650" spans="1:5" x14ac:dyDescent="0.25">
@@ -13155,16 +13203,16 @@
         <v>653</v>
       </c>
       <c r="B650" s="24">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C650" s="25">
-        <v>4</v>
+        <v>26.5</v>
       </c>
       <c r="D650" s="26">
-        <v>5.75</v>
+        <v>2.5</v>
       </c>
       <c r="E650" s="27">
-        <v>23</v>
+        <v>66.25</v>
       </c>
     </row>
     <row r="651" spans="1:5" x14ac:dyDescent="0.25">
@@ -13172,16 +13220,16 @@
         <v>654</v>
       </c>
       <c r="B651" s="24">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C651" s="25">
-        <v>6.5</v>
+        <v>15.5</v>
       </c>
       <c r="D651" s="26">
-        <v>5.8</v>
+        <v>7.31</v>
       </c>
       <c r="E651" s="27">
-        <v>37.700000000000003</v>
+        <v>113.34</v>
       </c>
     </row>
     <row r="652" spans="1:5" x14ac:dyDescent="0.25">
@@ -13189,16 +13237,16 @@
         <v>655</v>
       </c>
       <c r="B652" s="24">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C652" s="25">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="D652" s="26">
-        <v>2.25</v>
+        <v>5.75</v>
       </c>
       <c r="E652" s="27">
-        <v>132.75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="653" spans="1:5" x14ac:dyDescent="0.25">
@@ -13206,31 +13254,33 @@
         <v>656</v>
       </c>
       <c r="B653" s="24">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C653" s="25">
-        <v>62</v>
+        <v>6.5</v>
       </c>
       <c r="D653" s="26">
-        <v>2.25</v>
+        <v>5.8</v>
       </c>
       <c r="E653" s="27">
-        <v>139.5</v>
+        <v>37.700000000000003</v>
       </c>
     </row>
     <row r="654" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A654" s="23" t="s">
         <v>657</v>
       </c>
-      <c r="B654" s="24"/>
+      <c r="B654" s="24">
+        <v>10</v>
+      </c>
       <c r="C654" s="25">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D654" s="26">
-        <v>8.84</v>
+        <v>2.25</v>
       </c>
       <c r="E654" s="27">
-        <v>132.57</v>
+        <v>132.75</v>
       </c>
     </row>
     <row r="655" spans="1:5" x14ac:dyDescent="0.25">
@@ -13238,33 +13288,31 @@
         <v>658</v>
       </c>
       <c r="B655" s="24">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C655" s="25">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D655" s="26">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="E655" s="27">
-        <v>167.75</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A656" s="23" t="s">
         <v>659</v>
       </c>
-      <c r="B656" s="24">
-        <v>6</v>
-      </c>
+      <c r="B656" s="24"/>
       <c r="C656" s="25">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D656" s="26">
-        <v>2.75</v>
+        <v>8.84</v>
       </c>
       <c r="E656" s="27">
-        <v>187</v>
+        <v>132.57</v>
       </c>
     </row>
     <row r="657" spans="1:5" x14ac:dyDescent="0.25">
@@ -13275,13 +13323,13 @@
         <v>8</v>
       </c>
       <c r="C657" s="25">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D657" s="26">
         <v>2.75</v>
       </c>
       <c r="E657" s="27">
-        <v>159.5</v>
+        <v>167.75</v>
       </c>
     </row>
     <row r="658" spans="1:5" x14ac:dyDescent="0.25">
@@ -13289,16 +13337,16 @@
         <v>661</v>
       </c>
       <c r="B658" s="24">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C658" s="25">
-        <v>37.5</v>
+        <v>68</v>
       </c>
       <c r="D658" s="26">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="E658" s="27">
-        <v>150</v>
+        <v>187</v>
       </c>
     </row>
     <row r="659" spans="1:5" x14ac:dyDescent="0.25">
@@ -13306,16 +13354,16 @@
         <v>662</v>
       </c>
       <c r="B659" s="24">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C659" s="25">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="D659" s="26">
-        <v>2.66</v>
+        <v>2.75</v>
       </c>
       <c r="E659" s="27">
-        <v>58.52</v>
+        <v>159.5</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.25">
@@ -13323,16 +13371,16 @@
         <v>663</v>
       </c>
       <c r="B660" s="24">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C660" s="25">
-        <v>17.5</v>
+        <v>37.5</v>
       </c>
       <c r="D660" s="26">
-        <v>4.25</v>
+        <v>4</v>
       </c>
       <c r="E660" s="27">
-        <v>74.38</v>
+        <v>150</v>
       </c>
     </row>
     <row r="661" spans="1:5" x14ac:dyDescent="0.25">
@@ -13340,16 +13388,16 @@
         <v>664</v>
       </c>
       <c r="B661" s="24">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C661" s="25">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D661" s="26">
-        <v>4.25</v>
+        <v>2.66</v>
       </c>
       <c r="E661" s="27">
-        <v>102</v>
+        <v>58.52</v>
       </c>
     </row>
     <row r="662" spans="1:5" x14ac:dyDescent="0.25">
@@ -13357,16 +13405,16 @@
         <v>665</v>
       </c>
       <c r="B662" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C662" s="25">
-        <v>18.350000000000001</v>
+        <v>17.5</v>
       </c>
       <c r="D662" s="26">
-        <v>5.5</v>
+        <v>4.25</v>
       </c>
       <c r="E662" s="27">
-        <v>100.93</v>
+        <v>74.38</v>
       </c>
     </row>
     <row r="663" spans="1:5" x14ac:dyDescent="0.25">
@@ -13374,16 +13422,16 @@
         <v>666</v>
       </c>
       <c r="B663" s="24">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C663" s="25">
-        <v>26.5</v>
+        <v>24</v>
       </c>
       <c r="D663" s="26">
-        <v>5</v>
+        <v>4.25</v>
       </c>
       <c r="E663" s="27">
-        <v>132.5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="664" spans="1:5" x14ac:dyDescent="0.25">
@@ -13391,16 +13439,16 @@
         <v>667</v>
       </c>
       <c r="B664" s="24">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C664" s="25">
-        <v>30</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="D664" s="26">
-        <v>2.75</v>
+        <v>5.5</v>
       </c>
       <c r="E664" s="27">
-        <v>82.5</v>
+        <v>100.93</v>
       </c>
     </row>
     <row r="665" spans="1:5" x14ac:dyDescent="0.25">
@@ -13411,13 +13459,13 @@
         <v>6</v>
       </c>
       <c r="C665" s="25">
-        <v>34.5</v>
+        <v>26.5</v>
       </c>
       <c r="D665" s="26">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="E665" s="27">
-        <v>124.2</v>
+        <v>132.5</v>
       </c>
     </row>
     <row r="666" spans="1:5" x14ac:dyDescent="0.25">
@@ -13425,36 +13473,44 @@
         <v>669</v>
       </c>
       <c r="B666" s="24">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C666" s="25">
-        <v>28</v>
-      </c>
-      <c r="D666" s="29"/>
-      <c r="E666" s="28"/>
+        <v>30</v>
+      </c>
+      <c r="D666" s="26">
+        <v>2.75</v>
+      </c>
+      <c r="E666" s="27">
+        <v>82.5</v>
+      </c>
     </row>
     <row r="667" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A667" s="23" t="s">
         <v>670</v>
       </c>
       <c r="B667" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C667" s="25">
-        <v>30.5</v>
-      </c>
-      <c r="D667" s="29"/>
-      <c r="E667" s="28"/>
+        <v>34.5</v>
+      </c>
+      <c r="D667" s="26">
+        <v>3.6</v>
+      </c>
+      <c r="E667" s="27">
+        <v>124.2</v>
+      </c>
     </row>
     <row r="668" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A668" s="23" t="s">
         <v>671</v>
       </c>
       <c r="B668" s="24">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C668" s="25">
-        <v>41.69</v>
+        <v>28</v>
       </c>
       <c r="D668" s="29"/>
       <c r="E668" s="28"/>
@@ -13464,10 +13520,10 @@
         <v>672</v>
       </c>
       <c r="B669" s="24">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C669" s="25">
-        <v>26</v>
+        <v>30.5</v>
       </c>
       <c r="D669" s="29"/>
       <c r="E669" s="28"/>
@@ -13477,10 +13533,10 @@
         <v>673</v>
       </c>
       <c r="B670" s="24">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C670" s="25">
-        <v>8.5</v>
+        <v>41.69</v>
       </c>
       <c r="D670" s="29"/>
       <c r="E670" s="28"/>
@@ -13490,9 +13546,11 @@
         <v>674</v>
       </c>
       <c r="B671" s="24">
-        <v>11</v>
-      </c>
-      <c r="C671" s="28"/>
+        <v>2</v>
+      </c>
+      <c r="C671" s="25">
+        <v>26</v>
+      </c>
       <c r="D671" s="29"/>
       <c r="E671" s="28"/>
     </row>
@@ -13501,10 +13559,10 @@
         <v>675</v>
       </c>
       <c r="B672" s="24">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C672" s="25">
-        <v>12</v>
+        <v>3.5</v>
       </c>
       <c r="D672" s="29"/>
       <c r="E672" s="28"/>
@@ -13514,11 +13572,9 @@
         <v>676</v>
       </c>
       <c r="B673" s="24">
-        <v>30</v>
-      </c>
-      <c r="C673" s="25">
-        <v>59.5</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C673" s="28"/>
       <c r="D673" s="29"/>
       <c r="E673" s="28"/>
     </row>
@@ -13527,10 +13583,10 @@
         <v>677</v>
       </c>
       <c r="B674" s="24">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C674" s="25">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D674" s="29"/>
       <c r="E674" s="28"/>
@@ -13539,8 +13595,12 @@
       <c r="A675" s="23" t="s">
         <v>678</v>
       </c>
-      <c r="B675" s="24"/>
-      <c r="C675" s="28"/>
+      <c r="B675" s="24">
+        <v>30</v>
+      </c>
+      <c r="C675" s="25">
+        <v>59.5</v>
+      </c>
       <c r="D675" s="29"/>
       <c r="E675" s="28"/>
     </row>
@@ -13549,45 +13609,39 @@
         <v>679</v>
       </c>
       <c r="B676" s="24">
+        <v>18</v>
+      </c>
+      <c r="C676" s="25">
         <v>20</v>
       </c>
-      <c r="C676" s="25">
-        <v>106</v>
-      </c>
-      <c r="D676" s="26">
-        <v>2.9</v>
-      </c>
-      <c r="E676" s="27">
-        <v>307.18</v>
-      </c>
+      <c r="D676" s="29"/>
+      <c r="E676" s="28"/>
     </row>
     <row r="677" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A677" s="23" t="s">
         <v>680</v>
       </c>
       <c r="B677" s="24"/>
-      <c r="C677" s="25">
-        <v>14.5</v>
-      </c>
-      <c r="D677" s="26">
-        <v>3.8</v>
-      </c>
-      <c r="E677" s="27">
-        <v>55.1</v>
-      </c>
+      <c r="C677" s="28"/>
+      <c r="D677" s="29"/>
+      <c r="E677" s="28"/>
     </row>
     <row r="678" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A678" s="23" t="s">
         <v>681</v>
       </c>
       <c r="B678" s="24">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C678" s="25">
-        <v>-0.5</v>
-      </c>
-      <c r="D678" s="29"/>
-      <c r="E678" s="28"/>
+        <v>96</v>
+      </c>
+      <c r="D678" s="26">
+        <v>2.9</v>
+      </c>
+      <c r="E678" s="27">
+        <v>278.2</v>
+      </c>
     </row>
     <row r="679" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A679" s="23" t="s">
@@ -13595,63 +13649,67 @@
       </c>
       <c r="B679" s="24"/>
       <c r="C679" s="25">
-        <v>502</v>
+        <v>14.5</v>
       </c>
       <c r="D679" s="26">
-        <v>0.82</v>
+        <v>3.8</v>
       </c>
       <c r="E679" s="27">
-        <v>411.64</v>
+        <v>55.1</v>
       </c>
     </row>
     <row r="680" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A680" s="23" t="s">
         <v>683</v>
       </c>
-      <c r="B680" s="24"/>
+      <c r="B680" s="24">
+        <v>2</v>
+      </c>
       <c r="C680" s="25">
-        <v>500</v>
-      </c>
-      <c r="D680" s="26">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E680" s="27">
-        <v>575</v>
-      </c>
+        <v>-0.5</v>
+      </c>
+      <c r="D680" s="29"/>
+      <c r="E680" s="28"/>
     </row>
     <row r="681" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A681" s="23" t="s">
         <v>684</v>
       </c>
-      <c r="B681" s="24">
-        <v>1</v>
-      </c>
+      <c r="B681" s="24"/>
       <c r="C681" s="25">
-        <v>-0.5</v>
-      </c>
-      <c r="D681" s="29"/>
-      <c r="E681" s="28"/>
+        <v>502</v>
+      </c>
+      <c r="D681" s="26">
+        <v>0.82</v>
+      </c>
+      <c r="E681" s="27">
+        <v>411.64</v>
+      </c>
     </row>
     <row r="682" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A682" s="23" t="s">
         <v>685</v>
       </c>
-      <c r="B682" s="24">
-        <v>1</v>
-      </c>
-      <c r="C682" s="28"/>
-      <c r="D682" s="29"/>
-      <c r="E682" s="28"/>
+      <c r="B682" s="24"/>
+      <c r="C682" s="25">
+        <v>500</v>
+      </c>
+      <c r="D682" s="26">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E682" s="27">
+        <v>575</v>
+      </c>
     </row>
     <row r="683" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A683" s="23" t="s">
         <v>686</v>
       </c>
       <c r="B683" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C683" s="25">
-        <v>-0.02</v>
+        <v>-0.5</v>
       </c>
       <c r="D683" s="29"/>
       <c r="E683" s="28"/>
@@ -13661,24 +13719,22 @@
         <v>687</v>
       </c>
       <c r="B684" s="24">
-        <v>5</v>
-      </c>
-      <c r="C684" s="25">
-        <v>10</v>
-      </c>
-      <c r="D684" s="26">
-        <v>1.6</v>
-      </c>
-      <c r="E684" s="27">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C684" s="28"/>
+      <c r="D684" s="29"/>
+      <c r="E684" s="28"/>
     </row>
     <row r="685" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A685" s="23" t="s">
         <v>688</v>
       </c>
-      <c r="B685" s="24"/>
-      <c r="C685" s="28"/>
+      <c r="B685" s="24">
+        <v>2</v>
+      </c>
+      <c r="C685" s="25">
+        <v>-0.02</v>
+      </c>
       <c r="D685" s="29"/>
       <c r="E685" s="28"/>
     </row>
@@ -13687,24 +13743,24 @@
         <v>689</v>
       </c>
       <c r="B686" s="24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C686" s="25">
-        <v>-25</v>
-      </c>
-      <c r="D686" s="29"/>
-      <c r="E686" s="28"/>
+        <v>-5</v>
+      </c>
+      <c r="D686" s="26">
+        <v>1.6</v>
+      </c>
+      <c r="E686" s="27">
+        <v>-8</v>
+      </c>
     </row>
     <row r="687" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A687" s="23" t="s">
         <v>690</v>
       </c>
-      <c r="B687" s="24">
-        <v>39</v>
-      </c>
-      <c r="C687" s="25">
-        <v>-0.39</v>
-      </c>
+      <c r="B687" s="24"/>
+      <c r="C687" s="28"/>
       <c r="D687" s="29"/>
       <c r="E687" s="28"/>
     </row>
@@ -13713,10 +13769,10 @@
         <v>691</v>
       </c>
       <c r="B688" s="24">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C688" s="25">
-        <v>-0.59</v>
+        <v>-90</v>
       </c>
       <c r="D688" s="29"/>
       <c r="E688" s="28"/>
@@ -13726,27 +13782,23 @@
         <v>692</v>
       </c>
       <c r="B689" s="24">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C689" s="25">
-        <v>-94</v>
-      </c>
-      <c r="D689" s="26">
-        <v>1</v>
-      </c>
-      <c r="E689" s="27">
-        <v>-94</v>
-      </c>
+        <v>-0.39</v>
+      </c>
+      <c r="D689" s="29"/>
+      <c r="E689" s="28"/>
     </row>
     <row r="690" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A690" s="23" t="s">
         <v>693</v>
       </c>
       <c r="B690" s="24">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C690" s="25">
-        <v>-30.5</v>
+        <v>-0.63</v>
       </c>
       <c r="D690" s="29"/>
       <c r="E690" s="28"/>
@@ -13756,16 +13808,16 @@
         <v>694</v>
       </c>
       <c r="B691" s="24">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C691" s="25">
-        <v>21</v>
+        <v>-94</v>
       </c>
       <c r="D691" s="26">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E691" s="27">
-        <v>52.5</v>
+        <v>-94</v>
       </c>
     </row>
     <row r="692" spans="1:5" x14ac:dyDescent="0.25">
@@ -13773,33 +13825,29 @@
         <v>695</v>
       </c>
       <c r="B692" s="24">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C692" s="25">
-        <v>25.75</v>
-      </c>
-      <c r="D692" s="26">
-        <v>2.5</v>
-      </c>
-      <c r="E692" s="27">
-        <v>64.38</v>
-      </c>
+        <v>-31.5</v>
+      </c>
+      <c r="D692" s="29"/>
+      <c r="E692" s="28"/>
     </row>
     <row r="693" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A693" s="23" t="s">
         <v>696</v>
       </c>
       <c r="B693" s="24">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C693" s="25">
-        <v>45.75</v>
+        <v>21</v>
       </c>
       <c r="D693" s="26">
         <v>2.5</v>
       </c>
       <c r="E693" s="27">
-        <v>114.38</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="694" spans="1:5" x14ac:dyDescent="0.25">
@@ -13807,16 +13855,16 @@
         <v>697</v>
       </c>
       <c r="B694" s="24">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C694" s="25">
-        <v>68</v>
+        <v>25.25</v>
       </c>
       <c r="D694" s="26">
         <v>2.5</v>
       </c>
       <c r="E694" s="27">
-        <v>170</v>
+        <v>63.13</v>
       </c>
     </row>
     <row r="695" spans="1:5" x14ac:dyDescent="0.25">
@@ -13824,16 +13872,16 @@
         <v>698</v>
       </c>
       <c r="B695" s="24">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C695" s="25">
-        <v>28.5</v>
+        <v>37.25</v>
       </c>
       <c r="D695" s="26">
         <v>2.5</v>
       </c>
       <c r="E695" s="27">
-        <v>71.25</v>
+        <v>93.13</v>
       </c>
     </row>
     <row r="696" spans="1:5" x14ac:dyDescent="0.25">
@@ -13841,16 +13889,16 @@
         <v>699</v>
       </c>
       <c r="B696" s="24">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C696" s="25">
-        <v>11.75</v>
+        <v>67.5</v>
       </c>
       <c r="D696" s="26">
         <v>2.5</v>
       </c>
       <c r="E696" s="27">
-        <v>29.38</v>
+        <v>168.75</v>
       </c>
     </row>
     <row r="697" spans="1:5" x14ac:dyDescent="0.25">
@@ -13858,16 +13906,16 @@
         <v>700</v>
       </c>
       <c r="B697" s="24">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C697" s="25">
-        <v>25</v>
+        <v>27.5</v>
       </c>
       <c r="D697" s="26">
         <v>2.5</v>
       </c>
       <c r="E697" s="27">
-        <v>62.5</v>
+        <v>68.75</v>
       </c>
     </row>
     <row r="698" spans="1:5" x14ac:dyDescent="0.25">
@@ -13875,16 +13923,16 @@
         <v>701</v>
       </c>
       <c r="B698" s="24">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C698" s="25">
-        <v>42.75</v>
+        <v>8.75</v>
       </c>
       <c r="D698" s="26">
         <v>2.5</v>
       </c>
       <c r="E698" s="27">
-        <v>106.88</v>
+        <v>21.88</v>
       </c>
     </row>
     <row r="699" spans="1:5" x14ac:dyDescent="0.25">
@@ -13892,16 +13940,16 @@
         <v>702</v>
       </c>
       <c r="B699" s="24">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C699" s="25">
-        <v>45.5</v>
+        <v>24.5</v>
       </c>
       <c r="D699" s="26">
         <v>2.5</v>
       </c>
       <c r="E699" s="27">
-        <v>113.75</v>
+        <v>61.25</v>
       </c>
     </row>
     <row r="700" spans="1:5" x14ac:dyDescent="0.25">
@@ -13909,25 +13957,59 @@
         <v>703</v>
       </c>
       <c r="B700" s="24">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="C700" s="25">
-        <v>-202</v>
-      </c>
-      <c r="D700" s="29"/>
-      <c r="E700" s="28"/>
+        <v>39.25</v>
+      </c>
+      <c r="D700" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="E700" s="27">
+        <v>98.13</v>
+      </c>
     </row>
     <row r="701" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A701" s="30" t="s">
+      <c r="A701" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="B701" s="31"/>
-      <c r="C701" s="32">
-        <v>36597.43</v>
-      </c>
-      <c r="D701" s="33"/>
-      <c r="E701" s="34">
-        <v>107665.57</v>
+      <c r="B701" s="24">
+        <v>39</v>
+      </c>
+      <c r="C701" s="25">
+        <v>40</v>
+      </c>
+      <c r="D701" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="E701" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="702" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A702" s="23" t="s">
+        <v>705</v>
+      </c>
+      <c r="B702" s="24">
+        <v>78</v>
+      </c>
+      <c r="C702" s="25">
+        <v>-205</v>
+      </c>
+      <c r="D702" s="29"/>
+      <c r="E702" s="28"/>
+    </row>
+    <row r="703" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A703" s="30" t="s">
+        <v>706</v>
+      </c>
+      <c r="B703" s="31"/>
+      <c r="C703" s="32">
+        <v>38841.699999999997</v>
+      </c>
+      <c r="D703" s="33"/>
+      <c r="E703" s="34">
+        <v>107132.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil 10 dec @9.33
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -35,7 +35,7 @@
     <t>Stock Group Summary</t>
   </si>
   <si>
-    <t>1-Jul-25 to 9-Dec-25</t>
+    <t>1-Jul-25 to 10-Dec-25</t>
   </si>
   <si>
     <t/>
@@ -68,310 +68,310 @@
     <t>Value</t>
   </si>
   <si>
-    <t>.1001 PATRIKA (25/251)</t>
-  </si>
-  <si>
-    <t>1002 PATRIKA (25/262)</t>
-  </si>
-  <si>
-    <t>1003 PATRIKA (25/261)</t>
-  </si>
-  <si>
-    <t>1004 PATRIKA (25/361/861)</t>
-  </si>
-  <si>
-    <t>1005 PATRIKA (25/362/862)</t>
-  </si>
-  <si>
-    <t>1006 PATRIKA (25/282)</t>
-  </si>
-  <si>
-    <t>1007 PATRIKA (25/281)</t>
-  </si>
-  <si>
-    <t>1008 PATRIKA (JC) (2595 PINK)</t>
-  </si>
-  <si>
-    <t>1009 PATRIKA (JC) (2595 ORANGE)</t>
-  </si>
-  <si>
-    <t>1010 PATRIKA (6321)</t>
-  </si>
-  <si>
-    <t>1011 PATRIKA (2563 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1012 PATRIKA (2564 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1013 PATRIKA (2568 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1014 PATRIKA (11043 OFFSET)</t>
-  </si>
-  <si>
-    <t>1015 PATRIKA (DCU) (11041 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1016 PATRIKA (1011 OFFSET)</t>
-  </si>
-  <si>
-    <t>1017 PATRIKA (1014 OFFSET)</t>
-  </si>
-  <si>
-    <t>1018 PATRIKA (10081 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1019 PATRIKA (1222 SBC)</t>
-  </si>
-  <si>
-    <t>1020 PATRIKA (1235)</t>
-  </si>
-  <si>
-    <t>1021 PATRIKA (2101 VV)</t>
-  </si>
-  <si>
-    <t>1023 PATRIKA (25418)</t>
-  </si>
-  <si>
-    <t>1024 PATRIKA (25322)</t>
-  </si>
-  <si>
-    <t>1025 PATRIKA (25323)</t>
-  </si>
-  <si>
-    <t>1026 PATRIKA (JC) (1173 SBC)</t>
-  </si>
-  <si>
-    <t>1027 PATRIKA (JC) (5346)</t>
-  </si>
-  <si>
-    <t>1028 PATRIKA (JC) (2596)</t>
-  </si>
-  <si>
-    <t>1029 PATRIKA (1042)</t>
-  </si>
-  <si>
-    <t>1030 PATRIKA (1043)</t>
-  </si>
-  <si>
-    <t>1031 PATRIKA (GOPAL 11)</t>
-  </si>
-  <si>
-    <t>1032 PATRIKA (GOPAL 1)</t>
-  </si>
-  <si>
-    <t>1033 PATRIKA (2002 YLW)</t>
-  </si>
-  <si>
-    <t>1034 PATRIKA (2003 R)</t>
-  </si>
-  <si>
-    <t>1035 PATRIKA (DCU) (2201 ROSHAN)</t>
-  </si>
-  <si>
-    <t>1101 PATRIKA (O.2591) (2591 ORANGE)</t>
-  </si>
-  <si>
-    <t>1102 PATRIKA (P.2591) (2591 PINK)</t>
-  </si>
-  <si>
-    <t>1103 PATRIKA(N-271) (271 NEHA)</t>
-  </si>
-  <si>
-    <t>1104 PATRIKA(N-272) (272 NEHA)</t>
-  </si>
-  <si>
-    <t>1105 PATRIKA (276-A)</t>
-  </si>
-  <si>
-    <t>1106 PATRIKA-YELLOW (25419)</t>
-  </si>
-  <si>
-    <t>1107 PATRIKA-RED (25420)</t>
-  </si>
-  <si>
-    <t>1109 PATRIKA-BIG Y (25421)</t>
-  </si>
-  <si>
-    <t>1110 PATRIKA-BIG R (25422)</t>
-  </si>
-  <si>
-    <t>1112 PATRIKA (277-B)</t>
-  </si>
-  <si>
-    <t>1113 PATRIKA (1819 MONARCH)</t>
-  </si>
-  <si>
-    <t>1114 PATRIKA-BROWN (1709)</t>
-  </si>
-  <si>
-    <t>1115 PATRIKA-CREAM (1678 PRINCE)</t>
-  </si>
-  <si>
-    <t>1116 PATRIKA (1153) (1253 Jsk)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA (1155) (1155 JSK)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA - B (KRISHNA 1155-B)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA - B (DCU) (NEW SAVASHREE- 51)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA (सवाश्री-57) (NEW SAVASHREE-57)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA - B (DCU) (NEW SAVASHREE 52)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA(सवाश्री-55) (NEW SAVASHREE-55)</t>
-  </si>
-  <si>
-    <t>1120 PATRIKA(सवाश्री-59) (NEW SAVASHREE-59)</t>
-  </si>
-  <si>
-    <t>1121 PATRIKA(सवाश्री-53) (NEW SAVASHREE-53)</t>
-  </si>
-  <si>
-    <t>1122 PATRIKA (DCU) (NEW SAVASHREE-54)</t>
-  </si>
-  <si>
-    <t>1123 PATRIKA (LED-51) (LED-51)</t>
-  </si>
-  <si>
-    <t>1124 PATRIKA (LED-52) (LED-52)</t>
-  </si>
-  <si>
-    <t>1125 PATRIKA (LED-53) (LED-53)</t>
-  </si>
-  <si>
-    <t>1126 PATRIKA (LED-54) (LED-54)</t>
-  </si>
-  <si>
-    <t>1127 PATRIKA (Eco-52) (NEW ECO-52)</t>
-  </si>
-  <si>
-    <t>1128 PATRIKA (Eco-55) (NEW ECO-55)</t>
-  </si>
-  <si>
-    <t>1129 PATRIKA (Eco-56) (NEW ECO-56)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA - B (ECO-60) (DCU) (NEW ECO 60)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA (Eco-59) (NEW ECO-59)</t>
-  </si>
-  <si>
-    <t>1131 PATRIKA (DCU) Eco-51 (NEW ECO- 51)</t>
-  </si>
-  <si>
-    <t>1132 PATRIKA (DCU) Eco-53 (NEW ECO- 53)</t>
-  </si>
-  <si>
-    <t>1133 PATRIKA (DCU) Eco-57 (NEW ECO- 57)</t>
-  </si>
-  <si>
-    <t>1134 PATRIKA (DCU) Eco-58 (NEW ECO- 58)</t>
-  </si>
-  <si>
-    <t>1135 PATRIKA (DCU) Eco-54 (NEW ECO- 54)</t>
-  </si>
-  <si>
-    <t>1136 PATRIKA (R) (120 GSM RED)</t>
-  </si>
-  <si>
-    <t>1137 PATRIKA (P) (120 GSM YELLOW)</t>
-  </si>
-  <si>
-    <t>1138 PATRIKA (BR) (150 GSM FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1139 PATRIKA (BY) (150 GSM FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1140 PATRIKA (BB) (150 GSM FOIL (BROWN))</t>
-  </si>
-  <si>
-    <t>1141 PATRIKA (R) (120 GSM (RED)SELF)</t>
-  </si>
-  <si>
-    <t>1142 PATRIKA (P) (120 GSM (YELLOW) SELF)</t>
-  </si>
-  <si>
-    <t>1143 PATRIKA (G) (120 GSM (OLD GOLDEN))</t>
-  </si>
-  <si>
-    <t>1144 PATRIKA (BR) (170 GSM WITH FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1145 PATRIKA (BY) (170 GSM WITH FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1146 PATRIKA (DCU) (BROWN 170 GSM FOIL)</t>
-  </si>
-  <si>
-    <t>1147 PATRIKA (S.201) (201 WESTERN)</t>
-  </si>
-  <si>
-    <t>1148 PATRIKA (S.202) (202 WESTERN)</t>
-  </si>
-  <si>
-    <t>1149 PATRIKA (S.204) (204 WESTERN)</t>
-  </si>
-  <si>
-    <t>1150 PATRIKA (DCU) (NEW SAVASHREE-58)</t>
-  </si>
-  <si>
-    <t>1151 PATRIKA (DCU) (NEW SAVASHREE-56)</t>
-  </si>
-  <si>
-    <t>1152 PATRIKA (DCU) (WESTERN 202 OLD)</t>
-  </si>
-  <si>
-    <t>1153 PATRIKA (DCU) (201 WESTERN (OLD))</t>
-  </si>
-  <si>
-    <t>1154 PATRIKA (DCU) (203 WESTERN A)</t>
-  </si>
-  <si>
-    <t>1155 PATRIKA (DCU) (WESTERN (203) B)</t>
-  </si>
-  <si>
-    <t>1156 PATRIKA-YELLOW (LU-51 (YELLOW))</t>
-  </si>
-  <si>
-    <t>1157 PATRIKA-CREAM (LU-52 (CREAM))</t>
-  </si>
-  <si>
-    <t>1158 PATRIKA-GOLDEN (LU-53 (GOLDEN))</t>
-  </si>
-  <si>
-    <t>1159 PATRIKA-WHITE (LU-54 (WHITE))</t>
-  </si>
-  <si>
-    <t>1160 PATRIKA-PINK (LU-55 (PINK))</t>
-  </si>
-  <si>
-    <t>1161 PATRIKA (01) (JCC 01)</t>
-  </si>
-  <si>
-    <t>1162 PATRIKA (02) (JCC 02)</t>
-  </si>
-  <si>
-    <t>1163 PATRIKA (DCU) (BP RED)</t>
-  </si>
-  <si>
-    <t>1164 PATRIKA (DCU) (BP PINK RIYAZ)</t>
-  </si>
-  <si>
-    <t>1165 PATRIKA (DCU) (BP CREAM)</t>
-  </si>
-  <si>
-    <t>1166 PATRIKA (DCU) (BP YELLOW)</t>
+    <t>.1001 PATRIKA</t>
+  </si>
+  <si>
+    <t>1002 PATRIKA</t>
+  </si>
+  <si>
+    <t>1003 PATRIKA</t>
+  </si>
+  <si>
+    <t>1004 PATRIKA</t>
+  </si>
+  <si>
+    <t>1005 PATRIKA</t>
+  </si>
+  <si>
+    <t>1006 PATRIKA</t>
+  </si>
+  <si>
+    <t>1007 PATRIKA</t>
+  </si>
+  <si>
+    <t>1008 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1009 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1010 PATRIKA</t>
+  </si>
+  <si>
+    <t>1011 PATRIKA</t>
+  </si>
+  <si>
+    <t>1012 PATRIKA</t>
+  </si>
+  <si>
+    <t>1013 PATRIKA</t>
+  </si>
+  <si>
+    <t>1014 PATRIKA</t>
+  </si>
+  <si>
+    <t>1015 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1016 PATRIKA</t>
+  </si>
+  <si>
+    <t>1017 PATRIKA</t>
+  </si>
+  <si>
+    <t>1018 PATRIKA</t>
+  </si>
+  <si>
+    <t>1019 PATRIKA</t>
+  </si>
+  <si>
+    <t>1020 PATRIKA</t>
+  </si>
+  <si>
+    <t>1021 PATRIKA</t>
+  </si>
+  <si>
+    <t>1023 PATRIKA</t>
+  </si>
+  <si>
+    <t>1024 PATRIKA</t>
+  </si>
+  <si>
+    <t>1025 PATRIKA</t>
+  </si>
+  <si>
+    <t>1026 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1027 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1028 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1029 PATRIKA</t>
+  </si>
+  <si>
+    <t>1030 PATRIKA</t>
+  </si>
+  <si>
+    <t>1031 PATRIKA</t>
+  </si>
+  <si>
+    <t>1032 PATRIKA</t>
+  </si>
+  <si>
+    <t>1033 PATRIKA</t>
+  </si>
+  <si>
+    <t>1034 PATRIKA</t>
+  </si>
+  <si>
+    <t>1035 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1101 PATRIKA (O.2591)</t>
+  </si>
+  <si>
+    <t>1102 PATRIKA (P.2591)</t>
+  </si>
+  <si>
+    <t>1103 PATRIKA(N-271)</t>
+  </si>
+  <si>
+    <t>1104 PATRIKA(N-272)</t>
+  </si>
+  <si>
+    <t>1105 PATRIKA</t>
+  </si>
+  <si>
+    <t>1106 PATRIKA-YELLOW</t>
+  </si>
+  <si>
+    <t>1107 PATRIKA-RED</t>
+  </si>
+  <si>
+    <t>1109 PATRIKA-BIG Y</t>
+  </si>
+  <si>
+    <t>1110 PATRIKA-BIG R</t>
+  </si>
+  <si>
+    <t>1112 PATRIKA</t>
+  </si>
+  <si>
+    <t>1113 PATRIKA</t>
+  </si>
+  <si>
+    <t>1114 PATRIKA-BROWN</t>
+  </si>
+  <si>
+    <t>1115 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1116 PATRIKA (1153)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA (1155)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA - B</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA (सवाश्री-57)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA(सवाश्री-55)</t>
+  </si>
+  <si>
+    <t>1120 PATRIKA(सवाश्री-59)</t>
+  </si>
+  <si>
+    <t>1121 PATRIKA(सवाश्री-53)</t>
+  </si>
+  <si>
+    <t>1122 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1123 PATRIKA (LED-51)</t>
+  </si>
+  <si>
+    <t>1124 PATRIKA (LED-52)</t>
+  </si>
+  <si>
+    <t>1125 PATRIKA (LED-53)</t>
+  </si>
+  <si>
+    <t>1126 PATRIKA (LED-54)</t>
+  </si>
+  <si>
+    <t>1127 PATRIKA (Eco-52)</t>
+  </si>
+  <si>
+    <t>1128 PATRIKA (Eco-55)</t>
+  </si>
+  <si>
+    <t>1129 PATRIKA (Eco-56)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA - B (ECO-60) (DCU)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA (Eco-59)</t>
+  </si>
+  <si>
+    <t>1131 PATRIKA (DCU) Eco-51</t>
+  </si>
+  <si>
+    <t>1132 PATRIKA (DCU) Eco-53</t>
+  </si>
+  <si>
+    <t>1133 PATRIKA (DCU) Eco-57</t>
+  </si>
+  <si>
+    <t>1134 PATRIKA (DCU) Eco-58</t>
+  </si>
+  <si>
+    <t>1135 PATRIKA (DCU) Eco-54</t>
+  </si>
+  <si>
+    <t>1136 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1137 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1138 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1139 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1140 PATRIKA (BB)</t>
+  </si>
+  <si>
+    <t>1141 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1142 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1143 PATRIKA (G)</t>
+  </si>
+  <si>
+    <t>1144 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1145 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1146 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1147 PATRIKA (S.201)</t>
+  </si>
+  <si>
+    <t>1148 PATRIKA (S.202)</t>
+  </si>
+  <si>
+    <t>1149 PATRIKA (S.204)</t>
+  </si>
+  <si>
+    <t>1150 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1151 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1152 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1153 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1154 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1155 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1156 PATRIKA-YELLOW</t>
+  </si>
+  <si>
+    <t>1157 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1158 PATRIKA-GOLDEN</t>
+  </si>
+  <si>
+    <t>1159 PATRIKA-WHITE</t>
+  </si>
+  <si>
+    <t>1160 PATRIKA-PINK</t>
+  </si>
+  <si>
+    <t>1161 PATRIKA (01)</t>
+  </si>
+  <si>
+    <t>1162 PATRIKA (02)</t>
+  </si>
+  <si>
+    <t>1163 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1164 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1165 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1166 PATRIKA (DCU)</t>
   </si>
   <si>
     <t>190 NO. ENVELOPES (POCKET)</t>
@@ -407,109 +407,109 @@
     <t>2025- INVITAION (BOX) SAMPLES</t>
   </si>
   <si>
-    <t>2101 PATRIKA (L) (LUXYA - 51)</t>
-  </si>
-  <si>
-    <t>2102 PATRIKA *-* (M) (LUXYA - 52)</t>
-  </si>
-  <si>
-    <t>2103 PATRIKA (L) (LUXYA - 53)</t>
-  </si>
-  <si>
-    <t>2104 PATRIKA (LUXYA - 54)</t>
-  </si>
-  <si>
-    <t>2105 PATRIKA (LUXYA - 55)</t>
-  </si>
-  <si>
-    <t>2106 PATRIKA (L) (LUXYA - 56)</t>
-  </si>
-  <si>
-    <t>2107 PATRIKA *-* (M) (LUXYA - 57)</t>
-  </si>
-  <si>
-    <t>2108 PATRIKA *-* (M) (LUXYA - 59)</t>
-  </si>
-  <si>
-    <t>2109 PATRIKA (L) (LUXYA - 60)</t>
-  </si>
-  <si>
-    <t>2110 PATRIKA (LUXYA - 61)</t>
-  </si>
-  <si>
-    <t>2111 PATRIKA *-* (M) (LUXYA - 62)</t>
-  </si>
-  <si>
-    <t>2112 PATRIKA (L) (LEGACY - 01)</t>
-  </si>
-  <si>
-    <t>2113 PATRIKA (L) (LEGACY - 02)</t>
-  </si>
-  <si>
-    <t>2114 PATRIKA (L) (LEGACY - 03)</t>
-  </si>
-  <si>
-    <t>2115 PATRIKA (L) (LEGACY - 04)</t>
-  </si>
-  <si>
-    <t>2116 PATRIKA (L) (LEGACY - 05)</t>
-  </si>
-  <si>
-    <t>2117 PATRIKA *-* (M) (LEGACY - 06)</t>
-  </si>
-  <si>
-    <t>2118 PATRIKA (L) (LEGACY - 07)</t>
-  </si>
-  <si>
-    <t>2119 PATRIKA (L) (LEGACY - 08)</t>
-  </si>
-  <si>
-    <t>2120 PATRIKA (L) (LEGACY - 09)</t>
-  </si>
-  <si>
-    <t>2121 PATRIKA (LEGACY - 10)</t>
-  </si>
-  <si>
-    <t>2122 PATRIKA (LEGACY - 11)</t>
-  </si>
-  <si>
-    <t>2123 PATRIKA (LEGACY - 12)</t>
-  </si>
-  <si>
-    <t>2124 PATRIKA *-* (M) (LOTTERY - 71)</t>
-  </si>
-  <si>
-    <t>2125 PATRIKA *-* (M) (LOTTERY - 72)</t>
-  </si>
-  <si>
-    <t>2126 PATRIKA *-* (M) (LOTTERY - 73)</t>
-  </si>
-  <si>
-    <t>2127 PATRIKA *-* (M) (LOTTERY - 74)</t>
-  </si>
-  <si>
-    <t>2128 PATRIKA *-* (M) (LOTTERY - 75)</t>
-  </si>
-  <si>
-    <t>2129 PATRIKA *-* (M) (LOTTERY - 76)</t>
-  </si>
-  <si>
-    <t>2130 PATRIKA *-* (M) (LOTTERY - 77)</t>
-  </si>
-  <si>
-    <t>2131 PATRIKA *-* (M) (LOTTERY - 78)</t>
-  </si>
-  <si>
-    <t>2132 PATRIKA *-* (M) (LOTTERY - 79)</t>
-  </si>
-  <si>
-    <t>2133 PATRIKA (LOTTERY - 80)</t>
-  </si>
-  <si>
-    <t>2134 PATRIKA *-* (M) (LOTTERY - 81)</t>
-  </si>
-  <si>
-    <t>2135 PATRIKA *-* (M) (LOTTERY - 82)</t>
+    <t>2101 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2102 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2103 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2104 PATRIKA</t>
+  </si>
+  <si>
+    <t>2105 PATRIKA</t>
+  </si>
+  <si>
+    <t>2106 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2107 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2108 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2109 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2110 PATRIKA</t>
+  </si>
+  <si>
+    <t>2111 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2112 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2113 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2114 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2115 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2116 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2117 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2118 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2119 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2120 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2121 PATRIKA</t>
+  </si>
+  <si>
+    <t>2122 PATRIKA</t>
+  </si>
+  <si>
+    <t>2123 PATRIKA</t>
+  </si>
+  <si>
+    <t>2124 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2125 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2126 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2127 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2128 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2129 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2130 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2131 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2132 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2133 PATRIKA</t>
+  </si>
+  <si>
+    <t>2134 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2135 PATRIKA *-* (M)</t>
   </si>
   <si>
     <t>290 ENVELOPE 25-26</t>
@@ -527,1144 +527,1144 @@
     <t>330 ENVELOPE</t>
   </si>
   <si>
-    <t>4251 PATRIKA (JC) (5342)</t>
-  </si>
-  <si>
-    <t>4252 PATRIKA (5207)</t>
-  </si>
-  <si>
-    <t>4253 PATRIKA (5206)</t>
-  </si>
-  <si>
-    <t>4254 PATRIKA (4210) (10273/10277)</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA - B (DCU) (AS-02 (B))</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA (JC) (AS-02 (NEW))</t>
-  </si>
-  <si>
-    <t>4257 PATRIKA (82)</t>
-  </si>
-  <si>
-    <t>4258 PATRIKA (JC) (1129)</t>
-  </si>
-  <si>
-    <t>4259 PATRIKA (JC) (101 SBC)</t>
-  </si>
-  <si>
-    <t>4260 PATRIKA (1102)</t>
-  </si>
-  <si>
-    <t>4261 PATRIKA (JC) (959)</t>
-  </si>
-  <si>
-    <t>4262 PATRIKA (JC) (S-201 GANESH JI)</t>
-  </si>
-  <si>
-    <t>4264 PATRIKA (DCU) (1351)</t>
-  </si>
-  <si>
-    <t>4265 PATRIKA (83)</t>
-  </si>
-  <si>
-    <t>4266 PATRIKA (25-145)</t>
-  </si>
-  <si>
-    <t>4267 PATRIKA (JC) (25-046)</t>
-  </si>
-  <si>
-    <t>4268 PATRIKA (JC) *-* (M+T) (S-296)</t>
-  </si>
-  <si>
-    <t>4269 PATRIKA (111 SBC)</t>
-  </si>
-  <si>
-    <t>4270 PATRIKA (1151 GGN)</t>
-  </si>
-  <si>
-    <t>4271 PATRIKA (JC) (25216)</t>
-  </si>
-  <si>
-    <t>4272 PATRIKA (JC) (1231 SBC CRM)</t>
-  </si>
-  <si>
-    <t>4273 PATRIKA (2547)</t>
-  </si>
-  <si>
-    <t>4274 PATRIKA (JC) (25369)</t>
-  </si>
-  <si>
-    <t>4275 PATRIKA (25367)</t>
-  </si>
-  <si>
-    <t>4277 PATRIKA (JC) *-* (M) (25365)</t>
-  </si>
-  <si>
-    <t>4278 PATRIKA (25368)</t>
-  </si>
-  <si>
-    <t>4279 PATRIKA (1031)</t>
-  </si>
-  <si>
-    <t>4280 PATRIKA (25301)</t>
-  </si>
-  <si>
-    <t>4281 PATRIKA (25312 MYRA)</t>
-  </si>
-  <si>
-    <t>4282 PATRIKA (3117)</t>
-  </si>
-  <si>
-    <t>4283 PATRIKA - B (YELLOW) (3116-YLW)</t>
-  </si>
-  <si>
-    <t>4284 PATRIKA (1173 VV)</t>
-  </si>
-  <si>
-    <t>4285 PATRIKA (JC) *-* (M) (4626)</t>
-  </si>
-  <si>
-    <t>4286 PATRIKA (5254  RJN)</t>
-  </si>
-  <si>
-    <t>4287 PATRIKA (25402)</t>
-  </si>
-  <si>
-    <t>4288 PATRIKA (10001 NEW)</t>
-  </si>
-  <si>
-    <t>4289 PATRIKA (10002 NEW)</t>
-  </si>
-  <si>
-    <t>4290 PATRIKA (316 MYRA)</t>
-  </si>
-  <si>
-    <t>4291 PATRIKA (25401)</t>
-  </si>
-  <si>
-    <t>4292 PATRIKA (25311)</t>
-  </si>
-  <si>
-    <t>4293 PATRIKA (25312)</t>
-  </si>
-  <si>
-    <t>4294 PATRIKA (5273)</t>
-  </si>
-  <si>
-    <t>4295 PATRIKA (286-A)</t>
-  </si>
-  <si>
-    <t>4296 PATRIKA (1407)</t>
-  </si>
-  <si>
-    <t>4297 PATRIKA (306)</t>
-  </si>
-  <si>
-    <t>4298 PATRIKA (5501)</t>
-  </si>
-  <si>
-    <t>4299 PATRIKA (2011)</t>
-  </si>
-  <si>
-    <t>4300 PATRIKA (25314)</t>
-  </si>
-  <si>
-    <t>4301 PATRIKA (25315)</t>
-  </si>
-  <si>
-    <t>4302 PATRIKA (1402)</t>
-  </si>
-  <si>
-    <t>4303 PATRIKA (JC) (1234*-M)</t>
-  </si>
-  <si>
-    <t>4304 PATRIKA (5172)</t>
-  </si>
-  <si>
-    <t>4305 PATRIKA (25313)</t>
-  </si>
-  <si>
-    <t>4307 PATRIKA (BALAJI 5202)</t>
-  </si>
-  <si>
-    <t>4308 PATRIKA (LOTUS 430)</t>
-  </si>
-  <si>
-    <t>4309 PATRIKA (DCU) (3751 Patta)</t>
-  </si>
-  <si>
-    <t>4310 PATRIKA (DCU) (3752 Swastik)</t>
-  </si>
-  <si>
-    <t>4311 PATRIKA (DCU) (251 KBC)</t>
-  </si>
-  <si>
-    <t>4312 PATRIKA (DCU) (273-A)</t>
-  </si>
-  <si>
-    <t>4314 PATRIKA (DCU) (RED-YELLOW SWASTIK)</t>
-  </si>
-  <si>
-    <t>4315 PATRIKA (DCU) (WHITE-PINK PAN PATA)</t>
-  </si>
-  <si>
-    <t>4316 PATRIKA (DCU) (WHITE -ORANGE PAN PATTA)</t>
-  </si>
-  <si>
-    <t>5051 PATRIKA *-* (M) (5087)</t>
-  </si>
-  <si>
-    <t>5052 PATRIKA (5295)</t>
-  </si>
-  <si>
-    <t>5053 PATRIKA (5213)</t>
-  </si>
-  <si>
-    <t>5054 PATRIKA *-* (M) (25/162)</t>
-  </si>
-  <si>
-    <t>5055 PATRIKA (25/272)</t>
-  </si>
-  <si>
-    <t>5056 PATRIKA (JC) (25/271)</t>
-  </si>
-  <si>
-    <t>5057 PATRIKA (25/171)</t>
-  </si>
-  <si>
-    <t>5058 PATRIKA (8802)</t>
-  </si>
-  <si>
-    <t>5059 PATRIKA (8803)</t>
-  </si>
-  <si>
-    <t>5060 PATRIKA (JC) (7713)</t>
-  </si>
-  <si>
-    <t>5061 PATRIKA (DCU) (1405)</t>
-  </si>
-  <si>
-    <t>5062 PATRIKA (7705)</t>
-  </si>
-  <si>
-    <t>5063 PATRIKA (2522 GE)</t>
-  </si>
-  <si>
-    <t>5064 PATRIKA (2517 GE)</t>
-  </si>
-  <si>
-    <t>5065 PATRIKA (2527)</t>
-  </si>
-  <si>
-    <t>5066 PATRIKA (2536)</t>
-  </si>
-  <si>
-    <t>5067 PATRIKA (JC) (S-301)</t>
-  </si>
-  <si>
-    <t>5071 PATRIKA *-* (डोरी) (741)</t>
-  </si>
-  <si>
-    <t>5072 PATRIKA (5347 DIRECT)</t>
-  </si>
-  <si>
-    <t>5073 PATRIKA *-* (M) (3161)</t>
-  </si>
-  <si>
-    <t>5074 PATRIKA (1151 VV)</t>
-  </si>
-  <si>
-    <t>5075 PATRIKA (JC) (25-082)</t>
-  </si>
-  <si>
-    <t>5076 PATRIKA (JC) (3701 SBC)</t>
-  </si>
-  <si>
-    <t>5077 PATRIKA (2081)</t>
-  </si>
-  <si>
-    <t>5079 PATRIKA (296-A (NEHA)</t>
-  </si>
-  <si>
-    <t>5080 PATRIKA (2501 GE NEW)</t>
-  </si>
-  <si>
-    <t>5081 PATRIKA (2520 GE)</t>
-  </si>
-  <si>
-    <t>5083 PATRIKA (5267)</t>
-  </si>
-  <si>
-    <t>5084 PATRIKA (5258 RJ)</t>
-  </si>
-  <si>
-    <t>5085 PATRIKA (2023)</t>
-  </si>
-  <si>
-    <t>5086 PATRIKA (JC) *-* (M+D) (942)</t>
-  </si>
-  <si>
-    <t>5088 PATRIKA (25214)</t>
-  </si>
-  <si>
-    <t>5089 PATRIKA (2061 SBC)</t>
-  </si>
-  <si>
-    <t>5090 PATRIKA (5236 RJ)</t>
-  </si>
-  <si>
-    <t>5092 PATRIKA (05 NAVIN BHAI)</t>
-  </si>
-  <si>
-    <t>5093 PATRIKA (5350)</t>
-  </si>
-  <si>
-    <t>5094 PATRIKA (5251)</t>
-  </si>
-  <si>
-    <t>5095 PATRIKA (5240)</t>
-  </si>
-  <si>
-    <t>5096 PATRIKA (25316)</t>
-  </si>
-  <si>
-    <t>5097 PATRIKA (25321)</t>
-  </si>
-  <si>
-    <t>5098 PATRIKA *-* (M) (857)</t>
-  </si>
-  <si>
-    <t>5099 PATRIKA *-* (M) (852 DHANESH)</t>
-  </si>
-  <si>
-    <t>5100 PATRIKA (DCU) (5339)</t>
-  </si>
-  <si>
-    <t>5102 PATRIKA (5021) (2456)</t>
-  </si>
-  <si>
-    <t>5103 PATRIKA (2071)</t>
-  </si>
-  <si>
-    <t>5104 PATRIKA (5261 RJND)</t>
-  </si>
-  <si>
-    <t>5105 PATRIKA (JC) (5335)</t>
-  </si>
-  <si>
-    <t>5106 PATRIKA (253-A / 257-A)</t>
-  </si>
-  <si>
-    <t>5107 PATRIKA (5356 RJ)</t>
-  </si>
-  <si>
-    <t>5108 PATRIKA (5333)</t>
-  </si>
-  <si>
-    <t>5109 PATRIKA (5308)</t>
-  </si>
-  <si>
-    <t>5110 PATRIKA (JC) (AS-402)</t>
-  </si>
-  <si>
-    <t>5111 PATRIKA (JC) (5313)</t>
-  </si>
-  <si>
-    <t>5112 PATRIKA (JC) *-* (M) (25437)</t>
-  </si>
-  <si>
-    <t>5113 PATRIKA (5305)</t>
-  </si>
-  <si>
-    <t>5114 PATRIKA *-* (डोरी) (2091)</t>
-  </si>
-  <si>
-    <t>5115 PATRIKA (DCU) (5363 RJND)</t>
-  </si>
-  <si>
-    <t>5116 PATRIKA (2031)</t>
-  </si>
-  <si>
-    <t>5117 PATRIKA (DCU) (3331)</t>
-  </si>
-  <si>
-    <t>5118 PATRIKA (DCU) (25436)</t>
-  </si>
-  <si>
-    <t>5502 PATRIKA *-* (M) (5355 NICE)</t>
-  </si>
-  <si>
-    <t>5503 PATRIKA (5186)</t>
-  </si>
-  <si>
-    <t>5504 PATRIKA (JC) (7033)</t>
-  </si>
-  <si>
-    <t>5505 PATRIKA (JC) *-* (M) (2282)</t>
-  </si>
-  <si>
-    <t>5506 PATRIKA *-* (M) (25/122)</t>
-  </si>
-  <si>
-    <t>5508 PATRIKA (JC) (612 VV)</t>
-  </si>
-  <si>
-    <t>5509 PATRIKA (JC) (25/072)</t>
-  </si>
-  <si>
-    <t>5510 PATRIKA (JC) *-* (M) (AS-950)</t>
-  </si>
-  <si>
-    <t>5511 PATRIKA (JC) *-* (M) (2528)</t>
-  </si>
-  <si>
-    <t>5512 PATRIKA (JC) (2525 /2552)</t>
-  </si>
-  <si>
-    <t>5513 PATRIKA (2515)</t>
-  </si>
-  <si>
-    <t>5514 PATRIKA (2542)</t>
-  </si>
-  <si>
-    <t>5515 PATRIKA (2523)</t>
-  </si>
-  <si>
-    <t>5516 PATRIKA (JC) *-* (M) (5302 VV)</t>
-  </si>
-  <si>
-    <t>5517 PATRIKA *-* (M) (Patti Aayegi) (6301)</t>
-  </si>
-  <si>
-    <t>5518 PATRIKA (JC) *-* (M) (922)</t>
-  </si>
-  <si>
-    <t>5519 PATRIKA *-* (M) (7066)</t>
-  </si>
-  <si>
-    <t>5520 PATRIKA (1054)</t>
-  </si>
-  <si>
-    <t>5521 PATRIKA (JC) *-* (M) (35)</t>
-  </si>
-  <si>
-    <t>5522 PATRIKA (2231)</t>
-  </si>
-  <si>
-    <t>5523 PATRIKA (2232)</t>
-  </si>
-  <si>
-    <t>5524 PATRIKA (DCU) (5382)</t>
-  </si>
-  <si>
-    <t>5525 PATRIKA *-* (M) (5283)</t>
-  </si>
-  <si>
-    <t>5526 PATRIKA (DCU) (NEW LUSTER - 01)</t>
-  </si>
-  <si>
-    <t>5527 PATRIKA (DCU) (NEW LUSTER - 02)</t>
-  </si>
-  <si>
-    <t>5528 PATRIKA *-* (M) (NEW LUSTER - 03)</t>
-  </si>
-  <si>
-    <t>5529 PATRIKA *-* (M) (NEW LUSTER - 04)</t>
-  </si>
-  <si>
-    <t>5530 PATRIKA *-* (M) (NEW LUSTER - 05)</t>
-  </si>
-  <si>
-    <t>5531 PATRIKA (DCU) (NEW LUSTER - 06)</t>
-  </si>
-  <si>
-    <t>5532 PATRIKA *-* (M) (NEW LUSTER - 07)</t>
-  </si>
-  <si>
-    <t>5533 PATRIKA *-* (M) (NEW LUSTER - 08)</t>
-  </si>
-  <si>
-    <t>5534 PATRIKA *-* (M) (NEW LUSTER - 09)</t>
-  </si>
-  <si>
-    <t>5535 PATRIKA (JC) *-* (M) (1007)</t>
-  </si>
-  <si>
-    <t>5537 PATRIKA (JC) (25-052)</t>
-  </si>
-  <si>
-    <t>5538 PATRIKA (JC) *-* (M) (7073)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA-B (2942-B)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA (JC) (2942)</t>
-  </si>
-  <si>
-    <t>5540 PATRIKA *-* (M) (S-96)</t>
-  </si>
-  <si>
-    <t>5542 PATRIKA (2261)</t>
-  </si>
-  <si>
-    <t>5543 PATRIKA (2353)</t>
-  </si>
-  <si>
-    <t>5544 PATRIKA *-* (M) (2732)</t>
-  </si>
-  <si>
-    <t>5545 PATRIKA *-* (M) (2791)</t>
-  </si>
-  <si>
-    <t>5546 PATRIKA (718)</t>
-  </si>
-  <si>
-    <t>5547 PATRIKA *-* (M) (S-32)</t>
-  </si>
-  <si>
-    <t>5548 PATRIKA (DCU) (2792)</t>
-  </si>
-  <si>
-    <t>5549 PATRIKA (5261 NICE)</t>
-  </si>
-  <si>
-    <t>5550 PATRIKA *-* (M) (5424)</t>
-  </si>
-  <si>
-    <t>5551 PATRIKA (5231)</t>
-  </si>
-  <si>
-    <t>5552 PATRIKA (JC) *-* (M) (S-163)</t>
-  </si>
-  <si>
-    <t>5553 PATRIKA *-* (M) (5004)</t>
-  </si>
-  <si>
-    <t>5554 PATRIKA *-* (F/G) (5379)</t>
-  </si>
-  <si>
-    <t>5555 PATRIKA (2903)</t>
-  </si>
-  <si>
-    <t>5556 PATRIKA *-* (M) (2952)</t>
-  </si>
-  <si>
-    <t>5557 PATRIKA (2312 SBC)</t>
-  </si>
-  <si>
-    <t>5558 PATRIKA *-* (M) (121 NEHA)</t>
-  </si>
-  <si>
-    <t>5559 PATRIKA (2293)</t>
-  </si>
-  <si>
-    <t>5560 PATRIKA (F/G) *-* (2915)</t>
-  </si>
-  <si>
-    <t>5561 PATRIKA *-* (M) (25358)</t>
-  </si>
-  <si>
-    <t>5562 PATRIKA *-* (M) (114-B (NEHA))</t>
-  </si>
-  <si>
-    <t>5563 PATRIKA (5387)</t>
-  </si>
-  <si>
-    <t>5564 PATRIKA (JC) *-* (M) (S-107)</t>
-  </si>
-  <si>
-    <t>5565 PATRIKA (175)</t>
-  </si>
-  <si>
-    <t>5566 PATRIKA *-* (M) (1742-B)</t>
-  </si>
-  <si>
-    <t>5567 PATRIKA (1679)</t>
-  </si>
-  <si>
-    <t>5568 PATRIKA *-* (M) (3002)</t>
-  </si>
-  <si>
-    <t>5569 PATRIKA *-* (M) (S-39)</t>
-  </si>
-  <si>
-    <t>5570 PATRIKA *-* (M) (S-74)</t>
-  </si>
-  <si>
-    <t>5571 PATRIKA *-* (M) (25353)</t>
-  </si>
-  <si>
-    <t>5572 PATRIKA *-* (M) (25351)</t>
-  </si>
-  <si>
-    <t>5573 PATRIKA (2205)</t>
-  </si>
-  <si>
-    <t>5574 PATRIKA (25335)</t>
-  </si>
-  <si>
-    <t>5575 PATRIKA *-* (M) (S-77)</t>
-  </si>
-  <si>
-    <t>5576 PATRIKA (2531)</t>
-  </si>
-  <si>
-    <t>5577 PATRIKA *-* (M) (5808)</t>
-  </si>
-  <si>
-    <t>5578 PATRIKA (JC) *-* (M) (AS-104 / S-50)</t>
-  </si>
-  <si>
-    <t>5579 PATRIKA (JC) *-* (M) (AS-102)</t>
-  </si>
-  <si>
-    <t>5580 PATRIKA (S-326)</t>
-  </si>
-  <si>
-    <t>5581 PATRIKA *-* (M) (3471)</t>
-  </si>
-  <si>
-    <t>5582 PATRIKA *-* (M) (3512 SBC)</t>
-  </si>
-  <si>
-    <t>5583 PATRIKA (3211 SBC)</t>
-  </si>
-  <si>
-    <t>5584 PATRIKA (JC) (2202 SBC)</t>
-  </si>
-  <si>
-    <t>5585 PATRIKA *-* (M) (1201 KBC)</t>
-  </si>
-  <si>
-    <t>5586 PATRIKA *-* (M) (S-51)</t>
-  </si>
-  <si>
-    <t>5587 PATRIKA (2264)</t>
-  </si>
-  <si>
-    <t>5588 PATRIKA (JC) *-* (M) (1006)</t>
-  </si>
-  <si>
-    <t>5589 PATRIKA *-* (M) (25133)</t>
-  </si>
-  <si>
-    <t>5590 PATRIKA (3131 SBC)</t>
-  </si>
-  <si>
-    <t>5592 PATRIKA *-* (M) (2365)</t>
-  </si>
-  <si>
-    <t>5593 PATRIKA (2803)</t>
-  </si>
-  <si>
-    <t>5595 PATRIKA *-* (M) (226)</t>
-  </si>
-  <si>
-    <t>5596 PATRIKA *-* (M) (2541)</t>
-  </si>
-  <si>
-    <t>5597 PATRIKA (JC) *-* (M) (AS-104 (B))</t>
-  </si>
-  <si>
-    <t>5599 PATRIKA *-* (M) (77-B)</t>
-  </si>
-  <si>
-    <t>5601 PATRIKA (2771)</t>
-  </si>
-  <si>
-    <t>5602 PATRIKA (3271)</t>
-  </si>
-  <si>
-    <t>5603 PATRIKA *-* (M) (6125)</t>
-  </si>
-  <si>
-    <t>5604 PATRIKA (242-A)</t>
-  </si>
-  <si>
-    <t>5605 PATRIKA (JC) (3102)</t>
-  </si>
-  <si>
-    <t>5606 PATRIKA *-* (M) (221-A)</t>
-  </si>
-  <si>
-    <t>5607 PATRIKA (25442)</t>
-  </si>
-  <si>
-    <t>5608 PATRIKA (25440)</t>
-  </si>
-  <si>
-    <t>5609 PATRIKA (993)</t>
-  </si>
-  <si>
-    <t>5610 PATRIKA (JC) (2373)</t>
-  </si>
-  <si>
-    <t>5611 PATRIKA *-* (M) (1211)</t>
-  </si>
-  <si>
-    <t>5612 PATRIKA (DCU) (5276)</t>
-  </si>
-  <si>
-    <t>5614 PATRIKA *-* (M) (2331)</t>
-  </si>
-  <si>
-    <t>5615 PATRIKA (2111)</t>
-  </si>
-  <si>
-    <t>5616 PATRIKA (DCU) (7069)</t>
-  </si>
-  <si>
-    <t>5617 PATRIKA *-* (M) (7067)</t>
-  </si>
-  <si>
-    <t>5618 PATRIKA (JC) *-* (M) (S-52)</t>
-  </si>
-  <si>
-    <t>5619 PATRIKA (JC) (1131)</t>
-  </si>
-  <si>
-    <t>5621 PATRIKA (JC) *-* (M) (5297)</t>
-  </si>
-  <si>
-    <t>5622 PATRIKA *-* (M) (25337)</t>
-  </si>
-  <si>
-    <t>5623 PATRIKA (064)</t>
-  </si>
-  <si>
-    <t>5625 PATRIKA (DCU) (772)</t>
-  </si>
-  <si>
-    <t>6601 PATRIKA (L) (5164)</t>
-  </si>
-  <si>
-    <t>6602 PATRIKA (5126)</t>
-  </si>
-  <si>
-    <t>6603 PATRIKA (5111)</t>
-  </si>
-  <si>
-    <t>6604 PATRIKA *-* (M) (5196)</t>
-  </si>
-  <si>
-    <t>6605 PATRIKA (5191)</t>
-  </si>
-  <si>
-    <t>6606 PATRIKA (*-*) R (3023)</t>
-  </si>
-  <si>
-    <t>6607 PATRIKA *-* (M) (0523)</t>
-  </si>
-  <si>
-    <t>6608 PATRIKA (95)</t>
-  </si>
-  <si>
-    <t>6609 PATRIKA *-* (M) (3053)</t>
-  </si>
-  <si>
-    <t>6610 PATRIKA *-* (M) (3019)</t>
-  </si>
-  <si>
-    <t>6611 PATRIKA (3017 VV)</t>
-  </si>
-  <si>
-    <t>6612 PATRIKA (3015)</t>
-  </si>
-  <si>
-    <t>6613 PATRIKA (25164)</t>
-  </si>
-  <si>
-    <t>6614 PATRIKA (DCU) (25131)</t>
-  </si>
-  <si>
-    <t>6615 PATRIKA *-* (M) (915 GAGAN)</t>
-  </si>
-  <si>
-    <t>6616 PATRIKA *-* (M) (911 GAGAN)</t>
-  </si>
-  <si>
-    <t>6617 PATRIKA *-* (M) (3422)</t>
-  </si>
-  <si>
-    <t>6618 PATRIKA *-* (M) (3423)</t>
-  </si>
-  <si>
-    <t>6619 PATRIKA *-* (M) (1193)</t>
-  </si>
-  <si>
-    <t>6620 PATRIKA *-* (M) (1045 GGN (PADDING))</t>
-  </si>
-  <si>
-    <t>6621 PATRIKA *-* (M) (7108 (PADDING))</t>
-  </si>
-  <si>
-    <t>6622 PATRIKA *-* (M) (7259 (PADDING))</t>
-  </si>
-  <si>
-    <t>6623 PATRIKA (25184)</t>
-  </si>
-  <si>
-    <t>6624 PATRIKA *-* (M) (25135)</t>
-  </si>
-  <si>
-    <t>6625 PATRIKA *-* (M) (25116)</t>
-  </si>
-  <si>
-    <t>6626 PATRIKA *-* (M) (25161)</t>
-  </si>
-  <si>
-    <t>6627 PATRIKA *-* (M) (25111)</t>
-  </si>
-  <si>
-    <t>6628 PATRIKA *-* (M) (805 SBC)</t>
-  </si>
-  <si>
-    <t>6629 PATRIKA *-* (M) (812 NEW SBC)</t>
-  </si>
-  <si>
-    <t>6630 PATRIKA *-* (M) (5510 NICE)</t>
-  </si>
-  <si>
-    <t>6631 PATRIKA (DCU) (OLD AP ITEM)</t>
-  </si>
-  <si>
-    <t>6632 PATRIKA (DCU) (932)</t>
-  </si>
-  <si>
-    <t>6633 PATRIKA *-* (M) (7081 VP)</t>
-  </si>
-  <si>
-    <t>6634 PATRIKA (3562)</t>
-  </si>
-  <si>
-    <t>6635 PATRIKA *-* (M) (S-313)</t>
-  </si>
-  <si>
-    <t>6636 PATRIKA *-* (M) (25183)</t>
-  </si>
-  <si>
-    <t>6637 PATRIKA (25162 GE)</t>
-  </si>
-  <si>
-    <t>6638 PATRIKA *-* (M) (3014)</t>
-  </si>
-  <si>
-    <t>6639 PATRIKA (B) (2291-B)</t>
-  </si>
-  <si>
-    <t>6640 PATRIKA *-* (M) (5737 PADING)</t>
-  </si>
-  <si>
-    <t>6641 PATRIKA *-* (M) (5435)</t>
-  </si>
-  <si>
-    <t>6642 PATRIKA *-* (M) (5411 RJ)</t>
-  </si>
-  <si>
-    <t>6643 PATRIKA *-* (M) (25380)</t>
-  </si>
-  <si>
-    <t>6644 PATRIKA (DCU) (25132)</t>
-  </si>
-  <si>
-    <t>6645 PATRIKA *-* (M) (3031)</t>
-  </si>
-  <si>
-    <t>6646 PATRIKA *-* (M) (3034)</t>
-  </si>
-  <si>
-    <t>6647 PATRIKA *-* (M) (25382)</t>
-  </si>
-  <si>
-    <t>6648 PATRIKA *-* (M) (5011 (PADDING))</t>
-  </si>
-  <si>
-    <t>6649 PATRIKA *-* (M) (3402)</t>
-  </si>
-  <si>
-    <t>6650 PATRIKA *-* (M) (3431)</t>
-  </si>
-  <si>
-    <t>6651 PATRIKA (3421)</t>
-  </si>
-  <si>
-    <t>6652 PATRIKA *-* (M) (2764 SBC)</t>
-  </si>
-  <si>
-    <t>6653 PATRIKA *-* (M) (834 SBC NEW)</t>
-  </si>
-  <si>
-    <t>6654 PATRIKA *-* (M) (3461)</t>
-  </si>
-  <si>
-    <t>6655 PATRIKA *-* (M) (7129 (PADDING))</t>
-  </si>
-  <si>
-    <t>6656 PATRIKA (L) (7113 (PADDING))</t>
-  </si>
-  <si>
-    <t>6657 PATRIKA *-* (M) (563  DHANESH)</t>
-  </si>
-  <si>
-    <t>6658 PATRIKA *-* (M) (5319)</t>
-  </si>
-  <si>
-    <t>6659 PATRIKA (25193 (Padding))</t>
-  </si>
-  <si>
-    <t>6660 PATRIKA (25194 (Padding))</t>
-  </si>
-  <si>
-    <t>6661 PATRIKA *-* (M) (1281)</t>
-  </si>
-  <si>
-    <t>6662 PATRIKA (3424)</t>
-  </si>
-  <si>
-    <t>6663 PATRIKA (7103 (PADDING))</t>
-  </si>
-  <si>
-    <t>6664 PATRIKA *-* (M) (5823)</t>
-  </si>
-  <si>
-    <t>6665 PATRIKA *-* (M) (603 DHANESH)</t>
-  </si>
-  <si>
-    <t>6667 PATRIKA *-* (M) (1192 SBC)</t>
-  </si>
-  <si>
-    <t>6668 PATRIKA (DCU) (8102)</t>
-  </si>
-  <si>
-    <t>6669 PATRIKA (DCU) (6197)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA - B (M) (1868-B)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA *-* (M) (1868)</t>
-  </si>
-  <si>
-    <t>6671 PATRIKA *-* (M) (1872)</t>
-  </si>
-  <si>
-    <t>6672 PATRIKA *-* (M) (6132)</t>
-  </si>
-  <si>
-    <t>6673 PATRIKA (DCU) (6196)</t>
-  </si>
-  <si>
-    <t>6674 PATRIKA (DCU) (1503)</t>
-  </si>
-  <si>
-    <t>6675 PATRIKA *-* (M) (1282)</t>
-  </si>
-  <si>
-    <t>6676 PATRIKA (DCU) (533 KBC)</t>
-  </si>
-  <si>
-    <t>6677 PATRIKA (DCU) (25191 PADDING)</t>
-  </si>
-  <si>
-    <t>7265 PATRIKA (O.C.) (133)</t>
-  </si>
-  <si>
-    <t>7283 PATRIKA {F} (O.C.) (4148)</t>
-  </si>
-  <si>
-    <t>7287 PATRIKA (O.C.) (1522)</t>
-  </si>
-  <si>
-    <t>7288 PATRIKA (O.C.) (1178)</t>
-  </si>
-  <si>
-    <t>7293 PATRIKA (O.C.) (AS-20)</t>
-  </si>
-  <si>
-    <t>7309 PATRIKA (O.C.) (4087)</t>
-  </si>
-  <si>
-    <t>7312 PATRIKA (O.C.) (SBC 7312)</t>
-  </si>
-  <si>
-    <t>7319 PATRIKA (O.C.) (2204)</t>
-  </si>
-  <si>
-    <t>7332 PATRIKA (O.C.) (2482)</t>
-  </si>
-  <si>
-    <t>7342 PATRIKA (O.C.) (12)</t>
-  </si>
-  <si>
-    <t>7344 PATRIKA (O.C.) (INV B.P. RED (11))</t>
-  </si>
-  <si>
-    <t>7345 PATRIKA (O.C.) (INV B.P. GOLDEN (120) 5)</t>
-  </si>
-  <si>
-    <t>7401 PATRIKA (25/252)</t>
-  </si>
-  <si>
-    <t>7402 PATRIKA (25/264-263)</t>
-  </si>
-  <si>
-    <t>7403 PATRIKA (25/363/863)</t>
-  </si>
-  <si>
-    <t>7404 PATRIKA (25/283)</t>
-  </si>
-  <si>
-    <t>7405 PATRIKA (25/273)</t>
-  </si>
-  <si>
-    <t>7406 PATRIKA (25/172)</t>
-  </si>
-  <si>
-    <t>7407 PATRIKA *-* (F) (7145 VP)</t>
-  </si>
-  <si>
-    <t>7408 PATRIKA (DCU) (25895)</t>
-  </si>
-  <si>
-    <t>7409 PATRIKA (2521)</t>
-  </si>
-  <si>
-    <t>7410 PATRIKA (2526)</t>
-  </si>
-  <si>
-    <t>7411 PATRIKA (2535)</t>
-  </si>
-  <si>
-    <t>7413 PATRIKA (2543 INV OFFSET)</t>
-  </si>
-  <si>
-    <t>7414 PATRIKA (1015 GREEN OFFSET)</t>
-  </si>
-  <si>
-    <t>7415 PATRIKA *-* (F) (3162 SBC)</t>
-  </si>
-  <si>
-    <t>7416 PATRIKA (2234)</t>
-  </si>
-  <si>
-    <t>7417 PATRIKA (S-201 INV)</t>
-  </si>
-  <si>
-    <t>7418 PATRIKA *-* (डोरी) (1639)</t>
-  </si>
-  <si>
-    <t>7419 PATRIKA (5121)</t>
-  </si>
-  <si>
-    <t>7420 PATRIKA (720)</t>
-  </si>
-  <si>
-    <t>7421 PATRIKA *-* (F) (25-146)</t>
-  </si>
-  <si>
-    <t>7422 PATRIKA (3702)</t>
-  </si>
-  <si>
-    <t>7423 PATRIKA (254 SBC)</t>
-  </si>
-  <si>
-    <t>7424 PATRIKA *-* (F) (25-047)</t>
-  </si>
-  <si>
-    <t>7425 PATRIKA (2082)</t>
-  </si>
-  <si>
-    <t>7426 PATRIKA (F/G) *-* (4052)</t>
-  </si>
-  <si>
-    <t>7427 PATRIKA (2103)</t>
-  </si>
-  <si>
-    <t>7428 PATRIKA (1223 SBC)</t>
-  </si>
-  <si>
-    <t>7429 PATRIKA (F/G) *-* (1851 MONARCH)</t>
-  </si>
-  <si>
-    <t>7430 PATRIKA (6310 GE)</t>
-  </si>
-  <si>
-    <t>7431 PATRIKA (2532)</t>
-  </si>
-  <si>
-    <t>7432 PATRIKA (1174)</t>
-  </si>
-  <si>
-    <t>7433 PATRIKA (1034)</t>
-  </si>
-  <si>
-    <t>7434 PATRIKA (2204 INV)</t>
-  </si>
-  <si>
-    <t>7435 PATRIKA (06)</t>
-  </si>
-  <si>
-    <t>7436 PATRIKA (303)</t>
-  </si>
-  <si>
-    <t>7437 PATRIKA (25323 INV)</t>
-  </si>
-  <si>
-    <t>7438 PATRIKA (25413)</t>
-  </si>
-  <si>
-    <t>7439 PATRIKA (2597)</t>
-  </si>
-  <si>
-    <t>7440 PATRIKA (25896)</t>
-  </si>
-  <si>
-    <t>7441 PATRIKA *-* (F) (243-C)</t>
-  </si>
-  <si>
-    <t>7442 PATRIKA (1855)</t>
-  </si>
-  <si>
-    <t>7443 PATRIKA (1044 SBC)</t>
-  </si>
-  <si>
-    <t>7444 PATRIKA (2014)</t>
-  </si>
-  <si>
-    <t>7445 PATRIKA (2006)</t>
-  </si>
-  <si>
-    <t>7446 PATRIKA (DCU) (6106)</t>
-  </si>
-  <si>
-    <t>7447 PATRIKA (GOPAL 32)</t>
-  </si>
-  <si>
-    <t>7448 PATRIKA (2005- G)</t>
-  </si>
-  <si>
-    <t>7449 PATRIKA (5180)</t>
-  </si>
-  <si>
-    <t>7450 PATRIKA (DCU) (3753)</t>
-  </si>
-  <si>
-    <t>7451 PATRIKA (273 NEHA)</t>
-  </si>
-  <si>
-    <t>7452 PATRIKA (278-B)</t>
-  </si>
-  <si>
-    <t>7453 PATRIKA (ECO - 61) (NEW ECO 61)</t>
-  </si>
-  <si>
-    <t>7454 PATRIKA (ECO -63) (NEW ECO 63)</t>
-  </si>
-  <si>
-    <t>9001 CARD (O.C.) (2498 Cream)</t>
+    <t>4251 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4252 PATRIKA</t>
+  </si>
+  <si>
+    <t>4253 PATRIKA</t>
+  </si>
+  <si>
+    <t>4254 PATRIKA (4210)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4257 PATRIKA</t>
+  </si>
+  <si>
+    <t>4258 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4259 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4260 PATRIKA</t>
+  </si>
+  <si>
+    <t>4261 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4262 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4264 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4265 PATRIKA</t>
+  </si>
+  <si>
+    <t>4266 PATRIKA</t>
+  </si>
+  <si>
+    <t>4267 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4268 PATRIKA (JC) *-* (M+T)</t>
+  </si>
+  <si>
+    <t>4269 PATRIKA</t>
+  </si>
+  <si>
+    <t>4270 PATRIKA</t>
+  </si>
+  <si>
+    <t>4271 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4272 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4273 PATRIKA</t>
+  </si>
+  <si>
+    <t>4274 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4275 PATRIKA</t>
+  </si>
+  <si>
+    <t>4277 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4278 PATRIKA</t>
+  </si>
+  <si>
+    <t>4279 PATRIKA</t>
+  </si>
+  <si>
+    <t>4280 PATRIKA</t>
+  </si>
+  <si>
+    <t>4281 PATRIKA</t>
+  </si>
+  <si>
+    <t>4282 PATRIKA</t>
+  </si>
+  <si>
+    <t>4283 PATRIKA - B (YELLOW)</t>
+  </si>
+  <si>
+    <t>4284 PATRIKA</t>
+  </si>
+  <si>
+    <t>4285 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4286 PATRIKA</t>
+  </si>
+  <si>
+    <t>4287 PATRIKA</t>
+  </si>
+  <si>
+    <t>4288 PATRIKA</t>
+  </si>
+  <si>
+    <t>4289 PATRIKA</t>
+  </si>
+  <si>
+    <t>4290 PATRIKA</t>
+  </si>
+  <si>
+    <t>4291 PATRIKA</t>
+  </si>
+  <si>
+    <t>4292 PATRIKA</t>
+  </si>
+  <si>
+    <t>4293 PATRIKA</t>
+  </si>
+  <si>
+    <t>4294 PATRIKA</t>
+  </si>
+  <si>
+    <t>4295 PATRIKA</t>
+  </si>
+  <si>
+    <t>4296 PATRIKA</t>
+  </si>
+  <si>
+    <t>4297 PATRIKA</t>
+  </si>
+  <si>
+    <t>4298 PATRIKA</t>
+  </si>
+  <si>
+    <t>4299 PATRIKA</t>
+  </si>
+  <si>
+    <t>4300 PATRIKA</t>
+  </si>
+  <si>
+    <t>4301 PATRIKA</t>
+  </si>
+  <si>
+    <t>4302 PATRIKA</t>
+  </si>
+  <si>
+    <t>4303 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4304 PATRIKA</t>
+  </si>
+  <si>
+    <t>4305 PATRIKA</t>
+  </si>
+  <si>
+    <t>4307 PATRIKA</t>
+  </si>
+  <si>
+    <t>4308 PATRIKA</t>
+  </si>
+  <si>
+    <t>4309 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4310 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4311 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4312 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4314 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4315 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4316 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5051 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5052 PATRIKA</t>
+  </si>
+  <si>
+    <t>5053 PATRIKA</t>
+  </si>
+  <si>
+    <t>5054 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5055 PATRIKA</t>
+  </si>
+  <si>
+    <t>5056 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5057 PATRIKA</t>
+  </si>
+  <si>
+    <t>5058 PATRIKA</t>
+  </si>
+  <si>
+    <t>5059 PATRIKA</t>
+  </si>
+  <si>
+    <t>5060 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5061 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5062 PATRIKA</t>
+  </si>
+  <si>
+    <t>5063 PATRIKA</t>
+  </si>
+  <si>
+    <t>5064 PATRIKA</t>
+  </si>
+  <si>
+    <t>5065 PATRIKA</t>
+  </si>
+  <si>
+    <t>5066 PATRIKA</t>
+  </si>
+  <si>
+    <t>5067 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5071 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5072 PATRIKA</t>
+  </si>
+  <si>
+    <t>5073 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5074 PATRIKA</t>
+  </si>
+  <si>
+    <t>5075 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5076 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5077 PATRIKA</t>
+  </si>
+  <si>
+    <t>5079 PATRIKA</t>
+  </si>
+  <si>
+    <t>5080 PATRIKA</t>
+  </si>
+  <si>
+    <t>5081 PATRIKA</t>
+  </si>
+  <si>
+    <t>5083 PATRIKA</t>
+  </si>
+  <si>
+    <t>5084 PATRIKA</t>
+  </si>
+  <si>
+    <t>5085 PATRIKA</t>
+  </si>
+  <si>
+    <t>5086 PATRIKA (JC) *-* (M+D)</t>
+  </si>
+  <si>
+    <t>5088 PATRIKA</t>
+  </si>
+  <si>
+    <t>5089 PATRIKA</t>
+  </si>
+  <si>
+    <t>5090 PATRIKA</t>
+  </si>
+  <si>
+    <t>5092 PATRIKA</t>
+  </si>
+  <si>
+    <t>5093 PATRIKA</t>
+  </si>
+  <si>
+    <t>5094 PATRIKA</t>
+  </si>
+  <si>
+    <t>5095 PATRIKA</t>
+  </si>
+  <si>
+    <t>5096 PATRIKA</t>
+  </si>
+  <si>
+    <t>5097 PATRIKA</t>
+  </si>
+  <si>
+    <t>5098 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5099 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5100 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5102 PATRIKA (5021)</t>
+  </si>
+  <si>
+    <t>5103 PATRIKA</t>
+  </si>
+  <si>
+    <t>5104 PATRIKA</t>
+  </si>
+  <si>
+    <t>5105 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5106 PATRIKA</t>
+  </si>
+  <si>
+    <t>5107 PATRIKA</t>
+  </si>
+  <si>
+    <t>5108 PATRIKA</t>
+  </si>
+  <si>
+    <t>5109 PATRIKA</t>
+  </si>
+  <si>
+    <t>5110 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5111 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5112 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5113 PATRIKA</t>
+  </si>
+  <si>
+    <t>5114 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5115 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5116 PATRIKA</t>
+  </si>
+  <si>
+    <t>5117 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5118 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5502 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5503 PATRIKA</t>
+  </si>
+  <si>
+    <t>5504 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5505 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5506 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5508 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5509 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5510 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5511 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5512 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5513 PATRIKA</t>
+  </si>
+  <si>
+    <t>5514 PATRIKA</t>
+  </si>
+  <si>
+    <t>5515 PATRIKA</t>
+  </si>
+  <si>
+    <t>5516 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5517 PATRIKA *-* (M) (Patti Aayegi)</t>
+  </si>
+  <si>
+    <t>5518 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5519 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5520 PATRIKA</t>
+  </si>
+  <si>
+    <t>5521 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5522 PATRIKA</t>
+  </si>
+  <si>
+    <t>5523 PATRIKA</t>
+  </si>
+  <si>
+    <t>5524 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5525 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5526 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5527 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5528 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5529 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5530 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5531 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5532 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5533 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5534 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5535 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5537 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5538 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA-B</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5540 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5542 PATRIKA</t>
+  </si>
+  <si>
+    <t>5543 PATRIKA</t>
+  </si>
+  <si>
+    <t>5544 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5545 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5546 PATRIKA</t>
+  </si>
+  <si>
+    <t>5547 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5548 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5549 PATRIKA</t>
+  </si>
+  <si>
+    <t>5550 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5551 PATRIKA</t>
+  </si>
+  <si>
+    <t>5552 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5553 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5554 PATRIKA *-* (F/G)</t>
+  </si>
+  <si>
+    <t>5555 PATRIKA</t>
+  </si>
+  <si>
+    <t>5556 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5557 PATRIKA</t>
+  </si>
+  <si>
+    <t>5558 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5559 PATRIKA</t>
+  </si>
+  <si>
+    <t>5560 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>5561 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5562 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5563 PATRIKA</t>
+  </si>
+  <si>
+    <t>5564 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5565 PATRIKA</t>
+  </si>
+  <si>
+    <t>5566 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5567 PATRIKA</t>
+  </si>
+  <si>
+    <t>5568 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5569 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5570 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5571 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5572 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5573 PATRIKA</t>
+  </si>
+  <si>
+    <t>5574 PATRIKA</t>
+  </si>
+  <si>
+    <t>5575 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5576 PATRIKA</t>
+  </si>
+  <si>
+    <t>5577 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5578 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5579 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5580 PATRIKA</t>
+  </si>
+  <si>
+    <t>5581 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5582 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5583 PATRIKA</t>
+  </si>
+  <si>
+    <t>5584 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5585 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5586 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5587 PATRIKA</t>
+  </si>
+  <si>
+    <t>5588 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5589 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5590 PATRIKA</t>
+  </si>
+  <si>
+    <t>5592 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5593 PATRIKA</t>
+  </si>
+  <si>
+    <t>5595 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5596 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5597 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5599 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5601 PATRIKA</t>
+  </si>
+  <si>
+    <t>5602 PATRIKA</t>
+  </si>
+  <si>
+    <t>5603 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5604 PATRIKA</t>
+  </si>
+  <si>
+    <t>5605 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5606 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5607 PATRIKA</t>
+  </si>
+  <si>
+    <t>5608 PATRIKA</t>
+  </si>
+  <si>
+    <t>5609 PATRIKA</t>
+  </si>
+  <si>
+    <t>5610 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5611 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5612 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5614 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5615 PATRIKA</t>
+  </si>
+  <si>
+    <t>5616 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5618 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5619 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5621 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5623 PATRIKA</t>
+  </si>
+  <si>
+    <t>5625 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6601 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6602 PATRIKA</t>
+  </si>
+  <si>
+    <t>6603 PATRIKA</t>
+  </si>
+  <si>
+    <t>6604 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6605 PATRIKA</t>
+  </si>
+  <si>
+    <t>6606 PATRIKA (*-*) R</t>
+  </si>
+  <si>
+    <t>6607 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6608 PATRIKA</t>
+  </si>
+  <si>
+    <t>6609 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6610 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6611 PATRIKA</t>
+  </si>
+  <si>
+    <t>6612 PATRIKA</t>
+  </si>
+  <si>
+    <t>6613 PATRIKA</t>
+  </si>
+  <si>
+    <t>6614 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6615 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6616 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6618 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6619 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6620 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6621 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6623 PATRIKA</t>
+  </si>
+  <si>
+    <t>6624 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6625 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6626 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6627 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6628 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6629 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6630 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6631 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6632 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6633 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6634 PATRIKA</t>
+  </si>
+  <si>
+    <t>6635 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6636 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6637 PATRIKA</t>
+  </si>
+  <si>
+    <t>6638 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6639 PATRIKA (B)</t>
+  </si>
+  <si>
+    <t>6640 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6641 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6642 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6643 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6644 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6645 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6646 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6647 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6648 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6649 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6650 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6651 PATRIKA</t>
+  </si>
+  <si>
+    <t>6652 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6653 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6654 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6655 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6656 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6657 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6658 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6659 PATRIKA</t>
+  </si>
+  <si>
+    <t>6660 PATRIKA</t>
+  </si>
+  <si>
+    <t>6661 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6662 PATRIKA</t>
+  </si>
+  <si>
+    <t>6663 PATRIKA</t>
+  </si>
+  <si>
+    <t>6664 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6665 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6667 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6668 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6669 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA - B (M)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6671 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6672 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6673 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6674 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6675 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6676 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6677 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7265 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7283 PATRIKA {F} (O.C.)</t>
+  </si>
+  <si>
+    <t>7287 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7288 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7293 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7309 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7312 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7319 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7332 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7342 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7344 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7345 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7401 PATRIKA</t>
+  </si>
+  <si>
+    <t>7402 PATRIKA</t>
+  </si>
+  <si>
+    <t>7403 PATRIKA</t>
+  </si>
+  <si>
+    <t>7404 PATRIKA</t>
+  </si>
+  <si>
+    <t>7405 PATRIKA</t>
+  </si>
+  <si>
+    <t>7406 PATRIKA</t>
+  </si>
+  <si>
+    <t>7407 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7408 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7409 PATRIKA</t>
+  </si>
+  <si>
+    <t>7410 PATRIKA</t>
+  </si>
+  <si>
+    <t>7411 PATRIKA</t>
+  </si>
+  <si>
+    <t>7413 PATRIKA</t>
+  </si>
+  <si>
+    <t>7414 PATRIKA</t>
+  </si>
+  <si>
+    <t>7415 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7416 PATRIKA</t>
+  </si>
+  <si>
+    <t>7417 PATRIKA</t>
+  </si>
+  <si>
+    <t>7418 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>7419 PATRIKA</t>
+  </si>
+  <si>
+    <t>7420 PATRIKA</t>
+  </si>
+  <si>
+    <t>7421 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7422 PATRIKA</t>
+  </si>
+  <si>
+    <t>7423 PATRIKA</t>
+  </si>
+  <si>
+    <t>7424 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7425 PATRIKA</t>
+  </si>
+  <si>
+    <t>7426 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7427 PATRIKA</t>
+  </si>
+  <si>
+    <t>7428 PATRIKA</t>
+  </si>
+  <si>
+    <t>7429 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7430 PATRIKA</t>
+  </si>
+  <si>
+    <t>7431 PATRIKA</t>
+  </si>
+  <si>
+    <t>7432 PATRIKA</t>
+  </si>
+  <si>
+    <t>7433 PATRIKA</t>
+  </si>
+  <si>
+    <t>7434 PATRIKA</t>
+  </si>
+  <si>
+    <t>7435 PATRIKA</t>
+  </si>
+  <si>
+    <t>7436 PATRIKA</t>
+  </si>
+  <si>
+    <t>7437 PATRIKA</t>
+  </si>
+  <si>
+    <t>7438 PATRIKA</t>
+  </si>
+  <si>
+    <t>7439 PATRIKA</t>
+  </si>
+  <si>
+    <t>7440 PATRIKA</t>
+  </si>
+  <si>
+    <t>7441 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7442 PATRIKA</t>
+  </si>
+  <si>
+    <t>7443 PATRIKA</t>
+  </si>
+  <si>
+    <t>7444 PATRIKA</t>
+  </si>
+  <si>
+    <t>7445 PATRIKA</t>
+  </si>
+  <si>
+    <t>7446 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7447 PATRIKA</t>
+  </si>
+  <si>
+    <t>7448 PATRIKA</t>
+  </si>
+  <si>
+    <t>7449 PATRIKA</t>
+  </si>
+  <si>
+    <t>7450 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7451 PATRIKA</t>
+  </si>
+  <si>
+    <t>7452 PATRIKA</t>
+  </si>
+  <si>
+    <t>7453 PATRIKA (ECO - 61)</t>
+  </si>
+  <si>
+    <t>7454 PATRIKA (ECO -63)</t>
+  </si>
+  <si>
+    <t>9001 CARD (O.C.)</t>
   </si>
   <si>
     <t>9221 CARDS - YELLOW</t>
@@ -1688,268 +1688,268 @@
     <t>9227 CARDS (9*5 OFFSET)</t>
   </si>
   <si>
-    <t>9228 CARDS (Y) (ORANGE WITH ONLY FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS - B (DCU) (GOLDEN WITH GANESH JI &amp; FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS (C) (CREAM WITH GANESH JI &amp; FOIL)</t>
+    <t>9228 CARDS (Y)</t>
+  </si>
+  <si>
+    <t>9229 CARDS - B (DCU)</t>
+  </si>
+  <si>
+    <t>9229 CARDS (C)</t>
   </si>
   <si>
     <t>9230 (CARD) 9*5 SCREEN</t>
   </si>
   <si>
-    <t>9231 CARDS (DCU) (RIYAZ 9*5 PINK)</t>
-  </si>
-  <si>
-    <t>9232 CARDS (DCU) (RIYAZ 9*5 CREAM)</t>
-  </si>
-  <si>
-    <t>9233 CARDS (DCU) (RIYAZ 9*5 YELLOW)</t>
-  </si>
-  <si>
-    <t>9235 CARDS (DCU) (RIYAZ 9*4 CREAM)</t>
-  </si>
-  <si>
-    <t>9236 CARDS (DCU) (RIYAZ 9*4 YELLOW)</t>
-  </si>
-  <si>
-    <t>9237 CARDS (DCU) (DCU 9*4 RED)</t>
-  </si>
-  <si>
-    <t>9301 CARDS (4242)</t>
-  </si>
-  <si>
-    <t>9302 CARDS (5076)</t>
-  </si>
-  <si>
-    <t>9303 CARDS (5080 Pink)</t>
-  </si>
-  <si>
-    <t>9304 CARDS (5083 Blue)</t>
-  </si>
-  <si>
-    <t>9305 CARDS (9070) (4701 Nice)</t>
-  </si>
-  <si>
-    <t>9306 CARDS (0543 Nice)</t>
-  </si>
-  <si>
-    <t>9307 CARDS *-* (M) (5243 Nice)</t>
-  </si>
-  <si>
-    <t>9308 CARDS (9852)</t>
-  </si>
-  <si>
-    <t>9309 CARDS *-* (T) (9561 Vp)</t>
-  </si>
-  <si>
-    <t>9310 CARDS (3103)</t>
-  </si>
-  <si>
-    <t>9311 CARDS (3115)</t>
-  </si>
-  <si>
-    <t>9312 CARDS *-* (T) (208 VV)</t>
-  </si>
-  <si>
-    <t>9313 CARDS *-* (T) (216)</t>
-  </si>
-  <si>
-    <t>9314 CARDS (P-1)</t>
-  </si>
-  <si>
-    <t>9315 CARDS (DCU) (P-2)</t>
-  </si>
-  <si>
-    <t>9316 CARDS (DCU) (P-3)</t>
-  </si>
-  <si>
-    <t>9317 CARDS (P-4)</t>
-  </si>
-  <si>
-    <t>9318 CARDS (25905)</t>
-  </si>
-  <si>
-    <t>9320 CARDS (S-20)</t>
-  </si>
-  <si>
-    <t>9321 CARDS (22912 GANESH JI)</t>
-  </si>
-  <si>
-    <t>9322 CARDS *-* (M) (22912 COMMON)</t>
-  </si>
-  <si>
-    <t>9323 CARDS (9005 OLD) (9*5 CREAM FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9324 CARDS (9*5 PINK FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9325 CARDS (5229)</t>
-  </si>
-  <si>
-    <t>9326 CARDS (1601)</t>
-  </si>
-  <si>
-    <t>9327 CARDS (25908)</t>
-  </si>
-  <si>
-    <t>9328 CARDS (2543)</t>
-  </si>
-  <si>
-    <t>9329 CARDS (Desgin H/d) (3606)</t>
-  </si>
-  <si>
-    <t>9330 CARDS *-* (T) (9557)</t>
-  </si>
-  <si>
-    <t>9331 CARDS *-*  (T) (9560)</t>
-  </si>
-  <si>
-    <t>9332 CARDS (9847)</t>
-  </si>
-  <si>
-    <t>9333 CARDS (6042)</t>
-  </si>
-  <si>
-    <t>9334 CARDS (10X6 WHITE (2898))</t>
-  </si>
-  <si>
-    <t>9335 CARDS (9003 OLD) (9*5 WHITE)</t>
-  </si>
-  <si>
-    <t>9336 CARDS (2884)</t>
-  </si>
-  <si>
-    <t>9337 CARDS (1635 AP)</t>
-  </si>
-  <si>
-    <t>9338 CARDS (1637 AP)</t>
-  </si>
-  <si>
-    <t>9339 CARDS (5361)</t>
-  </si>
-  <si>
-    <t>9340 CARDS (5658)</t>
-  </si>
-  <si>
-    <t>9341 CARDS (5497)</t>
-  </si>
-  <si>
-    <t>9342 CARDS (2861)</t>
-  </si>
-  <si>
-    <t>9343 CARDS (9*5 WHTE GE HEAVY)</t>
-  </si>
-  <si>
-    <t>9344 CARDS (689)</t>
-  </si>
-  <si>
-    <t>9345 CARDS (358 KALYANI)</t>
-  </si>
-  <si>
-    <t>9346 CARDS (359)</t>
-  </si>
-  <si>
-    <t>9347 CARDS (2853)</t>
-  </si>
-  <si>
-    <t>9348 CARDS *-* (डोरी) (S-124)</t>
-  </si>
-  <si>
-    <t>9349 CARDS (W/o Window) (S-120)</t>
-  </si>
-  <si>
-    <t>9350 CARDS *-* (T) (1632)</t>
-  </si>
-  <si>
-    <t>9351 Card - B (1603 B)</t>
-  </si>
-  <si>
-    <t>9351 CARDS *-* (T) (1603)</t>
-  </si>
-  <si>
-    <t>9352 CARDS *-* (T) (1606 AP)</t>
-  </si>
-  <si>
-    <t>9353 CARDS (1618)</t>
-  </si>
-  <si>
-    <t>9354 CARDS (DCU) (345)</t>
-  </si>
-  <si>
-    <t>9355 CARDS (1624)</t>
-  </si>
-  <si>
-    <t>9356 CARDS (2895/2897)</t>
-  </si>
-  <si>
-    <t>9357 CARDS (2872)</t>
-  </si>
-  <si>
-    <t>9358 CARDS (WHITE PATTA)</t>
-  </si>
-  <si>
-    <t>9359 CARDS (PITCH PATTA)</t>
-  </si>
-  <si>
-    <t>9360 CARDS *-* (M) (GOL ANDA)</t>
-  </si>
-  <si>
-    <t>9361 CARDS (25426)</t>
-  </si>
-  <si>
-    <t>9362 CARDS (363)</t>
-  </si>
-  <si>
-    <t>9363 CARDS *-* (T) (1652)</t>
-  </si>
-  <si>
-    <t>9364 CARDS *-* (T) (1612)</t>
-  </si>
-  <si>
-    <t>9365 CARDS (25429)</t>
-  </si>
-  <si>
-    <t>9366 CARDS (25427 GOLDEN)</t>
-  </si>
-  <si>
-    <t>9367 CARDS (5652)</t>
-  </si>
-  <si>
-    <t>9368 CARDS (9*5 SET 25/26 GOLDEN (25425))</t>
-  </si>
-  <si>
-    <t>9369 CARDS (9*5 SET 25/26 YELLOW (25424))</t>
-  </si>
-  <si>
-    <t>9370 CARDS (9*5 SET 25/26 RED (25423))</t>
-  </si>
-  <si>
-    <t>9371 CARDS (3111 VP)</t>
-  </si>
-  <si>
-    <t>9372 CARDS (9*5 YLW SET (2841))</t>
-  </si>
-  <si>
-    <t>9373 CARDS (1482)</t>
-  </si>
-  <si>
-    <t>9374 CARDS (1485)</t>
-  </si>
-  <si>
-    <t>9375 CARDS (1452 WHITE)</t>
-  </si>
-  <si>
-    <t>9376 CARDS (1529 PRINCE)</t>
-  </si>
-  <si>
-    <t>9377 CARDS (DCU) (9*5 SET GREEN (009))</t>
-  </si>
-  <si>
-    <t>9378 CARDS (2892)</t>
+    <t>9231 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9232 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9233 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9235 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9236 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9237 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9301 CARDS</t>
+  </si>
+  <si>
+    <t>9302 CARDS</t>
+  </si>
+  <si>
+    <t>9303 CARDS</t>
+  </si>
+  <si>
+    <t>9304 CARDS</t>
+  </si>
+  <si>
+    <t>9305 CARDS (9070)</t>
+  </si>
+  <si>
+    <t>9306 CARDS</t>
+  </si>
+  <si>
+    <t>9307 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9308 CARDS</t>
+  </si>
+  <si>
+    <t>9309 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9310 CARDS</t>
+  </si>
+  <si>
+    <t>9311 CARDS</t>
+  </si>
+  <si>
+    <t>9312 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9313 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9314 CARDS</t>
+  </si>
+  <si>
+    <t>9315 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9316 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9317 CARDS</t>
+  </si>
+  <si>
+    <t>9318 CARDS</t>
+  </si>
+  <si>
+    <t>9320 CARDS</t>
+  </si>
+  <si>
+    <t>9321 CARDS</t>
+  </si>
+  <si>
+    <t>9322 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9323 CARDS (9005 OLD)</t>
+  </si>
+  <si>
+    <t>9324 CARDS</t>
+  </si>
+  <si>
+    <t>9325 CARDS</t>
+  </si>
+  <si>
+    <t>9326 CARDS</t>
+  </si>
+  <si>
+    <t>9327 CARDS</t>
+  </si>
+  <si>
+    <t>9328 CARDS</t>
+  </si>
+  <si>
+    <t>9329 CARDS (Desgin H/d)</t>
+  </si>
+  <si>
+    <t>9330 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9331 CARDS *-*  (T)</t>
+  </si>
+  <si>
+    <t>9332 CARDS</t>
+  </si>
+  <si>
+    <t>9333 CARDS</t>
+  </si>
+  <si>
+    <t>9334 CARDS</t>
+  </si>
+  <si>
+    <t>9335 CARDS (9003 OLD)</t>
+  </si>
+  <si>
+    <t>9336 CARDS</t>
+  </si>
+  <si>
+    <t>9337 CARDS</t>
+  </si>
+  <si>
+    <t>9338 CARDS</t>
+  </si>
+  <si>
+    <t>9339 CARDS</t>
+  </si>
+  <si>
+    <t>9340 CARDS</t>
+  </si>
+  <si>
+    <t>9341 CARDS</t>
+  </si>
+  <si>
+    <t>9342 CARDS</t>
+  </si>
+  <si>
+    <t>9343 CARDS</t>
+  </si>
+  <si>
+    <t>9344 CARDS</t>
+  </si>
+  <si>
+    <t>9345 CARDS</t>
+  </si>
+  <si>
+    <t>9346 CARDS</t>
+  </si>
+  <si>
+    <t>9347 CARDS</t>
+  </si>
+  <si>
+    <t>9348 CARDS *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>9349 CARDS (W/o Window)</t>
+  </si>
+  <si>
+    <t>9350 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9351 Card - B</t>
+  </si>
+  <si>
+    <t>9351 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9352 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9353 CARDS</t>
+  </si>
+  <si>
+    <t>9354 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9355 CARDS</t>
+  </si>
+  <si>
+    <t>9356 CARDS</t>
+  </si>
+  <si>
+    <t>9357 CARDS</t>
+  </si>
+  <si>
+    <t>9358 CARDS</t>
+  </si>
+  <si>
+    <t>9359 CARDS</t>
+  </si>
+  <si>
+    <t>9360 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9361 CARDS</t>
+  </si>
+  <si>
+    <t>9362 CARDS</t>
+  </si>
+  <si>
+    <t>9363 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9364 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9365 CARDS</t>
+  </si>
+  <si>
+    <t>9366 CARDS</t>
+  </si>
+  <si>
+    <t>9367 CARDS</t>
+  </si>
+  <si>
+    <t>9368 CARDS</t>
+  </si>
+  <si>
+    <t>9369 CARDS</t>
+  </si>
+  <si>
+    <t>9370 CARDS</t>
+  </si>
+  <si>
+    <t>9371 CARDS</t>
+  </si>
+  <si>
+    <t>9372 CARDS</t>
+  </si>
+  <si>
+    <t>9373 CARDS</t>
+  </si>
+  <si>
+    <t>9374 CARDS</t>
+  </si>
+  <si>
+    <t>9375 CARDS</t>
+  </si>
+  <si>
+    <t>9376 CARDS</t>
+  </si>
+  <si>
+    <t>9377 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9378 CARDS</t>
   </si>
   <si>
     <t>9379 CARDS - R</t>
@@ -1979,19 +1979,19 @@
     <t>9387 CARDS - GOLDEN (Mil Jayega)</t>
   </si>
   <si>
-    <t>9389 CARDS (9147 RJ)</t>
-  </si>
-  <si>
-    <t>9390 CARDS (DCU) (118KBC)</t>
+    <t>9389 CARDS</t>
+  </si>
+  <si>
+    <t>9390 CARDS (DCU)</t>
   </si>
   <si>
     <t>9391 CARDS</t>
   </si>
   <si>
-    <t>9*4 ENVELOPE (SBC) (CHOTA ENVELOPE (60/40 BILL))</t>
-  </si>
-  <si>
-    <t>9*5 ENVELOPE (FOIL) SBC (BADA ENVLP WITH FOIL (60/40 BILL))</t>
+    <t>9*4 ENVELOPE (SBC)</t>
+  </si>
+  <si>
+    <t>9*5 ENVELOPE (FOIL) SBC</t>
   </si>
   <si>
     <t>ACRYLIC NAME PLATE</t>
@@ -2000,7 +2000,7 @@
     <t>DEV SAMPLE SET</t>
   </si>
   <si>
-    <t>FANCY GIFT ENVELOPE-(SR) (SR ENVELOPES)</t>
+    <t>FANCY GIFT ENVELOPE-(SR)</t>
   </si>
   <si>
     <t>Gift Envelope (Pocket) SR...</t>
@@ -2018,34 +2018,34 @@
     <t>RIBBON (रिबीन)</t>
   </si>
   <si>
-    <t>RX-01 ENVELOPE (LX01)</t>
-  </si>
-  <si>
-    <t>RX-02 ENVELOPE (LX02)</t>
-  </si>
-  <si>
-    <t>RX-03 ENVELOPE (LX03)</t>
-  </si>
-  <si>
-    <t>RX-04 ENVELOPE (LX04)</t>
-  </si>
-  <si>
-    <t>RX-05 ENVELOPE (LX05)</t>
-  </si>
-  <si>
-    <t>RX-06 ENVELOPE (LX06)</t>
-  </si>
-  <si>
-    <t>RX-07 ENVELOPE (LX07)</t>
-  </si>
-  <si>
-    <t>RX-08 ENVELOPE (LX08)</t>
-  </si>
-  <si>
-    <t>RX-09 ENVELOPE (LX09)</t>
-  </si>
-  <si>
-    <t>गोल गणेश / गोल फ्लावर (GOL GANESH OR GOL FLOWER)</t>
+    <t>RX-01 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-02 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-03 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-04 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-05 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-06 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-07 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-08 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-09 ENVELOPE</t>
+  </si>
+  <si>
+    <t>गोल गणेश / गोल फ्लावर</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -2578,7 +2578,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -2751,16 +2751,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="25">
-        <v>104.5</v>
+        <v>101.5</v>
       </c>
       <c r="D14" s="26">
         <v>2</v>
       </c>
       <c r="E14" s="27">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2955,16 +2955,16 @@
         <v>29</v>
       </c>
       <c r="B26" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" s="25">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="26">
         <v>2</v>
       </c>
       <c r="E26" s="27">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3174,16 +3174,16 @@
         <v>42</v>
       </c>
       <c r="B39" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C39" s="25">
-        <v>53.5</v>
+        <v>49.5</v>
       </c>
       <c r="D39" s="26">
         <v>2.14</v>
       </c>
       <c r="E39" s="27">
-        <v>114.49</v>
+        <v>105.93</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3276,16 +3276,16 @@
         <v>48</v>
       </c>
       <c r="B45" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C45" s="25">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D45" s="26">
         <v>1.25</v>
       </c>
       <c r="E45" s="27">
-        <v>48.75</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3361,16 +3361,16 @@
         <v>53</v>
       </c>
       <c r="B50" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C50" s="25">
-        <v>144.5</v>
+        <v>143.5</v>
       </c>
       <c r="D50" s="26">
         <v>2.5</v>
       </c>
       <c r="E50" s="27">
-        <v>361.25</v>
+        <v>358.75</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3676,16 +3676,16 @@
         <v>72</v>
       </c>
       <c r="B69" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C69" s="25">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D69" s="26">
         <v>1.4</v>
       </c>
       <c r="E69" s="27">
-        <v>394.8</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3744,16 +3744,16 @@
         <v>76</v>
       </c>
       <c r="B73" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C73" s="25">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D73" s="26">
         <v>1.2</v>
       </c>
       <c r="E73" s="27">
-        <v>762</v>
+        <v>759.6</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3980,16 +3980,16 @@
         <v>90</v>
       </c>
       <c r="B87" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C87" s="25">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D87" s="26">
         <v>1.2</v>
       </c>
       <c r="E87" s="27">
-        <v>101.75</v>
+        <v>100.56</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4397,10 +4397,10 @@
         <v>119</v>
       </c>
       <c r="B116" s="24">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C116" s="25">
-        <v>-0.41</v>
+        <v>-0.42</v>
       </c>
       <c r="D116" s="28"/>
       <c r="E116" s="29"/>
@@ -4535,16 +4535,16 @@
         <v>129</v>
       </c>
       <c r="B126" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C126" s="25">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D126" s="26">
         <v>12.5</v>
       </c>
       <c r="E126" s="27">
-        <v>600</v>
+        <v>587.5</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4603,16 +4603,16 @@
         <v>133</v>
       </c>
       <c r="B130" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C130" s="25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D130" s="26">
         <v>12.5</v>
       </c>
       <c r="E130" s="27">
-        <v>287.5</v>
+        <v>275</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4856,16 +4856,16 @@
         <v>148</v>
       </c>
       <c r="B145" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C145" s="25">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="D145" s="26">
         <v>18.5</v>
       </c>
       <c r="E145" s="27">
-        <v>120.25</v>
+        <v>83.25</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -5160,16 +5160,16 @@
         <v>166</v>
       </c>
       <c r="B163" s="24">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C163" s="25">
-        <v>1.5</v>
+        <v>-6.5</v>
       </c>
       <c r="D163" s="26">
         <v>1.1499999999999999</v>
       </c>
       <c r="E163" s="27">
-        <v>1.72</v>
+        <v>-7.47</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5394,16 +5394,16 @@
         <v>180</v>
       </c>
       <c r="B177" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C177" s="25">
-        <v>30.5</v>
+        <v>28.5</v>
       </c>
       <c r="D177" s="26">
         <v>2.76</v>
       </c>
       <c r="E177" s="27">
-        <v>84.24</v>
+        <v>78.72</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5477,16 +5477,16 @@
         <v>185</v>
       </c>
       <c r="B182" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C182" s="25">
-        <v>32</v>
+        <v>30.5</v>
       </c>
       <c r="D182" s="26">
         <v>5</v>
       </c>
       <c r="E182" s="27">
-        <v>160</v>
+        <v>152.5</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5562,16 +5562,16 @@
         <v>190</v>
       </c>
       <c r="B187" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C187" s="25">
-        <v>44.5</v>
+        <v>42.5</v>
       </c>
       <c r="D187" s="26">
         <v>4.5</v>
       </c>
       <c r="E187" s="27">
-        <v>200.25</v>
+        <v>191.25</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5902,16 +5902,16 @@
         <v>210</v>
       </c>
       <c r="B207" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C207" s="25">
-        <v>70</v>
+        <v>66.5</v>
       </c>
       <c r="D207" s="26">
         <v>3.57</v>
       </c>
       <c r="E207" s="27">
-        <v>250.04</v>
+        <v>237.53</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -6209,16 +6209,16 @@
         <v>229</v>
       </c>
       <c r="B226" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C226" s="25">
-        <v>17</v>
+        <v>13.5</v>
       </c>
       <c r="D226" s="26">
         <v>8.25</v>
       </c>
       <c r="E226" s="27">
-        <v>140.25</v>
+        <v>111.38</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6260,16 +6260,16 @@
         <v>232</v>
       </c>
       <c r="B229" s="24">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C229" s="25">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D229" s="26">
         <v>6.3</v>
       </c>
       <c r="E229" s="27">
-        <v>264.60000000000002</v>
+        <v>245.7</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -6528,16 +6528,16 @@
         <v>248</v>
       </c>
       <c r="B245" s="24">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C245" s="25">
-        <v>419.5</v>
+        <v>417</v>
       </c>
       <c r="D245" s="26">
         <v>4.28</v>
       </c>
       <c r="E245" s="27">
-        <v>1795.46</v>
+        <v>1784.76</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -7022,13 +7022,13 @@
         <v>56</v>
       </c>
       <c r="C274" s="25">
-        <v>100.5</v>
+        <v>105.5</v>
       </c>
       <c r="D274" s="26">
         <v>6</v>
       </c>
       <c r="E274" s="27">
-        <v>602.95000000000005</v>
+        <v>632.95000000000005</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -7879,16 +7879,16 @@
         <v>329</v>
       </c>
       <c r="B326" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C326" s="25">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="D326" s="26">
         <v>6.4</v>
       </c>
       <c r="E326" s="27">
-        <v>67.2</v>
+        <v>60.8</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
@@ -8149,16 +8149,16 @@
         <v>345</v>
       </c>
       <c r="B342" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C342" s="25">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D342" s="26">
         <v>7.13</v>
       </c>
       <c r="E342" s="27">
-        <v>149.72999999999999</v>
+        <v>128.34</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
@@ -8251,16 +8251,16 @@
         <v>351</v>
       </c>
       <c r="B348" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C348" s="25">
-        <v>40</v>
+        <v>37.5</v>
       </c>
       <c r="D348" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E348" s="27">
-        <v>328</v>
+        <v>307.5</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -8370,16 +8370,16 @@
         <v>358</v>
       </c>
       <c r="B355" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C355" s="25">
-        <v>35.5</v>
+        <v>34.5</v>
       </c>
       <c r="D355" s="26">
         <v>3.6</v>
       </c>
       <c r="E355" s="27">
-        <v>127.8</v>
+        <v>124.2</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
@@ -9085,16 +9085,16 @@
         <v>401</v>
       </c>
       <c r="B398" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C398" s="25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D398" s="26">
         <v>6</v>
       </c>
       <c r="E398" s="27">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -9251,16 +9251,16 @@
         <v>411</v>
       </c>
       <c r="B408" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C408" s="25">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D408" s="26">
         <v>16</v>
       </c>
       <c r="E408" s="27">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
@@ -9621,16 +9621,16 @@
         <v>433</v>
       </c>
       <c r="B430" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C430" s="25">
-        <v>12</v>
+        <v>10.5</v>
       </c>
       <c r="D430" s="26">
         <v>15.5</v>
       </c>
       <c r="E430" s="27">
-        <v>186</v>
+        <v>162.75</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
@@ -9719,16 +9719,16 @@
         <v>439</v>
       </c>
       <c r="B436" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C436" s="25">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D436" s="26">
         <v>18</v>
       </c>
       <c r="E436" s="27">
-        <v>252</v>
+        <v>198</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
@@ -9753,16 +9753,16 @@
         <v>441</v>
       </c>
       <c r="B438" s="24">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C438" s="25">
-        <v>21.5</v>
+        <v>26.5</v>
       </c>
       <c r="D438" s="26">
         <v>9.5</v>
       </c>
       <c r="E438" s="27">
-        <v>204.25</v>
+        <v>251.75</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
@@ -9939,13 +9939,13 @@
         <v>5</v>
       </c>
       <c r="C449" s="25">
-        <v>18.5</v>
+        <v>19.5</v>
       </c>
       <c r="D449" s="26">
         <v>9.26</v>
       </c>
       <c r="E449" s="27">
-        <v>171.31</v>
+        <v>180.57</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
@@ -10087,16 +10087,16 @@
         <v>461</v>
       </c>
       <c r="B458" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C458" s="25">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D458" s="26">
         <v>11.15</v>
       </c>
       <c r="E458" s="27">
-        <v>401.54</v>
+        <v>356.92</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -10681,16 +10681,16 @@
         <v>497</v>
       </c>
       <c r="B494" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C494" s="25">
-        <v>37.5</v>
+        <v>35.5</v>
       </c>
       <c r="D494" s="26">
         <v>3</v>
       </c>
       <c r="E494" s="27">
-        <v>112.5</v>
+        <v>106.5</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.25">
@@ -10698,16 +10698,16 @@
         <v>498</v>
       </c>
       <c r="B495" s="24">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C495" s="25">
-        <v>58</v>
+        <v>55.5</v>
       </c>
       <c r="D495" s="26">
         <v>3.8</v>
       </c>
       <c r="E495" s="27">
-        <v>220.4</v>
+        <v>210.9</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -10813,16 +10813,16 @@
         <v>505</v>
       </c>
       <c r="B502" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C502" s="25">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D502" s="26">
         <v>2</v>
       </c>
       <c r="E502" s="27">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.25">
@@ -10847,16 +10847,16 @@
         <v>507</v>
       </c>
       <c r="B504" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C504" s="25">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="D504" s="26">
         <v>4.28</v>
       </c>
       <c r="E504" s="27">
-        <v>115.56</v>
+        <v>109.14</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
@@ -10915,16 +10915,16 @@
         <v>511</v>
       </c>
       <c r="B508" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C508" s="25">
-        <v>29.5</v>
+        <v>27.5</v>
       </c>
       <c r="D508" s="26">
         <v>4.75</v>
       </c>
       <c r="E508" s="27">
-        <v>140.13</v>
+        <v>130.63</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
@@ -11068,16 +11068,16 @@
         <v>520</v>
       </c>
       <c r="B517" s="24">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C517" s="25">
-        <v>123.5</v>
+        <v>124.5</v>
       </c>
       <c r="D517" s="26">
         <v>3.9</v>
       </c>
       <c r="E517" s="27">
-        <v>481.65</v>
+        <v>485.55</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
@@ -11187,16 +11187,16 @@
         <v>527</v>
       </c>
       <c r="B524" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C524" s="25">
-        <v>39.799999999999997</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="D524" s="26">
         <v>3.14</v>
       </c>
       <c r="E524" s="27">
-        <v>124.97</v>
+        <v>121.83</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
@@ -11255,16 +11255,16 @@
         <v>531</v>
       </c>
       <c r="B528" s="24">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C528" s="25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D528" s="26">
         <v>3.5</v>
       </c>
       <c r="E528" s="27">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -11323,16 +11323,16 @@
         <v>535</v>
       </c>
       <c r="B532" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C532" s="25">
-        <v>18.5</v>
+        <v>15.5</v>
       </c>
       <c r="D532" s="26">
         <v>2.66</v>
       </c>
       <c r="E532" s="27">
-        <v>49.21</v>
+        <v>41.23</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -11340,16 +11340,16 @@
         <v>536</v>
       </c>
       <c r="B533" s="24">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C533" s="25">
-        <v>54.5</v>
+        <v>50.5</v>
       </c>
       <c r="D533" s="26">
         <v>2.66</v>
       </c>
       <c r="E533" s="27">
-        <v>144.97</v>
+        <v>134.33000000000001</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
@@ -11438,16 +11438,16 @@
         <v>542</v>
       </c>
       <c r="B539" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C539" s="25">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D539" s="26">
         <v>1.4</v>
       </c>
       <c r="E539" s="27">
-        <v>253.4</v>
+        <v>250.6</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.25">
@@ -11603,16 +11603,16 @@
         <v>553</v>
       </c>
       <c r="B550" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C550" s="25">
-        <v>1190</v>
+        <v>1110</v>
       </c>
       <c r="D550" s="26">
         <v>0.57999999999999996</v>
       </c>
       <c r="E550" s="27">
-        <v>690.2</v>
+        <v>643.79999999999995</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.25">
@@ -12104,16 +12104,16 @@
         <v>584</v>
       </c>
       <c r="B581" s="24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C581" s="25">
-        <v>3.25</v>
+        <v>1.75</v>
       </c>
       <c r="D581" s="26">
         <v>1.5</v>
       </c>
       <c r="E581" s="27">
-        <v>4.88</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
@@ -12124,13 +12124,13 @@
         <v>38</v>
       </c>
       <c r="C582" s="25">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D582" s="26">
         <v>2.2799999999999998</v>
       </c>
       <c r="E582" s="27">
-        <v>13.68</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
@@ -12274,16 +12274,16 @@
         <v>594</v>
       </c>
       <c r="B591" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C591" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D591" s="26">
         <v>4.5</v>
       </c>
       <c r="E591" s="27">
-        <v>22.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
@@ -12444,16 +12444,16 @@
         <v>604</v>
       </c>
       <c r="B601" s="24">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C601" s="25">
-        <v>99.8</v>
+        <v>97.8</v>
       </c>
       <c r="D601" s="26">
         <v>2.85</v>
       </c>
       <c r="E601" s="27">
-        <v>284.43</v>
+        <v>278.73</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -12529,16 +12529,16 @@
         <v>609</v>
       </c>
       <c r="B606" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C606" s="25">
-        <v>32</v>
+        <v>29.5</v>
       </c>
       <c r="D606" s="26">
         <v>3.1</v>
       </c>
       <c r="E606" s="27">
-        <v>99.2</v>
+        <v>91.45</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12712,16 +12712,16 @@
         <v>620</v>
       </c>
       <c r="B617" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C617" s="25">
-        <v>44.5</v>
+        <v>43.5</v>
       </c>
       <c r="D617" s="26">
         <v>3.6</v>
       </c>
       <c r="E617" s="27">
-        <v>160.19999999999999</v>
+        <v>156.6</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12950,16 +12950,16 @@
         <v>634</v>
       </c>
       <c r="B631" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C631" s="25">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="D631" s="26">
         <v>4</v>
       </c>
       <c r="E631" s="27">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
@@ -13001,16 +13001,16 @@
         <v>637</v>
       </c>
       <c r="B634" s="24">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C634" s="25">
-        <v>16</v>
+        <v>17.5</v>
       </c>
       <c r="D634" s="26">
         <v>4.25</v>
       </c>
       <c r="E634" s="27">
-        <v>68</v>
+        <v>74.38</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.25">
@@ -13138,10 +13138,10 @@
         <v>646</v>
       </c>
       <c r="B643" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C643" s="25">
-        <v>48.5</v>
+        <v>44.5</v>
       </c>
       <c r="D643" s="28"/>
       <c r="E643" s="29"/>
@@ -13424,16 +13424,16 @@
         <v>666</v>
       </c>
       <c r="B663" s="24">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C663" s="25">
-        <v>30.25</v>
+        <v>28.25</v>
       </c>
       <c r="D663" s="26">
         <v>2.5</v>
       </c>
       <c r="E663" s="27">
-        <v>75.63</v>
+        <v>70.63</v>
       </c>
     </row>
     <row r="664" spans="1:5" x14ac:dyDescent="0.25">
@@ -13441,16 +13441,16 @@
         <v>667</v>
       </c>
       <c r="B664" s="24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C664" s="25">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D664" s="26">
         <v>2.5</v>
       </c>
       <c r="E664" s="27">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="665" spans="1:5" x14ac:dyDescent="0.25">
@@ -13475,16 +13475,16 @@
         <v>669</v>
       </c>
       <c r="B666" s="24">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C666" s="25">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="D666" s="26">
         <v>2.5</v>
       </c>
       <c r="E666" s="27">
-        <v>13.75</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="667" spans="1:5" x14ac:dyDescent="0.25">
@@ -13509,16 +13509,16 @@
         <v>671</v>
       </c>
       <c r="B668" s="24">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C668" s="25">
-        <v>22.25</v>
+        <v>19.25</v>
       </c>
       <c r="D668" s="26">
         <v>2.5</v>
       </c>
       <c r="E668" s="27">
-        <v>55.63</v>
+        <v>48.13</v>
       </c>
     </row>
     <row r="669" spans="1:5" x14ac:dyDescent="0.25">
@@ -13526,16 +13526,16 @@
         <v>672</v>
       </c>
       <c r="B669" s="24">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C669" s="25">
-        <v>33.5</v>
+        <v>32.5</v>
       </c>
       <c r="D669" s="26">
         <v>2.5</v>
       </c>
       <c r="E669" s="27">
-        <v>83.75</v>
+        <v>81.25</v>
       </c>
     </row>
     <row r="670" spans="1:5" x14ac:dyDescent="0.25">
@@ -13546,7 +13546,7 @@
         <v>86</v>
       </c>
       <c r="C670" s="25">
-        <v>-222</v>
+        <v>-224</v>
       </c>
       <c r="D670" s="28"/>
       <c r="E670" s="29"/>
@@ -13557,11 +13557,11 @@
       </c>
       <c r="B671" s="31"/>
       <c r="C671" s="32">
-        <v>38597.839999999997</v>
+        <v>38419.83</v>
       </c>
       <c r="D671" s="33"/>
       <c r="E671" s="34">
-        <v>107565.81</v>
+        <v>107116.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil 11 dec @ 8.22
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -68,310 +68,310 @@
     <t>Value</t>
   </si>
   <si>
-    <t>.1001 PATRIKA (25/251)</t>
-  </si>
-  <si>
-    <t>1002 PATRIKA (25/262)</t>
-  </si>
-  <si>
-    <t>1003 PATRIKA (25/261)</t>
-  </si>
-  <si>
-    <t>1004 PATRIKA (25/361/861)</t>
-  </si>
-  <si>
-    <t>1005 PATRIKA (25/362/862)</t>
-  </si>
-  <si>
-    <t>1006 PATRIKA (25/282)</t>
-  </si>
-  <si>
-    <t>1007 PATRIKA (25/281)</t>
-  </si>
-  <si>
-    <t>1008 PATRIKA (JC) (2595 PINK)</t>
-  </si>
-  <si>
-    <t>1009 PATRIKA (JC) (2595 ORANGE)</t>
-  </si>
-  <si>
-    <t>1010 PATRIKA (6321)</t>
-  </si>
-  <si>
-    <t>1011 PATRIKA (2563 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1012 PATRIKA (2564 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1013 PATRIKA (2568 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1014 PATRIKA (11043 OFFSET)</t>
-  </si>
-  <si>
-    <t>1015 PATRIKA (DCU) (11041 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1016 PATRIKA (1011 OFFSET)</t>
-  </si>
-  <si>
-    <t>1017 PATRIKA (1014 OFFSET)</t>
-  </si>
-  <si>
-    <t>1018 PATRIKA (10081 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1019 PATRIKA (1222 SBC)</t>
-  </si>
-  <si>
-    <t>1020 PATRIKA (1235)</t>
-  </si>
-  <si>
-    <t>1021 PATRIKA (2101 VV)</t>
-  </si>
-  <si>
-    <t>1023 PATRIKA (25418)</t>
-  </si>
-  <si>
-    <t>1024 PATRIKA (25322)</t>
-  </si>
-  <si>
-    <t>1025 PATRIKA (25323)</t>
-  </si>
-  <si>
-    <t>1026 PATRIKA (JC) (1173 SBC)</t>
-  </si>
-  <si>
-    <t>1027 PATRIKA (JC) (5346)</t>
-  </si>
-  <si>
-    <t>1028 PATRIKA (JC) (2596)</t>
-  </si>
-  <si>
-    <t>1029 PATRIKA (1042)</t>
-  </si>
-  <si>
-    <t>1030 PATRIKA (1043)</t>
-  </si>
-  <si>
-    <t>1031 PATRIKA (GOPAL 11)</t>
-  </si>
-  <si>
-    <t>1032 PATRIKA (GOPAL 1)</t>
-  </si>
-  <si>
-    <t>1033 PATRIKA (2002 YLW)</t>
-  </si>
-  <si>
-    <t>1034 PATRIKA (2003 R)</t>
-  </si>
-  <si>
-    <t>1035 PATRIKA (DCU) (2201 ROSHAN)</t>
-  </si>
-  <si>
-    <t>1101 PATRIKA (O.2591) (2591 ORANGE)</t>
-  </si>
-  <si>
-    <t>1102 PATRIKA (P.2591) (2591 PINK)</t>
-  </si>
-  <si>
-    <t>1103 PATRIKA(N-271) (271 NEHA)</t>
-  </si>
-  <si>
-    <t>1104 PATRIKA(N-272) (272 NEHA)</t>
-  </si>
-  <si>
-    <t>1105 PATRIKA (276-A)</t>
-  </si>
-  <si>
-    <t>1106 PATRIKA-YELLOW (25419)</t>
-  </si>
-  <si>
-    <t>1107 PATRIKA-RED (25420)</t>
-  </si>
-  <si>
-    <t>1109 PATRIKA-BIG Y (25421)</t>
-  </si>
-  <si>
-    <t>1110 PATRIKA-BIG R (25422)</t>
-  </si>
-  <si>
-    <t>1112 PATRIKA (277-B)</t>
-  </si>
-  <si>
-    <t>1113 PATRIKA (1819 MONARCH)</t>
-  </si>
-  <si>
-    <t>1114 PATRIKA-BROWN (1709)</t>
-  </si>
-  <si>
-    <t>1115 PATRIKA-CREAM (1678 PRINCE)</t>
-  </si>
-  <si>
-    <t>1116 PATRIKA (1153) (1253 Jsk)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA (1155) (1155 JSK)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA - B (KRISHNA 1155-B)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA - B (DCU) (NEW SAVASHREE- 51)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA (सवाश्री-57) (NEW SAVASHREE-57)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA - B (DCU) (NEW SAVASHREE 52)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA(सवाश्री-55) (NEW SAVASHREE-55)</t>
-  </si>
-  <si>
-    <t>1120 PATRIKA(सवाश्री-59) (NEW SAVASHREE-59)</t>
-  </si>
-  <si>
-    <t>1121 PATRIKA(सवाश्री-53) (NEW SAVASHREE-53)</t>
-  </si>
-  <si>
-    <t>1122 PATRIKA (DCU) (NEW SAVASHREE-54)</t>
-  </si>
-  <si>
-    <t>1123 PATRIKA (LED-51) (LED-51)</t>
-  </si>
-  <si>
-    <t>1124 PATRIKA (LED-52) (LED-52)</t>
-  </si>
-  <si>
-    <t>1125 PATRIKA (LED-53) (LED-53)</t>
-  </si>
-  <si>
-    <t>1126 PATRIKA (LED-54) (LED-54)</t>
-  </si>
-  <si>
-    <t>1127 PATRIKA (Eco-52) (NEW ECO-52)</t>
-  </si>
-  <si>
-    <t>1128 PATRIKA (Eco-55) (NEW ECO-55)</t>
-  </si>
-  <si>
-    <t>1129 PATRIKA (Eco-56) (NEW ECO-56)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA - B (ECO-60) (DCU) (NEW ECO 60)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA (Eco-59) (NEW ECO-59)</t>
-  </si>
-  <si>
-    <t>1131 PATRIKA (DCU) Eco-51 (NEW ECO- 51)</t>
-  </si>
-  <si>
-    <t>1132 PATRIKA (DCU) Eco-53 (NEW ECO- 53)</t>
-  </si>
-  <si>
-    <t>1133 PATRIKA (DCU) Eco-57 (NEW ECO- 57)</t>
-  </si>
-  <si>
-    <t>1134 PATRIKA (DCU) Eco-58 (NEW ECO- 58)</t>
-  </si>
-  <si>
-    <t>1135 PATRIKA (DCU) Eco-54 (NEW ECO- 54)</t>
-  </si>
-  <si>
-    <t>1136 PATRIKA (R) (120 GSM RED)</t>
-  </si>
-  <si>
-    <t>1137 PATRIKA (P) (120 GSM YELLOW)</t>
-  </si>
-  <si>
-    <t>1138 PATRIKA (BR) (150 GSM FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1139 PATRIKA (BY) (150 GSM FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1140 PATRIKA (BB) (150 GSM FOIL (BROWN))</t>
-  </si>
-  <si>
-    <t>1141 PATRIKA (R) (120 GSM (RED)SELF)</t>
-  </si>
-  <si>
-    <t>1142 PATRIKA (P) (120 GSM (YELLOW) SELF)</t>
-  </si>
-  <si>
-    <t>1143 PATRIKA (G) (120 GSM (OLD GOLDEN))</t>
-  </si>
-  <si>
-    <t>1144 PATRIKA (BR) (170 GSM WITH FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1145 PATRIKA (BY) (170 GSM WITH FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1146 PATRIKA (DCU) (BROWN 170 GSM FOIL)</t>
-  </si>
-  <si>
-    <t>1147 PATRIKA (S.201) (201 WESTERN)</t>
-  </si>
-  <si>
-    <t>1148 PATRIKA (S.202) (202 WESTERN)</t>
-  </si>
-  <si>
-    <t>1149 PATRIKA (S.204) (204 WESTERN)</t>
-  </si>
-  <si>
-    <t>1150 PATRIKA (DCU) (NEW SAVASHREE-58)</t>
-  </si>
-  <si>
-    <t>1151 PATRIKA (DCU) (NEW SAVASHREE-56)</t>
-  </si>
-  <si>
-    <t>1152 PATRIKA (DCU) (WESTERN 202 OLD)</t>
-  </si>
-  <si>
-    <t>1153 PATRIKA (DCU) (201 WESTERN (OLD))</t>
-  </si>
-  <si>
-    <t>1154 PATRIKA (DCU) (203 WESTERN A)</t>
-  </si>
-  <si>
-    <t>1155 PATRIKA (DCU) (WESTERN (203) B)</t>
-  </si>
-  <si>
-    <t>1156 PATRIKA-YELLOW (LU-51 (YELLOW))</t>
-  </si>
-  <si>
-    <t>1157 PATRIKA-CREAM (LU-52 (CREAM))</t>
-  </si>
-  <si>
-    <t>1158 PATRIKA-GOLDEN (LU-53 (GOLDEN))</t>
-  </si>
-  <si>
-    <t>1159 PATRIKA-WHITE (LU-54 (WHITE))</t>
-  </si>
-  <si>
-    <t>1160 PATRIKA-PINK (LU-55 (PINK))</t>
-  </si>
-  <si>
-    <t>1161 PATRIKA (01) (JCC 01)</t>
-  </si>
-  <si>
-    <t>1162 PATRIKA (02) (JCC 02)</t>
-  </si>
-  <si>
-    <t>1163 PATRIKA (DCU) (BP RED)</t>
-  </si>
-  <si>
-    <t>1164 PATRIKA (DCU) (BP PINK RIYAZ)</t>
-  </si>
-  <si>
-    <t>1165 PATRIKA (DCU) (BP CREAM)</t>
-  </si>
-  <si>
-    <t>1166 PATRIKA (DCU) (BP YELLOW)</t>
+    <t>.1001 PATRIKA</t>
+  </si>
+  <si>
+    <t>1002 PATRIKA</t>
+  </si>
+  <si>
+    <t>1003 PATRIKA</t>
+  </si>
+  <si>
+    <t>1004 PATRIKA</t>
+  </si>
+  <si>
+    <t>1005 PATRIKA</t>
+  </si>
+  <si>
+    <t>1006 PATRIKA</t>
+  </si>
+  <si>
+    <t>1007 PATRIKA</t>
+  </si>
+  <si>
+    <t>1008 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1009 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1010 PATRIKA</t>
+  </si>
+  <si>
+    <t>1011 PATRIKA</t>
+  </si>
+  <si>
+    <t>1012 PATRIKA</t>
+  </si>
+  <si>
+    <t>1013 PATRIKA</t>
+  </si>
+  <si>
+    <t>1014 PATRIKA</t>
+  </si>
+  <si>
+    <t>1015 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1016 PATRIKA</t>
+  </si>
+  <si>
+    <t>1017 PATRIKA</t>
+  </si>
+  <si>
+    <t>1018 PATRIKA</t>
+  </si>
+  <si>
+    <t>1019 PATRIKA</t>
+  </si>
+  <si>
+    <t>1020 PATRIKA</t>
+  </si>
+  <si>
+    <t>1021 PATRIKA</t>
+  </si>
+  <si>
+    <t>1023 PATRIKA</t>
+  </si>
+  <si>
+    <t>1024 PATRIKA</t>
+  </si>
+  <si>
+    <t>1025 PATRIKA</t>
+  </si>
+  <si>
+    <t>1026 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1027 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1028 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1029 PATRIKA</t>
+  </si>
+  <si>
+    <t>1030 PATRIKA</t>
+  </si>
+  <si>
+    <t>1031 PATRIKA</t>
+  </si>
+  <si>
+    <t>1032 PATRIKA</t>
+  </si>
+  <si>
+    <t>1033 PATRIKA</t>
+  </si>
+  <si>
+    <t>1034 PATRIKA</t>
+  </si>
+  <si>
+    <t>1035 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1101 PATRIKA (O.2591)</t>
+  </si>
+  <si>
+    <t>1102 PATRIKA (P.2591)</t>
+  </si>
+  <si>
+    <t>1103 PATRIKA(N-271)</t>
+  </si>
+  <si>
+    <t>1104 PATRIKA(N-272)</t>
+  </si>
+  <si>
+    <t>1105 PATRIKA</t>
+  </si>
+  <si>
+    <t>1106 PATRIKA-YELLOW</t>
+  </si>
+  <si>
+    <t>1107 PATRIKA-RED</t>
+  </si>
+  <si>
+    <t>1109 PATRIKA-BIG Y</t>
+  </si>
+  <si>
+    <t>1110 PATRIKA-BIG R</t>
+  </si>
+  <si>
+    <t>1112 PATRIKA</t>
+  </si>
+  <si>
+    <t>1113 PATRIKA</t>
+  </si>
+  <si>
+    <t>1114 PATRIKA-BROWN</t>
+  </si>
+  <si>
+    <t>1115 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1116 PATRIKA (1153)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA (1155)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA - B</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA (सवाश्री-57)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA(सवाश्री-55)</t>
+  </si>
+  <si>
+    <t>1120 PATRIKA(सवाश्री-59)</t>
+  </si>
+  <si>
+    <t>1121 PATRIKA(सवाश्री-53)</t>
+  </si>
+  <si>
+    <t>1122 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1123 PATRIKA (LED-51)</t>
+  </si>
+  <si>
+    <t>1124 PATRIKA (LED-52)</t>
+  </si>
+  <si>
+    <t>1125 PATRIKA (LED-53)</t>
+  </si>
+  <si>
+    <t>1126 PATRIKA (LED-54)</t>
+  </si>
+  <si>
+    <t>1127 PATRIKA (Eco-52)</t>
+  </si>
+  <si>
+    <t>1128 PATRIKA (Eco-55)</t>
+  </si>
+  <si>
+    <t>1129 PATRIKA (Eco-56)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA - B (ECO-60) (DCU)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA (Eco-59)</t>
+  </si>
+  <si>
+    <t>1131 PATRIKA (DCU) Eco-51</t>
+  </si>
+  <si>
+    <t>1132 PATRIKA (DCU) Eco-53</t>
+  </si>
+  <si>
+    <t>1133 PATRIKA (DCU) Eco-57</t>
+  </si>
+  <si>
+    <t>1134 PATRIKA (DCU) Eco-58</t>
+  </si>
+  <si>
+    <t>1135 PATRIKA (DCU) Eco-54</t>
+  </si>
+  <si>
+    <t>1136 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1137 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1138 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1139 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1140 PATRIKA (BB)</t>
+  </si>
+  <si>
+    <t>1141 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1142 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1143 PATRIKA (G)</t>
+  </si>
+  <si>
+    <t>1144 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1145 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1146 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1147 PATRIKA (S.201)</t>
+  </si>
+  <si>
+    <t>1148 PATRIKA (S.202)</t>
+  </si>
+  <si>
+    <t>1149 PATRIKA (S.204)</t>
+  </si>
+  <si>
+    <t>1150 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1151 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1152 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1153 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1154 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1155 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1156 PATRIKA-YELLOW</t>
+  </si>
+  <si>
+    <t>1157 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1158 PATRIKA-GOLDEN</t>
+  </si>
+  <si>
+    <t>1159 PATRIKA-WHITE</t>
+  </si>
+  <si>
+    <t>1160 PATRIKA-PINK</t>
+  </si>
+  <si>
+    <t>1161 PATRIKA (01)</t>
+  </si>
+  <si>
+    <t>1162 PATRIKA (02)</t>
+  </si>
+  <si>
+    <t>1163 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1164 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1165 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1166 PATRIKA (DCU)</t>
   </si>
   <si>
     <t>190 NO. ENVELOPES (POCKET)</t>
@@ -407,109 +407,109 @@
     <t>2025- INVITAION (BOX) SAMPLES</t>
   </si>
   <si>
-    <t>2101 PATRIKA (L) (LUXYA - 51)</t>
-  </si>
-  <si>
-    <t>2102 PATRIKA *-* (M) (LUXYA - 52)</t>
-  </si>
-  <si>
-    <t>2103 PATRIKA (L) (LUXYA - 53)</t>
-  </si>
-  <si>
-    <t>2104 PATRIKA (LUXYA - 54)</t>
-  </si>
-  <si>
-    <t>2105 PATRIKA (LUXYA - 55)</t>
-  </si>
-  <si>
-    <t>2106 PATRIKA (L) (LUXYA - 56)</t>
-  </si>
-  <si>
-    <t>2107 PATRIKA *-* (M) (LUXYA - 57)</t>
-  </si>
-  <si>
-    <t>2108 PATRIKA *-* (M) (LUXYA - 59)</t>
-  </si>
-  <si>
-    <t>2109 PATRIKA (L) (LUXYA - 60)</t>
-  </si>
-  <si>
-    <t>2110 PATRIKA (LUXYA - 61)</t>
-  </si>
-  <si>
-    <t>2111 PATRIKA *-* (M) (LUXYA - 62)</t>
-  </si>
-  <si>
-    <t>2112 PATRIKA (L) (LEGACY - 01)</t>
-  </si>
-  <si>
-    <t>2113 PATRIKA (L) (LEGACY - 02)</t>
-  </si>
-  <si>
-    <t>2114 PATRIKA (L) (LEGACY - 03)</t>
-  </si>
-  <si>
-    <t>2115 PATRIKA (L) (LEGACY - 04)</t>
-  </si>
-  <si>
-    <t>2116 PATRIKA (L) (LEGACY - 05)</t>
-  </si>
-  <si>
-    <t>2117 PATRIKA *-* (M) (LEGACY - 06)</t>
-  </si>
-  <si>
-    <t>2118 PATRIKA (L) (LEGACY - 07)</t>
-  </si>
-  <si>
-    <t>2119 PATRIKA (L) (LEGACY - 08)</t>
-  </si>
-  <si>
-    <t>2120 PATRIKA (L) (LEGACY - 09)</t>
-  </si>
-  <si>
-    <t>2121 PATRIKA (LEGACY - 10)</t>
-  </si>
-  <si>
-    <t>2122 PATRIKA (LEGACY - 11)</t>
-  </si>
-  <si>
-    <t>2123 PATRIKA (LEGACY - 12)</t>
-  </si>
-  <si>
-    <t>2124 PATRIKA *-* (M) (LOTTERY - 71)</t>
-  </si>
-  <si>
-    <t>2125 PATRIKA *-* (M) (LOTTERY - 72)</t>
-  </si>
-  <si>
-    <t>2126 PATRIKA *-* (M) (LOTTERY - 73)</t>
-  </si>
-  <si>
-    <t>2127 PATRIKA *-* (M) (LOTTERY - 74)</t>
-  </si>
-  <si>
-    <t>2128 PATRIKA *-* (M) (LOTTERY - 75)</t>
-  </si>
-  <si>
-    <t>2129 PATRIKA *-* (M) (LOTTERY - 76)</t>
-  </si>
-  <si>
-    <t>2130 PATRIKA *-* (M) (LOTTERY - 77)</t>
-  </si>
-  <si>
-    <t>2131 PATRIKA *-* (M) (LOTTERY - 78)</t>
-  </si>
-  <si>
-    <t>2132 PATRIKA *-* (M) (LOTTERY - 79)</t>
-  </si>
-  <si>
-    <t>2133 PATRIKA (LOTTERY - 80)</t>
-  </si>
-  <si>
-    <t>2134 PATRIKA *-* (M) (LOTTERY - 81)</t>
-  </si>
-  <si>
-    <t>2135 PATRIKA *-* (M) (LOTTERY - 82)</t>
+    <t>2101 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2102 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2103 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2104 PATRIKA</t>
+  </si>
+  <si>
+    <t>2105 PATRIKA</t>
+  </si>
+  <si>
+    <t>2106 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2107 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2108 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2109 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2110 PATRIKA</t>
+  </si>
+  <si>
+    <t>2111 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2112 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2113 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2114 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2115 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2116 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2117 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2118 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2119 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2120 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2121 PATRIKA</t>
+  </si>
+  <si>
+    <t>2122 PATRIKA</t>
+  </si>
+  <si>
+    <t>2123 PATRIKA</t>
+  </si>
+  <si>
+    <t>2124 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2125 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2126 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2127 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2128 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2129 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2130 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2131 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2132 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2133 PATRIKA</t>
+  </si>
+  <si>
+    <t>2134 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2135 PATRIKA *-* (M)</t>
   </si>
   <si>
     <t>290 ENVELOPE 25-26</t>
@@ -527,1144 +527,1144 @@
     <t>330 ENVELOPE</t>
   </si>
   <si>
-    <t>4251 PATRIKA (JC) (5342)</t>
-  </si>
-  <si>
-    <t>4252 PATRIKA (5207)</t>
-  </si>
-  <si>
-    <t>4253 PATRIKA (5206)</t>
-  </si>
-  <si>
-    <t>4254 PATRIKA (4210) (10273/10277)</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA - B (DCU) (AS-02 (B))</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA (JC) (AS-02 (NEW))</t>
-  </si>
-  <si>
-    <t>4257 PATRIKA (82)</t>
-  </si>
-  <si>
-    <t>4258 PATRIKA (JC) (1129)</t>
-  </si>
-  <si>
-    <t>4259 PATRIKA (JC) (101 SBC)</t>
-  </si>
-  <si>
-    <t>4260 PATRIKA (1102)</t>
-  </si>
-  <si>
-    <t>4261 PATRIKA (JC) (959)</t>
-  </si>
-  <si>
-    <t>4262 PATRIKA (JC) (S-201 GANESH JI)</t>
-  </si>
-  <si>
-    <t>4264 PATRIKA (DCU) (1351)</t>
-  </si>
-  <si>
-    <t>4265 PATRIKA (83)</t>
-  </si>
-  <si>
-    <t>4266 PATRIKA (25-145)</t>
-  </si>
-  <si>
-    <t>4267 PATRIKA (JC) (25-046)</t>
-  </si>
-  <si>
-    <t>4268 PATRIKA (JC) *-* (M+T) (S-296)</t>
-  </si>
-  <si>
-    <t>4269 PATRIKA (111 SBC)</t>
-  </si>
-  <si>
-    <t>4270 PATRIKA (1151 GGN)</t>
-  </si>
-  <si>
-    <t>4271 PATRIKA (JC) (25216)</t>
-  </si>
-  <si>
-    <t>4272 PATRIKA (JC) (1231 SBC CRM)</t>
-  </si>
-  <si>
-    <t>4273 PATRIKA (2547)</t>
-  </si>
-  <si>
-    <t>4274 PATRIKA (JC) (25369)</t>
-  </si>
-  <si>
-    <t>4275 PATRIKA (25367)</t>
-  </si>
-  <si>
-    <t>4277 PATRIKA (JC) *-* (M) (25365)</t>
-  </si>
-  <si>
-    <t>4278 PATRIKA (25368)</t>
-  </si>
-  <si>
-    <t>4279 PATRIKA (1031)</t>
-  </si>
-  <si>
-    <t>4280 PATRIKA (25301)</t>
-  </si>
-  <si>
-    <t>4281 PATRIKA (25312 MYRA)</t>
-  </si>
-  <si>
-    <t>4282 PATRIKA (3117)</t>
-  </si>
-  <si>
-    <t>4283 PATRIKA - B (YELLOW) (3116-YLW)</t>
-  </si>
-  <si>
-    <t>4284 PATRIKA (1173 VV)</t>
-  </si>
-  <si>
-    <t>4285 PATRIKA (JC) *-* (M) (4626)</t>
-  </si>
-  <si>
-    <t>4286 PATRIKA (5254  RJN)</t>
-  </si>
-  <si>
-    <t>4287 PATRIKA (25402)</t>
-  </si>
-  <si>
-    <t>4288 PATRIKA (10001 NEW)</t>
-  </si>
-  <si>
-    <t>4289 PATRIKA (10002 NEW)</t>
-  </si>
-  <si>
-    <t>4290 PATRIKA (316 MYRA)</t>
-  </si>
-  <si>
-    <t>4291 PATRIKA (25401)</t>
-  </si>
-  <si>
-    <t>4292 PATRIKA (25311)</t>
-  </si>
-  <si>
-    <t>4293 PATRIKA (25312)</t>
-  </si>
-  <si>
-    <t>4294 PATRIKA (5273)</t>
-  </si>
-  <si>
-    <t>4295 PATRIKA (286-A)</t>
-  </si>
-  <si>
-    <t>4296 PATRIKA (1407)</t>
-  </si>
-  <si>
-    <t>4297 PATRIKA (306)</t>
-  </si>
-  <si>
-    <t>4298 PATRIKA (5501)</t>
-  </si>
-  <si>
-    <t>4299 PATRIKA (2011)</t>
-  </si>
-  <si>
-    <t>4300 PATRIKA (25314)</t>
-  </si>
-  <si>
-    <t>4301 PATRIKA (25315)</t>
-  </si>
-  <si>
-    <t>4302 PATRIKA (1402)</t>
-  </si>
-  <si>
-    <t>4303 PATRIKA (JC) (1234*-M)</t>
-  </si>
-  <si>
-    <t>4304 PATRIKA (5172)</t>
-  </si>
-  <si>
-    <t>4305 PATRIKA (25313)</t>
-  </si>
-  <si>
-    <t>4307 PATRIKA (BALAJI 5202)</t>
-  </si>
-  <si>
-    <t>4308 PATRIKA (LOTUS 430)</t>
-  </si>
-  <si>
-    <t>4309 PATRIKA (DCU) (3751 Patta)</t>
-  </si>
-  <si>
-    <t>4310 PATRIKA (DCU) (3752 Swastik)</t>
-  </si>
-  <si>
-    <t>4311 PATRIKA (DCU) (251 KBC)</t>
-  </si>
-  <si>
-    <t>4312 PATRIKA (DCU) (273-A)</t>
-  </si>
-  <si>
-    <t>4314 PATRIKA (DCU) (RED-YELLOW SWASTIK)</t>
-  </si>
-  <si>
-    <t>4315 PATRIKA (DCU) (WHITE-PINK PAN PATA)</t>
-  </si>
-  <si>
-    <t>4316 PATRIKA (DCU) (WHITE -ORANGE PAN PATTA)</t>
-  </si>
-  <si>
-    <t>5051 PATRIKA *-* (M) (5087)</t>
-  </si>
-  <si>
-    <t>5052 PATRIKA (5295)</t>
-  </si>
-  <si>
-    <t>5053 PATRIKA (5213)</t>
-  </si>
-  <si>
-    <t>5054 PATRIKA *-* (M) (25/162)</t>
-  </si>
-  <si>
-    <t>5055 PATRIKA (25/272)</t>
-  </si>
-  <si>
-    <t>5056 PATRIKA (JC) (25/271)</t>
-  </si>
-  <si>
-    <t>5057 PATRIKA (25/171)</t>
-  </si>
-  <si>
-    <t>5058 PATRIKA (8802)</t>
-  </si>
-  <si>
-    <t>5059 PATRIKA (8803)</t>
-  </si>
-  <si>
-    <t>5060 PATRIKA (JC) (7713)</t>
-  </si>
-  <si>
-    <t>5061 PATRIKA (DCU) (1405)</t>
-  </si>
-  <si>
-    <t>5062 PATRIKA (7705)</t>
-  </si>
-  <si>
-    <t>5063 PATRIKA (2522 GE)</t>
-  </si>
-  <si>
-    <t>5064 PATRIKA (2517 GE)</t>
-  </si>
-  <si>
-    <t>5065 PATRIKA (2527)</t>
-  </si>
-  <si>
-    <t>5066 PATRIKA (2536)</t>
-  </si>
-  <si>
-    <t>5067 PATRIKA (JC) (S-301)</t>
-  </si>
-  <si>
-    <t>5071 PATRIKA *-* (डोरी) (741)</t>
-  </si>
-  <si>
-    <t>5072 PATRIKA (5347 DIRECT)</t>
-  </si>
-  <si>
-    <t>5073 PATRIKA *-* (M) (3161)</t>
-  </si>
-  <si>
-    <t>5074 PATRIKA (1151 VV)</t>
-  </si>
-  <si>
-    <t>5075 PATRIKA (JC) (25-082)</t>
-  </si>
-  <si>
-    <t>5076 PATRIKA (JC) (3701 SBC)</t>
-  </si>
-  <si>
-    <t>5077 PATRIKA (2081)</t>
-  </si>
-  <si>
-    <t>5079 PATRIKA (296-A (NEHA)</t>
-  </si>
-  <si>
-    <t>5080 PATRIKA (2501 GE NEW)</t>
-  </si>
-  <si>
-    <t>5081 PATRIKA (2520 GE)</t>
-  </si>
-  <si>
-    <t>5083 PATRIKA (5267)</t>
-  </si>
-  <si>
-    <t>5084 PATRIKA (5258 RJ)</t>
-  </si>
-  <si>
-    <t>5085 PATRIKA (2023)</t>
-  </si>
-  <si>
-    <t>5086 PATRIKA (JC) *-* (M+D) (942)</t>
-  </si>
-  <si>
-    <t>5088 PATRIKA (25214)</t>
-  </si>
-  <si>
-    <t>5089 PATRIKA (2061 SBC)</t>
-  </si>
-  <si>
-    <t>5090 PATRIKA (5236 RJ)</t>
-  </si>
-  <si>
-    <t>5092 PATRIKA (05 NAVIN BHAI)</t>
-  </si>
-  <si>
-    <t>5093 PATRIKA (5350)</t>
-  </si>
-  <si>
-    <t>5094 PATRIKA (5251)</t>
-  </si>
-  <si>
-    <t>5095 PATRIKA (5240)</t>
-  </si>
-  <si>
-    <t>5096 PATRIKA (25316)</t>
-  </si>
-  <si>
-    <t>5097 PATRIKA (25321)</t>
-  </si>
-  <si>
-    <t>5098 PATRIKA *-* (M) (857)</t>
-  </si>
-  <si>
-    <t>5099 PATRIKA *-* (M) (852 DHANESH)</t>
-  </si>
-  <si>
-    <t>5100 PATRIKA (DCU) (5339)</t>
-  </si>
-  <si>
-    <t>5102 PATRIKA (5021) (2456)</t>
-  </si>
-  <si>
-    <t>5103 PATRIKA (2071)</t>
-  </si>
-  <si>
-    <t>5104 PATRIKA (5261 RJND)</t>
-  </si>
-  <si>
-    <t>5105 PATRIKA (JC) (5335)</t>
-  </si>
-  <si>
-    <t>5106 PATRIKA (253-A / 257-A)</t>
-  </si>
-  <si>
-    <t>5107 PATRIKA (5356 RJ)</t>
-  </si>
-  <si>
-    <t>5108 PATRIKA (5333)</t>
-  </si>
-  <si>
-    <t>5109 PATRIKA (5308)</t>
-  </si>
-  <si>
-    <t>5110 PATRIKA (JC) (AS-402)</t>
-  </si>
-  <si>
-    <t>5111 PATRIKA (JC) (5313)</t>
-  </si>
-  <si>
-    <t>5112 PATRIKA (JC) *-* (M) (25437)</t>
-  </si>
-  <si>
-    <t>5113 PATRIKA (5305)</t>
-  </si>
-  <si>
-    <t>5114 PATRIKA *-* (डोरी) (2091)</t>
-  </si>
-  <si>
-    <t>5115 PATRIKA (DCU) (5363 RJND)</t>
-  </si>
-  <si>
-    <t>5116 PATRIKA (2031)</t>
-  </si>
-  <si>
-    <t>5117 PATRIKA (DCU) (3331)</t>
-  </si>
-  <si>
-    <t>5118 PATRIKA (DCU) (25436)</t>
-  </si>
-  <si>
-    <t>5502 PATRIKA *-* (M) (5355 NICE)</t>
-  </si>
-  <si>
-    <t>5503 PATRIKA (5186)</t>
-  </si>
-  <si>
-    <t>5504 PATRIKA (JC) (7033)</t>
-  </si>
-  <si>
-    <t>5505 PATRIKA (JC) *-* (M) (2282)</t>
-  </si>
-  <si>
-    <t>5506 PATRIKA *-* (M) (25/122)</t>
-  </si>
-  <si>
-    <t>5508 PATRIKA (JC) (612 VV)</t>
-  </si>
-  <si>
-    <t>5509 PATRIKA (JC) (25/072)</t>
-  </si>
-  <si>
-    <t>5510 PATRIKA (JC) *-* (M) (AS-950)</t>
-  </si>
-  <si>
-    <t>5511 PATRIKA (JC) *-* (M) (2528)</t>
-  </si>
-  <si>
-    <t>5512 PATRIKA (JC) (2525 /2552)</t>
-  </si>
-  <si>
-    <t>5513 PATRIKA (2515)</t>
-  </si>
-  <si>
-    <t>5514 PATRIKA (2542)</t>
-  </si>
-  <si>
-    <t>5515 PATRIKA (2523)</t>
-  </si>
-  <si>
-    <t>5516 PATRIKA (JC) *-* (M) (5302 VV)</t>
-  </si>
-  <si>
-    <t>5517 PATRIKA *-* (M) (Patti Aayegi) (6301)</t>
-  </si>
-  <si>
-    <t>5518 PATRIKA (JC) *-* (M) (922)</t>
-  </si>
-  <si>
-    <t>5519 PATRIKA *-* (M) (7066)</t>
-  </si>
-  <si>
-    <t>5520 PATRIKA (1054)</t>
-  </si>
-  <si>
-    <t>5521 PATRIKA (JC) *-* (M) (35)</t>
-  </si>
-  <si>
-    <t>5522 PATRIKA (2231)</t>
-  </si>
-  <si>
-    <t>5523 PATRIKA (2232)</t>
-  </si>
-  <si>
-    <t>5524 PATRIKA (DCU) (5382)</t>
-  </si>
-  <si>
-    <t>5525 PATRIKA *-* (M) (5283)</t>
-  </si>
-  <si>
-    <t>5526 PATRIKA (DCU) (NEW LUSTER - 01)</t>
-  </si>
-  <si>
-    <t>5527 PATRIKA (DCU) (NEW LUSTER - 02)</t>
-  </si>
-  <si>
-    <t>5528 PATRIKA *-* (M) (NEW LUSTER - 03)</t>
-  </si>
-  <si>
-    <t>5529 PATRIKA *-* (M) (NEW LUSTER - 04)</t>
-  </si>
-  <si>
-    <t>5530 PATRIKA *-* (M) (NEW LUSTER - 05)</t>
-  </si>
-  <si>
-    <t>5531 PATRIKA (DCU) (NEW LUSTER - 06)</t>
-  </si>
-  <si>
-    <t>5532 PATRIKA *-* (M) (NEW LUSTER - 07)</t>
-  </si>
-  <si>
-    <t>5533 PATRIKA *-* (M) (NEW LUSTER - 08)</t>
-  </si>
-  <si>
-    <t>5534 PATRIKA *-* (M) (NEW LUSTER - 09)</t>
-  </si>
-  <si>
-    <t>5535 PATRIKA (JC) *-* (M) (1007)</t>
-  </si>
-  <si>
-    <t>5537 PATRIKA (JC) (25-052)</t>
-  </si>
-  <si>
-    <t>5538 PATRIKA (JC) *-* (M) (7073)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA-B (2942-B)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA (JC) (2942)</t>
-  </si>
-  <si>
-    <t>5540 PATRIKA *-* (M) (S-96)</t>
-  </si>
-  <si>
-    <t>5542 PATRIKA (2261)</t>
-  </si>
-  <si>
-    <t>5543 PATRIKA (2353)</t>
-  </si>
-  <si>
-    <t>5544 PATRIKA *-* (M) (2732)</t>
-  </si>
-  <si>
-    <t>5545 PATRIKA *-* (M) (2791)</t>
-  </si>
-  <si>
-    <t>5546 PATRIKA (718)</t>
-  </si>
-  <si>
-    <t>5547 PATRIKA *-* (M) (S-32)</t>
-  </si>
-  <si>
-    <t>5548 PATRIKA (DCU) (2792)</t>
-  </si>
-  <si>
-    <t>5549 PATRIKA (5261 NICE)</t>
-  </si>
-  <si>
-    <t>5550 PATRIKA *-* (M) (5424)</t>
-  </si>
-  <si>
-    <t>5551 PATRIKA (5231)</t>
-  </si>
-  <si>
-    <t>5552 PATRIKA (JC) *-* (M) (S-163)</t>
-  </si>
-  <si>
-    <t>5553 PATRIKA *-* (M) (5004)</t>
-  </si>
-  <si>
-    <t>5554 PATRIKA *-* (F/G) (5379)</t>
-  </si>
-  <si>
-    <t>5555 PATRIKA (2903)</t>
-  </si>
-  <si>
-    <t>5556 PATRIKA *-* (M) (2952)</t>
-  </si>
-  <si>
-    <t>5557 PATRIKA (2312 SBC)</t>
-  </si>
-  <si>
-    <t>5558 PATRIKA *-* (M) (121 NEHA)</t>
-  </si>
-  <si>
-    <t>5559 PATRIKA (2293)</t>
-  </si>
-  <si>
-    <t>5560 PATRIKA (F/G) *-* (2915)</t>
-  </si>
-  <si>
-    <t>5561 PATRIKA *-* (M) (25358)</t>
-  </si>
-  <si>
-    <t>5562 PATRIKA *-* (M) (114-B (NEHA))</t>
-  </si>
-  <si>
-    <t>5563 PATRIKA (5387)</t>
-  </si>
-  <si>
-    <t>5564 PATRIKA (JC) *-* (M) (S-107)</t>
-  </si>
-  <si>
-    <t>5565 PATRIKA (175)</t>
-  </si>
-  <si>
-    <t>5566 PATRIKA *-* (M) (1742-B)</t>
-  </si>
-  <si>
-    <t>5567 PATRIKA (1679)</t>
-  </si>
-  <si>
-    <t>5568 PATRIKA *-* (M) (3002)</t>
-  </si>
-  <si>
-    <t>5569 PATRIKA *-* (M) (S-39)</t>
-  </si>
-  <si>
-    <t>5570 PATRIKA *-* (M) (S-74)</t>
-  </si>
-  <si>
-    <t>5571 PATRIKA *-* (M) (25353)</t>
-  </si>
-  <si>
-    <t>5572 PATRIKA *-* (M) (25351)</t>
-  </si>
-  <si>
-    <t>5573 PATRIKA (2205)</t>
-  </si>
-  <si>
-    <t>5574 PATRIKA (25335)</t>
-  </si>
-  <si>
-    <t>5575 PATRIKA *-* (M) (S-77)</t>
-  </si>
-  <si>
-    <t>5576 PATRIKA (2531)</t>
-  </si>
-  <si>
-    <t>5577 PATRIKA *-* (M) (5808)</t>
-  </si>
-  <si>
-    <t>5578 PATRIKA (JC) *-* (M) (AS-104 / S-50)</t>
-  </si>
-  <si>
-    <t>5579 PATRIKA (JC) *-* (M) (AS-102)</t>
-  </si>
-  <si>
-    <t>5580 PATRIKA (S-326)</t>
-  </si>
-  <si>
-    <t>5581 PATRIKA *-* (M) (3471)</t>
-  </si>
-  <si>
-    <t>5582 PATRIKA *-* (M) (3512 SBC)</t>
-  </si>
-  <si>
-    <t>5583 PATRIKA (3211 SBC)</t>
-  </si>
-  <si>
-    <t>5584 PATRIKA (JC) (2202 SBC)</t>
-  </si>
-  <si>
-    <t>5585 PATRIKA *-* (M) (1201 KBC)</t>
-  </si>
-  <si>
-    <t>5586 PATRIKA *-* (M) (S-51)</t>
-  </si>
-  <si>
-    <t>5587 PATRIKA (2264)</t>
-  </si>
-  <si>
-    <t>5588 PATRIKA (JC) *-* (M) (1006)</t>
-  </si>
-  <si>
-    <t>5589 PATRIKA *-* (M) (25133)</t>
-  </si>
-  <si>
-    <t>5590 PATRIKA (3131 SBC)</t>
-  </si>
-  <si>
-    <t>5592 PATRIKA *-* (M) (2365)</t>
-  </si>
-  <si>
-    <t>5593 PATRIKA (2803)</t>
-  </si>
-  <si>
-    <t>5595 PATRIKA *-* (M) (226)</t>
-  </si>
-  <si>
-    <t>5596 PATRIKA *-* (M) (2541)</t>
-  </si>
-  <si>
-    <t>5597 PATRIKA (JC) *-* (M) (AS-104 (B))</t>
-  </si>
-  <si>
-    <t>5599 PATRIKA *-* (M) (77-B)</t>
-  </si>
-  <si>
-    <t>5601 PATRIKA (2771)</t>
-  </si>
-  <si>
-    <t>5602 PATRIKA (3271)</t>
-  </si>
-  <si>
-    <t>5603 PATRIKA *-* (M) (6125)</t>
-  </si>
-  <si>
-    <t>5604 PATRIKA (242-A)</t>
-  </si>
-  <si>
-    <t>5605 PATRIKA (JC) (3102)</t>
-  </si>
-  <si>
-    <t>5606 PATRIKA *-* (M) (221-A)</t>
-  </si>
-  <si>
-    <t>5607 PATRIKA (25442)</t>
-  </si>
-  <si>
-    <t>5608 PATRIKA (25440)</t>
-  </si>
-  <si>
-    <t>5609 PATRIKA (993)</t>
-  </si>
-  <si>
-    <t>5610 PATRIKA (JC) (2373)</t>
-  </si>
-  <si>
-    <t>5611 PATRIKA *-* (M) (1211)</t>
-  </si>
-  <si>
-    <t>5612 PATRIKA (DCU) (5276)</t>
-  </si>
-  <si>
-    <t>5614 PATRIKA *-* (M) (2331)</t>
-  </si>
-  <si>
-    <t>5615 PATRIKA (2111)</t>
-  </si>
-  <si>
-    <t>5616 PATRIKA (DCU) (7069)</t>
-  </si>
-  <si>
-    <t>5617 PATRIKA *-* (M) (7067)</t>
-  </si>
-  <si>
-    <t>5618 PATRIKA (JC) *-* (M) (S-52)</t>
-  </si>
-  <si>
-    <t>5619 PATRIKA (JC) (1131)</t>
-  </si>
-  <si>
-    <t>5621 PATRIKA (JC) *-* (M) (5297)</t>
-  </si>
-  <si>
-    <t>5622 PATRIKA *-* (M) (25337)</t>
-  </si>
-  <si>
-    <t>5623 PATRIKA (064)</t>
-  </si>
-  <si>
-    <t>5625 PATRIKA (DCU) (772)</t>
-  </si>
-  <si>
-    <t>6601 PATRIKA (L) (5164)</t>
-  </si>
-  <si>
-    <t>6602 PATRIKA (5126)</t>
-  </si>
-  <si>
-    <t>6603 PATRIKA (5111)</t>
-  </si>
-  <si>
-    <t>6604 PATRIKA *-* (M) (5196)</t>
-  </si>
-  <si>
-    <t>6605 PATRIKA (5191)</t>
-  </si>
-  <si>
-    <t>6606 PATRIKA (*-*) R (3023)</t>
-  </si>
-  <si>
-    <t>6607 PATRIKA *-* (M) (0523)</t>
-  </si>
-  <si>
-    <t>6608 PATRIKA (95)</t>
-  </si>
-  <si>
-    <t>6609 PATRIKA *-* (M) (3053)</t>
-  </si>
-  <si>
-    <t>6610 PATRIKA *-* (M) (3019)</t>
-  </si>
-  <si>
-    <t>6611 PATRIKA (3017 VV)</t>
-  </si>
-  <si>
-    <t>6612 PATRIKA (3015)</t>
-  </si>
-  <si>
-    <t>6613 PATRIKA (25164)</t>
-  </si>
-  <si>
-    <t>6614 PATRIKA (DCU) (25131)</t>
-  </si>
-  <si>
-    <t>6615 PATRIKA *-* (M) (915 GAGAN)</t>
-  </si>
-  <si>
-    <t>6616 PATRIKA *-* (M) (911 GAGAN)</t>
-  </si>
-  <si>
-    <t>6617 PATRIKA *-* (M) (3422)</t>
-  </si>
-  <si>
-    <t>6618 PATRIKA *-* (M) (3423)</t>
-  </si>
-  <si>
-    <t>6619 PATRIKA *-* (M) (1193)</t>
-  </si>
-  <si>
-    <t>6620 PATRIKA *-* (M) (1045 GGN (PADDING))</t>
-  </si>
-  <si>
-    <t>6621 PATRIKA *-* (M) (7108 (PADDING))</t>
-  </si>
-  <si>
-    <t>6622 PATRIKA *-* (M) (7259 (PADDING))</t>
-  </si>
-  <si>
-    <t>6623 PATRIKA (25184)</t>
-  </si>
-  <si>
-    <t>6624 PATRIKA *-* (M) (25135)</t>
-  </si>
-  <si>
-    <t>6625 PATRIKA *-* (M) (25116)</t>
-  </si>
-  <si>
-    <t>6626 PATRIKA *-* (M) (25161)</t>
-  </si>
-  <si>
-    <t>6627 PATRIKA *-* (M) (25111)</t>
-  </si>
-  <si>
-    <t>6628 PATRIKA *-* (M) (805 SBC)</t>
-  </si>
-  <si>
-    <t>6629 PATRIKA *-* (M) (812 NEW SBC)</t>
-  </si>
-  <si>
-    <t>6630 PATRIKA *-* (M) (5510 NICE)</t>
-  </si>
-  <si>
-    <t>6631 PATRIKA (DCU) (OLD AP ITEM)</t>
-  </si>
-  <si>
-    <t>6632 PATRIKA (DCU) (932)</t>
-  </si>
-  <si>
-    <t>6633 PATRIKA *-* (M) (7081 VP)</t>
-  </si>
-  <si>
-    <t>6634 PATRIKA (3562)</t>
-  </si>
-  <si>
-    <t>6635 PATRIKA *-* (M) (S-313)</t>
-  </si>
-  <si>
-    <t>6636 PATRIKA *-* (M) (25183)</t>
-  </si>
-  <si>
-    <t>6637 PATRIKA (25162 GE)</t>
-  </si>
-  <si>
-    <t>6638 PATRIKA *-* (M) (3014)</t>
-  </si>
-  <si>
-    <t>6639 PATRIKA (B) (2291-B)</t>
-  </si>
-  <si>
-    <t>6640 PATRIKA *-* (M) (5737 PADING)</t>
-  </si>
-  <si>
-    <t>6641 PATRIKA *-* (M) (5435)</t>
-  </si>
-  <si>
-    <t>6642 PATRIKA *-* (M) (5411 RJ)</t>
-  </si>
-  <si>
-    <t>6643 PATRIKA *-* (M) (25380)</t>
-  </si>
-  <si>
-    <t>6644 PATRIKA (DCU) (25132)</t>
-  </si>
-  <si>
-    <t>6645 PATRIKA *-* (M) (3031)</t>
-  </si>
-  <si>
-    <t>6646 PATRIKA *-* (M) (3034)</t>
-  </si>
-  <si>
-    <t>6647 PATRIKA *-* (M) (25382)</t>
-  </si>
-  <si>
-    <t>6648 PATRIKA *-* (M) (5011 (PADDING))</t>
-  </si>
-  <si>
-    <t>6649 PATRIKA *-* (M) (3402)</t>
-  </si>
-  <si>
-    <t>6650 PATRIKA *-* (M) (3431)</t>
-  </si>
-  <si>
-    <t>6651 PATRIKA (3421)</t>
-  </si>
-  <si>
-    <t>6652 PATRIKA *-* (M) (2764 SBC)</t>
-  </si>
-  <si>
-    <t>6653 PATRIKA *-* (M) (834 SBC NEW)</t>
-  </si>
-  <si>
-    <t>6654 PATRIKA *-* (M) (3461)</t>
-  </si>
-  <si>
-    <t>6655 PATRIKA *-* (M) (7129 (PADDING))</t>
-  </si>
-  <si>
-    <t>6656 PATRIKA (L) (7113 (PADDING))</t>
-  </si>
-  <si>
-    <t>6657 PATRIKA *-* (M) (563  DHANESH)</t>
-  </si>
-  <si>
-    <t>6658 PATRIKA *-* (M) (5319)</t>
-  </si>
-  <si>
-    <t>6659 PATRIKA (25193 (Padding))</t>
-  </si>
-  <si>
-    <t>6660 PATRIKA (25194 (Padding))</t>
-  </si>
-  <si>
-    <t>6661 PATRIKA *-* (M) (1281)</t>
-  </si>
-  <si>
-    <t>6662 PATRIKA (3424)</t>
-  </si>
-  <si>
-    <t>6663 PATRIKA (7103 (PADDING))</t>
-  </si>
-  <si>
-    <t>6664 PATRIKA *-* (M) (5823)</t>
-  </si>
-  <si>
-    <t>6665 PATRIKA *-* (M) (603 DHANESH)</t>
-  </si>
-  <si>
-    <t>6667 PATRIKA *-* (M) (1192 SBC)</t>
-  </si>
-  <si>
-    <t>6668 PATRIKA (DCU) (8102)</t>
-  </si>
-  <si>
-    <t>6669 PATRIKA (DCU) (6197)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA - B (M) (1868-B)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA *-* (M) (1868)</t>
-  </si>
-  <si>
-    <t>6671 PATRIKA *-* (M) (1872)</t>
-  </si>
-  <si>
-    <t>6672 PATRIKA *-* (M) (6132)</t>
-  </si>
-  <si>
-    <t>6673 PATRIKA (DCU) (6196)</t>
-  </si>
-  <si>
-    <t>6674 PATRIKA (DCU) (1503)</t>
-  </si>
-  <si>
-    <t>6675 PATRIKA *-* (M) (1282)</t>
-  </si>
-  <si>
-    <t>6676 PATRIKA (DCU) (533 KBC)</t>
-  </si>
-  <si>
-    <t>6677 PATRIKA (DCU) (25191 PADDING)</t>
-  </si>
-  <si>
-    <t>7265 PATRIKA (O.C.) (133)</t>
-  </si>
-  <si>
-    <t>7283 PATRIKA {F} (O.C.) (4148)</t>
-  </si>
-  <si>
-    <t>7287 PATRIKA (O.C.) (1522)</t>
-  </si>
-  <si>
-    <t>7288 PATRIKA (O.C.) (1178)</t>
-  </si>
-  <si>
-    <t>7293 PATRIKA (O.C.) (AS-20)</t>
-  </si>
-  <si>
-    <t>7309 PATRIKA (O.C.) (4087)</t>
-  </si>
-  <si>
-    <t>7312 PATRIKA (O.C.) (SBC 7312)</t>
-  </si>
-  <si>
-    <t>7319 PATRIKA (O.C.) (2204)</t>
-  </si>
-  <si>
-    <t>7332 PATRIKA (O.C.) (2482)</t>
-  </si>
-  <si>
-    <t>7342 PATRIKA (O.C.) (12)</t>
-  </si>
-  <si>
-    <t>7344 PATRIKA (O.C.) (INV B.P. RED (11))</t>
-  </si>
-  <si>
-    <t>7345 PATRIKA (O.C.) (INV B.P. GOLDEN (120) 5)</t>
-  </si>
-  <si>
-    <t>7401 PATRIKA (25/252)</t>
-  </si>
-  <si>
-    <t>7402 PATRIKA (25/264-263)</t>
-  </si>
-  <si>
-    <t>7403 PATRIKA (25/363/863)</t>
-  </si>
-  <si>
-    <t>7404 PATRIKA (25/283)</t>
-  </si>
-  <si>
-    <t>7405 PATRIKA (25/273)</t>
-  </si>
-  <si>
-    <t>7406 PATRIKA (25/172)</t>
-  </si>
-  <si>
-    <t>7407 PATRIKA *-* (F) (7145 VP)</t>
-  </si>
-  <si>
-    <t>7408 PATRIKA (DCU) (25895)</t>
-  </si>
-  <si>
-    <t>7409 PATRIKA (2521)</t>
-  </si>
-  <si>
-    <t>7410 PATRIKA (2526)</t>
-  </si>
-  <si>
-    <t>7411 PATRIKA (2535)</t>
-  </si>
-  <si>
-    <t>7413 PATRIKA (2543 INV OFFSET)</t>
-  </si>
-  <si>
-    <t>7414 PATRIKA (1015 GREEN OFFSET)</t>
-  </si>
-  <si>
-    <t>7415 PATRIKA *-* (F) (3162 SBC)</t>
-  </si>
-  <si>
-    <t>7416 PATRIKA (2234)</t>
-  </si>
-  <si>
-    <t>7417 PATRIKA (S-201 INV)</t>
-  </si>
-  <si>
-    <t>7418 PATRIKA *-* (डोरी) (1639)</t>
-  </si>
-  <si>
-    <t>7419 PATRIKA (5121)</t>
-  </si>
-  <si>
-    <t>7420 PATRIKA (720)</t>
-  </si>
-  <si>
-    <t>7421 PATRIKA *-* (F) (25-146)</t>
-  </si>
-  <si>
-    <t>7422 PATRIKA (3702)</t>
-  </si>
-  <si>
-    <t>7423 PATRIKA (254 SBC)</t>
-  </si>
-  <si>
-    <t>7424 PATRIKA *-* (F) (25-047)</t>
-  </si>
-  <si>
-    <t>7425 PATRIKA (2082)</t>
-  </si>
-  <si>
-    <t>7426 PATRIKA (F/G) *-* (4052)</t>
-  </si>
-  <si>
-    <t>7427 PATRIKA (2103)</t>
-  </si>
-  <si>
-    <t>7428 PATRIKA (1223 SBC)</t>
-  </si>
-  <si>
-    <t>7429 PATRIKA (F/G) *-* (1851 MONARCH)</t>
-  </si>
-  <si>
-    <t>7430 PATRIKA (6310 GE)</t>
-  </si>
-  <si>
-    <t>7431 PATRIKA (2532)</t>
-  </si>
-  <si>
-    <t>7432 PATRIKA (1174)</t>
-  </si>
-  <si>
-    <t>7433 PATRIKA (1034)</t>
-  </si>
-  <si>
-    <t>7434 PATRIKA (2204 INV)</t>
-  </si>
-  <si>
-    <t>7435 PATRIKA (06)</t>
-  </si>
-  <si>
-    <t>7436 PATRIKA (303)</t>
-  </si>
-  <si>
-    <t>7437 PATRIKA (25323 INV)</t>
-  </si>
-  <si>
-    <t>7438 PATRIKA (25413)</t>
-  </si>
-  <si>
-    <t>7439 PATRIKA (2597)</t>
-  </si>
-  <si>
-    <t>7440 PATRIKA (25896)</t>
-  </si>
-  <si>
-    <t>7441 PATRIKA *-* (F) (243-C)</t>
-  </si>
-  <si>
-    <t>7442 PATRIKA (1855)</t>
-  </si>
-  <si>
-    <t>7443 PATRIKA (1044 SBC)</t>
-  </si>
-  <si>
-    <t>7444 PATRIKA (2014)</t>
-  </si>
-  <si>
-    <t>7445 PATRIKA (2006)</t>
-  </si>
-  <si>
-    <t>7446 PATRIKA (DCU) (6106)</t>
-  </si>
-  <si>
-    <t>7447 PATRIKA (GOPAL 32)</t>
-  </si>
-  <si>
-    <t>7448 PATRIKA (2005- G)</t>
-  </si>
-  <si>
-    <t>7449 PATRIKA (5180)</t>
-  </si>
-  <si>
-    <t>7450 PATRIKA (DCU) (3753)</t>
-  </si>
-  <si>
-    <t>7451 PATRIKA (273 NEHA)</t>
-  </si>
-  <si>
-    <t>7452 PATRIKA (278-B)</t>
-  </si>
-  <si>
-    <t>7453 PATRIKA (ECO - 61) (NEW ECO 61)</t>
-  </si>
-  <si>
-    <t>7454 PATRIKA (ECO -63) (NEW ECO 63)</t>
-  </si>
-  <si>
-    <t>9001 CARD (O.C.) (2498 Cream)</t>
+    <t>4251 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4252 PATRIKA</t>
+  </si>
+  <si>
+    <t>4253 PATRIKA</t>
+  </si>
+  <si>
+    <t>4254 PATRIKA (4210)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4257 PATRIKA</t>
+  </si>
+  <si>
+    <t>4258 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4259 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4260 PATRIKA</t>
+  </si>
+  <si>
+    <t>4261 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4262 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4264 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4265 PATRIKA</t>
+  </si>
+  <si>
+    <t>4266 PATRIKA</t>
+  </si>
+  <si>
+    <t>4267 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4268 PATRIKA (JC) *-* (M+T)</t>
+  </si>
+  <si>
+    <t>4269 PATRIKA</t>
+  </si>
+  <si>
+    <t>4270 PATRIKA</t>
+  </si>
+  <si>
+    <t>4271 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4272 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4273 PATRIKA</t>
+  </si>
+  <si>
+    <t>4274 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4275 PATRIKA</t>
+  </si>
+  <si>
+    <t>4277 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4278 PATRIKA</t>
+  </si>
+  <si>
+    <t>4279 PATRIKA</t>
+  </si>
+  <si>
+    <t>4280 PATRIKA</t>
+  </si>
+  <si>
+    <t>4281 PATRIKA</t>
+  </si>
+  <si>
+    <t>4282 PATRIKA</t>
+  </si>
+  <si>
+    <t>4283 PATRIKA - B (YELLOW)</t>
+  </si>
+  <si>
+    <t>4284 PATRIKA</t>
+  </si>
+  <si>
+    <t>4285 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4286 PATRIKA</t>
+  </si>
+  <si>
+    <t>4287 PATRIKA</t>
+  </si>
+  <si>
+    <t>4288 PATRIKA</t>
+  </si>
+  <si>
+    <t>4289 PATRIKA</t>
+  </si>
+  <si>
+    <t>4290 PATRIKA</t>
+  </si>
+  <si>
+    <t>4291 PATRIKA</t>
+  </si>
+  <si>
+    <t>4292 PATRIKA</t>
+  </si>
+  <si>
+    <t>4293 PATRIKA</t>
+  </si>
+  <si>
+    <t>4294 PATRIKA</t>
+  </si>
+  <si>
+    <t>4295 PATRIKA</t>
+  </si>
+  <si>
+    <t>4296 PATRIKA</t>
+  </si>
+  <si>
+    <t>4297 PATRIKA</t>
+  </si>
+  <si>
+    <t>4298 PATRIKA</t>
+  </si>
+  <si>
+    <t>4299 PATRIKA</t>
+  </si>
+  <si>
+    <t>4300 PATRIKA</t>
+  </si>
+  <si>
+    <t>4301 PATRIKA</t>
+  </si>
+  <si>
+    <t>4302 PATRIKA</t>
+  </si>
+  <si>
+    <t>4303 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4304 PATRIKA</t>
+  </si>
+  <si>
+    <t>4305 PATRIKA</t>
+  </si>
+  <si>
+    <t>4307 PATRIKA</t>
+  </si>
+  <si>
+    <t>4308 PATRIKA</t>
+  </si>
+  <si>
+    <t>4309 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4310 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4311 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4312 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4314 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4315 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4316 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5051 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5052 PATRIKA</t>
+  </si>
+  <si>
+    <t>5053 PATRIKA</t>
+  </si>
+  <si>
+    <t>5054 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5055 PATRIKA</t>
+  </si>
+  <si>
+    <t>5056 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5057 PATRIKA</t>
+  </si>
+  <si>
+    <t>5058 PATRIKA</t>
+  </si>
+  <si>
+    <t>5059 PATRIKA</t>
+  </si>
+  <si>
+    <t>5060 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5061 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5062 PATRIKA</t>
+  </si>
+  <si>
+    <t>5063 PATRIKA</t>
+  </si>
+  <si>
+    <t>5064 PATRIKA</t>
+  </si>
+  <si>
+    <t>5065 PATRIKA</t>
+  </si>
+  <si>
+    <t>5066 PATRIKA</t>
+  </si>
+  <si>
+    <t>5067 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5071 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5072 PATRIKA</t>
+  </si>
+  <si>
+    <t>5073 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5074 PATRIKA</t>
+  </si>
+  <si>
+    <t>5075 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5076 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5077 PATRIKA</t>
+  </si>
+  <si>
+    <t>5079 PATRIKA</t>
+  </si>
+  <si>
+    <t>5080 PATRIKA</t>
+  </si>
+  <si>
+    <t>5081 PATRIKA</t>
+  </si>
+  <si>
+    <t>5083 PATRIKA</t>
+  </si>
+  <si>
+    <t>5084 PATRIKA</t>
+  </si>
+  <si>
+    <t>5085 PATRIKA</t>
+  </si>
+  <si>
+    <t>5086 PATRIKA (JC) *-* (M+D)</t>
+  </si>
+  <si>
+    <t>5088 PATRIKA</t>
+  </si>
+  <si>
+    <t>5089 PATRIKA</t>
+  </si>
+  <si>
+    <t>5090 PATRIKA</t>
+  </si>
+  <si>
+    <t>5092 PATRIKA</t>
+  </si>
+  <si>
+    <t>5093 PATRIKA</t>
+  </si>
+  <si>
+    <t>5094 PATRIKA</t>
+  </si>
+  <si>
+    <t>5095 PATRIKA</t>
+  </si>
+  <si>
+    <t>5096 PATRIKA</t>
+  </si>
+  <si>
+    <t>5097 PATRIKA</t>
+  </si>
+  <si>
+    <t>5098 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5099 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5100 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5102 PATRIKA (5021)</t>
+  </si>
+  <si>
+    <t>5103 PATRIKA</t>
+  </si>
+  <si>
+    <t>5104 PATRIKA</t>
+  </si>
+  <si>
+    <t>5105 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5106 PATRIKA</t>
+  </si>
+  <si>
+    <t>5107 PATRIKA</t>
+  </si>
+  <si>
+    <t>5108 PATRIKA</t>
+  </si>
+  <si>
+    <t>5109 PATRIKA</t>
+  </si>
+  <si>
+    <t>5110 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5111 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5112 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5113 PATRIKA</t>
+  </si>
+  <si>
+    <t>5114 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5115 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5116 PATRIKA</t>
+  </si>
+  <si>
+    <t>5117 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5118 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5502 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5503 PATRIKA</t>
+  </si>
+  <si>
+    <t>5504 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5505 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5506 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5508 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5509 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5510 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5511 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5512 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5513 PATRIKA</t>
+  </si>
+  <si>
+    <t>5514 PATRIKA</t>
+  </si>
+  <si>
+    <t>5515 PATRIKA</t>
+  </si>
+  <si>
+    <t>5516 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5517 PATRIKA *-* (M) (Patti Aayegi)</t>
+  </si>
+  <si>
+    <t>5518 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5519 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5520 PATRIKA</t>
+  </si>
+  <si>
+    <t>5521 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5522 PATRIKA</t>
+  </si>
+  <si>
+    <t>5523 PATRIKA</t>
+  </si>
+  <si>
+    <t>5524 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5525 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5526 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5527 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5528 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5529 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5530 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5531 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5532 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5533 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5534 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5535 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5537 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5538 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA-B</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5540 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5542 PATRIKA</t>
+  </si>
+  <si>
+    <t>5543 PATRIKA</t>
+  </si>
+  <si>
+    <t>5544 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5545 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5546 PATRIKA</t>
+  </si>
+  <si>
+    <t>5547 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5548 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5549 PATRIKA</t>
+  </si>
+  <si>
+    <t>5550 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5551 PATRIKA</t>
+  </si>
+  <si>
+    <t>5552 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5553 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5554 PATRIKA *-* (F/G)</t>
+  </si>
+  <si>
+    <t>5555 PATRIKA</t>
+  </si>
+  <si>
+    <t>5556 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5557 PATRIKA</t>
+  </si>
+  <si>
+    <t>5558 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5559 PATRIKA</t>
+  </si>
+  <si>
+    <t>5560 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>5561 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5562 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5563 PATRIKA</t>
+  </si>
+  <si>
+    <t>5564 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5565 PATRIKA</t>
+  </si>
+  <si>
+    <t>5566 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5567 PATRIKA</t>
+  </si>
+  <si>
+    <t>5568 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5569 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5570 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5571 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5572 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5573 PATRIKA</t>
+  </si>
+  <si>
+    <t>5574 PATRIKA</t>
+  </si>
+  <si>
+    <t>5575 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5576 PATRIKA</t>
+  </si>
+  <si>
+    <t>5577 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5578 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5579 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5580 PATRIKA</t>
+  </si>
+  <si>
+    <t>5581 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5582 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5583 PATRIKA</t>
+  </si>
+  <si>
+    <t>5584 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5585 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5586 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5587 PATRIKA</t>
+  </si>
+  <si>
+    <t>5588 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5589 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5590 PATRIKA</t>
+  </si>
+  <si>
+    <t>5592 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5593 PATRIKA</t>
+  </si>
+  <si>
+    <t>5595 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5596 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5597 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5599 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5601 PATRIKA</t>
+  </si>
+  <si>
+    <t>5602 PATRIKA</t>
+  </si>
+  <si>
+    <t>5603 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5604 PATRIKA</t>
+  </si>
+  <si>
+    <t>5605 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5606 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5607 PATRIKA</t>
+  </si>
+  <si>
+    <t>5608 PATRIKA</t>
+  </si>
+  <si>
+    <t>5609 PATRIKA</t>
+  </si>
+  <si>
+    <t>5610 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5611 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5612 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5614 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5615 PATRIKA</t>
+  </si>
+  <si>
+    <t>5616 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5618 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5619 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5621 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5623 PATRIKA</t>
+  </si>
+  <si>
+    <t>5625 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6601 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6602 PATRIKA</t>
+  </si>
+  <si>
+    <t>6603 PATRIKA</t>
+  </si>
+  <si>
+    <t>6604 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6605 PATRIKA</t>
+  </si>
+  <si>
+    <t>6606 PATRIKA (*-*) R</t>
+  </si>
+  <si>
+    <t>6607 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6608 PATRIKA</t>
+  </si>
+  <si>
+    <t>6609 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6610 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6611 PATRIKA</t>
+  </si>
+  <si>
+    <t>6612 PATRIKA</t>
+  </si>
+  <si>
+    <t>6613 PATRIKA</t>
+  </si>
+  <si>
+    <t>6614 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6615 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6616 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6618 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6619 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6620 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6621 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6623 PATRIKA</t>
+  </si>
+  <si>
+    <t>6624 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6625 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6626 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6627 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6628 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6629 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6630 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6631 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6632 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6633 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6634 PATRIKA</t>
+  </si>
+  <si>
+    <t>6635 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6636 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6637 PATRIKA</t>
+  </si>
+  <si>
+    <t>6638 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6639 PATRIKA (B)</t>
+  </si>
+  <si>
+    <t>6640 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6641 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6642 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6643 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6644 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6645 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6646 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6647 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6648 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6649 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6650 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6651 PATRIKA</t>
+  </si>
+  <si>
+    <t>6652 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6653 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6654 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6655 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6656 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6657 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6658 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6659 PATRIKA</t>
+  </si>
+  <si>
+    <t>6660 PATRIKA</t>
+  </si>
+  <si>
+    <t>6661 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6662 PATRIKA</t>
+  </si>
+  <si>
+    <t>6663 PATRIKA</t>
+  </si>
+  <si>
+    <t>6664 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6665 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6667 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6668 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6669 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA - B (M)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6671 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6672 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6673 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6674 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6675 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6676 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6677 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7265 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7283 PATRIKA {F} (O.C.)</t>
+  </si>
+  <si>
+    <t>7287 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7288 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7293 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7309 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7312 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7319 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7332 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7342 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7344 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7345 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7401 PATRIKA</t>
+  </si>
+  <si>
+    <t>7402 PATRIKA</t>
+  </si>
+  <si>
+    <t>7403 PATRIKA</t>
+  </si>
+  <si>
+    <t>7404 PATRIKA</t>
+  </si>
+  <si>
+    <t>7405 PATRIKA</t>
+  </si>
+  <si>
+    <t>7406 PATRIKA</t>
+  </si>
+  <si>
+    <t>7407 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7408 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7409 PATRIKA</t>
+  </si>
+  <si>
+    <t>7410 PATRIKA</t>
+  </si>
+  <si>
+    <t>7411 PATRIKA</t>
+  </si>
+  <si>
+    <t>7413 PATRIKA</t>
+  </si>
+  <si>
+    <t>7414 PATRIKA</t>
+  </si>
+  <si>
+    <t>7415 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7416 PATRIKA</t>
+  </si>
+  <si>
+    <t>7417 PATRIKA</t>
+  </si>
+  <si>
+    <t>7418 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>7419 PATRIKA</t>
+  </si>
+  <si>
+    <t>7420 PATRIKA</t>
+  </si>
+  <si>
+    <t>7421 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7422 PATRIKA</t>
+  </si>
+  <si>
+    <t>7423 PATRIKA</t>
+  </si>
+  <si>
+    <t>7424 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7425 PATRIKA</t>
+  </si>
+  <si>
+    <t>7426 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7427 PATRIKA</t>
+  </si>
+  <si>
+    <t>7428 PATRIKA</t>
+  </si>
+  <si>
+    <t>7429 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7430 PATRIKA</t>
+  </si>
+  <si>
+    <t>7431 PATRIKA</t>
+  </si>
+  <si>
+    <t>7432 PATRIKA</t>
+  </si>
+  <si>
+    <t>7433 PATRIKA</t>
+  </si>
+  <si>
+    <t>7434 PATRIKA</t>
+  </si>
+  <si>
+    <t>7435 PATRIKA</t>
+  </si>
+  <si>
+    <t>7436 PATRIKA</t>
+  </si>
+  <si>
+    <t>7437 PATRIKA</t>
+  </si>
+  <si>
+    <t>7438 PATRIKA</t>
+  </si>
+  <si>
+    <t>7439 PATRIKA</t>
+  </si>
+  <si>
+    <t>7440 PATRIKA</t>
+  </si>
+  <si>
+    <t>7441 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7442 PATRIKA</t>
+  </si>
+  <si>
+    <t>7443 PATRIKA</t>
+  </si>
+  <si>
+    <t>7444 PATRIKA</t>
+  </si>
+  <si>
+    <t>7445 PATRIKA</t>
+  </si>
+  <si>
+    <t>7446 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7447 PATRIKA</t>
+  </si>
+  <si>
+    <t>7448 PATRIKA</t>
+  </si>
+  <si>
+    <t>7449 PATRIKA</t>
+  </si>
+  <si>
+    <t>7450 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7451 PATRIKA</t>
+  </si>
+  <si>
+    <t>7452 PATRIKA</t>
+  </si>
+  <si>
+    <t>7453 PATRIKA (ECO - 61)</t>
+  </si>
+  <si>
+    <t>7454 PATRIKA (ECO -63)</t>
+  </si>
+  <si>
+    <t>9001 CARD (O.C.)</t>
   </si>
   <si>
     <t>9221 CARDS - YELLOW</t>
@@ -1688,268 +1688,268 @@
     <t>9227 CARDS (9*5 OFFSET)</t>
   </si>
   <si>
-    <t>9228 CARDS (Y) (ORANGE WITH ONLY FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS - B (DCU) (GOLDEN WITH GANESH JI &amp; FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS (C) (CREAM WITH GANESH JI &amp; FOIL)</t>
+    <t>9228 CARDS (Y)</t>
+  </si>
+  <si>
+    <t>9229 CARDS - B (DCU)</t>
+  </si>
+  <si>
+    <t>9229 CARDS (C)</t>
   </si>
   <si>
     <t>9230 (CARD) 9*5 SCREEN</t>
   </si>
   <si>
-    <t>9231 CARDS (DCU) (RIYAZ 9*5 PINK)</t>
-  </si>
-  <si>
-    <t>9232 CARDS (DCU) (RIYAZ 9*5 CREAM)</t>
-  </si>
-  <si>
-    <t>9233 CARDS (DCU) (RIYAZ 9*5 YELLOW)</t>
-  </si>
-  <si>
-    <t>9235 CARDS (DCU) (RIYAZ 9*4 CREAM)</t>
-  </si>
-  <si>
-    <t>9236 CARDS (DCU) (RIYAZ 9*4 YELLOW)</t>
-  </si>
-  <si>
-    <t>9237 CARDS (DCU) (DCU 9*4 RED)</t>
-  </si>
-  <si>
-    <t>9301 CARDS (4242)</t>
-  </si>
-  <si>
-    <t>9302 CARDS (5076)</t>
-  </si>
-  <si>
-    <t>9303 CARDS (5080 Pink)</t>
-  </si>
-  <si>
-    <t>9304 CARDS (5083 Blue)</t>
-  </si>
-  <si>
-    <t>9305 CARDS (9070) (4701 Nice)</t>
-  </si>
-  <si>
-    <t>9306 CARDS (0543 Nice)</t>
-  </si>
-  <si>
-    <t>9307 CARDS *-* (M) (5243 Nice)</t>
-  </si>
-  <si>
-    <t>9308 CARDS (9852)</t>
-  </si>
-  <si>
-    <t>9309 CARDS *-* (T) (9561 Vp)</t>
-  </si>
-  <si>
-    <t>9310 CARDS (3103)</t>
-  </si>
-  <si>
-    <t>9311 CARDS (3115)</t>
-  </si>
-  <si>
-    <t>9312 CARDS *-* (T) (208 VV)</t>
-  </si>
-  <si>
-    <t>9313 CARDS *-* (T) (216)</t>
-  </si>
-  <si>
-    <t>9314 CARDS (P-1)</t>
-  </si>
-  <si>
-    <t>9315 CARDS (DCU) (P-2)</t>
-  </si>
-  <si>
-    <t>9316 CARDS (DCU) (P-3)</t>
-  </si>
-  <si>
-    <t>9317 CARDS (P-4)</t>
-  </si>
-  <si>
-    <t>9318 CARDS (25905)</t>
-  </si>
-  <si>
-    <t>9320 CARDS (S-20)</t>
-  </si>
-  <si>
-    <t>9321 CARDS (22912 GANESH JI)</t>
-  </si>
-  <si>
-    <t>9322 CARDS *-* (M) (22912 COMMON)</t>
-  </si>
-  <si>
-    <t>9323 CARDS (9005 OLD) (9*5 CREAM FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9324 CARDS (9*5 PINK FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9325 CARDS (5229)</t>
-  </si>
-  <si>
-    <t>9326 CARDS (1601)</t>
-  </si>
-  <si>
-    <t>9327 CARDS (25908)</t>
-  </si>
-  <si>
-    <t>9328 CARDS (2543)</t>
-  </si>
-  <si>
-    <t>9329 CARDS (Desgin H/d) (3606)</t>
-  </si>
-  <si>
-    <t>9330 CARDS *-* (T) (9557)</t>
-  </si>
-  <si>
-    <t>9331 CARDS *-*  (T) (9560)</t>
-  </si>
-  <si>
-    <t>9332 CARDS (9847)</t>
-  </si>
-  <si>
-    <t>9333 CARDS (6042)</t>
-  </si>
-  <si>
-    <t>9334 CARDS (10X6 WHITE (2898))</t>
-  </si>
-  <si>
-    <t>9335 CARDS (9003 OLD) (9*5 WHITE)</t>
-  </si>
-  <si>
-    <t>9336 CARDS (2884)</t>
-  </si>
-  <si>
-    <t>9337 CARDS (1635 AP)</t>
-  </si>
-  <si>
-    <t>9338 CARDS (1637 AP)</t>
-  </si>
-  <si>
-    <t>9339 CARDS (5361)</t>
-  </si>
-  <si>
-    <t>9340 CARDS (5658)</t>
-  </si>
-  <si>
-    <t>9341 CARDS (5497)</t>
-  </si>
-  <si>
-    <t>9342 CARDS (2861)</t>
-  </si>
-  <si>
-    <t>9343 CARDS (9*5 WHTE GE HEAVY)</t>
-  </si>
-  <si>
-    <t>9344 CARDS (689)</t>
-  </si>
-  <si>
-    <t>9345 CARDS (358 KALYANI)</t>
-  </si>
-  <si>
-    <t>9346 CARDS (359)</t>
-  </si>
-  <si>
-    <t>9347 CARDS (2853)</t>
-  </si>
-  <si>
-    <t>9348 CARDS *-* (डोरी) (S-124)</t>
-  </si>
-  <si>
-    <t>9349 CARDS (W/o Window) (S-120)</t>
-  </si>
-  <si>
-    <t>9350 CARDS *-* (T) (1632)</t>
-  </si>
-  <si>
-    <t>9351 Card - B (1603 B)</t>
-  </si>
-  <si>
-    <t>9351 CARDS *-* (T) (1603)</t>
-  </si>
-  <si>
-    <t>9352 CARDS *-* (T) (1606 AP)</t>
-  </si>
-  <si>
-    <t>9353 CARDS (1618)</t>
-  </si>
-  <si>
-    <t>9354 CARDS (DCU) (345)</t>
-  </si>
-  <si>
-    <t>9355 CARDS (1624)</t>
-  </si>
-  <si>
-    <t>9356 CARDS (2895/2897)</t>
-  </si>
-  <si>
-    <t>9357 CARDS (2872)</t>
-  </si>
-  <si>
-    <t>9358 CARDS (WHITE PATTA)</t>
-  </si>
-  <si>
-    <t>9359 CARDS (PITCH PATTA)</t>
-  </si>
-  <si>
-    <t>9360 CARDS *-* (M) (GOL ANDA)</t>
-  </si>
-  <si>
-    <t>9361 CARDS (25426)</t>
-  </si>
-  <si>
-    <t>9362 CARDS (363)</t>
-  </si>
-  <si>
-    <t>9363 CARDS *-* (T) (1652)</t>
-  </si>
-  <si>
-    <t>9364 CARDS *-* (T) (1612)</t>
-  </si>
-  <si>
-    <t>9365 CARDS (25429)</t>
-  </si>
-  <si>
-    <t>9366 CARDS (25427 GOLDEN)</t>
-  </si>
-  <si>
-    <t>9367 CARDS (5652)</t>
-  </si>
-  <si>
-    <t>9368 CARDS (9*5 SET 25/26 GOLDEN (25425))</t>
-  </si>
-  <si>
-    <t>9369 CARDS (9*5 SET 25/26 YELLOW (25424))</t>
-  </si>
-  <si>
-    <t>9370 CARDS (9*5 SET 25/26 RED (25423))</t>
-  </si>
-  <si>
-    <t>9371 CARDS (3111 VP)</t>
-  </si>
-  <si>
-    <t>9372 CARDS (9*5 YLW SET (2841))</t>
-  </si>
-  <si>
-    <t>9373 CARDS (1482)</t>
-  </si>
-  <si>
-    <t>9374 CARDS (1485)</t>
-  </si>
-  <si>
-    <t>9375 CARDS (1452 WHITE)</t>
-  </si>
-  <si>
-    <t>9376 CARDS (1529 PRINCE)</t>
-  </si>
-  <si>
-    <t>9377 CARDS (DCU) (9*5 SET GREEN (009))</t>
-  </si>
-  <si>
-    <t>9378 CARDS (2892)</t>
+    <t>9231 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9232 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9233 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9235 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9236 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9237 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9301 CARDS</t>
+  </si>
+  <si>
+    <t>9302 CARDS</t>
+  </si>
+  <si>
+    <t>9303 CARDS</t>
+  </si>
+  <si>
+    <t>9304 CARDS</t>
+  </si>
+  <si>
+    <t>9305 CARDS (9070)</t>
+  </si>
+  <si>
+    <t>9306 CARDS</t>
+  </si>
+  <si>
+    <t>9307 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9308 CARDS</t>
+  </si>
+  <si>
+    <t>9309 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9310 CARDS</t>
+  </si>
+  <si>
+    <t>9311 CARDS</t>
+  </si>
+  <si>
+    <t>9312 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9313 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9314 CARDS</t>
+  </si>
+  <si>
+    <t>9315 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9316 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9317 CARDS</t>
+  </si>
+  <si>
+    <t>9318 CARDS</t>
+  </si>
+  <si>
+    <t>9320 CARDS</t>
+  </si>
+  <si>
+    <t>9321 CARDS</t>
+  </si>
+  <si>
+    <t>9322 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9323 CARDS (9005 OLD)</t>
+  </si>
+  <si>
+    <t>9324 CARDS</t>
+  </si>
+  <si>
+    <t>9325 CARDS</t>
+  </si>
+  <si>
+    <t>9326 CARDS</t>
+  </si>
+  <si>
+    <t>9327 CARDS</t>
+  </si>
+  <si>
+    <t>9328 CARDS</t>
+  </si>
+  <si>
+    <t>9329 CARDS (Desgin H/d)</t>
+  </si>
+  <si>
+    <t>9330 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9331 CARDS *-*  (T)</t>
+  </si>
+  <si>
+    <t>9332 CARDS</t>
+  </si>
+  <si>
+    <t>9333 CARDS</t>
+  </si>
+  <si>
+    <t>9334 CARDS</t>
+  </si>
+  <si>
+    <t>9335 CARDS (9003 OLD)</t>
+  </si>
+  <si>
+    <t>9336 CARDS</t>
+  </si>
+  <si>
+    <t>9337 CARDS</t>
+  </si>
+  <si>
+    <t>9338 CARDS</t>
+  </si>
+  <si>
+    <t>9339 CARDS</t>
+  </si>
+  <si>
+    <t>9340 CARDS</t>
+  </si>
+  <si>
+    <t>9341 CARDS</t>
+  </si>
+  <si>
+    <t>9342 CARDS</t>
+  </si>
+  <si>
+    <t>9343 CARDS</t>
+  </si>
+  <si>
+    <t>9344 CARDS</t>
+  </si>
+  <si>
+    <t>9345 CARDS</t>
+  </si>
+  <si>
+    <t>9346 CARDS</t>
+  </si>
+  <si>
+    <t>9347 CARDS</t>
+  </si>
+  <si>
+    <t>9348 CARDS *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>9349 CARDS (W/o Window)</t>
+  </si>
+  <si>
+    <t>9350 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9351 Card - B</t>
+  </si>
+  <si>
+    <t>9351 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9352 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9353 CARDS</t>
+  </si>
+  <si>
+    <t>9354 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9355 CARDS</t>
+  </si>
+  <si>
+    <t>9356 CARDS</t>
+  </si>
+  <si>
+    <t>9357 CARDS</t>
+  </si>
+  <si>
+    <t>9358 CARDS</t>
+  </si>
+  <si>
+    <t>9359 CARDS</t>
+  </si>
+  <si>
+    <t>9360 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9361 CARDS</t>
+  </si>
+  <si>
+    <t>9362 CARDS</t>
+  </si>
+  <si>
+    <t>9363 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9364 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9365 CARDS</t>
+  </si>
+  <si>
+    <t>9366 CARDS</t>
+  </si>
+  <si>
+    <t>9367 CARDS</t>
+  </si>
+  <si>
+    <t>9368 CARDS</t>
+  </si>
+  <si>
+    <t>9369 CARDS</t>
+  </si>
+  <si>
+    <t>9370 CARDS</t>
+  </si>
+  <si>
+    <t>9371 CARDS</t>
+  </si>
+  <si>
+    <t>9372 CARDS</t>
+  </si>
+  <si>
+    <t>9373 CARDS</t>
+  </si>
+  <si>
+    <t>9374 CARDS</t>
+  </si>
+  <si>
+    <t>9375 CARDS</t>
+  </si>
+  <si>
+    <t>9376 CARDS</t>
+  </si>
+  <si>
+    <t>9377 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9378 CARDS</t>
   </si>
   <si>
     <t>9379 CARDS - R</t>
@@ -1979,19 +1979,19 @@
     <t>9387 CARDS - GOLDEN (Mil Jayega)</t>
   </si>
   <si>
-    <t>9389 CARDS (9147 RJ)</t>
-  </si>
-  <si>
-    <t>9390 CARDS (DCU) (118KBC)</t>
+    <t>9389 CARDS</t>
+  </si>
+  <si>
+    <t>9390 CARDS (DCU)</t>
   </si>
   <si>
     <t>9391 CARDS</t>
   </si>
   <si>
-    <t>9*4 ENVELOPE (SBC) (CHOTA ENVELOPE (60/40 BILL))</t>
-  </si>
-  <si>
-    <t>9*5 ENVELOPE (FOIL) SBC (BADA ENVLP WITH FOIL (60/40 BILL))</t>
+    <t>9*4 ENVELOPE (SBC)</t>
+  </si>
+  <si>
+    <t>9*5 ENVELOPE (FOIL) SBC</t>
   </si>
   <si>
     <t>ACRYLIC NAME PLATE</t>
@@ -2000,7 +2000,7 @@
     <t>DEV SAMPLE SET</t>
   </si>
   <si>
-    <t>FANCY GIFT ENVELOPE-(SR) (SR ENVELOPES)</t>
+    <t>FANCY GIFT ENVELOPE-(SR)</t>
   </si>
   <si>
     <t>Gift Envelope (Pocket) SR...</t>
@@ -2018,34 +2018,34 @@
     <t>RIBBON (रिबीन)</t>
   </si>
   <si>
-    <t>RX-01 ENVELOPE (LX01)</t>
-  </si>
-  <si>
-    <t>RX-02 ENVELOPE (LX02)</t>
-  </si>
-  <si>
-    <t>RX-03 ENVELOPE (LX03)</t>
-  </si>
-  <si>
-    <t>RX-04 ENVELOPE (LX04)</t>
-  </si>
-  <si>
-    <t>RX-05 ENVELOPE (LX05)</t>
-  </si>
-  <si>
-    <t>RX-06 ENVELOPE (LX06)</t>
-  </si>
-  <si>
-    <t>RX-07 ENVELOPE (LX07)</t>
-  </si>
-  <si>
-    <t>RX-08 ENVELOPE (LX08)</t>
-  </si>
-  <si>
-    <t>RX-09 ENVELOPE (LX09)</t>
-  </si>
-  <si>
-    <t>गोल गणेश / गोल फ्लावर (GOL GANESH OR GOL FLOWER)</t>
+    <t>RX-01 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-02 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-03 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-04 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-05 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-06 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-07 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-08 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-09 ENVELOPE</t>
+  </si>
+  <si>
+    <t>गोल गणेश / गोल फ्लावर</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -2578,7 +2578,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -2768,16 +2768,16 @@
         <v>18</v>
       </c>
       <c r="B15" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="25">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="26">
         <v>2</v>
       </c>
       <c r="E15" s="27">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3659,16 +3659,16 @@
         <v>71</v>
       </c>
       <c r="B68" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C68" s="25">
-        <v>273.5</v>
+        <v>267.5</v>
       </c>
       <c r="D68" s="26">
         <v>1.4</v>
       </c>
       <c r="E68" s="27">
-        <v>382.9</v>
+        <v>374.5</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3676,16 +3676,16 @@
         <v>72</v>
       </c>
       <c r="B69" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C69" s="25">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D69" s="26">
         <v>1.4</v>
       </c>
       <c r="E69" s="27">
-        <v>392</v>
+        <v>386.4</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3744,16 +3744,16 @@
         <v>76</v>
       </c>
       <c r="B73" s="24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C73" s="25">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="D73" s="26">
         <v>1.2</v>
       </c>
       <c r="E73" s="27">
-        <v>752.4</v>
+        <v>742.8</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3761,16 +3761,16 @@
         <v>77</v>
       </c>
       <c r="B74" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C74" s="25">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>795.6</v>
+        <v>790.8</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4354,16 +4354,16 @@
         <v>116</v>
       </c>
       <c r="B113" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C113" s="25">
-        <v>346.5</v>
+        <v>306.5</v>
       </c>
       <c r="D113" s="26">
         <v>0.7</v>
       </c>
       <c r="E113" s="27">
-        <v>242.55</v>
+        <v>214.55</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4569,16 +4569,16 @@
         <v>131</v>
       </c>
       <c r="B128" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C128" s="25">
-        <v>21</v>
+        <v>19.5</v>
       </c>
       <c r="D128" s="26">
         <v>12.5</v>
       </c>
       <c r="E128" s="27">
-        <v>262.5</v>
+        <v>243.75</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4805,16 +4805,16 @@
         <v>145</v>
       </c>
       <c r="B142" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C142" s="25">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D142" s="26">
         <v>18.5</v>
       </c>
       <c r="E142" s="27">
-        <v>92.5</v>
+        <v>277.5</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -5111,16 +5111,16 @@
         <v>163</v>
       </c>
       <c r="B160" s="24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C160" s="25">
-        <v>83.25</v>
+        <v>58.25</v>
       </c>
       <c r="D160" s="26">
         <v>1</v>
       </c>
       <c r="E160" s="27">
-        <v>83.25</v>
+        <v>58.25</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -5144,15 +5144,17 @@
       <c r="A162" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B162" s="24"/>
+      <c r="B162" s="24">
+        <v>1</v>
+      </c>
       <c r="C162" s="25">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D162" s="26">
         <v>1.3</v>
       </c>
       <c r="E162" s="27">
-        <v>390</v>
+        <v>384.8</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -5163,13 +5165,13 @@
         <v>65</v>
       </c>
       <c r="C163" s="25">
-        <v>-6.5</v>
+        <v>-22.5</v>
       </c>
       <c r="D163" s="26">
         <v>1.1499999999999999</v>
       </c>
       <c r="E163" s="27">
-        <v>-7.47</v>
+        <v>-25.87</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5394,16 +5396,16 @@
         <v>180</v>
       </c>
       <c r="B177" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C177" s="25">
-        <v>28.5</v>
+        <v>26.5</v>
       </c>
       <c r="D177" s="26">
         <v>2.76</v>
       </c>
       <c r="E177" s="27">
-        <v>78.72</v>
+        <v>73.19</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5565,13 +5567,13 @@
         <v>21</v>
       </c>
       <c r="C187" s="25">
-        <v>42.5</v>
+        <v>86.5</v>
       </c>
       <c r="D187" s="26">
         <v>4.5</v>
       </c>
       <c r="E187" s="27">
-        <v>191.25</v>
+        <v>389.25</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -6246,13 +6248,13 @@
         <v>17</v>
       </c>
       <c r="C228" s="25">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="D228" s="26">
         <v>4.8</v>
       </c>
       <c r="E228" s="27">
-        <v>211.2</v>
+        <v>360</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6260,16 +6262,16 @@
         <v>232</v>
       </c>
       <c r="B229" s="24">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C229" s="25">
-        <v>35</v>
+        <v>33.5</v>
       </c>
       <c r="D229" s="26">
         <v>6.3</v>
       </c>
       <c r="E229" s="27">
-        <v>220.5</v>
+        <v>211.05</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -6528,16 +6530,16 @@
         <v>248</v>
       </c>
       <c r="B245" s="24">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C245" s="25">
-        <v>417</v>
+        <v>414.5</v>
       </c>
       <c r="D245" s="26">
         <v>4.28</v>
       </c>
       <c r="E245" s="27">
-        <v>1784.76</v>
+        <v>1774.06</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6647,16 +6649,16 @@
         <v>255</v>
       </c>
       <c r="B252" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C252" s="25">
-        <v>35.369999999999997</v>
+        <v>133.87</v>
       </c>
       <c r="D252" s="26">
         <v>4.25</v>
       </c>
       <c r="E252" s="27">
-        <v>150.32</v>
+        <v>568.95000000000005</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6800,16 +6802,16 @@
         <v>264</v>
       </c>
       <c r="B261" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C261" s="25">
-        <v>63.5</v>
+        <v>62</v>
       </c>
       <c r="D261" s="26">
         <v>6.18</v>
       </c>
       <c r="E261" s="27">
-        <v>392.45</v>
+        <v>383.18</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6854,13 +6856,13 @@
         <v>26</v>
       </c>
       <c r="C264" s="25">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="D264" s="26">
         <v>5</v>
       </c>
       <c r="E264" s="27">
-        <v>55</v>
+        <v>805</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6871,13 +6873,13 @@
         <v>6</v>
       </c>
       <c r="C265" s="25">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D265" s="26">
         <v>6</v>
       </c>
       <c r="E265" s="27">
-        <v>120</v>
+        <v>312</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -6939,13 +6941,13 @@
         <v>17</v>
       </c>
       <c r="C269" s="25">
-        <v>47</v>
+        <v>147</v>
       </c>
       <c r="D269" s="26">
         <v>4.5</v>
       </c>
       <c r="E269" s="27">
-        <v>211.5</v>
+        <v>661.5</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -7019,16 +7021,16 @@
         <v>277</v>
       </c>
       <c r="B274" s="24">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C274" s="25">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D274" s="26">
         <v>6</v>
       </c>
       <c r="E274" s="27">
-        <v>599.96</v>
+        <v>629.95000000000005</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -7056,13 +7058,13 @@
         <v>22</v>
       </c>
       <c r="C276" s="25">
-        <v>129</v>
+        <v>319</v>
       </c>
       <c r="D276" s="26">
-        <v>4.24</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="E276" s="27">
-        <v>546.78</v>
+        <v>1361.58</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -7122,13 +7124,13 @@
         <v>23</v>
       </c>
       <c r="C280" s="25">
-        <v>120</v>
+        <v>270</v>
       </c>
       <c r="D280" s="26">
         <v>4.29</v>
       </c>
       <c r="E280" s="27">
-        <v>514.23</v>
+        <v>1158.78</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
@@ -7484,13 +7486,13 @@
         <v>16</v>
       </c>
       <c r="C302" s="25">
-        <v>6.2</v>
+        <v>26.2</v>
       </c>
       <c r="D302" s="26">
         <v>10</v>
       </c>
       <c r="E302" s="27">
-        <v>62</v>
+        <v>262</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7896,16 +7898,16 @@
         <v>330</v>
       </c>
       <c r="B327" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C327" s="25">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="D327" s="26">
         <v>7.36</v>
       </c>
       <c r="E327" s="27">
-        <v>92</v>
+        <v>77.28</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -8152,13 +8154,13 @@
         <v>22</v>
       </c>
       <c r="C342" s="25">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D342" s="26">
         <v>7.13</v>
       </c>
       <c r="E342" s="27">
-        <v>128.34</v>
+        <v>385.02</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
@@ -8217,16 +8219,16 @@
         <v>349</v>
       </c>
       <c r="B346" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C346" s="25">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D346" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E346" s="27">
-        <v>106.6</v>
+        <v>131.19999999999999</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
@@ -8390,13 +8392,13 @@
         <v>15</v>
       </c>
       <c r="C356" s="25">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D356" s="26">
         <v>6</v>
       </c>
       <c r="E356" s="27">
-        <v>246</v>
+        <v>402</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
@@ -9088,13 +9090,13 @@
         <v>6</v>
       </c>
       <c r="C398" s="25">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D398" s="26">
         <v>6</v>
       </c>
       <c r="E398" s="27">
-        <v>66</v>
+        <v>210</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -9285,16 +9287,16 @@
         <v>413</v>
       </c>
       <c r="B410" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C410" s="25">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="D410" s="26">
         <v>11</v>
       </c>
       <c r="E410" s="27">
-        <v>88</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
@@ -9621,16 +9623,16 @@
         <v>433</v>
       </c>
       <c r="B430" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C430" s="25">
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="D430" s="26">
         <v>15.5</v>
       </c>
       <c r="E430" s="27">
-        <v>139.5</v>
+        <v>162.75</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
@@ -11255,16 +11257,16 @@
         <v>531</v>
       </c>
       <c r="B528" s="24">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C528" s="25">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="D528" s="26">
         <v>3.5</v>
       </c>
       <c r="E528" s="27">
-        <v>84</v>
+        <v>238</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -11547,10 +11549,10 @@
         <v>549</v>
       </c>
       <c r="B546" s="24">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C546" s="25">
-        <v>96.5</v>
+        <v>94.5</v>
       </c>
       <c r="D546" s="28"/>
       <c r="E546" s="29"/>
@@ -11573,10 +11575,10 @@
         <v>551</v>
       </c>
       <c r="B548" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C548" s="25">
-        <v>149.9</v>
+        <v>146.9</v>
       </c>
       <c r="D548" s="28"/>
       <c r="E548" s="29"/>
@@ -11603,16 +11605,16 @@
         <v>553</v>
       </c>
       <c r="B550" s="24">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C550" s="25">
-        <v>1106</v>
+        <v>1088</v>
       </c>
       <c r="D550" s="26">
         <v>0.57999999999999996</v>
       </c>
       <c r="E550" s="27">
-        <v>641.48</v>
+        <v>631.04</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.25">
@@ -11620,16 +11622,16 @@
         <v>554</v>
       </c>
       <c r="B551" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C551" s="25">
-        <v>564.5</v>
+        <v>554.5</v>
       </c>
       <c r="D551" s="26">
         <v>0.85</v>
       </c>
       <c r="E551" s="27">
-        <v>479.83</v>
+        <v>471.33</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11815,16 +11817,16 @@
         <v>567</v>
       </c>
       <c r="B564" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C564" s="25">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="D564" s="26">
         <v>8.25</v>
       </c>
       <c r="E564" s="27">
-        <v>61.88</v>
+        <v>45.38</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
@@ -13001,16 +13003,16 @@
         <v>637</v>
       </c>
       <c r="B634" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C634" s="25">
-        <v>17.5</v>
+        <v>17</v>
       </c>
       <c r="D634" s="26">
         <v>4.25</v>
       </c>
       <c r="E634" s="27">
-        <v>74.38</v>
+        <v>72.25</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.25">
@@ -13321,10 +13323,10 @@
         <v>659</v>
       </c>
       <c r="B656" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C656" s="25">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="D656" s="28"/>
       <c r="E656" s="29"/>
@@ -13475,16 +13477,16 @@
         <v>669</v>
       </c>
       <c r="B666" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C666" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D666" s="26">
         <v>2.5</v>
       </c>
       <c r="E666" s="27">
-        <v>10</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="667" spans="1:5" x14ac:dyDescent="0.25">
@@ -13557,11 +13559,11 @@
       </c>
       <c r="B671" s="31"/>
       <c r="C671" s="32">
-        <v>38316.33</v>
+        <v>39112.33</v>
       </c>
       <c r="D671" s="33"/>
       <c r="E671" s="34">
-        <v>106673.88</v>
+        <v>111232.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil @ 25 dec @8.57
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -65,307 +65,307 @@
     <t>Value</t>
   </si>
   <si>
-    <t>.1001 PATRIKA (25/251)</t>
-  </si>
-  <si>
-    <t>1002 PATRIKA (25/262)</t>
-  </si>
-  <si>
-    <t>1003 PATRIKA (25/261)</t>
-  </si>
-  <si>
-    <t>1004 PATRIKA (25/361/861)</t>
-  </si>
-  <si>
-    <t>1005 PATRIKA (25/362/862)</t>
-  </si>
-  <si>
-    <t>1006 PATRIKA (25/282)</t>
-  </si>
-  <si>
-    <t>1007 PATRIKA (25/281)</t>
-  </si>
-  <si>
-    <t>1008 PATRIKA (JC) (2595 PINK)</t>
-  </si>
-  <si>
-    <t>1009 PATRIKA (JC) (2595 ORANGE)</t>
-  </si>
-  <si>
-    <t>1010 PATRIKA (6321)</t>
-  </si>
-  <si>
-    <t>1011 PATRIKA (2563 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1012 PATRIKA (2564 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1013 PATRIKA (2568 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1014 PATRIKA (11043 OFFSET)</t>
-  </si>
-  <si>
-    <t>1015 PATRIKA (DCU) (11041 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1016 PATRIKA (1011 OFFSET)</t>
-  </si>
-  <si>
-    <t>1017 PATRIKA (1014 OFFSET)</t>
-  </si>
-  <si>
-    <t>1018 PATRIKA (10081 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1019 PATRIKA (1222 SBC)</t>
-  </si>
-  <si>
-    <t>1020 PATRIKA (1235)</t>
-  </si>
-  <si>
-    <t>1021 PATRIKA (2101 VV)</t>
-  </si>
-  <si>
-    <t>1023 PATRIKA (25418)</t>
-  </si>
-  <si>
-    <t>1024 PATRIKA (25322)</t>
-  </si>
-  <si>
-    <t>1025 PATRIKA (25323)</t>
-  </si>
-  <si>
-    <t>1026 PATRIKA (JC) (1173 SBC)</t>
-  </si>
-  <si>
-    <t>1027 PATRIKA (JC) (5346)</t>
-  </si>
-  <si>
-    <t>1028 PATRIKA (JC) (2596)</t>
-  </si>
-  <si>
-    <t>1029 PATRIKA (1042)</t>
-  </si>
-  <si>
-    <t>1030 PATRIKA (1043)</t>
-  </si>
-  <si>
-    <t>1031 PATRIKA (GOPAL 11)</t>
-  </si>
-  <si>
-    <t>1032 PATRIKA (GOPAL 1)</t>
-  </si>
-  <si>
-    <t>1033 PATRIKA (2002 YLW)</t>
-  </si>
-  <si>
-    <t>1034 PATRIKA (2003 R)</t>
-  </si>
-  <si>
-    <t>1035 PATRIKA (DCU) (2201 ROSHAN)</t>
-  </si>
-  <si>
-    <t>1101 PATRIKA (O.2591) (2591 ORANGE)</t>
-  </si>
-  <si>
-    <t>1102 PATRIKA (P.2591) (2591 PINK)</t>
-  </si>
-  <si>
-    <t>1103 PATRIKA(N-271) (271 NEHA)</t>
-  </si>
-  <si>
-    <t>1104 PATRIKA(N-272) (272 NEHA)</t>
-  </si>
-  <si>
-    <t>1105 PATRIKA (276-A)</t>
-  </si>
-  <si>
-    <t>1106 PATRIKA-YELLOW (25419)</t>
-  </si>
-  <si>
-    <t>1107 PATRIKA-RED (25420)</t>
-  </si>
-  <si>
-    <t>1109 PATRIKA-BIG Y (25421)</t>
-  </si>
-  <si>
-    <t>1110 PATRIKA-BIG R (25422)</t>
-  </si>
-  <si>
-    <t>1112 PATRIKA (277-B)</t>
-  </si>
-  <si>
-    <t>1113 PATRIKA (1819 MONARCH)</t>
-  </si>
-  <si>
-    <t>1114 PATRIKA-BROWN (1709)</t>
-  </si>
-  <si>
-    <t>1115 PATRIKA-CREAM (1678 PRINCE)</t>
-  </si>
-  <si>
-    <t>1116 PATRIKA (1153) (1253 Jsk)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA (1155) (1155 JSK)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA - B (KRISHNA 1155-B)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA - B (DCU) (NEW SAVASHREE- 51)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA (सवाश्री-57) (NEW SAVASHREE-57)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA - B (DCU) (NEW SAVASHREE 52)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA(सवाश्री-55) (NEW SAVASHREE-55)</t>
-  </si>
-  <si>
-    <t>1120 PATRIKA(सवाश्री-59) (NEW SAVASHREE-59)</t>
-  </si>
-  <si>
-    <t>1121 PATRIKA(सवाश्री-53) (NEW SAVASHREE-53)</t>
-  </si>
-  <si>
-    <t>1122 PATRIKA (DCU) (NEW SAVASHREE-54)</t>
-  </si>
-  <si>
-    <t>1123 PATRIKA (LED-51) (LED-51)</t>
-  </si>
-  <si>
-    <t>1124 PATRIKA (LED-52) (LED-52)</t>
-  </si>
-  <si>
-    <t>1125 PATRIKA (LED-53) (LED-53)</t>
-  </si>
-  <si>
-    <t>1126 PATRIKA (LED-54) (LED-54)</t>
-  </si>
-  <si>
-    <t>1127 PATRIKA (Eco-52) (NEW ECO-52)</t>
-  </si>
-  <si>
-    <t>1128 PATRIKA (Eco-55) (NEW ECO-55)</t>
-  </si>
-  <si>
-    <t>1129 PATRIKA (Eco-56) (NEW ECO-56)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA - B (ECO-60) (DCU) (NEW ECO 60)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA (Eco-59) (NEW ECO-59)</t>
-  </si>
-  <si>
-    <t>1131 PATRIKA (DCU) Eco-51 (NEW ECO- 51)</t>
-  </si>
-  <si>
-    <t>1132 PATRIKA (DCU) Eco-53 (NEW ECO- 53)</t>
-  </si>
-  <si>
-    <t>1133 PATRIKA (DCU) Eco-57 (NEW ECO- 57)</t>
-  </si>
-  <si>
-    <t>1134 PATRIKA (DCU) Eco-58 (NEW ECO- 58)</t>
-  </si>
-  <si>
-    <t>1135 PATRIKA (DCU) Eco-54 (NEW ECO- 54)</t>
-  </si>
-  <si>
-    <t>1136 PATRIKA (R) (120 GSM RED)</t>
-  </si>
-  <si>
-    <t>1137 PATRIKA (P) (120 GSM YELLOW)</t>
-  </si>
-  <si>
-    <t>1138 PATRIKA (BR) (150 GSM FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1139 PATRIKA (BY) (150 GSM FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1140 PATRIKA (BB) (150 GSM FOIL (BROWN))</t>
-  </si>
-  <si>
-    <t>1141 PATRIKA (R) (120 GSM (RED)SELF)</t>
-  </si>
-  <si>
-    <t>1142 PATRIKA (P) (120 GSM (YELLOW) SELF)</t>
-  </si>
-  <si>
-    <t>1143 PATRIKA (G) (120 GSM (OLD GOLDEN))</t>
-  </si>
-  <si>
-    <t>1144 PATRIKA (BR) (170 GSM WITH FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1145 PATRIKA (BY) (170 GSM WITH FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1146 PATRIKA (DCU) (BROWN 170 GSM FOIL)</t>
-  </si>
-  <si>
-    <t>1147 PATRIKA (S.201) (201 WESTERN)</t>
-  </si>
-  <si>
-    <t>1148 PATRIKA (S.202) (202 WESTERN)</t>
-  </si>
-  <si>
-    <t>1149 PATRIKA (S.204) (204 WESTERN)</t>
-  </si>
-  <si>
-    <t>1150 PATRIKA (DCU) (NEW SAVASHREE-58)</t>
-  </si>
-  <si>
-    <t>1151 PATRIKA (DCU) (NEW SAVASHREE-56)</t>
-  </si>
-  <si>
-    <t>1152 PATRIKA (DCU) (WESTERN 202 OLD)</t>
-  </si>
-  <si>
-    <t>1153 PATRIKA (DCU) (201 WESTERN (OLD))</t>
-  </si>
-  <si>
-    <t>1154 PATRIKA (DCU) (203 WESTERN A)</t>
-  </si>
-  <si>
-    <t>1155 PATRIKA (DCU) (WESTERN (203) B)</t>
-  </si>
-  <si>
-    <t>1157 PATRIKA-CREAM (LU-52 (CREAM))</t>
-  </si>
-  <si>
-    <t>1158 PATRIKA-GOLDEN (LU-53 (GOLDEN))</t>
-  </si>
-  <si>
-    <t>1159 PATRIKA-WHITE (LU-54 (WHITE))</t>
-  </si>
-  <si>
-    <t>1160 PATRIKA-PINK (LU-55 (PINK))</t>
-  </si>
-  <si>
-    <t>1161 PATRIKA (01) (JCC 01)</t>
-  </si>
-  <si>
-    <t>1162 PATRIKA (02) (JCC 02)</t>
-  </si>
-  <si>
-    <t>1163 PATRIKA (DCU) (BP RED)</t>
-  </si>
-  <si>
-    <t>1164 PATRIKA (DCU) (BP PINK RIYAZ)</t>
-  </si>
-  <si>
-    <t>1165 PATRIKA (DCU) (BP CREAM)</t>
-  </si>
-  <si>
-    <t>1166 PATRIKA (DCU) (BP YELLOW)</t>
+    <t>.1001 PATRIKA</t>
+  </si>
+  <si>
+    <t>1002 PATRIKA</t>
+  </si>
+  <si>
+    <t>1003 PATRIKA</t>
+  </si>
+  <si>
+    <t>1004 PATRIKA</t>
+  </si>
+  <si>
+    <t>1005 PATRIKA</t>
+  </si>
+  <si>
+    <t>1006 PATRIKA</t>
+  </si>
+  <si>
+    <t>1007 PATRIKA</t>
+  </si>
+  <si>
+    <t>1008 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1009 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1010 PATRIKA</t>
+  </si>
+  <si>
+    <t>1011 PATRIKA</t>
+  </si>
+  <si>
+    <t>1012 PATRIKA</t>
+  </si>
+  <si>
+    <t>1013 PATRIKA</t>
+  </si>
+  <si>
+    <t>1014 PATRIKA</t>
+  </si>
+  <si>
+    <t>1015 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1016 PATRIKA</t>
+  </si>
+  <si>
+    <t>1017 PATRIKA</t>
+  </si>
+  <si>
+    <t>1018 PATRIKA</t>
+  </si>
+  <si>
+    <t>1019 PATRIKA</t>
+  </si>
+  <si>
+    <t>1020 PATRIKA</t>
+  </si>
+  <si>
+    <t>1021 PATRIKA</t>
+  </si>
+  <si>
+    <t>1023 PATRIKA</t>
+  </si>
+  <si>
+    <t>1024 PATRIKA</t>
+  </si>
+  <si>
+    <t>1025 PATRIKA</t>
+  </si>
+  <si>
+    <t>1026 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1027 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1028 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1029 PATRIKA</t>
+  </si>
+  <si>
+    <t>1030 PATRIKA</t>
+  </si>
+  <si>
+    <t>1031 PATRIKA</t>
+  </si>
+  <si>
+    <t>1032 PATRIKA</t>
+  </si>
+  <si>
+    <t>1033 PATRIKA</t>
+  </si>
+  <si>
+    <t>1034 PATRIKA</t>
+  </si>
+  <si>
+    <t>1035 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1101 PATRIKA (O.2591)</t>
+  </si>
+  <si>
+    <t>1102 PATRIKA (P.2591)</t>
+  </si>
+  <si>
+    <t>1103 PATRIKA(N-271)</t>
+  </si>
+  <si>
+    <t>1104 PATRIKA(N-272)</t>
+  </si>
+  <si>
+    <t>1105 PATRIKA</t>
+  </si>
+  <si>
+    <t>1106 PATRIKA-YELLOW</t>
+  </si>
+  <si>
+    <t>1107 PATRIKA-RED</t>
+  </si>
+  <si>
+    <t>1109 PATRIKA-BIG Y</t>
+  </si>
+  <si>
+    <t>1110 PATRIKA-BIG R</t>
+  </si>
+  <si>
+    <t>1112 PATRIKA</t>
+  </si>
+  <si>
+    <t>1113 PATRIKA</t>
+  </si>
+  <si>
+    <t>1114 PATRIKA-BROWN</t>
+  </si>
+  <si>
+    <t>1115 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1116 PATRIKA (1153)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA (1155)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA - B</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA (सवाश्री-57)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA(सवाश्री-55)</t>
+  </si>
+  <si>
+    <t>1120 PATRIKA(सवाश्री-59)</t>
+  </si>
+  <si>
+    <t>1121 PATRIKA(सवाश्री-53)</t>
+  </si>
+  <si>
+    <t>1122 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1123 PATRIKA (LED-51)</t>
+  </si>
+  <si>
+    <t>1124 PATRIKA (LED-52)</t>
+  </si>
+  <si>
+    <t>1125 PATRIKA (LED-53)</t>
+  </si>
+  <si>
+    <t>1126 PATRIKA (LED-54)</t>
+  </si>
+  <si>
+    <t>1127 PATRIKA (Eco-52)</t>
+  </si>
+  <si>
+    <t>1128 PATRIKA (Eco-55)</t>
+  </si>
+  <si>
+    <t>1129 PATRIKA (Eco-56)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA - B (ECO-60) (DCU)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA (Eco-59)</t>
+  </si>
+  <si>
+    <t>1131 PATRIKA (DCU) Eco-51</t>
+  </si>
+  <si>
+    <t>1132 PATRIKA (DCU) Eco-53</t>
+  </si>
+  <si>
+    <t>1133 PATRIKA (DCU) Eco-57</t>
+  </si>
+  <si>
+    <t>1134 PATRIKA (DCU) Eco-58</t>
+  </si>
+  <si>
+    <t>1135 PATRIKA (DCU) Eco-54</t>
+  </si>
+  <si>
+    <t>1136 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1137 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1138 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1139 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1140 PATRIKA (BB)</t>
+  </si>
+  <si>
+    <t>1141 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1142 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1143 PATRIKA (G)</t>
+  </si>
+  <si>
+    <t>1144 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1145 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1146 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1147 PATRIKA (S.201)</t>
+  </si>
+  <si>
+    <t>1148 PATRIKA (S.202)</t>
+  </si>
+  <si>
+    <t>1149 PATRIKA (S.204)</t>
+  </si>
+  <si>
+    <t>1150 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1151 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1152 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1153 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1154 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1155 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1157 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1158 PATRIKA-GOLDEN</t>
+  </si>
+  <si>
+    <t>1159 PATRIKA-WHITE</t>
+  </si>
+  <si>
+    <t>1160 PATRIKA-PINK</t>
+  </si>
+  <si>
+    <t>1161 PATRIKA (01)</t>
+  </si>
+  <si>
+    <t>1162 PATRIKA (02)</t>
+  </si>
+  <si>
+    <t>1163 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1164 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1165 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1166 PATRIKA (DCU)</t>
   </si>
   <si>
     <t>190 NO. ENVELOPES (POCKET)</t>
@@ -401,106 +401,106 @@
     <t>2025- INVITAION (BOX) SAMPLES</t>
   </si>
   <si>
-    <t>2101 PATRIKA (L) (LUXYA - 51)</t>
-  </si>
-  <si>
-    <t>2102 PATRIKA *-* (M) (LUXYA - 52)</t>
-  </si>
-  <si>
-    <t>2103 PATRIKA (L) (LUXYA - 53)</t>
-  </si>
-  <si>
-    <t>2104 PATRIKA (LUXYA - 54)</t>
-  </si>
-  <si>
-    <t>2105 PATRIKA (LUXYA - 55)</t>
-  </si>
-  <si>
-    <t>2106 PATRIKA (L) (LUXYA - 56)</t>
-  </si>
-  <si>
-    <t>2107 PATRIKA *-* (M) (LUXYA - 57)</t>
-  </si>
-  <si>
-    <t>2108 PATRIKA *-* (M) (LUXYA - 59)</t>
-  </si>
-  <si>
-    <t>2109 PATRIKA (L) (LUXYA - 60)</t>
-  </si>
-  <si>
-    <t>2110 PATRIKA (LUXYA - 61)</t>
-  </si>
-  <si>
-    <t>2111 PATRIKA *-* (M) (LUXYA - 62)</t>
-  </si>
-  <si>
-    <t>2112 PATRIKA (L) (LEGACY - 01)</t>
-  </si>
-  <si>
-    <t>2113 PATRIKA (L) (LEGACY - 02)</t>
-  </si>
-  <si>
-    <t>2114 PATRIKA (L) (LEGACY - 03)</t>
-  </si>
-  <si>
-    <t>2115 PATRIKA (L) (LEGACY - 04)</t>
-  </si>
-  <si>
-    <t>2116 PATRIKA (L) (LEGACY - 05)</t>
-  </si>
-  <si>
-    <t>2117 PATRIKA *-* (M) (LEGACY - 06)</t>
-  </si>
-  <si>
-    <t>2118 PATRIKA (L) (LEGACY - 07)</t>
-  </si>
-  <si>
-    <t>2119 PATRIKA (L) (LEGACY - 08)</t>
-  </si>
-  <si>
-    <t>2120 PATRIKA (L) (LEGACY - 09)</t>
-  </si>
-  <si>
-    <t>2121 PATRIKA (LEGACY - 10)</t>
-  </si>
-  <si>
-    <t>2123 PATRIKA (LEGACY - 12)</t>
-  </si>
-  <si>
-    <t>2124 PATRIKA *-* (M) (LOTTERY - 71)</t>
-  </si>
-  <si>
-    <t>2125 PATRIKA *-* (M) (LOTTERY - 72)</t>
-  </si>
-  <si>
-    <t>2126 PATRIKA *-* (M) (LOTTERY - 73)</t>
-  </si>
-  <si>
-    <t>2127 PATRIKA *-* (M) (LOTTERY - 74)</t>
-  </si>
-  <si>
-    <t>2128 PATRIKA *-* (M) (LOTTERY - 75)</t>
-  </si>
-  <si>
-    <t>2129 PATRIKA *-* (M) (LOTTERY - 76)</t>
-  </si>
-  <si>
-    <t>2130 PATRIKA *-* (M) (LOTTERY - 77)</t>
-  </si>
-  <si>
-    <t>2131 PATRIKA *-* (M) (LOTTERY - 78)</t>
-  </si>
-  <si>
-    <t>2132 PATRIKA *-* (M) (LOTTERY - 79)</t>
-  </si>
-  <si>
-    <t>2133 PATRIKA (LOTTERY - 80)</t>
-  </si>
-  <si>
-    <t>2134 PATRIKA *-* (M) (LOTTERY - 81)</t>
-  </si>
-  <si>
-    <t>2135 PATRIKA *-* (M) (LOTTERY - 82)</t>
+    <t>2101 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2102 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2103 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2104 PATRIKA</t>
+  </si>
+  <si>
+    <t>2105 PATRIKA</t>
+  </si>
+  <si>
+    <t>2106 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2107 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2108 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2109 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2110 PATRIKA</t>
+  </si>
+  <si>
+    <t>2111 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2112 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2113 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2114 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2115 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2116 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2117 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2118 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2119 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2120 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2121 PATRIKA</t>
+  </si>
+  <si>
+    <t>2123 PATRIKA</t>
+  </si>
+  <si>
+    <t>2124 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2125 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2126 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2127 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2128 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2129 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2130 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2131 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2132 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2133 PATRIKA</t>
+  </si>
+  <si>
+    <t>2134 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2135 PATRIKA *-* (M)</t>
   </si>
   <si>
     <t>290 ENVELOPE 25-26</t>
@@ -518,1153 +518,1153 @@
     <t>330 ENVELOPE</t>
   </si>
   <si>
-    <t>4251 PATRIKA (JC) (5342)</t>
-  </si>
-  <si>
-    <t>4252 PATRIKA (5207)</t>
-  </si>
-  <si>
-    <t>4253 PATRIKA (5206)</t>
-  </si>
-  <si>
-    <t>4254 PATRIKA (4210) (10273/10277)</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA - B (DCU) (AS-02 (B))</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA (JC) (AS-02 (NEW))</t>
-  </si>
-  <si>
-    <t>4257 PATRIKA (82)</t>
-  </si>
-  <si>
-    <t>4258 PATRIKA (JC) (1129)</t>
-  </si>
-  <si>
-    <t>4259 PATRIKA (JC) (101 SBC)</t>
-  </si>
-  <si>
-    <t>4260 PATRIKA (1102)</t>
-  </si>
-  <si>
-    <t>4261 PATRIKA (JC) (959)</t>
-  </si>
-  <si>
-    <t>4262 PATRIKA (JC) (S-201 GANESH JI)</t>
-  </si>
-  <si>
-    <t>4264 PATRIKA (DCU) (1351)</t>
-  </si>
-  <si>
-    <t>4265 PATRIKA (83)</t>
-  </si>
-  <si>
-    <t>4266 PATRIKA (25-145)</t>
-  </si>
-  <si>
-    <t>4267 PATRIKA (JC) (25-046)</t>
-  </si>
-  <si>
-    <t>4268 PATRIKA (JC) *-* (M+T) (S-296)</t>
-  </si>
-  <si>
-    <t>4269 PATRIKA (111 SBC)</t>
-  </si>
-  <si>
-    <t>4270 PATRIKA (1151 GGN)</t>
-  </si>
-  <si>
-    <t>4271 PATRIKA (JC) (25216)</t>
-  </si>
-  <si>
-    <t>4272 PATRIKA (JC) (1231 SBC CRM)</t>
-  </si>
-  <si>
-    <t>4273 PATRIKA (2547)</t>
-  </si>
-  <si>
-    <t>4274 PATRIKA (JC) (25369)</t>
-  </si>
-  <si>
-    <t>4275 PATRIKA (25367)</t>
-  </si>
-  <si>
-    <t>4277 PATRIKA (JC) *-* (M) (25365)</t>
-  </si>
-  <si>
-    <t>4278 PATRIKA (25368)</t>
-  </si>
-  <si>
-    <t>4279 PATRIKA (1031)</t>
-  </si>
-  <si>
-    <t>4280 PATRIKA (25301)</t>
-  </si>
-  <si>
-    <t>4281 PATRIKA (25312 MYRA)</t>
-  </si>
-  <si>
-    <t>4282 PATRIKA (3117)</t>
-  </si>
-  <si>
-    <t>4283 PATRIKA - B (YELLOW) (3116-YLW)</t>
-  </si>
-  <si>
-    <t>4284 PATRIKA (1173 VV)</t>
-  </si>
-  <si>
-    <t>4285 PATRIKA (JC) *-* (M) (4626)</t>
-  </si>
-  <si>
-    <t>4286 PATRIKA (5254  RJN)</t>
-  </si>
-  <si>
-    <t>4287 PATRIKA (25402)</t>
-  </si>
-  <si>
-    <t>4288 PATRIKA (10001 NEW)</t>
-  </si>
-  <si>
-    <t>4289 PATRIKA (10002 NEW)</t>
-  </si>
-  <si>
-    <t>4290 PATRIKA (316 MYRA)</t>
-  </si>
-  <si>
-    <t>4291 PATRIKA (25401)</t>
-  </si>
-  <si>
-    <t>4292 PATRIKA (25311)</t>
-  </si>
-  <si>
-    <t>4293 PATRIKA (25312)</t>
-  </si>
-  <si>
-    <t>4294 PATRIKA (5273)</t>
-  </si>
-  <si>
-    <t>4295 PATRIKA (286-A)</t>
-  </si>
-  <si>
-    <t>4296 PATRIKA (1407)</t>
-  </si>
-  <si>
-    <t>4297 PATRIKA (306)</t>
-  </si>
-  <si>
-    <t>4298 PATRIKA (5501)</t>
-  </si>
-  <si>
-    <t>4299 PATRIKA (2011)</t>
-  </si>
-  <si>
-    <t>4300 PATRIKA (25314)</t>
-  </si>
-  <si>
-    <t>4301 PATRIKA (25315)</t>
-  </si>
-  <si>
-    <t>4302 PATRIKA (1402)</t>
-  </si>
-  <si>
-    <t>4303 PATRIKA (JC) (1234*-M)</t>
-  </si>
-  <si>
-    <t>4304 PATRIKA (5172)</t>
-  </si>
-  <si>
-    <t>4305 PATRIKA (25313)</t>
-  </si>
-  <si>
-    <t>4307 PATRIKA (BALAJI 5202)</t>
-  </si>
-  <si>
-    <t>4308 PATRIKA (LOTUS 430)</t>
-  </si>
-  <si>
-    <t>4309 PATRIKA (DCU) (3751 Patta)</t>
-  </si>
-  <si>
-    <t>4310 PATRIKA (DCU) (3752 Swastik)</t>
-  </si>
-  <si>
-    <t>4311 PATRIKA (DCU) (251 KBC)</t>
-  </si>
-  <si>
-    <t>4312 PATRIKA (DCU) (273-A)</t>
-  </si>
-  <si>
-    <t>4314 PATRIKA (DCU) (RED-YELLOW SWASTIK)</t>
-  </si>
-  <si>
-    <t>4315 PATRIKA (DCU) (WHITE-PINK PAN PATA)</t>
-  </si>
-  <si>
-    <t>4316 PATRIKA (DCU) (WHITE -ORANGE PAN PATTA)</t>
-  </si>
-  <si>
-    <t>5051 PATRIKA *-* (M) (5087)</t>
-  </si>
-  <si>
-    <t>5052 PATRIKA (5295)</t>
-  </si>
-  <si>
-    <t>5053 PATRIKA (5213)</t>
-  </si>
-  <si>
-    <t>5054 PATRIKA *-* (M) (25/162)</t>
-  </si>
-  <si>
-    <t>5055 PATRIKA (25/272)</t>
-  </si>
-  <si>
-    <t>5056 PATRIKA (JC) (25/271)</t>
-  </si>
-  <si>
-    <t>5057 PATRIKA (25/171)</t>
-  </si>
-  <si>
-    <t>5058 PATRIKA (8802)</t>
-  </si>
-  <si>
-    <t>5059 PATRIKA (8803)</t>
-  </si>
-  <si>
-    <t>5061 PATRIKA (DCU) (1405)</t>
-  </si>
-  <si>
-    <t>5062 PATRIKA (7705)</t>
-  </si>
-  <si>
-    <t>5063 PATRIKA (2522 GE)</t>
-  </si>
-  <si>
-    <t>5064 PATRIKA (2517 GE)</t>
-  </si>
-  <si>
-    <t>5065 PATRIKA (2527)</t>
-  </si>
-  <si>
-    <t>5066 PATRIKA (2536)</t>
-  </si>
-  <si>
-    <t>5067 PATRIKA (JC) (S-301)</t>
-  </si>
-  <si>
-    <t>5069 PATRIKA (JC) (1103)</t>
-  </si>
-  <si>
-    <t>5071 PATRIKA *-* (डोरी) (741)</t>
-  </si>
-  <si>
-    <t>5072 PATRIKA (5347 DIRECT)</t>
-  </si>
-  <si>
-    <t>5073 PATRIKA *-* (M) (3161)</t>
-  </si>
-  <si>
-    <t>5074 PATRIKA (1151 VV)</t>
-  </si>
-  <si>
-    <t>5075 PATRIKA (JC) (25-082)</t>
-  </si>
-  <si>
-    <t>5077 PATRIKA (2081)</t>
-  </si>
-  <si>
-    <t>5079 PATRIKA (296-A (NEHA)</t>
-  </si>
-  <si>
-    <t>5080 PATRIKA (2501 GE NEW)</t>
-  </si>
-  <si>
-    <t>5081 PATRIKA (2520 GE)</t>
-  </si>
-  <si>
-    <t>5083 PATRIKA (5267)</t>
-  </si>
-  <si>
-    <t>5084 PATRIKA (5258 RJ)</t>
-  </si>
-  <si>
-    <t>5085 PATRIKA (2023)</t>
-  </si>
-  <si>
-    <t>5086 PATRIKA (JC) *-* (M+D) (942)</t>
-  </si>
-  <si>
-    <t>5088 PATRIKA (25214)</t>
-  </si>
-  <si>
-    <t>5089 PATRIKA (2061 SBC)</t>
-  </si>
-  <si>
-    <t>5090 PATRIKA (5236 RJ)</t>
-  </si>
-  <si>
-    <t>5092 PATRIKA (05 NAVIN BHAI)</t>
-  </si>
-  <si>
-    <t>5093 PATRIKA (5350)</t>
-  </si>
-  <si>
-    <t>5094 PATRIKA (5251)</t>
-  </si>
-  <si>
-    <t>5095 PATRIKA (5240)</t>
-  </si>
-  <si>
-    <t>5096 PATRIKA (25316)</t>
-  </si>
-  <si>
-    <t>5097 PATRIKA (25321)</t>
-  </si>
-  <si>
-    <t>5098 PATRIKA *-* (M) (31.12) (857)</t>
-  </si>
-  <si>
-    <t>5099 PATRIKA *-* (M) (852 DHANESH)</t>
-  </si>
-  <si>
-    <t>5100 PATRIKA (DCU) (5339)</t>
-  </si>
-  <si>
-    <t>5102 PATRIKA (5021) (2456)</t>
-  </si>
-  <si>
-    <t>5103 PATRIKA (2071)</t>
-  </si>
-  <si>
-    <t>5104 PATRIKA (5261 RJND)</t>
-  </si>
-  <si>
-    <t>5105 PATRIKA (JC) (5335)</t>
-  </si>
-  <si>
-    <t>5106 PATRIKA (253-A / 257-A)</t>
-  </si>
-  <si>
-    <t>5107 PATRIKA (5356 RJ)</t>
-  </si>
-  <si>
-    <t>5108 PATRIKA (5333)</t>
-  </si>
-  <si>
-    <t>5109 PATRIKA (5308)</t>
-  </si>
-  <si>
-    <t>5110 PATRIKA (JC) (AS-402)</t>
-  </si>
-  <si>
-    <t>5111 PATRIKA (JC) (5313)</t>
-  </si>
-  <si>
-    <t>5112 PATRIKA (JC) *-* (M) (25437)</t>
-  </si>
-  <si>
-    <t>5113 PATRIKA (5305)</t>
-  </si>
-  <si>
-    <t>5114 PATRIKA *-* (डोरी) (2091)</t>
-  </si>
-  <si>
-    <t>5115 PATRIKA (DCU) (5363 RJND)</t>
-  </si>
-  <si>
-    <t>5116 PATRIKA (2031)</t>
-  </si>
-  <si>
-    <t>5117 PATRIKA (DCU) (3331)</t>
-  </si>
-  <si>
-    <t>5118 PATRIKA (DCU) (25436)</t>
-  </si>
-  <si>
-    <t>5502 PATRIKA *-* (M) (5355 NICE)</t>
-  </si>
-  <si>
-    <t>5503 PATRIKA (5186)</t>
-  </si>
-  <si>
-    <t>5504 PATRIKA (JC) (7033)</t>
-  </si>
-  <si>
-    <t>5505 PATRIKA (JC) *-* (M) (2282)</t>
-  </si>
-  <si>
-    <t>5506 PATRIKA *-* (M) (25/122)</t>
-  </si>
-  <si>
-    <t>5508 PATRIKA (JC) (612 VV)</t>
-  </si>
-  <si>
-    <t>5509 PATRIKA (JC) (25/072)</t>
-  </si>
-  <si>
-    <t>5510 PATRIKA (JC) *-* (M) (AS-950)</t>
-  </si>
-  <si>
-    <t>5511 PATRIKA (JC) *-* (M) (2528)</t>
-  </si>
-  <si>
-    <t>5512 PATRIKA (JC) (2525 /2552)</t>
-  </si>
-  <si>
-    <t>5513 PATRIKA (2515)</t>
-  </si>
-  <si>
-    <t>5514 PATRIKA (2542)</t>
-  </si>
-  <si>
-    <t>5515 PATRIKA (2523)</t>
-  </si>
-  <si>
-    <t>5516 PATRIKA (JC) *-* (M) (5302 VV)</t>
-  </si>
-  <si>
-    <t>5517 PATRIKA *-* (M) (Patti Aayegi) (6301)</t>
-  </si>
-  <si>
-    <t>5518 PATRIKA (JC) *-* (M) (922)</t>
-  </si>
-  <si>
-    <t>5519 PATRIKA *-* (M) (7066)</t>
-  </si>
-  <si>
-    <t>5520 PATRIKA (1054)</t>
-  </si>
-  <si>
-    <t>5521 PATRIKA (JC) *-* (M) (35)</t>
-  </si>
-  <si>
-    <t>5522 PATRIKA (2231)</t>
-  </si>
-  <si>
-    <t>5523 PATRIKA (2232)</t>
-  </si>
-  <si>
-    <t>5524 PATRIKA (DCU) (5382)</t>
-  </si>
-  <si>
-    <t>5525 PATRIKA *-* (M) (5283)</t>
-  </si>
-  <si>
-    <t>5526 PATRIKA (DCU) (NEW LUSTER - 01)</t>
-  </si>
-  <si>
-    <t>5528 PATRIKA *-* (M) (NEW LUSTER - 03)</t>
-  </si>
-  <si>
-    <t>5529 PATRIKA *-* (M) (NEW LUSTER - 04)</t>
-  </si>
-  <si>
-    <t>5530 PATRIKA *-* (M) (NEW LUSTER - 05)</t>
-  </si>
-  <si>
-    <t>5532 PATRIKA *-* (M) (NEW LUSTER - 07)</t>
-  </si>
-  <si>
-    <t>5533 PATRIKA *-* (M) (NEW LUSTER - 08)</t>
-  </si>
-  <si>
-    <t>5534 PATRIKA *-* (M) (NEW LUSTER - 09)</t>
-  </si>
-  <si>
-    <t>5535 PATRIKA (JC) *-* (M) (1007)</t>
-  </si>
-  <si>
-    <t>5537 PATRIKA (JC) (25-052)</t>
-  </si>
-  <si>
-    <t>5538 PATRIKA (JC) *-* (M) (7073)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA-B (2942-B)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA (JC) (2942)</t>
-  </si>
-  <si>
-    <t>5540 PATRIKA *-* (M) (S-96)</t>
-  </si>
-  <si>
-    <t>5542 PATRIKA (2261)</t>
-  </si>
-  <si>
-    <t>5543 PATRIKA (2353)</t>
-  </si>
-  <si>
-    <t>5544 PATRIKA *-* (M) (2732)</t>
-  </si>
-  <si>
-    <t>5545 PATRIKA *-* (M) (2791)</t>
-  </si>
-  <si>
-    <t>5546 PATRIKA (718)</t>
-  </si>
-  <si>
-    <t>5547 PATRIKA *-* (M) (S-32)</t>
-  </si>
-  <si>
-    <t>5548 PATRIKA (DCU) (2792)</t>
-  </si>
-  <si>
-    <t>5549 PATRIKA (5261 NICE)</t>
-  </si>
-  <si>
-    <t>5550 PATRIKA *-* (M) (5424)</t>
-  </si>
-  <si>
-    <t>5551 PATRIKA (5231)</t>
-  </si>
-  <si>
-    <t>5552 PATRIKA (JC) *-* (M) (S-163)</t>
-  </si>
-  <si>
-    <t>5553 PATRIKA *-* (M) (5004)</t>
-  </si>
-  <si>
-    <t>5554 PATRIKA *-* (F/G) (5379)</t>
-  </si>
-  <si>
-    <t>5555 PATRIKA (2903)</t>
-  </si>
-  <si>
-    <t>5556 PATRIKA *-* (M) (2952)</t>
-  </si>
-  <si>
-    <t>5557 PATRIKA (2312 SBC)</t>
-  </si>
-  <si>
-    <t>5558 PATRIKA *-* (M) (121 NEHA)</t>
-  </si>
-  <si>
-    <t>5559 PATRIKA (2293)</t>
-  </si>
-  <si>
-    <t>5560 PATRIKA (F/G) *-* (2915)</t>
-  </si>
-  <si>
-    <t>5561 PATRIKA *-* (M) (25358)</t>
-  </si>
-  <si>
-    <t>5562 PATRIKA *-* (M) (114-B (NEHA))</t>
-  </si>
-  <si>
-    <t>5563 PATRIKA (5387)</t>
-  </si>
-  <si>
-    <t>5564 PATRIKA (JC) *-* (M) (S-107)</t>
-  </si>
-  <si>
-    <t>5565 PATRIKA (175)</t>
-  </si>
-  <si>
-    <t>5566 PATRIKA *-* (M) (1742-B)</t>
-  </si>
-  <si>
-    <t>5567 PATRIKA (1679)</t>
-  </si>
-  <si>
-    <t>5568 PATRIKA *-* (M) (3002)</t>
-  </si>
-  <si>
-    <t>5569 PATRIKA *-* (M) (S-39)</t>
-  </si>
-  <si>
-    <t>5570 PATRIKA *-* (M) (S-74)</t>
-  </si>
-  <si>
-    <t>5571 PATRIKA *-* (M) (25353)</t>
-  </si>
-  <si>
-    <t>5572 PATRIKA *-* (M) (25351)</t>
-  </si>
-  <si>
-    <t>5573 PATRIKA (2205)</t>
-  </si>
-  <si>
-    <t>5574 PATRIKA (25335)</t>
-  </si>
-  <si>
-    <t>5575 PATRIKA *-* (M) (S-77)</t>
-  </si>
-  <si>
-    <t>5576 PATRIKA (2531)</t>
-  </si>
-  <si>
-    <t>5577 PATRIKA *-* (M) (5808)</t>
-  </si>
-  <si>
-    <t>5578 PATRIKA (JC) *-* (M) (AS-104 / S-50)</t>
-  </si>
-  <si>
-    <t>5579 PATRIKA (JC) *-* (M) (AS-102)</t>
-  </si>
-  <si>
-    <t>5580 PATRIKA (S-326)</t>
-  </si>
-  <si>
-    <t>5581 PATRIKA *-* (M) (3471)</t>
-  </si>
-  <si>
-    <t>5582 PATRIKA *-* (M) (3512 SBC)</t>
-  </si>
-  <si>
-    <t>5583 PATRIKA (3211 SBC)</t>
-  </si>
-  <si>
-    <t>5584 PATRIKA (JC) (2202 SBC)</t>
-  </si>
-  <si>
-    <t>5585 PATRIKA *-* (M) (1201 KBC)</t>
-  </si>
-  <si>
-    <t>5586 PATRIKA *-* (M) (S-51)</t>
-  </si>
-  <si>
-    <t>5587 PATRIKA (2264)</t>
-  </si>
-  <si>
-    <t>5588 PATRIKA (JC) *-* (M) (1006)</t>
-  </si>
-  <si>
-    <t>5589 PATRIKA *-* (M) (25133)</t>
-  </si>
-  <si>
-    <t>5590 PATRIKA (3131 SBC)</t>
-  </si>
-  <si>
-    <t>5592 PATRIKA *-* (M) (2365)</t>
-  </si>
-  <si>
-    <t>5593 PATRIKA (2803)</t>
-  </si>
-  <si>
-    <t>5595 PATRIKA *-* (M) (226)</t>
-  </si>
-  <si>
-    <t>5596 PATRIKA *-* (M) (2541)</t>
-  </si>
-  <si>
-    <t>5597 PATRIKA (JC) *-* (M) (AS-104 (B))</t>
-  </si>
-  <si>
-    <t>5599 PATRIKA *-* (M) (77-B)</t>
-  </si>
-  <si>
-    <t>5601 PATRIKA (2771)</t>
-  </si>
-  <si>
-    <t>5602 PATRIKA (3271)</t>
-  </si>
-  <si>
-    <t>5603 PATRIKA *-* (M) (6125)</t>
-  </si>
-  <si>
-    <t>5604 PATRIKA (242-A)</t>
-  </si>
-  <si>
-    <t>5605 PATRIKA (JC) (3102)</t>
-  </si>
-  <si>
-    <t>5606 PATRIKA *-* (M) (221-A)</t>
-  </si>
-  <si>
-    <t>5607 PATRIKA (25442)</t>
-  </si>
-  <si>
-    <t>5608 PATRIKA (25440)</t>
-  </si>
-  <si>
-    <t>5609 PATRIKA (993)</t>
-  </si>
-  <si>
-    <t>5610 PATRIKA (JC) (2373)</t>
-  </si>
-  <si>
-    <t>5611 PATRIKA *-* (M) (1211)</t>
-  </si>
-  <si>
-    <t>5612 PATRIKA (DCU) (5276)</t>
-  </si>
-  <si>
-    <t>5614 PATRIKA *-* (M) (2331)</t>
-  </si>
-  <si>
-    <t>5615 PATRIKA (2111)</t>
-  </si>
-  <si>
-    <t>5616 PATRIKA (DCU) (7069)</t>
-  </si>
-  <si>
-    <t>5617 PATRIKA *-* (M) (7067)</t>
-  </si>
-  <si>
-    <t>5618 PATRIKA (JC) *-* (M) (S-52)</t>
-  </si>
-  <si>
-    <t>5621 PATRIKA (JC) *-* (M) (5297)</t>
-  </si>
-  <si>
-    <t>5622 PATRIKA *-* (M) (25337)</t>
-  </si>
-  <si>
-    <t>5623 PATRIKA (064)</t>
-  </si>
-  <si>
-    <t>5625 PATRIKA (DCU) (772)</t>
-  </si>
-  <si>
-    <t>5626 PATRIKA (DCU) (FULL JALI)</t>
-  </si>
-  <si>
-    <t>5627 PATRIKA (DCU) (HALF JALI)</t>
-  </si>
-  <si>
-    <t>5628 PATRIKA (DCU) (GOL)</t>
-  </si>
-  <si>
-    <t>5629 PATRIKA (DCU) (9*5 X 6*5 PATTA)</t>
-  </si>
-  <si>
-    <t>5630 PATRIKA (DCU) (SATHIYA)</t>
-  </si>
-  <si>
-    <t>6601 PATRIKA (L) (5164)</t>
-  </si>
-  <si>
-    <t>6602 PATRIKA (5126)</t>
-  </si>
-  <si>
-    <t>6603 PATRIKA (5111)</t>
-  </si>
-  <si>
-    <t>6604 PATRIKA *-* (M) (5196)</t>
-  </si>
-  <si>
-    <t>6605 PATRIKA (5191)</t>
-  </si>
-  <si>
-    <t>6606 PATRIKA (*-*) R (3023)</t>
-  </si>
-  <si>
-    <t>6607 PATRIKA *-* (M) (0523)</t>
-  </si>
-  <si>
-    <t>6608 PATRIKA (95)</t>
-  </si>
-  <si>
-    <t>6609 PATRIKA *-* (M) (3053)</t>
-  </si>
-  <si>
-    <t>6610 PATRIKA *-* (M) (3019)</t>
-  </si>
-  <si>
-    <t>6611 PATRIKA (3017 VV)</t>
-  </si>
-  <si>
-    <t>6612 PATRIKA (3015)</t>
-  </si>
-  <si>
-    <t>6613 PATRIKA (25164)</t>
-  </si>
-  <si>
-    <t>6614 PATRIKA (DCU) (25131)</t>
-  </si>
-  <si>
-    <t>6615 PATRIKA *-* (M) (915 GAGAN)</t>
-  </si>
-  <si>
-    <t>6616 PATRIKA *-* (M) (911 GAGAN)</t>
-  </si>
-  <si>
-    <t>6617 PATRIKA *-* (M) (3422)</t>
-  </si>
-  <si>
-    <t>6618 PATRIKA *-* (M) (3423)</t>
-  </si>
-  <si>
-    <t>6619 PATRIKA *-* (M) (1193)</t>
-  </si>
-  <si>
-    <t>6620 PATRIKA *-* (M) (1045 GGN (PADDING))</t>
-  </si>
-  <si>
-    <t>6621 PATRIKA *-* (M) (7108 (PADDING))</t>
-  </si>
-  <si>
-    <t>6622 PATRIKA *-* (M) (7259 (PADDING))</t>
-  </si>
-  <si>
-    <t>6623 PATRIKA (25184)</t>
-  </si>
-  <si>
-    <t>6624 PATRIKA *-* (M) (25135)</t>
-  </si>
-  <si>
-    <t>6625 PATRIKA *-* (M) (25116)</t>
-  </si>
-  <si>
-    <t>6626 PATRIKA *-* (M) (25161)</t>
-  </si>
-  <si>
-    <t>6627 PATRIKA *-* (M) (25111)</t>
-  </si>
-  <si>
-    <t>6628 PATRIKA *-* (M) (805 SBC)</t>
-  </si>
-  <si>
-    <t>6629 PATRIKA *-* (M) (812 NEW SBC)</t>
-  </si>
-  <si>
-    <t>6630 PATRIKA *-* (M) (5510 NICE)</t>
-  </si>
-  <si>
-    <t>6631 PATRIKA (DCU) (OLD AP ITEM)</t>
-  </si>
-  <si>
-    <t>6632 PATRIKA (DCU) (932)</t>
-  </si>
-  <si>
-    <t>6633 PATRIKA *-* (M) (7081 VP)</t>
-  </si>
-  <si>
-    <t>6634 PATRIKA (3562)</t>
-  </si>
-  <si>
-    <t>6635 PATRIKA *-* (M) (S-313)</t>
-  </si>
-  <si>
-    <t>6636 PATRIKA *-* (M) (25183)</t>
-  </si>
-  <si>
-    <t>6637 PATRIKA (25162 GE)</t>
-  </si>
-  <si>
-    <t>6638 PATRIKA *-* (M) (3014)</t>
-  </si>
-  <si>
-    <t>6639 PATRIKA (B) (2291-B)</t>
-  </si>
-  <si>
-    <t>6640 PATRIKA *-* (M) (5737 PADING)</t>
-  </si>
-  <si>
-    <t>6641 PATRIKA *-* (M) (5435)</t>
-  </si>
-  <si>
-    <t>6642 PATRIKA *-* (M) (5411 RJ)</t>
-  </si>
-  <si>
-    <t>6643 PATRIKA *-* (M) (25380)</t>
-  </si>
-  <si>
-    <t>6644 PATRIKA (DCU) (25132)</t>
-  </si>
-  <si>
-    <t>6645 PATRIKA *-* (M) (3031)</t>
-  </si>
-  <si>
-    <t>6646 PATRIKA *-* (M) (3034)</t>
-  </si>
-  <si>
-    <t>6647 PATRIKA *-* (M) (25382)</t>
-  </si>
-  <si>
-    <t>6648 PATRIKA *-* (M) (5011 (PADDING))</t>
-  </si>
-  <si>
-    <t>6649 PATRIKA *-* (M) (3402)</t>
-  </si>
-  <si>
-    <t>6650 PATRIKA *-* (M) (3431)</t>
-  </si>
-  <si>
-    <t>6651 PATRIKA (3421)</t>
-  </si>
-  <si>
-    <t>6652 PATRIKA *-* (M) (2764 SBC)</t>
-  </si>
-  <si>
-    <t>6653 PATRIKA *-* (M) (834 SBC NEW)</t>
-  </si>
-  <si>
-    <t>6654 PATRIKA *-* (M) (3461)</t>
-  </si>
-  <si>
-    <t>6655 PATRIKA *-* (M) (7129 (PADDING))</t>
-  </si>
-  <si>
-    <t>6656 PATRIKA (L) (7113 (PADDING))</t>
-  </si>
-  <si>
-    <t>6657 PATRIKA *-* (M) (563  DHANESH)</t>
-  </si>
-  <si>
-    <t>6658 PATRIKA *-* (M) (5319)</t>
-  </si>
-  <si>
-    <t>6659 PATRIKA (25193 (Padding))</t>
-  </si>
-  <si>
-    <t>6660 PATRIKA (25194 (Padding))</t>
-  </si>
-  <si>
-    <t>6661 PATRIKA *-* (M) (1281)</t>
-  </si>
-  <si>
-    <t>6662 PATRIKA (3424)</t>
-  </si>
-  <si>
-    <t>6663 PATRIKA (7103 (PADDING))</t>
-  </si>
-  <si>
-    <t>6664 PATRIKA *-* (M) (5823)</t>
-  </si>
-  <si>
-    <t>6665 PATRIKA *-* (M) (603 DHANESH)</t>
-  </si>
-  <si>
-    <t>6667 PATRIKA *-* (M) (1192 SBC)</t>
-  </si>
-  <si>
-    <t>6668 PATRIKA (DCU) (8102)</t>
-  </si>
-  <si>
-    <t>6669 PATRIKA (DCU) (6197)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA - B (M) (1868-B)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA *-* (M) (1868)</t>
-  </si>
-  <si>
-    <t>6671 PATRIKA *-* (M) (1872)</t>
-  </si>
-  <si>
-    <t>6672 PATRIKA *-* (M) (6132)</t>
-  </si>
-  <si>
-    <t>6673 PATRIKA (DCU) (6196)</t>
-  </si>
-  <si>
-    <t>6674 PATRIKA (DCU) (1503)</t>
-  </si>
-  <si>
-    <t>6675 PATRIKA *-* (M) (1282)</t>
-  </si>
-  <si>
-    <t>6676 PATRIKA (DCU) (533 KBC)</t>
-  </si>
-  <si>
-    <t>6677 PATRIKA (DCU) (25191 PADDING)</t>
-  </si>
-  <si>
-    <t>7265 PATRIKA (O.C.) (133)</t>
-  </si>
-  <si>
-    <t>7283 PATRIKA {F} (O.C.) (4148)</t>
-  </si>
-  <si>
-    <t>7287 PATRIKA (O.C.) (1522)</t>
-  </si>
-  <si>
-    <t>7288 PATRIKA (O.C.) (1178)</t>
-  </si>
-  <si>
-    <t>7293 PATRIKA (O.C.) (AS-20)</t>
-  </si>
-  <si>
-    <t>7309 PATRIKA (O.C.) (4087)</t>
-  </si>
-  <si>
-    <t>7312 PATRIKA (O.C.) (SBC 7312)</t>
-  </si>
-  <si>
-    <t>7319 PATRIKA (O.C.) (2204)</t>
-  </si>
-  <si>
-    <t>7332 PATRIKA (O.C.) (2482)</t>
-  </si>
-  <si>
-    <t>7342 PATRIKA (O.C.) (12)</t>
-  </si>
-  <si>
-    <t>7344 PATRIKA (O.C.) (INV B.P. RED (11))</t>
-  </si>
-  <si>
-    <t>7345 PATRIKA (O.C.) (INV B.P. GOLDEN (120) 5)</t>
-  </si>
-  <si>
-    <t>7401 PATRIKA (25/252)</t>
-  </si>
-  <si>
-    <t>7402 PATRIKA (25/264-263)</t>
-  </si>
-  <si>
-    <t>7403 PATRIKA (25/363/863)</t>
-  </si>
-  <si>
-    <t>7404 PATRIKA (25/283)</t>
-  </si>
-  <si>
-    <t>7405 PATRIKA (25/273)</t>
-  </si>
-  <si>
-    <t>7406 PATRIKA (25/172)</t>
-  </si>
-  <si>
-    <t>7407 PATRIKA *-* (F) (7145 VP)</t>
-  </si>
-  <si>
-    <t>7408 PATRIKA (DCU) (25895)</t>
-  </si>
-  <si>
-    <t>7409 PATRIKA (2521)</t>
-  </si>
-  <si>
-    <t>7410 PATRIKA (2526)</t>
-  </si>
-  <si>
-    <t>7411 PATRIKA (2535)</t>
-  </si>
-  <si>
-    <t>7412 PATRIKA (84)</t>
-  </si>
-  <si>
-    <t>7413 PATRIKA (2543 INV OFFSET)</t>
-  </si>
-  <si>
-    <t>7414 PATRIKA (1015 GREEN OFFSET)</t>
-  </si>
-  <si>
-    <t>7415 PATRIKA *-* (F) (3162 SBC)</t>
-  </si>
-  <si>
-    <t>7416 PATRIKA (2234)</t>
-  </si>
-  <si>
-    <t>7417 PATRIKA (S-201 INV)</t>
-  </si>
-  <si>
-    <t>7418 PATRIKA *-* (डोरी) (1639)</t>
-  </si>
-  <si>
-    <t>7419 PATRIKA (5121)</t>
-  </si>
-  <si>
-    <t>7420 PATRIKA (720)</t>
-  </si>
-  <si>
-    <t>7421 PATRIKA *-* (F) (25-146)</t>
-  </si>
-  <si>
-    <t>7422 PATRIKA (3702)</t>
-  </si>
-  <si>
-    <t>7423 PATRIKA (254 SBC)</t>
-  </si>
-  <si>
-    <t>7424 PATRIKA *-* (F) (25-047)</t>
-  </si>
-  <si>
-    <t>7425 PATRIKA (2082)</t>
-  </si>
-  <si>
-    <t>7426 PATRIKA (F/G) *-* (4052)</t>
-  </si>
-  <si>
-    <t>7427 PATRIKA (2103)</t>
-  </si>
-  <si>
-    <t>7428 PATRIKA (1223 SBC)</t>
-  </si>
-  <si>
-    <t>7429 PATRIKA (F/G) *-* (1851 MONARCH)</t>
-  </si>
-  <si>
-    <t>7430 PATRIKA (6310 GE)</t>
-  </si>
-  <si>
-    <t>7431 PATRIKA (2532)</t>
-  </si>
-  <si>
-    <t>7432 PATRIKA (1174)</t>
-  </si>
-  <si>
-    <t>7433 PATRIKA (1034)</t>
-  </si>
-  <si>
-    <t>7434 PATRIKA (2204 INV)</t>
-  </si>
-  <si>
-    <t>7435 PATRIKA (06)</t>
-  </si>
-  <si>
-    <t>7436 PATRIKA (303)</t>
-  </si>
-  <si>
-    <t>7437 PATRIKA (25323 INV)</t>
-  </si>
-  <si>
-    <t>7438 PATRIKA (25413)</t>
-  </si>
-  <si>
-    <t>7439 PATRIKA (2597)</t>
-  </si>
-  <si>
-    <t>7440 PATRIKA (25896)</t>
-  </si>
-  <si>
-    <t>7441 PATRIKA *-* (F) (243-C)</t>
-  </si>
-  <si>
-    <t>7442 PATRIKA (1855)</t>
-  </si>
-  <si>
-    <t>7443 PATRIKA (1044 SBC)</t>
-  </si>
-  <si>
-    <t>7444 PATRIKA (2014)</t>
-  </si>
-  <si>
-    <t>7445 PATRIKA (2006)</t>
-  </si>
-  <si>
-    <t>7446 PATRIKA (DCU) (6106)</t>
-  </si>
-  <si>
-    <t>7447 PATRIKA (GOPAL 32)</t>
-  </si>
-  <si>
-    <t>7448 PATRIKA (2005- G)</t>
-  </si>
-  <si>
-    <t>7449 PATRIKA (5180)</t>
-  </si>
-  <si>
-    <t>7450 PATRIKA (DCU) (3753)</t>
-  </si>
-  <si>
-    <t>7451 PATRIKA (273 NEHA)</t>
-  </si>
-  <si>
-    <t>7452 PATRIKA (278-B)</t>
-  </si>
-  <si>
-    <t>7453 PATRIKA (ECO - 61) (NEW ECO 61)</t>
-  </si>
-  <si>
-    <t>7454 PATRIKA (ECO -63) (NEW ECO 63)</t>
+    <t>4251 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4252 PATRIKA</t>
+  </si>
+  <si>
+    <t>4253 PATRIKA</t>
+  </si>
+  <si>
+    <t>4254 PATRIKA (4210)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4257 PATRIKA</t>
+  </si>
+  <si>
+    <t>4258 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4259 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4260 PATRIKA</t>
+  </si>
+  <si>
+    <t>4261 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4262 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4264 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4265 PATRIKA</t>
+  </si>
+  <si>
+    <t>4266 PATRIKA</t>
+  </si>
+  <si>
+    <t>4267 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4268 PATRIKA (JC) *-* (M+T)</t>
+  </si>
+  <si>
+    <t>4269 PATRIKA</t>
+  </si>
+  <si>
+    <t>4270 PATRIKA</t>
+  </si>
+  <si>
+    <t>4271 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4272 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4273 PATRIKA</t>
+  </si>
+  <si>
+    <t>4274 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4275 PATRIKA</t>
+  </si>
+  <si>
+    <t>4277 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4278 PATRIKA</t>
+  </si>
+  <si>
+    <t>4279 PATRIKA</t>
+  </si>
+  <si>
+    <t>4280 PATRIKA</t>
+  </si>
+  <si>
+    <t>4281 PATRIKA</t>
+  </si>
+  <si>
+    <t>4282 PATRIKA</t>
+  </si>
+  <si>
+    <t>4283 PATRIKA - B (YELLOW)</t>
+  </si>
+  <si>
+    <t>4284 PATRIKA</t>
+  </si>
+  <si>
+    <t>4285 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4286 PATRIKA</t>
+  </si>
+  <si>
+    <t>4287 PATRIKA</t>
+  </si>
+  <si>
+    <t>4288 PATRIKA</t>
+  </si>
+  <si>
+    <t>4289 PATRIKA</t>
+  </si>
+  <si>
+    <t>4290 PATRIKA</t>
+  </si>
+  <si>
+    <t>4291 PATRIKA</t>
+  </si>
+  <si>
+    <t>4292 PATRIKA</t>
+  </si>
+  <si>
+    <t>4293 PATRIKA</t>
+  </si>
+  <si>
+    <t>4294 PATRIKA</t>
+  </si>
+  <si>
+    <t>4295 PATRIKA</t>
+  </si>
+  <si>
+    <t>4296 PATRIKA</t>
+  </si>
+  <si>
+    <t>4297 PATRIKA</t>
+  </si>
+  <si>
+    <t>4298 PATRIKA</t>
+  </si>
+  <si>
+    <t>4299 PATRIKA</t>
+  </si>
+  <si>
+    <t>4300 PATRIKA</t>
+  </si>
+  <si>
+    <t>4301 PATRIKA</t>
+  </si>
+  <si>
+    <t>4302 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4303 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4304 PATRIKA</t>
+  </si>
+  <si>
+    <t>4305 PATRIKA</t>
+  </si>
+  <si>
+    <t>4307 PATRIKA</t>
+  </si>
+  <si>
+    <t>4308 PATRIKA</t>
+  </si>
+  <si>
+    <t>4309 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4310 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4311 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4312 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4314 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4315 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4316 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5051 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5052 PATRIKA</t>
+  </si>
+  <si>
+    <t>5053 PATRIKA</t>
+  </si>
+  <si>
+    <t>5054 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5055 PATRIKA</t>
+  </si>
+  <si>
+    <t>5056 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5057 PATRIKA</t>
+  </si>
+  <si>
+    <t>5058 PATRIKA</t>
+  </si>
+  <si>
+    <t>5059 PATRIKA</t>
+  </si>
+  <si>
+    <t>5061 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5062 PATRIKA</t>
+  </si>
+  <si>
+    <t>5063 PATRIKA</t>
+  </si>
+  <si>
+    <t>5064 PATRIKA</t>
+  </si>
+  <si>
+    <t>5065 PATRIKA</t>
+  </si>
+  <si>
+    <t>5066 PATRIKA</t>
+  </si>
+  <si>
+    <t>5067 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5069 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5071 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5072 PATRIKA</t>
+  </si>
+  <si>
+    <t>5073 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5074 PATRIKA</t>
+  </si>
+  <si>
+    <t>5075 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5077 PATRIKA</t>
+  </si>
+  <si>
+    <t>5079 PATRIKA</t>
+  </si>
+  <si>
+    <t>5080 PATRIKA</t>
+  </si>
+  <si>
+    <t>5081 PATRIKA</t>
+  </si>
+  <si>
+    <t>5083 PATRIKA</t>
+  </si>
+  <si>
+    <t>5084 PATRIKA</t>
+  </si>
+  <si>
+    <t>5085 PATRIKA</t>
+  </si>
+  <si>
+    <t>5086 PATRIKA (JC) *-* (M+D)</t>
+  </si>
+  <si>
+    <t>5088 PATRIKA</t>
+  </si>
+  <si>
+    <t>5089 PATRIKA</t>
+  </si>
+  <si>
+    <t>5090 PATRIKA</t>
+  </si>
+  <si>
+    <t>5092 PATRIKA</t>
+  </si>
+  <si>
+    <t>5093 PATRIKA</t>
+  </si>
+  <si>
+    <t>5094 PATRIKA</t>
+  </si>
+  <si>
+    <t>5095 PATRIKA</t>
+  </si>
+  <si>
+    <t>5096 PATRIKA</t>
+  </si>
+  <si>
+    <t>5097 PATRIKA</t>
+  </si>
+  <si>
+    <t>5098 PATRIKA *-* (M) (31.12)</t>
+  </si>
+  <si>
+    <t>5099 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5100 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5102 PATRIKA (5021)</t>
+  </si>
+  <si>
+    <t>5103 PATRIKA</t>
+  </si>
+  <si>
+    <t>5104 PATRIKA</t>
+  </si>
+  <si>
+    <t>5105 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5106 PATRIKA</t>
+  </si>
+  <si>
+    <t>5107 PATRIKA</t>
+  </si>
+  <si>
+    <t>5108 PATRIKA</t>
+  </si>
+  <si>
+    <t>5109 PATRIKA</t>
+  </si>
+  <si>
+    <t>5110 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5111 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5112 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5113 PATRIKA</t>
+  </si>
+  <si>
+    <t>5114 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5115 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5116 PATRIKA</t>
+  </si>
+  <si>
+    <t>5117 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5118 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5502 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5503 PATRIKA</t>
+  </si>
+  <si>
+    <t>5504 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5505 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5506 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5508 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5509 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5510 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5511 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5512 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5513 PATRIKA</t>
+  </si>
+  <si>
+    <t>5514 PATRIKA</t>
+  </si>
+  <si>
+    <t>5515 PATRIKA</t>
+  </si>
+  <si>
+    <t>5516 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5517 PATRIKA *-* (M) (Patti Aayegi)</t>
+  </si>
+  <si>
+    <t>5518 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5519 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5520 PATRIKA</t>
+  </si>
+  <si>
+    <t>5521 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5522 PATRIKA</t>
+  </si>
+  <si>
+    <t>5523 PATRIKA</t>
+  </si>
+  <si>
+    <t>5524 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5525 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5526 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5528 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5529 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5530 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5532 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5533 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5534 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5535 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5537 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5538 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA-B</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5540 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5542 PATRIKA</t>
+  </si>
+  <si>
+    <t>5543 PATRIKA</t>
+  </si>
+  <si>
+    <t>5544 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5545 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5546 PATRIKA</t>
+  </si>
+  <si>
+    <t>5547 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5548 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5549 PATRIKA</t>
+  </si>
+  <si>
+    <t>5550 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5551 PATRIKA</t>
+  </si>
+  <si>
+    <t>5552 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5553 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5554 PATRIKA *-* (F/G)</t>
+  </si>
+  <si>
+    <t>5555 PATRIKA</t>
+  </si>
+  <si>
+    <t>5556 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5557 PATRIKA</t>
+  </si>
+  <si>
+    <t>5558 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5559 PATRIKA</t>
+  </si>
+  <si>
+    <t>5560 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>5561 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5562 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5563 PATRIKA</t>
+  </si>
+  <si>
+    <t>5564 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5565 PATRIKA</t>
+  </si>
+  <si>
+    <t>5566 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5567 PATRIKA</t>
+  </si>
+  <si>
+    <t>5568 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5569 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5570 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5571 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5572 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5573 PATRIKA</t>
+  </si>
+  <si>
+    <t>5574 PATRIKA</t>
+  </si>
+  <si>
+    <t>5575 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5576 PATRIKA</t>
+  </si>
+  <si>
+    <t>5577 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5578 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5579 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5580 PATRIKA</t>
+  </si>
+  <si>
+    <t>5581 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5582 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5583 PATRIKA</t>
+  </si>
+  <si>
+    <t>5584 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5585 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5586 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5587 PATRIKA</t>
+  </si>
+  <si>
+    <t>5588 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5589 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5590 PATRIKA</t>
+  </si>
+  <si>
+    <t>5592 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5593 PATRIKA</t>
+  </si>
+  <si>
+    <t>5595 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5596 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5597 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5599 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5601 PATRIKA</t>
+  </si>
+  <si>
+    <t>5602 PATRIKA</t>
+  </si>
+  <si>
+    <t>5603 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5604 PATRIKA</t>
+  </si>
+  <si>
+    <t>5605 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5606 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5607 PATRIKA</t>
+  </si>
+  <si>
+    <t>5608 PATRIKA</t>
+  </si>
+  <si>
+    <t>5609 PATRIKA</t>
+  </si>
+  <si>
+    <t>5610 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5611 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5612 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5614 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5615 PATRIKA</t>
+  </si>
+  <si>
+    <t>5616 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5618 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5621 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5623 PATRIKA</t>
+  </si>
+  <si>
+    <t>5625 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5626 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5627 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5628 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5629 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5630 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6601 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6602 PATRIKA</t>
+  </si>
+  <si>
+    <t>6603 PATRIKA</t>
+  </si>
+  <si>
+    <t>6604 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6605 PATRIKA</t>
+  </si>
+  <si>
+    <t>6606 PATRIKA (*-*) R</t>
+  </si>
+  <si>
+    <t>6607 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6608 PATRIKA</t>
+  </si>
+  <si>
+    <t>6609 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6610 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6611 PATRIKA</t>
+  </si>
+  <si>
+    <t>6612 PATRIKA</t>
+  </si>
+  <si>
+    <t>6613 PATRIKA</t>
+  </si>
+  <si>
+    <t>6614 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6615 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6616 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6618 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6619 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6620 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6621 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6623 PATRIKA</t>
+  </si>
+  <si>
+    <t>6624 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6625 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6626 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6627 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6628 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6629 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6630 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6631 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6632 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6633 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6634 PATRIKA</t>
+  </si>
+  <si>
+    <t>6635 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6636 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6637 PATRIKA</t>
+  </si>
+  <si>
+    <t>6638 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6639 PATRIKA (B)</t>
+  </si>
+  <si>
+    <t>6640 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6641 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6642 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6643 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6644 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6645 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6646 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6647 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6648 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6649 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6650 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6651 PATRIKA</t>
+  </si>
+  <si>
+    <t>6652 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6653 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6654 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6655 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6656 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6657 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6658 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6659 PATRIKA</t>
+  </si>
+  <si>
+    <t>6660 PATRIKA</t>
+  </si>
+  <si>
+    <t>6661 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6662 PATRIKA</t>
+  </si>
+  <si>
+    <t>6663 PATRIKA</t>
+  </si>
+  <si>
+    <t>6664 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6665 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6667 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6668 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6669 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA - B (M)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6671 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6672 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6673 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6674 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6675 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6676 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6677 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7265 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7283 PATRIKA {F} (O.C.)</t>
+  </si>
+  <si>
+    <t>7287 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7288 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7293 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7309 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7312 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7319 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7332 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7342 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7344 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7345 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7401 PATRIKA</t>
+  </si>
+  <si>
+    <t>7402 PATRIKA</t>
+  </si>
+  <si>
+    <t>7403 PATRIKA</t>
+  </si>
+  <si>
+    <t>7404 PATRIKA</t>
+  </si>
+  <si>
+    <t>7405 PATRIKA</t>
+  </si>
+  <si>
+    <t>7406 PATRIKA</t>
+  </si>
+  <si>
+    <t>7407 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7408 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7409 PATRIKA</t>
+  </si>
+  <si>
+    <t>7410 PATRIKA</t>
+  </si>
+  <si>
+    <t>7411 PATRIKA</t>
+  </si>
+  <si>
+    <t>7412 PATRIKA</t>
+  </si>
+  <si>
+    <t>7413 PATRIKA</t>
+  </si>
+  <si>
+    <t>7414 PATRIKA</t>
+  </si>
+  <si>
+    <t>7415 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7416 PATRIKA</t>
+  </si>
+  <si>
+    <t>7417 PATRIKA</t>
+  </si>
+  <si>
+    <t>7418 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>7419 PATRIKA</t>
+  </si>
+  <si>
+    <t>7420 PATRIKA</t>
+  </si>
+  <si>
+    <t>7421 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7422 PATRIKA</t>
+  </si>
+  <si>
+    <t>7423 PATRIKA</t>
+  </si>
+  <si>
+    <t>7424 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7425 PATRIKA</t>
+  </si>
+  <si>
+    <t>7426 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7427 PATRIKA</t>
+  </si>
+  <si>
+    <t>7428 PATRIKA</t>
+  </si>
+  <si>
+    <t>7429 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7430 PATRIKA</t>
+  </si>
+  <si>
+    <t>7431 PATRIKA</t>
+  </si>
+  <si>
+    <t>7432 PATRIKA</t>
+  </si>
+  <si>
+    <t>7433 PATRIKA</t>
+  </si>
+  <si>
+    <t>7434 PATRIKA</t>
+  </si>
+  <si>
+    <t>7435 PATRIKA</t>
+  </si>
+  <si>
+    <t>7436 PATRIKA</t>
+  </si>
+  <si>
+    <t>7437 PATRIKA</t>
+  </si>
+  <si>
+    <t>7438 PATRIKA</t>
+  </si>
+  <si>
+    <t>7439 PATRIKA</t>
+  </si>
+  <si>
+    <t>7440 PATRIKA</t>
+  </si>
+  <si>
+    <t>7441 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7442 PATRIKA</t>
+  </si>
+  <si>
+    <t>7443 PATRIKA</t>
+  </si>
+  <si>
+    <t>7444 PATRIKA</t>
+  </si>
+  <si>
+    <t>7445 PATRIKA</t>
+  </si>
+  <si>
+    <t>7446 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7447 PATRIKA</t>
+  </si>
+  <si>
+    <t>7448 PATRIKA</t>
+  </si>
+  <si>
+    <t>7449 PATRIKA</t>
+  </si>
+  <si>
+    <t>7450 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7451 PATRIKA</t>
+  </si>
+  <si>
+    <t>7452 PATRIKA</t>
+  </si>
+  <si>
+    <t>7453 PATRIKA (ECO - 61)</t>
+  </si>
+  <si>
+    <t>7454 PATRIKA (ECO -63)</t>
   </si>
   <si>
     <t>7604 PATRIKA</t>
   </si>
   <si>
-    <t>9001 CARD (O.C.) (2498 Cream)</t>
+    <t>9001 CARD (O.C.)</t>
   </si>
   <si>
     <t>9221 CARDS - YELLOW</t>
@@ -1688,262 +1688,262 @@
     <t>9227 CARDS (9*5 OFFSET)</t>
   </si>
   <si>
-    <t>9228 CARDS (Y) (ORANGE WITH ONLY FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS - B (DCU) (GOLDEN WITH GANESH JI &amp; FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS (C) (CREAM WITH GANESH JI &amp; FOIL)</t>
+    <t>9228 CARDS (Y)</t>
+  </si>
+  <si>
+    <t>9229 CARDS - B (DCU)</t>
+  </si>
+  <si>
+    <t>9229 CARDS (C)</t>
   </si>
   <si>
     <t>9230 (CARD) 9*5 SCREEN</t>
   </si>
   <si>
-    <t>9232 CARDS (DCU) (RIYAZ 9*5 CREAM)</t>
-  </si>
-  <si>
-    <t>9233 CARDS (DCU) (RIYAZ 9*5 YELLOW)</t>
-  </si>
-  <si>
-    <t>9235 CARDS (DCU) (RIYAZ 9*4 CREAM)</t>
-  </si>
-  <si>
-    <t>9236 CARDS (DCU) (RIYAZ 9*4 YELLOW)</t>
-  </si>
-  <si>
-    <t>9237 CARDS (DCU) (DCU 9*4 RED)</t>
-  </si>
-  <si>
-    <t>9301 CARDS (4242)</t>
-  </si>
-  <si>
-    <t>9302 CARDS (5076)</t>
-  </si>
-  <si>
-    <t>9303 CARDS (5080 Pink)</t>
-  </si>
-  <si>
-    <t>9304 CARDS (5083 Blue)</t>
-  </si>
-  <si>
-    <t>9305 CARDS (9070) (4701 Nice)</t>
-  </si>
-  <si>
-    <t>9306 CARDS (0543 Nice)</t>
-  </si>
-  <si>
-    <t>9307 CARDS *-* (M) (5243 Nice)</t>
-  </si>
-  <si>
-    <t>9308 CARDS (9852)</t>
-  </si>
-  <si>
-    <t>9309 CARDS *-* (T) (9561 Vp)</t>
-  </si>
-  <si>
-    <t>9310 CARDS (3103)</t>
-  </si>
-  <si>
-    <t>9311 CARDS (3115)</t>
-  </si>
-  <si>
-    <t>9312 CARDS *-* (T) (208 VV)</t>
-  </si>
-  <si>
-    <t>9313 CARDS *-* (T) (216)</t>
-  </si>
-  <si>
-    <t>9314 CARDS (P-1)</t>
-  </si>
-  <si>
-    <t>9315 CARDS (DCU) (P-2)</t>
-  </si>
-  <si>
-    <t>9316 CARDS (DCU) (P-3)</t>
-  </si>
-  <si>
-    <t>9317 CARDS (P-4)</t>
-  </si>
-  <si>
-    <t>9318 CARDS (25905)</t>
-  </si>
-  <si>
-    <t>9320 CARDS (S-20)</t>
-  </si>
-  <si>
-    <t>9321 CARDS (22912 GANESH JI)</t>
-  </si>
-  <si>
-    <t>9322 CARDS *-* (M) (22912 COMMON)</t>
-  </si>
-  <si>
-    <t>9323 CARDS (9005 OLD) (9*5 CREAM FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9324 CARDS (9*5 PINK FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9325 CARDS (5229)</t>
-  </si>
-  <si>
-    <t>9326 CARDS (1601)</t>
-  </si>
-  <si>
-    <t>9327 CARDS (25908)</t>
-  </si>
-  <si>
-    <t>9328 CARDS (2543)</t>
-  </si>
-  <si>
-    <t>9329 CARDS (Desgin H/d) (3606)</t>
-  </si>
-  <si>
-    <t>9330 CARDS *-* (T) (9557)</t>
-  </si>
-  <si>
-    <t>9331 CARDS *-*  (T) (9560)</t>
-  </si>
-  <si>
-    <t>9332 CARDS (9847)</t>
-  </si>
-  <si>
-    <t>9333 CARDS (6042)</t>
-  </si>
-  <si>
-    <t>9334 CARDS (10X6 WHITE (2898))</t>
-  </si>
-  <si>
-    <t>9335 CARDS (9003 OLD) (9*5 WHITE)</t>
-  </si>
-  <si>
-    <t>9336 CARDS (2884)</t>
-  </si>
-  <si>
-    <t>9337 CARDS (1635 AP)</t>
-  </si>
-  <si>
-    <t>9338 CARDS (1637 AP)</t>
-  </si>
-  <si>
-    <t>9339 CARDS (5361)</t>
-  </si>
-  <si>
-    <t>9340 CARDS (5658)</t>
-  </si>
-  <si>
-    <t>9341 CARDS (5497)</t>
-  </si>
-  <si>
-    <t>9342 CARDS (2861)</t>
-  </si>
-  <si>
-    <t>9343 CARDS (9*5 WHTE GE HEAVY)</t>
-  </si>
-  <si>
-    <t>9344 CARDS (689)</t>
-  </si>
-  <si>
-    <t>9345 CARDS (358 KALYANI)</t>
-  </si>
-  <si>
-    <t>9346 CARDS (359)</t>
-  </si>
-  <si>
-    <t>9347 CARDS (2853)</t>
-  </si>
-  <si>
-    <t>9348 CARDS *-* (डोरी) (S-124)</t>
-  </si>
-  <si>
-    <t>9349 CARDS (W/o Window) (S-120)</t>
-  </si>
-  <si>
-    <t>9350 CARDS *-* (T) (1632)</t>
-  </si>
-  <si>
-    <t>9351 Card - B (1603 B)</t>
-  </si>
-  <si>
-    <t>9351 CARDS *-* (T) (1603)</t>
-  </si>
-  <si>
-    <t>9352 CARDS *-* (T) (1606 AP)</t>
-  </si>
-  <si>
-    <t>9353 CARDS (1618)</t>
-  </si>
-  <si>
-    <t>9354 CARDS (DCU) (345)</t>
-  </si>
-  <si>
-    <t>9355 CARDS (1624)</t>
-  </si>
-  <si>
-    <t>9356 CARDS (2895/2897)</t>
-  </si>
-  <si>
-    <t>9357 CARDS (2872)</t>
-  </si>
-  <si>
-    <t>9358 CARDS (WHITE PATTA)</t>
-  </si>
-  <si>
-    <t>9359 CARDS (PITCH PATTA)</t>
-  </si>
-  <si>
-    <t>9360 CARDS *-* (M) (GOL ANDA)</t>
-  </si>
-  <si>
-    <t>9361 CARDS (25426)</t>
-  </si>
-  <si>
-    <t>9362 CARDS (363)</t>
-  </si>
-  <si>
-    <t>9363 CARDS *-* (T) (1652)</t>
-  </si>
-  <si>
-    <t>9364 CARDS *-* (T) (1612)</t>
-  </si>
-  <si>
-    <t>9365 CARDS (25429)</t>
-  </si>
-  <si>
-    <t>9366 CARDS (25427 GOLDEN)</t>
-  </si>
-  <si>
-    <t>9367 CARDS (5652)</t>
-  </si>
-  <si>
-    <t>9368 CARDS (9*5 SET 25/26 GOLDEN (25425))</t>
-  </si>
-  <si>
-    <t>9369 CARDS (9*5 SET 25/26 YELLOW (25424))</t>
-  </si>
-  <si>
-    <t>9370 CARDS (9*5 SET 25/26 RED (25423))</t>
-  </si>
-  <si>
-    <t>9371 CARDS (3111 VP)</t>
-  </si>
-  <si>
-    <t>9372 CARDS (9*5 YLW SET (2841))</t>
-  </si>
-  <si>
-    <t>9373 CARDS (1482)</t>
-  </si>
-  <si>
-    <t>9374 CARDS (1485)</t>
-  </si>
-  <si>
-    <t>9375 CARDS (1452 WHITE)</t>
-  </si>
-  <si>
-    <t>9376 CARDS (1529 PRINCE)</t>
-  </si>
-  <si>
-    <t>9378 CARDS (2892)</t>
+    <t>9232 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9233 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9235 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9236 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9237 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9301 CARDS</t>
+  </si>
+  <si>
+    <t>9302 CARDS</t>
+  </si>
+  <si>
+    <t>9303 CARDS</t>
+  </si>
+  <si>
+    <t>9304 CARDS</t>
+  </si>
+  <si>
+    <t>9305 CARDS (9070)</t>
+  </si>
+  <si>
+    <t>9306 CARDS</t>
+  </si>
+  <si>
+    <t>9307 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9308 CARDS</t>
+  </si>
+  <si>
+    <t>9309 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9310 CARDS</t>
+  </si>
+  <si>
+    <t>9311 CARDS</t>
+  </si>
+  <si>
+    <t>9312 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9313 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9314 CARDS</t>
+  </si>
+  <si>
+    <t>9315 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9316 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9317 CARDS</t>
+  </si>
+  <si>
+    <t>9318 CARDS</t>
+  </si>
+  <si>
+    <t>9320 CARDS</t>
+  </si>
+  <si>
+    <t>9321 CARDS</t>
+  </si>
+  <si>
+    <t>9322 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9323 CARDS (9005 OLD)</t>
+  </si>
+  <si>
+    <t>9324 CARDS</t>
+  </si>
+  <si>
+    <t>9325 CARDS</t>
+  </si>
+  <si>
+    <t>9326 CARDS</t>
+  </si>
+  <si>
+    <t>9327 CARDS</t>
+  </si>
+  <si>
+    <t>9328 CARDS</t>
+  </si>
+  <si>
+    <t>9329 CARDS (Desgin H/d)</t>
+  </si>
+  <si>
+    <t>9330 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9331 CARDS *-*  (T)</t>
+  </si>
+  <si>
+    <t>9332 CARDS</t>
+  </si>
+  <si>
+    <t>9333 CARDS</t>
+  </si>
+  <si>
+    <t>9334 CARDS</t>
+  </si>
+  <si>
+    <t>9335 CARDS (9003 OLD)</t>
+  </si>
+  <si>
+    <t>9336 CARDS</t>
+  </si>
+  <si>
+    <t>9337 CARDS</t>
+  </si>
+  <si>
+    <t>9338 CARDS</t>
+  </si>
+  <si>
+    <t>9339 CARDS</t>
+  </si>
+  <si>
+    <t>9340 CARDS</t>
+  </si>
+  <si>
+    <t>9341 CARDS</t>
+  </si>
+  <si>
+    <t>9342 CARDS</t>
+  </si>
+  <si>
+    <t>9343 CARDS</t>
+  </si>
+  <si>
+    <t>9344 CARDS</t>
+  </si>
+  <si>
+    <t>9345 CARDS</t>
+  </si>
+  <si>
+    <t>9346 CARDS</t>
+  </si>
+  <si>
+    <t>9347 CARDS</t>
+  </si>
+  <si>
+    <t>9348 CARDS *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>9349 CARDS (W/o Window)</t>
+  </si>
+  <si>
+    <t>9350 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9351 Card - B</t>
+  </si>
+  <si>
+    <t>9351 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9352 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9353 CARDS</t>
+  </si>
+  <si>
+    <t>9354 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9355 CARDS</t>
+  </si>
+  <si>
+    <t>9356 CARDS</t>
+  </si>
+  <si>
+    <t>9357 CARDS</t>
+  </si>
+  <si>
+    <t>9358 CARDS</t>
+  </si>
+  <si>
+    <t>9359 CARDS</t>
+  </si>
+  <si>
+    <t>9360 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9361 CARDS</t>
+  </si>
+  <si>
+    <t>9362 CARDS</t>
+  </si>
+  <si>
+    <t>9363 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9364 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9365 CARDS</t>
+  </si>
+  <si>
+    <t>9366 CARDS</t>
+  </si>
+  <si>
+    <t>9367 CARDS</t>
+  </si>
+  <si>
+    <t>9368 CARDS</t>
+  </si>
+  <si>
+    <t>9369 CARDS</t>
+  </si>
+  <si>
+    <t>9370 CARDS</t>
+  </si>
+  <si>
+    <t>9371 CARDS</t>
+  </si>
+  <si>
+    <t>9372 CARDS</t>
+  </si>
+  <si>
+    <t>9373 CARDS</t>
+  </si>
+  <si>
+    <t>9374 CARDS</t>
+  </si>
+  <si>
+    <t>9375 CARDS</t>
+  </si>
+  <si>
+    <t>9376 CARDS</t>
+  </si>
+  <si>
+    <t>9378 CARDS</t>
   </si>
   <si>
     <t>9379 CARDS - R</t>
@@ -1973,19 +1973,19 @@
     <t>9387 CARDS - GOLDEN (Mil Jayega)</t>
   </si>
   <si>
-    <t>9389 CARDS (9147 RJ)</t>
-  </si>
-  <si>
-    <t>9390 CARDS (DCU) (118KBC)</t>
+    <t>9389 CARDS</t>
+  </si>
+  <si>
+    <t>9390 CARDS (DCU)</t>
   </si>
   <si>
     <t>9391 CARDS</t>
   </si>
   <si>
-    <t>9*4 ENVELOPE (SBC) (CHOTA ENVELOPE (60/40 BILL))</t>
-  </si>
-  <si>
-    <t>9*5 ENVELOPE (FOIL) SBC (BADA ENVLP WITH FOIL (60/40 BILL))</t>
+    <t>9*4 ENVELOPE (SBC)</t>
+  </si>
+  <si>
+    <t>9*5 ENVELOPE (FOIL) SBC</t>
   </si>
   <si>
     <t>ACRYLIC NAME PLATE</t>
@@ -1994,7 +1994,7 @@
     <t>DEV SAMPLE SET</t>
   </si>
   <si>
-    <t>FANCY GIFT ENVELOPE-(SR) (SR ENVELOPES)</t>
+    <t>FANCY GIFT ENVELOPE-(SR)</t>
   </si>
   <si>
     <t>Gift Envelope (Pocket) SR...</t>
@@ -2012,31 +2012,31 @@
     <t>RIBBON (रिबीन)</t>
   </si>
   <si>
-    <t>RX-01 ENVELOPE (LX01)</t>
-  </si>
-  <si>
-    <t>RX-02 ENVELOPE (LX02)</t>
-  </si>
-  <si>
-    <t>RX-03 ENVELOPE (LX03)</t>
-  </si>
-  <si>
-    <t>RX-04 ENVELOPE (LX04)</t>
-  </si>
-  <si>
-    <t>RX-05 ENVELOPE (LX05)</t>
-  </si>
-  <si>
-    <t>RX-07 ENVELOPE (LX07)</t>
-  </si>
-  <si>
-    <t>RX-08 ENVELOPE (LX08)</t>
-  </si>
-  <si>
-    <t>RX-09 ENVELOPE (LX09)</t>
-  </si>
-  <si>
-    <t>गोल गणेश / गोल फ्लावर (GOL GANESH OR GOL FLOWER)</t>
+    <t>RX-01 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-02 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-03 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-04 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-05 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-07 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-08 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-09 ENVELOPE</t>
+  </si>
+  <si>
+    <t>गोल गणेश / गोल फ्लावर</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -2569,7 +2569,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -2691,16 +2691,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="25">
-        <v>47.5</v>
+        <v>46.5</v>
       </c>
       <c r="D11" s="26">
         <v>1.8</v>
       </c>
       <c r="E11" s="27">
-        <v>85.5</v>
+        <v>83.7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2844,16 +2844,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="25">
-        <v>19.5</v>
+        <v>17.5</v>
       </c>
       <c r="D20" s="26">
         <v>2.6</v>
       </c>
       <c r="E20" s="27">
-        <v>50.7</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3201,16 +3201,16 @@
         <v>43</v>
       </c>
       <c r="B41" s="24">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" s="25">
-        <v>34.5</v>
+        <v>34</v>
       </c>
       <c r="D41" s="26">
         <v>2.35</v>
       </c>
       <c r="E41" s="27">
-        <v>81.08</v>
+        <v>79.900000000000006</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3286,16 +3286,16 @@
         <v>48</v>
       </c>
       <c r="B46" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C46" s="25">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="D46" s="26">
         <v>1.26</v>
       </c>
       <c r="E46" s="27">
-        <v>6.93</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3337,16 +3337,16 @@
         <v>51</v>
       </c>
       <c r="B49" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C49" s="25">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D49" s="26">
         <v>1.8</v>
       </c>
       <c r="E49" s="27">
-        <v>203.4</v>
+        <v>192.6</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3425,13 +3425,13 @@
         <v>14</v>
       </c>
       <c r="C54" s="25">
-        <v>63.5</v>
+        <v>183.5</v>
       </c>
       <c r="D54" s="26">
         <v>1.8</v>
       </c>
       <c r="E54" s="27">
-        <v>114.3</v>
+        <v>330.3</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3490,16 +3490,16 @@
         <v>60</v>
       </c>
       <c r="B58" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C58" s="25">
-        <v>275.5</v>
+        <v>245.5</v>
       </c>
       <c r="D58" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E58" s="27">
-        <v>305.81</v>
+        <v>272.51</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3507,16 +3507,16 @@
         <v>61</v>
       </c>
       <c r="B59" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C59" s="25">
-        <v>248.5</v>
+        <v>218.5</v>
       </c>
       <c r="D59" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E59" s="27">
-        <v>275.83999999999997</v>
+        <v>242.54</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3554,16 +3554,16 @@
         <v>64</v>
       </c>
       <c r="B62" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C62" s="25">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D62" s="26">
         <v>1.65</v>
       </c>
       <c r="E62" s="27">
-        <v>166.65</v>
+        <v>150.15</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3586,16 +3586,16 @@
         <v>66</v>
       </c>
       <c r="B64" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C64" s="25">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D64" s="26">
         <v>1.65</v>
       </c>
       <c r="E64" s="27">
-        <v>66</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3737,16 +3737,16 @@
         <v>75</v>
       </c>
       <c r="B73" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C73" s="25">
-        <v>547</v>
+        <v>527</v>
       </c>
       <c r="D73" s="26">
         <v>1.2</v>
       </c>
       <c r="E73" s="27">
-        <v>656.4</v>
+        <v>632.4</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3754,16 +3754,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C74" s="25">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>750</v>
+        <v>726</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3786,16 +3786,16 @@
         <v>78</v>
       </c>
       <c r="B76" s="24">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C76" s="25">
-        <v>650.5</v>
+        <v>626.5</v>
       </c>
       <c r="D76" s="26">
         <v>1.2</v>
       </c>
       <c r="E76" s="27">
-        <v>780.6</v>
+        <v>751.8</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3891,13 +3891,13 @@
         <v>19</v>
       </c>
       <c r="C82" s="25">
-        <v>87.5</v>
+        <v>1259.5</v>
       </c>
       <c r="D82" s="26">
         <v>1.3</v>
       </c>
       <c r="E82" s="27">
-        <v>113.75</v>
+        <v>1637.35</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3922,16 +3922,16 @@
         <v>86</v>
       </c>
       <c r="B84" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C84" s="25">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D84" s="26">
         <v>1.7</v>
       </c>
       <c r="E84" s="27">
-        <v>13.6</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3976,13 +3976,13 @@
         <v>20</v>
       </c>
       <c r="C87" s="25">
-        <v>258</v>
+        <v>325</v>
       </c>
       <c r="D87" s="26">
-        <v>1.34</v>
+        <v>1.37</v>
       </c>
       <c r="E87" s="27">
-        <v>346.96</v>
+        <v>446.14</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4398,10 +4398,10 @@
         <v>118</v>
       </c>
       <c r="B116" s="24">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C116" s="25">
-        <v>-1.73</v>
+        <v>-1.78</v>
       </c>
       <c r="D116" s="28"/>
       <c r="E116" s="29"/>
@@ -4591,16 +4591,16 @@
         <v>131</v>
       </c>
       <c r="B129" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C129" s="25">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="D129" s="26">
         <v>12.5</v>
       </c>
       <c r="E129" s="27">
-        <v>118.75</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4625,16 +4625,16 @@
         <v>133</v>
       </c>
       <c r="B131" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C131" s="25">
-        <v>17.5</v>
+        <v>14.5</v>
       </c>
       <c r="D131" s="26">
         <v>12.89</v>
       </c>
       <c r="E131" s="27">
-        <v>225.49</v>
+        <v>186.84</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4674,16 +4674,16 @@
         <v>136</v>
       </c>
       <c r="B134" s="24">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C134" s="25">
-        <v>27.5</v>
+        <v>25.5</v>
       </c>
       <c r="D134" s="26">
         <v>18.5</v>
       </c>
       <c r="E134" s="27">
-        <v>508.75</v>
+        <v>471.75</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4708,16 +4708,16 @@
         <v>138</v>
       </c>
       <c r="B136" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C136" s="25">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="D136" s="26">
         <v>18.5</v>
       </c>
       <c r="E136" s="27">
-        <v>157.25</v>
+        <v>138.75</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4810,16 +4810,16 @@
         <v>144</v>
       </c>
       <c r="B142" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C142" s="25">
-        <v>16.5</v>
+        <v>14.5</v>
       </c>
       <c r="D142" s="26">
         <v>18.5</v>
       </c>
       <c r="E142" s="27">
-        <v>305.25</v>
+        <v>268.25</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4881,13 +4881,13 @@
         <v>14</v>
       </c>
       <c r="C146" s="25">
-        <v>15.5</v>
+        <v>30.5</v>
       </c>
       <c r="D146" s="26">
         <v>11.5</v>
       </c>
       <c r="E146" s="27">
-        <v>178.25</v>
+        <v>350.75</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -5201,16 +5201,16 @@
         <v>167</v>
       </c>
       <c r="B165" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C165" s="25">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D165" s="26">
         <v>2.7</v>
       </c>
       <c r="E165" s="27">
-        <v>229.5</v>
+        <v>221.4</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5386,16 +5386,16 @@
         <v>178</v>
       </c>
       <c r="B176" s="24">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C176" s="25">
-        <v>100</v>
+        <v>94.5</v>
       </c>
       <c r="D176" s="26">
         <v>2.65</v>
       </c>
       <c r="E176" s="27">
-        <v>265</v>
+        <v>250.43</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5455,13 +5455,13 @@
         <v>14</v>
       </c>
       <c r="C180" s="25">
-        <v>30.5</v>
+        <v>60</v>
       </c>
       <c r="D180" s="26">
         <v>5</v>
       </c>
       <c r="E180" s="27">
-        <v>152.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5812,13 +5812,13 @@
         <v>16</v>
       </c>
       <c r="C201" s="25">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D201" s="26">
         <v>3</v>
       </c>
       <c r="E201" s="27">
-        <v>9</v>
+        <v>225</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5897,13 +5897,13 @@
         <v>29</v>
       </c>
       <c r="C206" s="25">
-        <v>38.5</v>
+        <v>40</v>
       </c>
       <c r="D206" s="26">
         <v>2.7</v>
       </c>
       <c r="E206" s="27">
-        <v>103.95</v>
+        <v>108</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -6252,16 +6252,16 @@
         <v>230</v>
       </c>
       <c r="B228" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C228" s="25">
-        <v>35.5</v>
+        <v>32.5</v>
       </c>
       <c r="D228" s="26">
         <v>3</v>
       </c>
       <c r="E228" s="27">
-        <v>106.5</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6286,16 +6286,16 @@
         <v>232</v>
       </c>
       <c r="B230" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C230" s="25">
-        <v>53.5</v>
+        <v>50.5</v>
       </c>
       <c r="D230" s="26">
         <v>3.8</v>
       </c>
       <c r="E230" s="27">
-        <v>203.3</v>
+        <v>191.9</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6303,16 +6303,16 @@
         <v>233</v>
       </c>
       <c r="B231" s="24">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C231" s="25">
-        <v>135.5</v>
+        <v>133</v>
       </c>
       <c r="D231" s="26">
         <v>3.9</v>
       </c>
       <c r="E231" s="27">
-        <v>528.45000000000005</v>
+        <v>518.70000000000005</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6320,16 +6320,16 @@
         <v>234</v>
       </c>
       <c r="B232" s="24">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C232" s="25">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D232" s="26">
         <v>3.9</v>
       </c>
       <c r="E232" s="27">
-        <v>507</v>
+        <v>499.2</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -6573,16 +6573,16 @@
         <v>249</v>
       </c>
       <c r="B247" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C247" s="25">
-        <v>92.5</v>
+        <v>91.5</v>
       </c>
       <c r="D247" s="26">
         <v>4.5</v>
       </c>
       <c r="E247" s="27">
-        <v>416.25</v>
+        <v>411.75</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -6777,16 +6777,16 @@
         <v>261</v>
       </c>
       <c r="B259" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C259" s="25">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D259" s="26">
         <v>5.16</v>
       </c>
       <c r="E259" s="27">
-        <v>598.55999999999995</v>
+        <v>583.08000000000004</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6933,13 +6933,13 @@
         <v>33</v>
       </c>
       <c r="C268" s="25">
-        <v>192</v>
+        <v>232</v>
       </c>
       <c r="D268" s="26">
         <v>4.8899999999999997</v>
       </c>
       <c r="E268" s="27">
-        <v>938.74</v>
+        <v>1134.04</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -7509,16 +7509,16 @@
         <v>305</v>
       </c>
       <c r="B303" s="24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C303" s="25">
-        <v>131.5</v>
+        <v>132.5</v>
       </c>
       <c r="D303" s="26">
         <v>4.28</v>
       </c>
       <c r="E303" s="27">
-        <v>562.82000000000005</v>
+        <v>567.1</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7662,16 +7662,16 @@
         <v>314</v>
       </c>
       <c r="B312" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C312" s="25">
-        <v>11.5</v>
+        <v>10</v>
       </c>
       <c r="D312" s="26">
         <v>9</v>
       </c>
       <c r="E312" s="27">
-        <v>103.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -7928,16 +7928,16 @@
         <v>330</v>
       </c>
       <c r="B328" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C328" s="25">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D328" s="26">
         <v>6.64</v>
       </c>
       <c r="E328" s="27">
-        <v>378.55</v>
+        <v>371.91</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -8115,16 +8115,16 @@
         <v>341</v>
       </c>
       <c r="B339" s="24">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C339" s="25">
-        <v>236</v>
+        <v>236.5</v>
       </c>
       <c r="D339" s="26">
         <v>6.6</v>
       </c>
       <c r="E339" s="27">
-        <v>1557.6</v>
+        <v>1560.9</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -8183,16 +8183,16 @@
         <v>345</v>
       </c>
       <c r="B343" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C343" s="25">
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="D343" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E343" s="27">
-        <v>168.1</v>
+        <v>143.5</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -8772,16 +8772,16 @@
         <v>380</v>
       </c>
       <c r="B378" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C378" s="25">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D378" s="26">
         <v>7.6</v>
       </c>
       <c r="E378" s="27">
-        <v>19</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
@@ -8789,16 +8789,16 @@
         <v>381</v>
       </c>
       <c r="B379" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C379" s="25">
-        <v>91</v>
+        <v>89.5</v>
       </c>
       <c r="D379" s="26">
         <v>5.2</v>
       </c>
       <c r="E379" s="27">
-        <v>473.2</v>
+        <v>465.4</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
@@ -9747,16 +9747,16 @@
         <v>439</v>
       </c>
       <c r="B437" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C437" s="25">
-        <v>22.5</v>
+        <v>20</v>
       </c>
       <c r="D437" s="26">
         <v>9.5</v>
       </c>
       <c r="E437" s="27">
-        <v>213.75</v>
+        <v>190</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -10088,13 +10088,13 @@
         <v>13</v>
       </c>
       <c r="C457" s="25">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D457" s="26">
         <v>11.15</v>
       </c>
       <c r="E457" s="27">
-        <v>267.69</v>
+        <v>245.38</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
@@ -10136,16 +10136,16 @@
         <v>462</v>
       </c>
       <c r="B460" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C460" s="25">
-        <v>16</v>
+        <v>13.5</v>
       </c>
       <c r="D460" s="26">
         <v>13.39</v>
       </c>
       <c r="E460" s="27">
-        <v>214.27</v>
+        <v>180.79</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
@@ -10185,16 +10185,16 @@
         <v>465</v>
       </c>
       <c r="B463" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C463" s="25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D463" s="26">
         <v>11.25</v>
       </c>
       <c r="E463" s="27">
-        <v>146.25</v>
+        <v>135</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
@@ -11083,16 +11083,16 @@
         <v>519</v>
       </c>
       <c r="B517" s="24">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C517" s="25">
-        <v>111.5</v>
+        <v>212</v>
       </c>
       <c r="D517" s="26">
         <v>3.9</v>
       </c>
       <c r="E517" s="27">
-        <v>434.85</v>
+        <v>826.8</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
@@ -11338,16 +11338,16 @@
         <v>534</v>
       </c>
       <c r="B532" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C532" s="25">
-        <v>3.5</v>
+        <v>-1.5</v>
       </c>
       <c r="D532" s="26">
         <v>2.66</v>
       </c>
       <c r="E532" s="27">
-        <v>9.31</v>
+        <v>-3.99</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -11577,10 +11577,10 @@
         <v>549</v>
       </c>
       <c r="B547" s="24">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C547" s="25">
-        <v>41.5</v>
+        <v>37.5</v>
       </c>
       <c r="D547" s="28"/>
       <c r="E547" s="29"/>
@@ -11590,10 +11590,10 @@
         <v>550</v>
       </c>
       <c r="B548" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C548" s="25">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D548" s="28"/>
       <c r="E548" s="29"/>
@@ -11616,16 +11616,16 @@
         <v>552</v>
       </c>
       <c r="B550" s="24">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C550" s="25">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D550" s="26">
         <v>0.87</v>
       </c>
       <c r="E550" s="27">
-        <v>122.67</v>
+        <v>121.8</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.25">
@@ -11684,16 +11684,16 @@
         <v>556</v>
       </c>
       <c r="B554" s="24">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C554" s="25">
-        <v>445.5</v>
+        <v>444.5</v>
       </c>
       <c r="D554" s="26">
         <v>0.85</v>
       </c>
       <c r="E554" s="27">
-        <v>378.68</v>
+        <v>377.83</v>
       </c>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.25">
@@ -11917,16 +11917,16 @@
         <v>571</v>
       </c>
       <c r="B569" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C569" s="25">
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
       <c r="D569" s="26">
         <v>3.5</v>
       </c>
       <c r="E569" s="27">
-        <v>71.75</v>
+        <v>68.25</v>
       </c>
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.25">
@@ -11951,16 +11951,16 @@
         <v>573</v>
       </c>
       <c r="B571" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C571" s="25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D571" s="26">
         <v>4</v>
       </c>
       <c r="E571" s="27">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
@@ -12070,16 +12070,16 @@
         <v>580</v>
       </c>
       <c r="B578" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C578" s="25">
-        <v>35.5</v>
+        <v>30.5</v>
       </c>
       <c r="D578" s="26">
         <v>4</v>
       </c>
       <c r="E578" s="27">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
@@ -12087,16 +12087,16 @@
         <v>581</v>
       </c>
       <c r="B579" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C579" s="25">
-        <v>47.5</v>
+        <v>42.5</v>
       </c>
       <c r="D579" s="26">
         <v>1.5</v>
       </c>
       <c r="E579" s="27">
-        <v>71.25</v>
+        <v>63.75</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -12342,16 +12342,16 @@
         <v>596</v>
       </c>
       <c r="B594" s="24">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C594" s="25">
-        <v>399.5</v>
+        <v>390.5</v>
       </c>
       <c r="D594" s="26">
         <v>1.7</v>
       </c>
       <c r="E594" s="27">
-        <v>679.15</v>
+        <v>663.85</v>
       </c>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
@@ -12461,16 +12461,16 @@
         <v>603</v>
       </c>
       <c r="B601" s="24">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C601" s="25">
-        <v>94.8</v>
+        <v>94.3</v>
       </c>
       <c r="D601" s="26">
         <v>2.85</v>
       </c>
       <c r="E601" s="27">
-        <v>270.18</v>
+        <v>268.76</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -12580,16 +12580,16 @@
         <v>610</v>
       </c>
       <c r="B608" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C608" s="25">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D608" s="26">
         <v>3.97</v>
       </c>
       <c r="E608" s="27">
-        <v>214.29</v>
+        <v>202.39</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
@@ -12712,16 +12712,16 @@
         <v>618</v>
       </c>
       <c r="B616" s="24">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C616" s="25">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D616" s="26">
         <v>3.1</v>
       </c>
       <c r="E616" s="27">
-        <v>486.7</v>
+        <v>471.2</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12746,16 +12746,16 @@
         <v>620</v>
       </c>
       <c r="B618" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C618" s="25">
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="D618" s="26">
         <v>3.5</v>
       </c>
       <c r="E618" s="27">
-        <v>64.75</v>
+        <v>57.75</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12865,16 +12865,16 @@
         <v>627</v>
       </c>
       <c r="B625" s="24">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C625" s="25">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D625" s="26">
         <v>2.25</v>
       </c>
       <c r="E625" s="27">
-        <v>119.25</v>
+        <v>110.25</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -13001,16 +13001,16 @@
         <v>635</v>
       </c>
       <c r="B633" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C633" s="25">
-        <v>17.5</v>
+        <v>15</v>
       </c>
       <c r="D633" s="26">
         <v>4.25</v>
       </c>
       <c r="E633" s="27">
-        <v>74.38</v>
+        <v>63.75</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
@@ -13167,7 +13167,7 @@
         <v>34</v>
       </c>
       <c r="C644" s="25">
-        <v>73.5</v>
+        <v>77</v>
       </c>
       <c r="D644" s="28"/>
       <c r="E644" s="29"/>
@@ -13321,10 +13321,10 @@
         <v>657</v>
       </c>
       <c r="B655" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C655" s="25">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="D655" s="28"/>
       <c r="E655" s="29"/>
@@ -13377,10 +13377,10 @@
         <v>661</v>
       </c>
       <c r="B659" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C659" s="25">
-        <v>-61.65</v>
+        <v>-62.65</v>
       </c>
       <c r="D659" s="28"/>
       <c r="E659" s="29"/>
@@ -13526,10 +13526,10 @@
         <v>670</v>
       </c>
       <c r="B668" s="24">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C668" s="25">
-        <v>-237</v>
+        <v>-238.5</v>
       </c>
       <c r="D668" s="28"/>
       <c r="E668" s="29"/>
@@ -13540,11 +13540,11 @@
       </c>
       <c r="B669" s="31"/>
       <c r="C669" s="32">
-        <v>39177.54</v>
+        <v>40525.99</v>
       </c>
       <c r="D669" s="33"/>
       <c r="E669" s="34">
-        <v>112024.44</v>
+        <v>114289.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil 30 dec @ 8.40
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -35,7 +35,7 @@
     <t>Stock Group Summary</t>
   </si>
   <si>
-    <t>1-Jul-25 to 29-Dec-25</t>
+    <t>1-Jul-25 to 30-Dec-25</t>
   </si>
   <si>
     <t/>
@@ -1526,7 +1526,7 @@
     <t>6665 PATRIKA *-* (M)</t>
   </si>
   <si>
-    <t>6666 PATRIKA *-* (M)</t>
+    <t>6666 PATRIKA *-* (M) (DC)</t>
   </si>
   <si>
     <t>6667 PATRIKA *-* (M)</t>
@@ -2877,16 +2877,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="25">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="26">
         <v>2</v>
       </c>
       <c r="E14" s="27">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2894,16 +2894,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="25">
-        <v>72.5</v>
+        <v>67.5</v>
       </c>
       <c r="D15" s="26">
         <v>2</v>
       </c>
       <c r="E15" s="27">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2996,16 +2996,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="25">
-        <v>124.5</v>
+        <v>104.5</v>
       </c>
       <c r="D21" s="26">
         <v>1.8</v>
       </c>
       <c r="E21" s="27">
-        <v>224.1</v>
+        <v>188.1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3013,16 +3013,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="25">
-        <v>130.5</v>
+        <v>110.5</v>
       </c>
       <c r="D22" s="26">
         <v>1.8</v>
       </c>
       <c r="E22" s="27">
-        <v>234.9</v>
+        <v>198.9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3432,16 +3432,16 @@
         <v>49</v>
       </c>
       <c r="B47" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C47" s="25">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D47" s="26">
         <v>1.26</v>
       </c>
       <c r="E47" s="27">
-        <v>1.89</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3449,16 +3449,16 @@
         <v>50</v>
       </c>
       <c r="B48" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C48" s="25">
-        <v>113</v>
+        <v>100.5</v>
       </c>
       <c r="D48" s="26">
         <v>1.4</v>
       </c>
       <c r="E48" s="27">
-        <v>158.19999999999999</v>
+        <v>140.69999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3486,13 +3486,13 @@
         <v>14</v>
       </c>
       <c r="C50" s="25">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D50" s="26">
         <v>1.8</v>
       </c>
       <c r="E50" s="27">
-        <v>176.4</v>
+        <v>149.4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3568,16 +3568,16 @@
         <v>57</v>
       </c>
       <c r="B55" s="24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C55" s="25">
-        <v>179.5</v>
+        <v>154.5</v>
       </c>
       <c r="D55" s="26">
         <v>1.8</v>
       </c>
       <c r="E55" s="27">
-        <v>323.10000000000002</v>
+        <v>278.10000000000002</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3636,16 +3636,16 @@
         <v>61</v>
       </c>
       <c r="B59" s="24">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C59" s="25">
-        <v>241.5</v>
+        <v>219.5</v>
       </c>
       <c r="D59" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E59" s="27">
-        <v>268.07</v>
+        <v>243.65</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3669,15 +3669,17 @@
       <c r="A61" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B61" s="24"/>
+      <c r="B61" s="24">
+        <v>1</v>
+      </c>
       <c r="C61" s="25">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D61" s="26">
         <v>1.05</v>
       </c>
       <c r="E61" s="27">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3749,16 +3751,16 @@
         <v>68</v>
       </c>
       <c r="B66" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C66" s="25">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D66" s="26">
         <v>1.65</v>
       </c>
       <c r="E66" s="27">
-        <v>123.75</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3817,16 +3819,16 @@
         <v>72</v>
       </c>
       <c r="B70" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C70" s="25">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D70" s="26">
         <v>1.4</v>
       </c>
       <c r="E70" s="27">
-        <v>302.39999999999998</v>
+        <v>274.39999999999998</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3834,16 +3836,16 @@
         <v>73</v>
       </c>
       <c r="B71" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C71" s="25">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="D71" s="26">
         <v>1.4</v>
       </c>
       <c r="E71" s="27">
-        <v>484.4</v>
+        <v>456.4</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4121,16 +4123,16 @@
         <v>90</v>
       </c>
       <c r="B88" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C88" s="25">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D88" s="26">
         <v>1.37</v>
       </c>
       <c r="E88" s="27">
-        <v>339.06</v>
+        <v>334.95</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4172,16 +4174,16 @@
         <v>93</v>
       </c>
       <c r="B91" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C91" s="25">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="D91" s="26">
-        <v>1.52</v>
+        <v>1.58</v>
       </c>
       <c r="E91" s="27">
-        <v>441.57</v>
+        <v>474.74</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4189,16 +4191,16 @@
         <v>94</v>
       </c>
       <c r="B92" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C92" s="25">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D92" s="26">
         <v>2.76</v>
       </c>
       <c r="E92" s="27">
-        <v>146.25</v>
+        <v>91.06</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4219,16 +4221,16 @@
         <v>96</v>
       </c>
       <c r="B94" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C94" s="25">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="D94" s="26">
         <v>0.73</v>
       </c>
       <c r="E94" s="27">
-        <v>119.06</v>
+        <v>104.36</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -4236,16 +4238,16 @@
         <v>97</v>
       </c>
       <c r="B95" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C95" s="25">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="D95" s="26">
         <v>0.81</v>
       </c>
       <c r="E95" s="27">
-        <v>320.08</v>
+        <v>303.88</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4596,10 +4598,10 @@
         <v>123</v>
       </c>
       <c r="B121" s="24">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C121" s="25">
-        <v>-2.38</v>
+        <v>-2.4</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="28"/>
@@ -4691,16 +4693,16 @@
         <v>130</v>
       </c>
       <c r="B128" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C128" s="25">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="D128" s="26">
         <v>12.5</v>
       </c>
       <c r="E128" s="27">
-        <v>118.75</v>
+        <v>93.75</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4725,16 +4727,16 @@
         <v>132</v>
       </c>
       <c r="B130" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C130" s="25">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D130" s="26">
         <v>12.5</v>
       </c>
       <c r="E130" s="27">
-        <v>312.5</v>
+        <v>287.5</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4742,16 +4744,16 @@
         <v>133</v>
       </c>
       <c r="B131" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C131" s="25">
-        <v>21</v>
+        <v>18.5</v>
       </c>
       <c r="D131" s="26">
         <v>12.5</v>
       </c>
       <c r="E131" s="27">
-        <v>262.5</v>
+        <v>231.25</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -5323,16 +5325,16 @@
         <v>168</v>
       </c>
       <c r="B166" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C166" s="25">
-        <v>237.5</v>
+        <v>187.5</v>
       </c>
       <c r="D166" s="26">
         <v>1.3</v>
       </c>
       <c r="E166" s="27">
-        <v>308.75</v>
+        <v>243.75</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5385,16 +5387,16 @@
         <v>172</v>
       </c>
       <c r="B170" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C170" s="25">
-        <v>40.5</v>
+        <v>40</v>
       </c>
       <c r="D170" s="26">
         <v>3.25</v>
       </c>
       <c r="E170" s="27">
-        <v>131.63</v>
+        <v>130</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5479,16 +5481,16 @@
         <v>178</v>
       </c>
       <c r="B176" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C176" s="25">
-        <v>156.5</v>
+        <v>155</v>
       </c>
       <c r="D176" s="26">
         <v>2.78</v>
       </c>
       <c r="E176" s="27">
-        <v>435.72</v>
+        <v>431.54</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5592,17 +5594,11 @@
         <v>185</v>
       </c>
       <c r="B183" s="24">
-        <v>1</v>
-      </c>
-      <c r="C183" s="25">
-        <v>12</v>
-      </c>
-      <c r="D183" s="26">
-        <v>4.75</v>
-      </c>
-      <c r="E183" s="27">
-        <v>57</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C183" s="28"/>
+      <c r="D183" s="29"/>
+      <c r="E183" s="28"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="23" t="s">
@@ -5692,16 +5688,16 @@
         <v>191</v>
       </c>
       <c r="B189" s="24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C189" s="25">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D189" s="26">
         <v>5</v>
       </c>
       <c r="E189" s="27">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5805,16 +5801,16 @@
         <v>198</v>
       </c>
       <c r="B196" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C196" s="25">
-        <v>17.5</v>
+        <v>7.5</v>
       </c>
       <c r="D196" s="26">
         <v>4.5</v>
       </c>
       <c r="E196" s="27">
-        <v>78.75</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5890,16 +5886,16 @@
         <v>203</v>
       </c>
       <c r="B201" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C201" s="25">
-        <v>44.5</v>
+        <v>39</v>
       </c>
       <c r="D201" s="26">
         <v>2.6</v>
       </c>
       <c r="E201" s="27">
-        <v>115.7</v>
+        <v>101.4</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -6023,13 +6019,13 @@
         <v>42</v>
       </c>
       <c r="C209" s="25">
-        <v>172.5</v>
+        <v>172</v>
       </c>
       <c r="D209" s="26">
         <v>2.7</v>
       </c>
       <c r="E209" s="27">
-        <v>465.75</v>
+        <v>464.4</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -6037,16 +6033,16 @@
         <v>212</v>
       </c>
       <c r="B210" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C210" s="25">
-        <v>97.5</v>
+        <v>97</v>
       </c>
       <c r="D210" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E210" s="27">
-        <v>224.25</v>
+        <v>223.1</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -6105,16 +6101,16 @@
         <v>216</v>
       </c>
       <c r="B214" s="24">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C214" s="25">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D214" s="26">
         <v>3.92</v>
       </c>
       <c r="E214" s="27">
-        <v>576.36</v>
+        <v>544.99</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -6156,16 +6152,16 @@
         <v>219</v>
       </c>
       <c r="B217" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C217" s="25">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D217" s="26">
         <v>2.7</v>
       </c>
       <c r="E217" s="27">
-        <v>89.1</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -6190,16 +6186,16 @@
         <v>221</v>
       </c>
       <c r="B219" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C219" s="25">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D219" s="26">
         <v>2.66</v>
       </c>
       <c r="E219" s="27">
-        <v>255.36</v>
+        <v>228.76</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -6241,16 +6237,16 @@
         <v>224</v>
       </c>
       <c r="B222" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C222" s="25">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D222" s="26">
         <v>3.5</v>
       </c>
       <c r="E222" s="27">
-        <v>217</v>
+        <v>182</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -6320,16 +6316,16 @@
         <v>229</v>
       </c>
       <c r="B227" s="24">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C227" s="25">
-        <v>76.5</v>
+        <v>55.5</v>
       </c>
       <c r="D227" s="26">
         <v>3.25</v>
       </c>
       <c r="E227" s="27">
-        <v>248.63</v>
+        <v>180.38</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6337,16 +6333,16 @@
         <v>230</v>
       </c>
       <c r="B228" s="24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C228" s="25">
-        <v>70.5</v>
+        <v>62.5</v>
       </c>
       <c r="D228" s="26">
         <v>3.25</v>
       </c>
       <c r="E228" s="27">
-        <v>229.13</v>
+        <v>203.13</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6587,16 +6583,16 @@
         <v>246</v>
       </c>
       <c r="B244" s="24">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C244" s="25">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D244" s="26">
         <v>3.9</v>
       </c>
       <c r="E244" s="27">
-        <v>483.6</v>
+        <v>444.6</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6604,16 +6600,16 @@
         <v>247</v>
       </c>
       <c r="B245" s="24">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C245" s="25">
-        <v>128</v>
+        <v>116.5</v>
       </c>
       <c r="D245" s="26">
         <v>3.9</v>
       </c>
       <c r="E245" s="27">
-        <v>499.2</v>
+        <v>454.35</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6816,16 +6812,16 @@
         <v>261</v>
       </c>
       <c r="B259" s="24">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C259" s="25">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D259" s="26">
         <v>4.28</v>
       </c>
       <c r="E259" s="27">
-        <v>1532.24</v>
+        <v>1523.68</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -7098,16 +7094,16 @@
         <v>279</v>
       </c>
       <c r="B277" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C277" s="25">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D277" s="26">
         <v>4.5999999999999996</v>
       </c>
       <c r="E277" s="27">
-        <v>179.31</v>
+        <v>170.12</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -7115,16 +7111,16 @@
         <v>280</v>
       </c>
       <c r="B278" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C278" s="25">
-        <v>102</v>
+        <v>99.5</v>
       </c>
       <c r="D278" s="26">
         <v>6.2</v>
       </c>
       <c r="E278" s="27">
-        <v>631.98</v>
+        <v>616.5</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -7234,16 +7230,16 @@
         <v>287</v>
       </c>
       <c r="B285" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C285" s="25">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D285" s="26">
         <v>5.76</v>
       </c>
       <c r="E285" s="27">
-        <v>74.88</v>
+        <v>17.28</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -7301,15 +7297,17 @@
       <c r="A289" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="B289" s="24"/>
+      <c r="B289" s="24">
+        <v>1</v>
+      </c>
       <c r="C289" s="25">
-        <v>27.5</v>
+        <v>17.5</v>
       </c>
       <c r="D289" s="26">
         <v>5.76</v>
       </c>
       <c r="E289" s="27">
-        <v>158.4</v>
+        <v>100.8</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7385,16 +7383,16 @@
         <v>296</v>
       </c>
       <c r="B294" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C294" s="25">
-        <v>16.5</v>
+        <v>6.5</v>
       </c>
       <c r="D294" s="26">
         <v>5.7</v>
       </c>
       <c r="E294" s="27">
-        <v>94.05</v>
+        <v>37.049999999999997</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -7703,17 +7701,11 @@
         <v>316</v>
       </c>
       <c r="B314" s="24">
-        <v>1</v>
-      </c>
-      <c r="C314" s="25">
-        <v>7.5</v>
-      </c>
-      <c r="D314" s="26">
-        <v>7.75</v>
-      </c>
-      <c r="E314" s="27">
-        <v>58.13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C314" s="28"/>
+      <c r="D314" s="29"/>
+      <c r="E314" s="28"/>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="23" t="s">
@@ -7754,16 +7746,16 @@
         <v>319</v>
       </c>
       <c r="B317" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C317" s="25">
-        <v>26</v>
+        <v>24.5</v>
       </c>
       <c r="D317" s="26">
         <v>5.25</v>
       </c>
       <c r="E317" s="27">
-        <v>136.5</v>
+        <v>128.63</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
@@ -8061,16 +8053,16 @@
         <v>338</v>
       </c>
       <c r="B336" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C336" s="25">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="D336" s="26">
         <v>9</v>
       </c>
       <c r="E336" s="27">
-        <v>31.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -8255,16 +8247,16 @@
         <v>350</v>
       </c>
       <c r="B348" s="24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C348" s="25">
-        <v>50.35</v>
+        <v>48.85</v>
       </c>
       <c r="D348" s="26">
         <v>4.75</v>
       </c>
       <c r="E348" s="27">
-        <v>239.16</v>
+        <v>232.04</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -8389,16 +8381,16 @@
         <v>358</v>
       </c>
       <c r="B356" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C356" s="25">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D356" s="26">
         <v>7.76</v>
       </c>
       <c r="E356" s="27">
-        <v>961.91</v>
+        <v>884.33</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
@@ -8406,16 +8398,16 @@
         <v>359</v>
       </c>
       <c r="B357" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C357" s="25">
-        <v>58.5</v>
+        <v>48.5</v>
       </c>
       <c r="D357" s="26">
         <v>7.13</v>
       </c>
       <c r="E357" s="27">
-        <v>417.11</v>
+        <v>345.81</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -8525,16 +8517,16 @@
         <v>366</v>
       </c>
       <c r="B364" s="24">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C364" s="25">
-        <v>236.5</v>
+        <v>229.5</v>
       </c>
       <c r="D364" s="26">
         <v>6.6</v>
       </c>
       <c r="E364" s="27">
-        <v>1560.9</v>
+        <v>1514.7</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
@@ -8899,16 +8891,16 @@
         <v>388</v>
       </c>
       <c r="B386" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C386" s="25">
-        <v>25.5</v>
+        <v>15.5</v>
       </c>
       <c r="D386" s="26">
         <v>3.6</v>
       </c>
       <c r="E386" s="27">
-        <v>91.8</v>
+        <v>55.8</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -8982,16 +8974,16 @@
         <v>393</v>
       </c>
       <c r="B391" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C391" s="25">
-        <v>17</v>
+        <v>13.5</v>
       </c>
       <c r="D391" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E391" s="27">
-        <v>145.35</v>
+        <v>115.43</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
@@ -9044,16 +9036,16 @@
         <v>397</v>
       </c>
       <c r="B395" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C395" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D395" s="26">
         <v>6.4</v>
       </c>
       <c r="E395" s="27">
-        <v>128</v>
+        <v>64</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
@@ -9405,16 +9397,16 @@
         <v>420</v>
       </c>
       <c r="B418" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C418" s="25">
-        <v>21.5</v>
+        <v>17</v>
       </c>
       <c r="D418" s="26">
         <v>9</v>
       </c>
       <c r="E418" s="27">
-        <v>193.5</v>
+        <v>153</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
@@ -9459,16 +9451,16 @@
         <v>424</v>
       </c>
       <c r="B422" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C422" s="25">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D422" s="26">
         <v>8.35</v>
       </c>
       <c r="E422" s="27">
-        <v>342.18</v>
+        <v>258.72000000000003</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -9537,45 +9529,45 @@
       <c r="A427" s="23" t="s">
         <v>429</v>
       </c>
-      <c r="B427" s="24"/>
-      <c r="C427" s="25">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="D427" s="26">
-        <v>5.19</v>
-      </c>
-      <c r="E427" s="27">
-        <v>50.83</v>
-      </c>
+      <c r="B427" s="24">
+        <v>1</v>
+      </c>
+      <c r="C427" s="28"/>
+      <c r="D427" s="29"/>
+      <c r="E427" s="28"/>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" s="23" t="s">
         <v>430</v>
       </c>
-      <c r="B428" s="24"/>
+      <c r="B428" s="24">
+        <v>1</v>
+      </c>
       <c r="C428" s="25">
-        <v>28.2</v>
+        <v>18.2</v>
       </c>
       <c r="D428" s="26">
         <v>5.31</v>
       </c>
       <c r="E428" s="27">
-        <v>149.81</v>
+        <v>96.69</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="B429" s="24"/>
+      <c r="B429" s="24">
+        <v>1</v>
+      </c>
       <c r="C429" s="25">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D429" s="26">
         <v>4.8499999999999996</v>
       </c>
       <c r="E429" s="27">
-        <v>140.65</v>
+        <v>92.15</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -9583,16 +9575,16 @@
         <v>432</v>
       </c>
       <c r="B430" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C430" s="25">
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
       <c r="D430" s="26">
         <v>5.35</v>
       </c>
       <c r="E430" s="27">
-        <v>29.43</v>
+        <v>8.0299999999999994</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
@@ -9817,16 +9809,16 @@
         <v>446</v>
       </c>
       <c r="B444" s="24">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C444" s="25">
-        <v>14</v>
+        <v>16.5</v>
       </c>
       <c r="D444" s="26">
         <v>10.5</v>
       </c>
       <c r="E444" s="27">
-        <v>147</v>
+        <v>173.25</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
@@ -9834,16 +9826,16 @@
         <v>447</v>
       </c>
       <c r="B445" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C445" s="25">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="D445" s="26">
         <v>18</v>
       </c>
       <c r="E445" s="27">
-        <v>171</v>
+        <v>144</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
@@ -10015,16 +10007,16 @@
         <v>458</v>
       </c>
       <c r="B456" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C456" s="25">
-        <v>19.5</v>
+        <v>15.5</v>
       </c>
       <c r="D456" s="26">
         <v>10.5</v>
       </c>
       <c r="E456" s="27">
-        <v>204.75</v>
+        <v>162.75</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
@@ -10032,16 +10024,16 @@
         <v>459</v>
       </c>
       <c r="B457" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C457" s="25">
-        <v>8.5</v>
+        <v>11</v>
       </c>
       <c r="D457" s="26">
         <v>10</v>
       </c>
       <c r="E457" s="27">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
@@ -10213,16 +10205,16 @@
         <v>470</v>
       </c>
       <c r="B468" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C468" s="25">
-        <v>18</v>
+        <v>17.5</v>
       </c>
       <c r="D468" s="26">
         <v>10</v>
       </c>
       <c r="E468" s="27">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.25">
@@ -10230,16 +10222,16 @@
         <v>471</v>
       </c>
       <c r="B469" s="24">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C469" s="25">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D469" s="26">
         <v>9.5</v>
       </c>
       <c r="E469" s="27">
-        <v>133</v>
+        <v>161.5</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
@@ -10292,16 +10284,16 @@
         <v>475</v>
       </c>
       <c r="B473" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C473" s="25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D473" s="26">
         <v>10</v>
       </c>
       <c r="E473" s="27">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
@@ -10429,13 +10421,13 @@
         <v>7</v>
       </c>
       <c r="C481" s="25">
-        <v>14.5</v>
+        <v>14</v>
       </c>
       <c r="D481" s="26">
         <v>9.26</v>
       </c>
       <c r="E481" s="27">
-        <v>134.27000000000001</v>
+        <v>129.63999999999999</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.25">
@@ -10511,16 +10503,16 @@
         <v>488</v>
       </c>
       <c r="B486" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C486" s="25">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="D486" s="26">
         <v>10</v>
       </c>
       <c r="E486" s="27">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
@@ -10579,16 +10571,16 @@
         <v>492</v>
       </c>
       <c r="B490" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C490" s="25">
-        <v>18</v>
+        <v>15.5</v>
       </c>
       <c r="D490" s="26">
         <v>11.15</v>
       </c>
       <c r="E490" s="27">
-        <v>200.77</v>
+        <v>172.88</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10679,16 +10671,16 @@
         <v>498</v>
       </c>
       <c r="B496" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C496" s="25">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D496" s="26">
         <v>11.25</v>
       </c>
       <c r="E496" s="27">
-        <v>123.75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -11401,16 +11393,16 @@
         <v>542</v>
       </c>
       <c r="B540" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C540" s="25">
-        <v>10.4</v>
+        <v>7.9</v>
       </c>
       <c r="D540" s="26">
         <v>4.5</v>
       </c>
       <c r="E540" s="27">
-        <v>46.8</v>
+        <v>35.549999999999997</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
@@ -11503,16 +11495,16 @@
         <v>548</v>
       </c>
       <c r="B546" s="24">
+        <v>14</v>
+      </c>
+      <c r="C546" s="25">
         <v>13</v>
-      </c>
-      <c r="C546" s="25">
-        <v>14</v>
       </c>
       <c r="D546" s="26">
         <v>3.45</v>
       </c>
       <c r="E546" s="27">
-        <v>48.3</v>
+        <v>44.85</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
@@ -11588,16 +11580,16 @@
         <v>553</v>
       </c>
       <c r="B551" s="24">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C551" s="25">
-        <v>173.7</v>
+        <v>172.2</v>
       </c>
       <c r="D551" s="26">
         <v>3.9</v>
       </c>
       <c r="E551" s="27">
-        <v>677.43</v>
+        <v>671.58</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11892,16 +11884,16 @@
         <v>571</v>
       </c>
       <c r="B569" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C569" s="25">
-        <v>28.5</v>
+        <v>25.5</v>
       </c>
       <c r="D569" s="26">
         <v>2.35</v>
       </c>
       <c r="E569" s="27">
-        <v>66.98</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.25">
@@ -11960,16 +11952,16 @@
         <v>575</v>
       </c>
       <c r="B573" s="24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C573" s="25">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D573" s="26">
         <v>1.4</v>
       </c>
       <c r="E573" s="27">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
@@ -12095,10 +12087,10 @@
         <v>584</v>
       </c>
       <c r="B582" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C582" s="25">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D582" s="29"/>
       <c r="E582" s="28"/>
@@ -12108,10 +12100,10 @@
         <v>585</v>
       </c>
       <c r="B583" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C583" s="25">
-        <v>21.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="D583" s="29"/>
       <c r="E583" s="28"/>
@@ -12189,16 +12181,16 @@
         <v>590</v>
       </c>
       <c r="B588" s="24">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C588" s="25">
-        <v>336.5</v>
+        <v>331.5</v>
       </c>
       <c r="D588" s="26">
         <v>0.85</v>
       </c>
       <c r="E588" s="27">
-        <v>286.02999999999997</v>
+        <v>281.77999999999997</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
@@ -12223,10 +12215,10 @@
         <v>592</v>
       </c>
       <c r="B590" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C590" s="25">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D590" s="29"/>
       <c r="E590" s="28"/>
@@ -12249,10 +12241,10 @@
         <v>594</v>
       </c>
       <c r="B592" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C592" s="25">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="D592" s="29"/>
       <c r="E592" s="28"/>
@@ -12262,10 +12254,10 @@
         <v>595</v>
       </c>
       <c r="B593" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C593" s="25">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D593" s="29"/>
       <c r="E593" s="28"/>
@@ -12612,16 +12604,16 @@
         <v>617</v>
       </c>
       <c r="B615" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C615" s="25">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D615" s="26">
         <v>4</v>
       </c>
       <c r="E615" s="27">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12691,16 +12683,16 @@
         <v>622</v>
       </c>
       <c r="B620" s="24">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C620" s="25">
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="D620" s="26">
         <v>2.2799999999999998</v>
       </c>
       <c r="E620" s="27">
-        <v>20.52</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -13014,16 +13006,16 @@
         <v>641</v>
       </c>
       <c r="B639" s="24">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C639" s="25">
-        <v>90.8</v>
+        <v>89.3</v>
       </c>
       <c r="D639" s="26">
         <v>2.85</v>
       </c>
       <c r="E639" s="27">
-        <v>258.77999999999997</v>
+        <v>254.51</v>
       </c>
     </row>
     <row r="640" spans="1:5" x14ac:dyDescent="0.25">
@@ -13116,16 +13108,16 @@
         <v>647</v>
       </c>
       <c r="B645" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C645" s="25">
-        <v>24</v>
+        <v>22.5</v>
       </c>
       <c r="D645" s="26">
         <v>5.68</v>
       </c>
       <c r="E645" s="27">
-        <v>136.32</v>
+        <v>127.8</v>
       </c>
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.25">
@@ -13261,16 +13253,16 @@
         <v>656</v>
       </c>
       <c r="B654" s="24">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C654" s="25">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="D654" s="26">
         <v>3.1</v>
       </c>
       <c r="E654" s="27">
-        <v>440.2</v>
+        <v>331.7</v>
       </c>
     </row>
     <row r="655" spans="1:5" x14ac:dyDescent="0.25">
@@ -13278,16 +13270,16 @@
         <v>657</v>
       </c>
       <c r="B655" s="24">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C655" s="25">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D655" s="26">
         <v>3.6</v>
       </c>
       <c r="E655" s="27">
-        <v>129.6</v>
+        <v>104.4</v>
       </c>
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.25">
@@ -13346,16 +13338,16 @@
         <v>661</v>
       </c>
       <c r="B659" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C659" s="25">
-        <v>20.5</v>
+        <v>17</v>
       </c>
       <c r="D659" s="26">
         <v>2.5</v>
       </c>
       <c r="E659" s="27">
-        <v>51.25</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.25">
@@ -13431,16 +13423,16 @@
         <v>666</v>
       </c>
       <c r="B664" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C664" s="25">
-        <v>48.5</v>
+        <v>48</v>
       </c>
       <c r="D664" s="26">
         <v>2.25</v>
       </c>
       <c r="E664" s="27">
-        <v>109.13</v>
+        <v>108</v>
       </c>
     </row>
     <row r="665" spans="1:5" x14ac:dyDescent="0.25">
@@ -13711,10 +13703,10 @@
         <v>684</v>
       </c>
       <c r="B682" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C682" s="25">
-        <v>115.5</v>
+        <v>114.5</v>
       </c>
       <c r="D682" s="29"/>
       <c r="E682" s="28"/>
@@ -13772,16 +13764,16 @@
         <v>689</v>
       </c>
       <c r="B687" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C687" s="25">
-        <v>86.5</v>
+        <v>83.5</v>
       </c>
       <c r="D687" s="26">
         <v>2.9</v>
       </c>
       <c r="E687" s="27">
-        <v>250.67</v>
+        <v>241.98</v>
       </c>
     </row>
     <row r="688" spans="1:5" x14ac:dyDescent="0.25">
@@ -13906,16 +13898,16 @@
         <v>699</v>
       </c>
       <c r="B697" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C697" s="25">
-        <v>-5</v>
+        <v>-35</v>
       </c>
       <c r="D697" s="26">
         <v>1.6</v>
       </c>
       <c r="E697" s="27">
-        <v>-8</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="698" spans="1:5" x14ac:dyDescent="0.25">
@@ -13958,10 +13950,10 @@
         <v>703</v>
       </c>
       <c r="B701" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C701" s="25">
-        <v>-0.67</v>
+        <v>-0.68</v>
       </c>
       <c r="D701" s="29"/>
       <c r="E701" s="28"/>
@@ -13988,10 +13980,10 @@
         <v>705</v>
       </c>
       <c r="B703" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C703" s="25">
-        <v>-68.150000000000006</v>
+        <v>-71.150000000000006</v>
       </c>
       <c r="D703" s="29"/>
       <c r="E703" s="28"/>
@@ -14154,10 +14146,10 @@
         <v>715</v>
       </c>
       <c r="B713" s="24">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C713" s="25">
-        <v>-281.5</v>
+        <v>-283</v>
       </c>
       <c r="D713" s="29"/>
       <c r="E713" s="28"/>
@@ -14168,11 +14160,11 @@
       </c>
       <c r="B714" s="31"/>
       <c r="C714" s="32">
-        <v>41751.18</v>
+        <v>40998.85</v>
       </c>
       <c r="D714" s="33"/>
       <c r="E714" s="34">
-        <v>113746.5</v>
+        <v>111495.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil jan 1st @933
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -65,316 +65,316 @@
     <t>Value</t>
   </si>
   <si>
-    <t>.1001 PATRIKA (25/251)</t>
-  </si>
-  <si>
-    <t>1002 PATRIKA (25/262)</t>
-  </si>
-  <si>
-    <t>1003 PATRIKA (25/261)</t>
-  </si>
-  <si>
-    <t>1004 PATRIKA (25/361/861)</t>
-  </si>
-  <si>
-    <t>1005 PATRIKA (25/362/862)</t>
-  </si>
-  <si>
-    <t>1006 PATRIKA (25/282)</t>
-  </si>
-  <si>
-    <t>1007 PATRIKA (25/281)</t>
-  </si>
-  <si>
-    <t>1008 PATRIKA (JC) (2595 PINK)</t>
-  </si>
-  <si>
-    <t>1009 PATRIKA (JC) (2595 ORANGE)</t>
+    <t>.1001 PATRIKA</t>
+  </si>
+  <si>
+    <t>1002 PATRIKA</t>
+  </si>
+  <si>
+    <t>1003 PATRIKA</t>
+  </si>
+  <si>
+    <t>1004 PATRIKA</t>
+  </si>
+  <si>
+    <t>1005 PATRIKA</t>
+  </si>
+  <si>
+    <t>1006 PATRIKA</t>
+  </si>
+  <si>
+    <t>1007 PATRIKA</t>
+  </si>
+  <si>
+    <t>1008 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1009 PATRIKA (JC)</t>
   </si>
   <si>
     <t>100 ENVELOPE (SR) OFFSET</t>
   </si>
   <si>
-    <t>1010 PATRIKA (6321)</t>
-  </si>
-  <si>
-    <t>1011 PATRIKA (2563 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1012 PATRIKA (2564 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1013 PATRIKA (2568 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1014 PATRIKA (11043 OFFSET)</t>
-  </si>
-  <si>
-    <t>1015 PATRIKA (DCU) (11041 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1016 PATRIKA (1011 OFFSET)</t>
-  </si>
-  <si>
-    <t>1017 PATRIKA (1014 OFFSET)</t>
-  </si>
-  <si>
-    <t>1018 PATRIKA (10081 OFFSET NEW)</t>
-  </si>
-  <si>
-    <t>1019 PATRIKA (1222 SBC)</t>
-  </si>
-  <si>
-    <t>1020 PATRIKA (1235)</t>
-  </si>
-  <si>
-    <t>1021 PATRIKA (2101 VV)</t>
-  </si>
-  <si>
-    <t>1022 PATRIKA (JC) (25409)</t>
-  </si>
-  <si>
-    <t>1023 PATRIKA (25418)</t>
-  </si>
-  <si>
-    <t>1024 PATRIKA (25322)</t>
-  </si>
-  <si>
-    <t>1025 PATRIKA (25323)</t>
-  </si>
-  <si>
-    <t>1026 PATRIKA (JC) (1173 SBC)</t>
-  </si>
-  <si>
-    <t>1027 PATRIKA (JC) (5346)</t>
-  </si>
-  <si>
-    <t>1028 PATRIKA (JC) (2596)</t>
-  </si>
-  <si>
-    <t>1029 PATRIKA (1042)</t>
-  </si>
-  <si>
-    <t>1030 PATRIKA (1043)</t>
-  </si>
-  <si>
-    <t>1031 PATRIKA (GOPAL 11)</t>
-  </si>
-  <si>
-    <t>1032 PATRIKA (GOPAL 1)</t>
-  </si>
-  <si>
-    <t>1033 PATRIKA (2002 YLW)</t>
-  </si>
-  <si>
-    <t>1034 PATRIKA (2003 R)</t>
-  </si>
-  <si>
-    <t>1035 PATRIKA (DCU) (2201 ROSHAN)</t>
-  </si>
-  <si>
-    <t>1101 PATRIKA (O.2591) (2591 ORANGE)</t>
-  </si>
-  <si>
-    <t>1102 PATRIKA (P.2591) (2591 PINK)</t>
-  </si>
-  <si>
-    <t>1103 PATRIKA(N-271) (271 NEHA)</t>
-  </si>
-  <si>
-    <t>1104 PATRIKA(N-272) (272 NEHA)</t>
-  </si>
-  <si>
-    <t>1105 PATRIKA (276-A)</t>
-  </si>
-  <si>
-    <t>1106 PATRIKA-YELLOW (25419)</t>
-  </si>
-  <si>
-    <t>1107 PATRIKA-RED (25420)</t>
-  </si>
-  <si>
-    <t>1109 PATRIKA-BIG Y (25421)</t>
-  </si>
-  <si>
-    <t>1110 PATRIKA-BIG R (25422)</t>
-  </si>
-  <si>
-    <t>1112 PATRIKA (277-B)</t>
-  </si>
-  <si>
-    <t>1113 PATRIKA (1819 MONARCH)</t>
-  </si>
-  <si>
-    <t>1114 PATRIKA-BROWN (1709)</t>
-  </si>
-  <si>
-    <t>1115 PATRIKA-CREAM (1678 PRINCE)</t>
-  </si>
-  <si>
-    <t>1116 PATRIKA (1153) (1253 Jsk)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA (1155) (1155 JSK)</t>
-  </si>
-  <si>
-    <t>1117 PATRIKA - B (KRISHNA 1155-B)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA - B (DCU) (NEW SAVASHREE- 51)</t>
-  </si>
-  <si>
-    <t>1118 PATRIKA (सवाश्री-57) (NEW SAVASHREE-57)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA - B (DCU) (NEW SAVASHREE 52)</t>
-  </si>
-  <si>
-    <t>1119 PATRIKA(सवाश्री-55) (NEW SAVASHREE-55)</t>
-  </si>
-  <si>
-    <t>1120 PATRIKA(सवाश्री-59) (NEW SAVASHREE-59)</t>
-  </si>
-  <si>
-    <t>1121 PATRIKA(सवाश्री-53) (NEW SAVASHREE-53)</t>
-  </si>
-  <si>
-    <t>1122 PATRIKA (DCU) (NEW SAVASHREE-54)</t>
-  </si>
-  <si>
-    <t>1123 PATRIKA (LED-51) (LED-51)</t>
-  </si>
-  <si>
-    <t>1124 PATRIKA (LED-52) (LED-52)</t>
-  </si>
-  <si>
-    <t>1125 PATRIKA (LED-53) (LED-53)</t>
-  </si>
-  <si>
-    <t>1126 PATRIKA (LED-54) (LED-54)</t>
-  </si>
-  <si>
-    <t>1127 PATRIKA (Eco-52) (NEW ECO-52)</t>
-  </si>
-  <si>
-    <t>1128 PATRIKA (Eco-55) (NEW ECO-55)</t>
-  </si>
-  <si>
-    <t>1129 PATRIKA (Eco-56) (NEW ECO-56)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA - B (ECO-60) (DCU) (NEW ECO 60)</t>
-  </si>
-  <si>
-    <t>1130 PATRIKA (Eco-59) (NEW ECO-59)</t>
-  </si>
-  <si>
-    <t>1131 PATRIKA (DCU) Eco-51 (NEW ECO- 51)</t>
-  </si>
-  <si>
-    <t>1132 PATRIKA (DCU) Eco-53 (NEW ECO- 53)</t>
-  </si>
-  <si>
-    <t>1133 PATRIKA (DCU) Eco-57 (NEW ECO- 57)</t>
-  </si>
-  <si>
-    <t>1134 PATRIKA (DCU) Eco-58 (NEW ECO- 58)</t>
-  </si>
-  <si>
-    <t>1135 PATRIKA (DCU) Eco-54 (NEW ECO- 54)</t>
-  </si>
-  <si>
-    <t>1136 PATRIKA (R) (120 GSM RED)</t>
-  </si>
-  <si>
-    <t>1137 PATRIKA (P) (120 GSM YELLOW)</t>
-  </si>
-  <si>
-    <t>1138 PATRIKA (BR) (150 GSM FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1139 PATRIKA (BY) (150 GSM FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1140 PATRIKA (BB) (150 GSM FOIL (BROWN))</t>
-  </si>
-  <si>
-    <t>1141 PATRIKA (R) (120 GSM (RED)SELF)</t>
-  </si>
-  <si>
-    <t>1142 PATRIKA (P) (120 GSM (YELLOW) SELF)</t>
-  </si>
-  <si>
-    <t>1143 PATRIKA (G) (120 GSM (OLD GOLDEN))</t>
-  </si>
-  <si>
-    <t>1144 PATRIKA (BR) (170 GSM WITH FOIL (RED))</t>
-  </si>
-  <si>
-    <t>1145 PATRIKA (BY) (170 GSM WITH FOIL (YELLOW))</t>
-  </si>
-  <si>
-    <t>1146 PATRIKA (DCU) (BROWN 170 GSM FOIL)</t>
-  </si>
-  <si>
-    <t>1147 PATRIKA (S.201) (201 WESTERN)</t>
-  </si>
-  <si>
-    <t>1148 PATRIKA (S.202) (202 WESTERN)</t>
-  </si>
-  <si>
-    <t>1149 PATRIKA (S.204) (204 WESTERN)</t>
-  </si>
-  <si>
-    <t>1150 PATRIKA (DCU) (NEW SAVASHREE-58)</t>
-  </si>
-  <si>
-    <t>1151 PATRIKA (DCU) (NEW SAVASHREE-56)</t>
-  </si>
-  <si>
-    <t>1152 PATRIKA (DCU) (WESTERN 202 OLD)</t>
-  </si>
-  <si>
-    <t>1153 PATRIKA (DCU) (201 WESTERN (OLD))</t>
-  </si>
-  <si>
-    <t>1154 PATRIKA (DCU) (203 WESTERN A)</t>
-  </si>
-  <si>
-    <t>1155 PATRIKA (DCU) (WESTERN (203) B)</t>
-  </si>
-  <si>
-    <t>1156 PATRIKA-YELLOW (LU-51 (YELLOW))</t>
-  </si>
-  <si>
-    <t>1157 PATRIKA-CREAM (LU-52 (CREAM))</t>
-  </si>
-  <si>
-    <t>1158 PATRIKA-GOLDEN (LU-53 (GOLDEN))</t>
-  </si>
-  <si>
-    <t>1159 PATRIKA-WHITE (LU-54 (WHITE))</t>
-  </si>
-  <si>
-    <t>1160 PATRIKA-PINK (LU-55 (PINK))</t>
-  </si>
-  <si>
-    <t>1161 PATRIKA (01) (JCC 01)</t>
-  </si>
-  <si>
-    <t>1162 PATRIKA (02) (JCC 02)</t>
-  </si>
-  <si>
-    <t>1163 PATRIKA (DCU) (BP RED)</t>
-  </si>
-  <si>
-    <t>1164 PATRIKA (DCU) (BP PINK RIYAZ)</t>
-  </si>
-  <si>
-    <t>1165 PATRIKA (DCU) (BP CREAM)</t>
-  </si>
-  <si>
-    <t>1166 PATRIKA (DCU) (BP YELLOW)</t>
+    <t>1010 PATRIKA</t>
+  </si>
+  <si>
+    <t>1011 PATRIKA</t>
+  </si>
+  <si>
+    <t>1012 PATRIKA</t>
+  </si>
+  <si>
+    <t>1013 PATRIKA</t>
+  </si>
+  <si>
+    <t>1014 PATRIKA</t>
+  </si>
+  <si>
+    <t>1015 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1016 PATRIKA</t>
+  </si>
+  <si>
+    <t>1017 PATRIKA</t>
+  </si>
+  <si>
+    <t>1018 PATRIKA</t>
+  </si>
+  <si>
+    <t>1019 PATRIKA</t>
+  </si>
+  <si>
+    <t>1020 PATRIKA</t>
+  </si>
+  <si>
+    <t>1021 PATRIKA</t>
+  </si>
+  <si>
+    <t>1022 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1023 PATRIKA</t>
+  </si>
+  <si>
+    <t>1024 PATRIKA</t>
+  </si>
+  <si>
+    <t>1025 PATRIKA</t>
+  </si>
+  <si>
+    <t>1026 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1027 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1028 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>1029 PATRIKA</t>
+  </si>
+  <si>
+    <t>1030 PATRIKA</t>
+  </si>
+  <si>
+    <t>1031 PATRIKA</t>
+  </si>
+  <si>
+    <t>1032 PATRIKA</t>
+  </si>
+  <si>
+    <t>1033 PATRIKA</t>
+  </si>
+  <si>
+    <t>1034 PATRIKA</t>
+  </si>
+  <si>
+    <t>1035 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1101 PATRIKA (O.2591)</t>
+  </si>
+  <si>
+    <t>1102 PATRIKA (P.2591)</t>
+  </si>
+  <si>
+    <t>1103 PATRIKA(N-271)</t>
+  </si>
+  <si>
+    <t>1104 PATRIKA(N-272)</t>
+  </si>
+  <si>
+    <t>1105 PATRIKA</t>
+  </si>
+  <si>
+    <t>1106 PATRIKA-YELLOW</t>
+  </si>
+  <si>
+    <t>1107 PATRIKA-RED</t>
+  </si>
+  <si>
+    <t>1109 PATRIKA-BIG Y</t>
+  </si>
+  <si>
+    <t>1110 PATRIKA-BIG R</t>
+  </si>
+  <si>
+    <t>1112 PATRIKA</t>
+  </si>
+  <si>
+    <t>1113 PATRIKA</t>
+  </si>
+  <si>
+    <t>1114 PATRIKA-BROWN</t>
+  </si>
+  <si>
+    <t>1115 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1116 PATRIKA (1153)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA (1155)</t>
+  </si>
+  <si>
+    <t>1117 PATRIKA - B</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1118 PATRIKA (सवाश्री-57)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>1119 PATRIKA(सवाश्री-55)</t>
+  </si>
+  <si>
+    <t>1120 PATRIKA(सवाश्री-59)</t>
+  </si>
+  <si>
+    <t>1121 PATRIKA(सवाश्री-53)</t>
+  </si>
+  <si>
+    <t>1122 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1123 PATRIKA (LED-51)</t>
+  </si>
+  <si>
+    <t>1124 PATRIKA (LED-52)</t>
+  </si>
+  <si>
+    <t>1125 PATRIKA (LED-53)</t>
+  </si>
+  <si>
+    <t>1126 PATRIKA (LED-54)</t>
+  </si>
+  <si>
+    <t>1127 PATRIKA (Eco-52)</t>
+  </si>
+  <si>
+    <t>1128 PATRIKA (Eco-55)</t>
+  </si>
+  <si>
+    <t>1129 PATRIKA (Eco-56)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA - B (ECO-60) (DCU)</t>
+  </si>
+  <si>
+    <t>1130 PATRIKA (Eco-59)</t>
+  </si>
+  <si>
+    <t>1131 PATRIKA (DCU) Eco-51</t>
+  </si>
+  <si>
+    <t>1132 PATRIKA (DCU) Eco-53</t>
+  </si>
+  <si>
+    <t>1133 PATRIKA (DCU) Eco-57</t>
+  </si>
+  <si>
+    <t>1134 PATRIKA (DCU) Eco-58</t>
+  </si>
+  <si>
+    <t>1135 PATRIKA (DCU) Eco-54</t>
+  </si>
+  <si>
+    <t>1136 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1137 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1138 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1139 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1140 PATRIKA (BB)</t>
+  </si>
+  <si>
+    <t>1141 PATRIKA (R)</t>
+  </si>
+  <si>
+    <t>1142 PATRIKA (P)</t>
+  </si>
+  <si>
+    <t>1143 PATRIKA (G)</t>
+  </si>
+  <si>
+    <t>1144 PATRIKA (BR)</t>
+  </si>
+  <si>
+    <t>1145 PATRIKA (BY)</t>
+  </si>
+  <si>
+    <t>1146 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1147 PATRIKA (S.201)</t>
+  </si>
+  <si>
+    <t>1148 PATRIKA (S.202)</t>
+  </si>
+  <si>
+    <t>1149 PATRIKA (S.204)</t>
+  </si>
+  <si>
+    <t>1150 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1151 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1152 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1153 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1154 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1155 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1156 PATRIKA-YELLOW</t>
+  </si>
+  <si>
+    <t>1157 PATRIKA-CREAM</t>
+  </si>
+  <si>
+    <t>1158 PATRIKA-GOLDEN</t>
+  </si>
+  <si>
+    <t>1159 PATRIKA-WHITE</t>
+  </si>
+  <si>
+    <t>1160 PATRIKA-PINK</t>
+  </si>
+  <si>
+    <t>1161 PATRIKA (01)</t>
+  </si>
+  <si>
+    <t>1162 PATRIKA (02)</t>
+  </si>
+  <si>
+    <t>1163 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1164 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1165 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>1166 PATRIKA (DCU)</t>
   </si>
   <si>
     <t>1167 PATRIKA (DCU) BROWN</t>
@@ -416,109 +416,109 @@
     <t>2025- INVITAION (BOX) SAMPLES</t>
   </si>
   <si>
-    <t>2101 PATRIKA (L) (LUXYA - 51)</t>
-  </si>
-  <si>
-    <t>2102 PATRIKA *-* (M) (LUXYA - 52)</t>
-  </si>
-  <si>
-    <t>2103 PATRIKA (L) (LUXYA - 53)</t>
-  </si>
-  <si>
-    <t>2104 PATRIKA (LUXYA - 54)</t>
-  </si>
-  <si>
-    <t>2105 PATRIKA (LUXYA - 55)</t>
-  </si>
-  <si>
-    <t>2106 PATRIKA (L) (LUXYA - 56)</t>
-  </si>
-  <si>
-    <t>2107 PATRIKA *-* (M) (LUXYA - 57)</t>
-  </si>
-  <si>
-    <t>2108 PATRIKA *-* (M) (LUXYA - 59)</t>
-  </si>
-  <si>
-    <t>2109 PATRIKA (L) (LUXYA - 60)</t>
-  </si>
-  <si>
-    <t>2110 PATRIKA (LUXYA - 61)</t>
-  </si>
-  <si>
-    <t>2111 PATRIKA *-* (M) (LUXYA - 62)</t>
-  </si>
-  <si>
-    <t>2112 PATRIKA (L) (LEGACY - 01)</t>
-  </si>
-  <si>
-    <t>2113 PATRIKA (L) (LEGACY - 02)</t>
-  </si>
-  <si>
-    <t>2114 PATRIKA (L) (LEGACY - 03)</t>
-  </si>
-  <si>
-    <t>2115 PATRIKA (L) (LEGACY - 04)</t>
-  </si>
-  <si>
-    <t>2116 PATRIKA (L) (LEGACY - 05)</t>
-  </si>
-  <si>
-    <t>2117 PATRIKA *-* (M) (LEGACY - 06)</t>
-  </si>
-  <si>
-    <t>2118 PATRIKA (L) (LEGACY - 07)</t>
-  </si>
-  <si>
-    <t>2119 PATRIKA (L) (LEGACY - 08)</t>
-  </si>
-  <si>
-    <t>2120 PATRIKA (L) (LEGACY - 09)</t>
-  </si>
-  <si>
-    <t>2121 PATRIKA (LEGACY - 10)</t>
-  </si>
-  <si>
-    <t>2122 PATRIKA (LEGACY - 11)</t>
-  </si>
-  <si>
-    <t>2123 PATRIKA (LEGACY - 12)</t>
-  </si>
-  <si>
-    <t>2124 PATRIKA *-* (M) (LOTTERY - 71)</t>
-  </si>
-  <si>
-    <t>2125 PATRIKA *-* (M) (LOTTERY - 72)</t>
-  </si>
-  <si>
-    <t>2126 PATRIKA *-* (M) (LOTTERY - 73)</t>
-  </si>
-  <si>
-    <t>2127 PATRIKA *-* (M) (DCU) (LOTTERY - 74)</t>
-  </si>
-  <si>
-    <t>2128 PATRIKA *-* (M) (LOTTERY - 75)</t>
-  </si>
-  <si>
-    <t>2129 PATRIKA *-* (M) (DCU) (LOTTERY - 76)</t>
-  </si>
-  <si>
-    <t>2130 PATRIKA *-* (M) (LOTTERY - 77)</t>
-  </si>
-  <si>
-    <t>2131 PATRIKA *-* (M) (DCU) (LOTTERY - 78)</t>
-  </si>
-  <si>
-    <t>2132 PATRIKA *-* (M) (LOTTERY - 79)</t>
-  </si>
-  <si>
-    <t>2133 PATRIKA (LOTTERY - 80)</t>
-  </si>
-  <si>
-    <t>2134 PATRIKA *-* (M) (LOTTERY - 81)</t>
-  </si>
-  <si>
-    <t>2135 PATRIKA *-* (M) (LOTTERY - 82)</t>
+    <t>2101 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2102 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2103 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2104 PATRIKA</t>
+  </si>
+  <si>
+    <t>2105 PATRIKA</t>
+  </si>
+  <si>
+    <t>2106 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2107 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2108 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2109 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2110 PATRIKA</t>
+  </si>
+  <si>
+    <t>2111 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2112 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2113 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2114 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2115 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2116 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2117 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2118 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2119 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2120 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>2121 PATRIKA</t>
+  </si>
+  <si>
+    <t>2122 PATRIKA</t>
+  </si>
+  <si>
+    <t>2123 PATRIKA</t>
+  </si>
+  <si>
+    <t>2124 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2125 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2126 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2127 PATRIKA *-* (M) (DCU)</t>
+  </si>
+  <si>
+    <t>2128 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2129 PATRIKA *-* (M) (DCU)</t>
+  </si>
+  <si>
+    <t>2130 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2131 PATRIKA *-* (M) (DCU)</t>
+  </si>
+  <si>
+    <t>2132 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2133 PATRIKA</t>
+  </si>
+  <si>
+    <t>2134 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>2135 PATRIKA *-* (M)</t>
   </si>
   <si>
     <t>240 ENVELOPE</t>
@@ -542,1234 +542,1234 @@
     <t>330 ENVELOPE (B)</t>
   </si>
   <si>
-    <t>4251 PATRIKA (JC) (5342)</t>
-  </si>
-  <si>
-    <t>4252 PATRIKA (5207)</t>
-  </si>
-  <si>
-    <t>4253 PATRIKA (5206)</t>
-  </si>
-  <si>
-    <t>4254 PATRIKA (4210) (10273/10277)</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA - B (DCU) (AS-02 (B))</t>
-  </si>
-  <si>
-    <t>4255 PATRIKA (JC) (AS-02 (NEW))</t>
-  </si>
-  <si>
-    <t>4256 PATRIKA (JC) *-* (M) (1352 VV)</t>
-  </si>
-  <si>
-    <t>4257 PATRIKA (82)</t>
-  </si>
-  <si>
-    <t>4258 PATRIKA (JC) (1129)</t>
-  </si>
-  <si>
-    <t>4259 PATRIKA (JC) (101 SBC)</t>
-  </si>
-  <si>
-    <t>4260 PATRIKA (1102)</t>
-  </si>
-  <si>
-    <t>4261 PATRIKA (JC) (959)</t>
-  </si>
-  <si>
-    <t>4262 PATRIKA (JC) (S-201 GANESH JI)</t>
-  </si>
-  <si>
-    <t>4263 PATRIKA (JC) (2571)</t>
-  </si>
-  <si>
-    <t>4264 PATRIKA (DCU) (1351)</t>
-  </si>
-  <si>
-    <t>4265 PATRIKA (83)</t>
-  </si>
-  <si>
-    <t>4266 PATRIKA (25-145)</t>
-  </si>
-  <si>
-    <t>4267 PATRIKA (JC) (25-046)</t>
-  </si>
-  <si>
-    <t>4268 PATRIKA (JC) *-* (M+T) (S-296)</t>
-  </si>
-  <si>
-    <t>4269 PATRIKA (111 SBC)</t>
-  </si>
-  <si>
-    <t>4270 PATRIKA (1151 GGN)</t>
-  </si>
-  <si>
-    <t>4271 PATRIKA (JC) (25216)</t>
-  </si>
-  <si>
-    <t>4272 PATRIKA (JC) (1231 SBC CRM)</t>
-  </si>
-  <si>
-    <t>4273 PATRIKA (2547)</t>
-  </si>
-  <si>
-    <t>4274 PATRIKA (JC) (25369)</t>
-  </si>
-  <si>
-    <t>4275 PATRIKA (25367)</t>
-  </si>
-  <si>
-    <t>4276 PATRIKA (JC) *-* (M) (2632)</t>
-  </si>
-  <si>
-    <t>4277 PATRIKA (JC) *-* (M) (25365)</t>
-  </si>
-  <si>
-    <t>4278 PATRIKA (25368)</t>
-  </si>
-  <si>
-    <t>4279 PATRIKA (1031)</t>
-  </si>
-  <si>
-    <t>4280 PATRIKA (25301)</t>
-  </si>
-  <si>
-    <t>4281 PATRIKA (25312 MYRA)</t>
-  </si>
-  <si>
-    <t>4282 PATRIKA (3117)</t>
-  </si>
-  <si>
-    <t>4283 PATRIKA - B (YELLOW) (3116-YLW)</t>
-  </si>
-  <si>
-    <t>4283 PATRIKA (GOLDEN) (3116)</t>
-  </si>
-  <si>
-    <t>4284 PATRIKA (1173 VV)</t>
-  </si>
-  <si>
-    <t>4285 PATRIKA (JC) *-* (M) (4626)</t>
-  </si>
-  <si>
-    <t>4286 PATRIKA (5254  RJN)</t>
-  </si>
-  <si>
-    <t>4287 PATRIKA (25402)</t>
-  </si>
-  <si>
-    <t>4288 PATRIKA (10001 NEW)</t>
-  </si>
-  <si>
-    <t>4289 PATRIKA (10002 NEW)</t>
-  </si>
-  <si>
-    <t>4290 PATRIKA (316 MYRA)</t>
-  </si>
-  <si>
-    <t>4291 PATRIKA (25401)</t>
-  </si>
-  <si>
-    <t>4292 PATRIKA (25311)</t>
-  </si>
-  <si>
-    <t>4293 PATRIKA (25312)</t>
-  </si>
-  <si>
-    <t>4294 PATRIKA (5273)</t>
-  </si>
-  <si>
-    <t>4295 PATRIKA (286-A)</t>
-  </si>
-  <si>
-    <t>4296 PATRIKA (1407)</t>
-  </si>
-  <si>
-    <t>4297 PATRIKA (306)</t>
-  </si>
-  <si>
-    <t>4298 PATRIKA (5501)</t>
-  </si>
-  <si>
-    <t>4299 PATRIKA (2011)</t>
-  </si>
-  <si>
-    <t>4300 PATRIKA (25314)</t>
-  </si>
-  <si>
-    <t>4301 PATRIKA (25315)</t>
-  </si>
-  <si>
-    <t>4302 PATRIKA (DCU) (1402)</t>
-  </si>
-  <si>
-    <t>4303 PATRIKA (JC) (1234*-M)</t>
-  </si>
-  <si>
-    <t>4304 PATRIKA (5172)</t>
-  </si>
-  <si>
-    <t>4305 PATRIKA (25313)</t>
-  </si>
-  <si>
-    <t>4306 PATRIKA (JC) (427 LOTUS)</t>
-  </si>
-  <si>
-    <t>4307 PATRIKA (BALAJI 5202)</t>
-  </si>
-  <si>
-    <t>4308 PATRIKA (LOTUS 430)</t>
-  </si>
-  <si>
-    <t>4309 PATRIKA (DCU) (3751 Patta)</t>
-  </si>
-  <si>
-    <t>4310 PATRIKA (DCU) (3752 Swastik)</t>
-  </si>
-  <si>
-    <t>4311 PATRIKA (DCU) (251 KBC)</t>
-  </si>
-  <si>
-    <t>4312 PATRIKA (DCU) (273-A)</t>
-  </si>
-  <si>
-    <t>4313 PATRIKA (DCU) (RED- YELLOW PAN PATTA)</t>
-  </si>
-  <si>
-    <t>4314 PATRIKA (DCU) (RED-YELLOW SWASTIK)</t>
-  </si>
-  <si>
-    <t>4315 PATRIKA (DCU) (WHITE-PINK PAN PATA)</t>
-  </si>
-  <si>
-    <t>4316 PATRIKA (DCU) (WHITE -ORANGE PAN PATTA)</t>
-  </si>
-  <si>
-    <t>5051 PATRIKA *-* (M) (5087)</t>
-  </si>
-  <si>
-    <t>5052 PATRIKA (5295)</t>
-  </si>
-  <si>
-    <t>5053 PATRIKA (5213)</t>
-  </si>
-  <si>
-    <t>5054 PATRIKA *-* (M) (25/162)</t>
-  </si>
-  <si>
-    <t>5055 PATRIKA (25/272)</t>
-  </si>
-  <si>
-    <t>5056 PATRIKA (JC) (25/271)</t>
-  </si>
-  <si>
-    <t>5057 PATRIKA (25/171)</t>
-  </si>
-  <si>
-    <t>5058 PATRIKA (8802)</t>
-  </si>
-  <si>
-    <t>5059 PATRIKA (8803)</t>
-  </si>
-  <si>
-    <t>5060 PATRIKA (JC) (7713)</t>
-  </si>
-  <si>
-    <t>5061 PATRIKA (DCU) (1405)</t>
-  </si>
-  <si>
-    <t>5062 PATRIKA (7705)</t>
-  </si>
-  <si>
-    <t>5063 PATRIKA (2522 GE)</t>
-  </si>
-  <si>
-    <t>5064 PATRIKA (2517 GE)</t>
-  </si>
-  <si>
-    <t>5065 PATRIKA (2527)</t>
-  </si>
-  <si>
-    <t>5066 PATRIKA (2536)</t>
-  </si>
-  <si>
-    <t>5067 PATRIKA (JC) (S-301)</t>
-  </si>
-  <si>
-    <t>5068 PATRIKA (DCU) (S-305)</t>
-  </si>
-  <si>
-    <t>5069 PATRIKA (JC) (1103)</t>
-  </si>
-  <si>
-    <t>5070 PATRIKA (JC) (2156  YELLOW)</t>
-  </si>
-  <si>
-    <t>5071 PATRIKA *-* (डोरी) (741)</t>
-  </si>
-  <si>
-    <t>5072 PATRIKA (5347 DIRECT)</t>
-  </si>
-  <si>
-    <t>5073 PATRIKA *-* (M) (3161)</t>
-  </si>
-  <si>
-    <t>5074 PATRIKA (1151 VV)</t>
-  </si>
-  <si>
-    <t>5075 PATRIKA (JC) (25-082)</t>
-  </si>
-  <si>
-    <t>5076 PATRIKA (JC) (3701 SBC)</t>
-  </si>
-  <si>
-    <t>5077 PATRIKA (2081)</t>
-  </si>
-  <si>
-    <t>5078 PATRIKA (DCU) (2156 CREAM)</t>
-  </si>
-  <si>
-    <t>5079 PATRIKA (296-A (NEHA)</t>
-  </si>
-  <si>
-    <t>5080 PATRIKA (2501 GE NEW)</t>
-  </si>
-  <si>
-    <t>5081 PATRIKA (2520 GE)</t>
-  </si>
-  <si>
-    <t>5083 PATRIKA (5267)</t>
-  </si>
-  <si>
-    <t>5084 PATRIKA (5258 RJ)</t>
-  </si>
-  <si>
-    <t>5085 PATRIKA (2023)</t>
-  </si>
-  <si>
-    <t>5086 PATRIKA (JC) *-* (M+D) (942)</t>
-  </si>
-  <si>
-    <t>5087 PATRIKA (JC) (2206)</t>
-  </si>
-  <si>
-    <t>5088 PATRIKA (25214)</t>
-  </si>
-  <si>
-    <t>5089 PATRIKA (2061 SBC)</t>
-  </si>
-  <si>
-    <t>5090 PATRIKA (5236 RJ)</t>
-  </si>
-  <si>
-    <t>5091 PATRIKA (JC) (1411 KBC)</t>
-  </si>
-  <si>
-    <t>5092 PATRIKA (05 NAVIN BHAI)</t>
-  </si>
-  <si>
-    <t>5093 PATRIKA (5350)</t>
-  </si>
-  <si>
-    <t>5094 PATRIKA (5251)</t>
-  </si>
-  <si>
-    <t>5095 PATRIKA (5240)</t>
-  </si>
-  <si>
-    <t>5096 PATRIKA (25316)</t>
-  </si>
-  <si>
-    <t>5097 PATRIKA (25321)</t>
-  </si>
-  <si>
-    <t>5098 PATRIKA *-* (M) (31.12) (857)</t>
-  </si>
-  <si>
-    <t>5099 PATRIKA *-* (M) (852 DHANESH)</t>
-  </si>
-  <si>
-    <t>5100 PATRIKA (DCU) (5339)</t>
-  </si>
-  <si>
-    <t>5102 PATRIKA (5021) (2456)</t>
-  </si>
-  <si>
-    <t>5103 PATRIKA (2071)</t>
-  </si>
-  <si>
-    <t>5104 PATRIKA (5261 RJND)</t>
-  </si>
-  <si>
-    <t>5105 PATRIKA (JC) (5335)</t>
-  </si>
-  <si>
-    <t>5106 PATRIKA (253-A / 257-A)</t>
-  </si>
-  <si>
-    <t>5107 PATRIKA (5356 RJ)</t>
-  </si>
-  <si>
-    <t>5108 PATRIKA (5333)</t>
-  </si>
-  <si>
-    <t>5109 PATRIKA (5308)</t>
-  </si>
-  <si>
-    <t>5110 PATRIKA (JC) (AS-402)</t>
-  </si>
-  <si>
-    <t>5111 PATRIKA (JC) (5313)</t>
-  </si>
-  <si>
-    <t>5112 PATRIKA (JC) *-* (M) (25437)</t>
-  </si>
-  <si>
-    <t>5113 PATRIKA (5305)</t>
-  </si>
-  <si>
-    <t>5114 PATRIKA *-* (डोरी) (2091)</t>
-  </si>
-  <si>
-    <t>5115 PATRIKA (DCU) (5363 RJND)</t>
-  </si>
-  <si>
-    <t>5116 PATRIKA (2031)</t>
-  </si>
-  <si>
-    <t>5117 PATRIKA (DCU) (3331)</t>
-  </si>
-  <si>
-    <t>5118 PATRIKA (DCU) (25436)</t>
-  </si>
-  <si>
-    <t>5501 PATRIKA (DCU) (985 PISTA)</t>
-  </si>
-  <si>
-    <t>5502 PATRIKA *-* (M) (5355 NICE)</t>
-  </si>
-  <si>
-    <t>5503 PATRIKA (5186)</t>
-  </si>
-  <si>
-    <t>5504 PATRIKA (JC) (7033)</t>
-  </si>
-  <si>
-    <t>5505 PATRIKA (JC) *-* (M) (2282)</t>
-  </si>
-  <si>
-    <t>5506 PATRIKA *-* (M) (25/122)</t>
-  </si>
-  <si>
-    <t>5507 PATRIKA (JC) (8055 VV)</t>
-  </si>
-  <si>
-    <t>5508 PATRIKA (JC) (612 VV)</t>
-  </si>
-  <si>
-    <t>5509 PATRIKA (JC) (25/072)</t>
-  </si>
-  <si>
-    <t>5510 PATRIKA (JC) *-* (M) (AS-950)</t>
-  </si>
-  <si>
-    <t>5511 PATRIKA (JC) *-* (M) (2528)</t>
-  </si>
-  <si>
-    <t>5512 PATRIKA (JC) (2525 /2552)</t>
-  </si>
-  <si>
-    <t>5513 PATRIKA (2515)</t>
-  </si>
-  <si>
-    <t>5514 PATRIKA (2542)</t>
-  </si>
-  <si>
-    <t>5515 PATRIKA (2523)</t>
-  </si>
-  <si>
-    <t>5516 PATRIKA (JC) *-* (M) (5302 VV)</t>
-  </si>
-  <si>
-    <t>5517 PATRIKA *-* (M) (Patti Aayegi) (6301)</t>
-  </si>
-  <si>
-    <t>5518 PATRIKA (JC) *-* (M) (922)</t>
-  </si>
-  <si>
-    <t>5519 PATRIKA *-* (M) (7066)</t>
-  </si>
-  <si>
-    <t>5520 PATRIKA (1054)</t>
-  </si>
-  <si>
-    <t>5521 PATRIKA (JC) *-* (M) (35)</t>
-  </si>
-  <si>
-    <t>5522 PATRIKA (2231)</t>
-  </si>
-  <si>
-    <t>5523 PATRIKA (2232)</t>
-  </si>
-  <si>
-    <t>5524 PATRIKA (DCU) (5382)</t>
-  </si>
-  <si>
-    <t>5525 PATRIKA *-* (M) (5283)</t>
-  </si>
-  <si>
-    <t>5526 PATRIKA (DCU) (NEW LUSTER - 01)</t>
-  </si>
-  <si>
-    <t>5527 PATRIKA (DCU) (NEW LUSTER - 02)</t>
-  </si>
-  <si>
-    <t>5528 PATRIKA *-* (M) (NEW LUSTER - 03)</t>
-  </si>
-  <si>
-    <t>5529 PATRIKA *-* (M) (NEW LUSTER - 04)</t>
-  </si>
-  <si>
-    <t>5530 PATRIKA *-* (M) (NEW LUSTER - 05)</t>
-  </si>
-  <si>
-    <t>5531 PATRIKA (DCU) (NEW LUSTER - 06)</t>
-  </si>
-  <si>
-    <t>5532 PATRIKA *-* (M) (NEW LUSTER - 07)</t>
-  </si>
-  <si>
-    <t>5533 PATRIKA *-* (M) (NEW LUSTER - 08)</t>
-  </si>
-  <si>
-    <t>5534 PATRIKA *-* (M) (NEW LUSTER - 09)</t>
-  </si>
-  <si>
-    <t>5535 PATRIKA (JC) *-* (M) (1007)</t>
-  </si>
-  <si>
-    <t>5537 PATRIKA (JC) (25-052)</t>
-  </si>
-  <si>
-    <t>5538 PATRIKA (JC) *-* (M) (7073)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA-B (2942-B)</t>
-  </si>
-  <si>
-    <t>5539 PATRIKA (JC) (2942)</t>
-  </si>
-  <si>
-    <t>5540 PATRIKA *-* (M) (S-96)</t>
-  </si>
-  <si>
-    <t>5541 PATRIKA (JC) (2101)</t>
-  </si>
-  <si>
-    <t>5542 PATRIKA (2261)</t>
-  </si>
-  <si>
-    <t>5543 PATRIKA (2353)</t>
-  </si>
-  <si>
-    <t>5544 PATRIKA *-* (M) (2732)</t>
-  </si>
-  <si>
-    <t>5545 PATRIKA *-* (M) (2791)</t>
-  </si>
-  <si>
-    <t>5546 PATRIKA (718)</t>
-  </si>
-  <si>
-    <t>5547 PATRIKA *-* (M) (S-32)</t>
-  </si>
-  <si>
-    <t>5548 PATRIKA (DCU) (2792)</t>
-  </si>
-  <si>
-    <t>5549 PATRIKA (5261 NICE)</t>
-  </si>
-  <si>
-    <t>5550 PATRIKA *-* (M) (5424)</t>
-  </si>
-  <si>
-    <t>5551 PATRIKA (5231)</t>
-  </si>
-  <si>
-    <t>5552 PATRIKA (JC) *-* (M) (S-163)</t>
-  </si>
-  <si>
-    <t>5553 PATRIKA *-* (M) (5004)</t>
-  </si>
-  <si>
-    <t>5554 PATRIKA *-* (F/G) (5379)</t>
-  </si>
-  <si>
-    <t>5555 PATRIKA (2903)</t>
-  </si>
-  <si>
-    <t>5556 PATRIKA *-* (M) (2952)</t>
-  </si>
-  <si>
-    <t>5557 PATRIKA (2312 SBC)</t>
-  </si>
-  <si>
-    <t>5558 PATRIKA *-* (M) (121 NEHA)</t>
-  </si>
-  <si>
-    <t>5559 PATRIKA (2293)</t>
-  </si>
-  <si>
-    <t>5560 PATRIKA (F/G) *-* (2915)</t>
-  </si>
-  <si>
-    <t>5561 PATRIKA *-* (M) (25358)</t>
-  </si>
-  <si>
-    <t>5562 PATRIKA *-* (M) (114-B (NEHA))</t>
-  </si>
-  <si>
-    <t>5563 PATRIKA (5387)</t>
-  </si>
-  <si>
-    <t>5564 PATRIKA (JC) *-* (M) (S-107)</t>
-  </si>
-  <si>
-    <t>5565 PATRIKA (175)</t>
-  </si>
-  <si>
-    <t>5566 PATRIKA *-* (M) (1742-B)</t>
-  </si>
-  <si>
-    <t>5567 PATRIKA (1679)</t>
-  </si>
-  <si>
-    <t>5568 PATRIKA *-* (M) (3002)</t>
-  </si>
-  <si>
-    <t>5569 PATRIKA *-* (M) (S-39)</t>
-  </si>
-  <si>
-    <t>5570 PATRIKA *-* (M) (S-74)</t>
-  </si>
-  <si>
-    <t>5571 PATRIKA *-* (M) (25353)</t>
-  </si>
-  <si>
-    <t>5572 PATRIKA *-* (M) (25351)</t>
-  </si>
-  <si>
-    <t>5573 PATRIKA (2205)</t>
-  </si>
-  <si>
-    <t>5574 PATRIKA (25335)</t>
-  </si>
-  <si>
-    <t>5575 PATRIKA *-* (M) (S-77)</t>
-  </si>
-  <si>
-    <t>5576 PATRIKA (2531)</t>
-  </si>
-  <si>
-    <t>5577 PATRIKA *-* (M) (5808)</t>
-  </si>
-  <si>
-    <t>5578 PATRIKA (JC) *-* (M) (AS-104 / S-50)</t>
-  </si>
-  <si>
-    <t>5579 PATRIKA (JC) *-* (M) (AS-102)</t>
-  </si>
-  <si>
-    <t>5580 PATRIKA (S-326)</t>
-  </si>
-  <si>
-    <t>5581 PATRIKA *-* (M) (3471)</t>
-  </si>
-  <si>
-    <t>5582 PATRIKA *-* (M) (3512 SBC)</t>
-  </si>
-  <si>
-    <t>5583 PATRIKA (3211 SBC)</t>
-  </si>
-  <si>
-    <t>5584 PATRIKA (JC) (2202 SBC)</t>
-  </si>
-  <si>
-    <t>5585 PATRIKA *-* (M) (1201 KBC)</t>
-  </si>
-  <si>
-    <t>5586 PATRIKA *-* (M) (S-51)</t>
-  </si>
-  <si>
-    <t>5587 PATRIKA (2264)</t>
-  </si>
-  <si>
-    <t>5588 PATRIKA (JC) *-* (M) (1006)</t>
-  </si>
-  <si>
-    <t>5589 PATRIKA *-* (M) (25133)</t>
-  </si>
-  <si>
-    <t>5590 PATRIKA (3131 SBC)</t>
-  </si>
-  <si>
-    <t>5591 PATRIKA (DCU) (3735 YLW)</t>
-  </si>
-  <si>
-    <t>5592 PATRIKA *-* (M) (2365)</t>
-  </si>
-  <si>
-    <t>5593 PATRIKA (2803)</t>
-  </si>
-  <si>
-    <t>5594 PATRIKA (JC) (2931)</t>
-  </si>
-  <si>
-    <t>5595 PATRIKA *-* (M) (226)</t>
-  </si>
-  <si>
-    <t>5596 PATRIKA *-* (M) (2541)</t>
-  </si>
-  <si>
-    <t>5597 PATRIKA (JC) *-* (M) (AS-104 (B))</t>
-  </si>
-  <si>
-    <t>5599 PATRIKA *-* (M) (77-B)</t>
-  </si>
-  <si>
-    <t>5600 PATRIKA (JC) (25324)</t>
-  </si>
-  <si>
-    <t>5601 PATRIKA (2771)</t>
-  </si>
-  <si>
-    <t>5602 PATRIKA (3271)</t>
-  </si>
-  <si>
-    <t>5603 PATRIKA *-* (M) (6125)</t>
-  </si>
-  <si>
-    <t>5604 PATRIKA (242-A)</t>
-  </si>
-  <si>
-    <t>5605 PATRIKA (JC) (3102)</t>
-  </si>
-  <si>
-    <t>5606 PATRIKA *-* (M) (221-A)</t>
-  </si>
-  <si>
-    <t>5607 PATRIKA (25442)</t>
-  </si>
-  <si>
-    <t>5608 PATRIKA (25440)</t>
-  </si>
-  <si>
-    <t>5609 PATRIKA (993)</t>
-  </si>
-  <si>
-    <t>5610 PATRIKA (JC) (2373)</t>
-  </si>
-  <si>
-    <t>5611 PATRIKA *-* (M) (1211)</t>
-  </si>
-  <si>
-    <t>5612 PATRIKA (DCU) (5276)</t>
-  </si>
-  <si>
-    <t>5613 PATRIKA (JC) (DC) (1841-A)</t>
-  </si>
-  <si>
-    <t>5614 PATRIKA *-* (M) (2331)</t>
-  </si>
-  <si>
-    <t>5615 PATRIKA (2111)</t>
-  </si>
-  <si>
-    <t>5616 PATRIKA (DCU) (7069)</t>
-  </si>
-  <si>
-    <t>5617 PATRIKA *-* (M) (7067)</t>
-  </si>
-  <si>
-    <t>5618 PATRIKA (JC) *-* (M) (S-52)</t>
-  </si>
-  <si>
-    <t>5619 PATRIKA (JC) (1131)</t>
-  </si>
-  <si>
-    <t>5620 PATRIKA (JC) (15)</t>
-  </si>
-  <si>
-    <t>5621 PATRIKA (JC) *-* (M) (5297)</t>
-  </si>
-  <si>
-    <t>5622 PATRIKA *-* (M) (25337)</t>
-  </si>
-  <si>
-    <t>5623 PATRIKA (064)</t>
-  </si>
-  <si>
-    <t>5624 PATRIKA (JC) (2753)</t>
-  </si>
-  <si>
-    <t>5625 PATRIKA (DCU) (772)</t>
-  </si>
-  <si>
-    <t>5626 PATRIKA (DCU) (FULL JALI)</t>
-  </si>
-  <si>
-    <t>5627 PATRIKA (DCU) (HALF JALI)</t>
-  </si>
-  <si>
-    <t>5628 PATRIKA (DCU) (GOL)</t>
-  </si>
-  <si>
-    <t>5629 PATRIKA (DCU) (9*5 X 6*5 PATTA)</t>
-  </si>
-  <si>
-    <t>5630 PATRIKA (DCU) (SATHIYA)</t>
-  </si>
-  <si>
-    <t>6601 PATRIKA (L) (5164)</t>
-  </si>
-  <si>
-    <t>6602 PATRIKA (5126)</t>
-  </si>
-  <si>
-    <t>6603 PATRIKA (5111)</t>
-  </si>
-  <si>
-    <t>6604 PATRIKA *-* (M) (5196)</t>
-  </si>
-  <si>
-    <t>6605 PATRIKA (5191)</t>
-  </si>
-  <si>
-    <t>6606 PATRIKA (*-*) R (3023)</t>
-  </si>
-  <si>
-    <t>6607 PATRIKA *-* (M) (0523)</t>
-  </si>
-  <si>
-    <t>6608 PATRIKA (95)</t>
-  </si>
-  <si>
-    <t>6609 PATRIKA *-* (M) (3053)</t>
-  </si>
-  <si>
-    <t>6610 PATRIKA *-* (M) (3019)</t>
-  </si>
-  <si>
-    <t>6611 PATRIKA (3017 VV)</t>
-  </si>
-  <si>
-    <t>6612 PATRIKA (3015)</t>
-  </si>
-  <si>
-    <t>6613 PATRIKA (25164)</t>
-  </si>
-  <si>
-    <t>6614 PATRIKA (DCU) (25131)</t>
-  </si>
-  <si>
-    <t>6615 PATRIKA *-* (M) (915 GAGAN)</t>
-  </si>
-  <si>
-    <t>6616 PATRIKA *-* (M) (911 GAGAN)</t>
-  </si>
-  <si>
-    <t>6617 PATRIKA *-* (M) (3422)</t>
-  </si>
-  <si>
-    <t>6618 PATRIKA *-* (M) (3423)</t>
-  </si>
-  <si>
-    <t>6619 PATRIKA *-* (M) (1193)</t>
-  </si>
-  <si>
-    <t>6620 PATRIKA *-* (M) (1045 GGN (PADDING))</t>
-  </si>
-  <si>
-    <t>6621 PATRIKA *-* (M) (300 01.01.26) (7108 (PADDING))</t>
-  </si>
-  <si>
-    <t>6622 PATRIKA *-* (M) (7259 (PADDING))</t>
-  </si>
-  <si>
-    <t>6623 PATRIKA (25184)</t>
-  </si>
-  <si>
-    <t>6624 PATRIKA *-* (M) (25135)</t>
-  </si>
-  <si>
-    <t>6625 PATRIKA *-* (M) (25116)</t>
-  </si>
-  <si>
-    <t>6626 PATRIKA *-* (M) (25161)</t>
-  </si>
-  <si>
-    <t>6627 PATRIKA *-* (M) (25111)</t>
-  </si>
-  <si>
-    <t>6628 PATRIKA *-* (M) (805 SBC)</t>
-  </si>
-  <si>
-    <t>6629 PATRIKA *-* (M) (812 NEW SBC)</t>
-  </si>
-  <si>
-    <t>6630 PATRIKA *-* (M) (5510 NICE)</t>
-  </si>
-  <si>
-    <t>6631 PATRIKA (DCU) (OLD AP ITEM)</t>
-  </si>
-  <si>
-    <t>6632 PATRIKA (DCU) (932)</t>
-  </si>
-  <si>
-    <t>6633 PATRIKA *-* (M) (7081 VP)</t>
-  </si>
-  <si>
-    <t>6634 PATRIKA (3562)</t>
-  </si>
-  <si>
-    <t>6635 PATRIKA *-* (M) (S-313)</t>
-  </si>
-  <si>
-    <t>6636 PATRIKA *-* (M) (25183)</t>
-  </si>
-  <si>
-    <t>6637 PATRIKA (25162 GE)</t>
-  </si>
-  <si>
-    <t>6638 PATRIKA *-* (M) (3014)</t>
-  </si>
-  <si>
-    <t>6639 PATRIKA (2291)</t>
-  </si>
-  <si>
-    <t>6639 PATRIKA (B) (2291-B)</t>
-  </si>
-  <si>
-    <t>6640 PATRIKA *-* (M) (5737 PADING)</t>
-  </si>
-  <si>
-    <t>6641 PATRIKA *-* (M) (5435)</t>
-  </si>
-  <si>
-    <t>6642 PATRIKA *-* (M) (5411 RJ)</t>
-  </si>
-  <si>
-    <t>6643 PATRIKA *-* (M) (25380)</t>
-  </si>
-  <si>
-    <t>6644 PATRIKA (DCU) (25132)</t>
-  </si>
-  <si>
-    <t>6645 PATRIKA *-* (M) (3031)</t>
-  </si>
-  <si>
-    <t>6646 PATRIKA *-* (M) (3034)</t>
-  </si>
-  <si>
-    <t>6647 PATRIKA *-* (M) (25382)</t>
-  </si>
-  <si>
-    <t>6648 PATRIKA *-* (M) (5011 (PADDING))</t>
-  </si>
-  <si>
-    <t>6649 PATRIKA *-* (M) (3402)</t>
-  </si>
-  <si>
-    <t>6650 PATRIKA *-* (M) (3431)</t>
-  </si>
-  <si>
-    <t>6651 PATRIKA (3421)</t>
-  </si>
-  <si>
-    <t>6652 PATRIKA *-* (M) (2764 SBC)</t>
-  </si>
-  <si>
-    <t>6653 PATRIKA *-* (M) (834 SBC NEW)</t>
-  </si>
-  <si>
-    <t>6654 PATRIKA *-* (M) (3461)</t>
-  </si>
-  <si>
-    <t>6655 PATRIKA *-* (M) (7129 (PADDING))</t>
-  </si>
-  <si>
-    <t>6656 PATRIKA (L) (7113 (PADDING))</t>
-  </si>
-  <si>
-    <t>6657 PATRIKA *-* (M) (563  DHANESH)</t>
-  </si>
-  <si>
-    <t>6658 PATRIKA *-* (M) (5319)</t>
-  </si>
-  <si>
-    <t>6659 PATRIKA (25193 (Padding))</t>
-  </si>
-  <si>
-    <t>6660 PATRIKA (25194 (Padding))</t>
-  </si>
-  <si>
-    <t>6661 PATRIKA *-* (M) (1281)</t>
-  </si>
-  <si>
-    <t>6662 PATRIKA (3424)</t>
-  </si>
-  <si>
-    <t>6663 PATRIKA (7103 (PADDING))</t>
-  </si>
-  <si>
-    <t>6664 PATRIKA *-* (M) (5823)</t>
-  </si>
-  <si>
-    <t>6665 PATRIKA *-* (M) (603 DHANESH)</t>
-  </si>
-  <si>
-    <t>6666 PATRIKA *-* (M) (DC) (1192 KBC)</t>
-  </si>
-  <si>
-    <t>6667 PATRIKA *-* (M) (1192 SBC)</t>
-  </si>
-  <si>
-    <t>6668 PATRIKA (DCU) (8102)</t>
-  </si>
-  <si>
-    <t>6669 PATRIKA (DCU) (6197)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA - B (M) (1868-B)</t>
-  </si>
-  <si>
-    <t>6670 PATRIKA *-* (M) (1868)</t>
-  </si>
-  <si>
-    <t>6671 PATRIKA *-* (M) (1872)</t>
-  </si>
-  <si>
-    <t>6672 PATRIKA *-* (M) (6132)</t>
-  </si>
-  <si>
-    <t>6673 PATRIKA (DCU) (6196)</t>
-  </si>
-  <si>
-    <t>6674 PATRIKA (DCU) (1503)</t>
-  </si>
-  <si>
-    <t>6675 PATRIKA *-* (M) (1282)</t>
-  </si>
-  <si>
-    <t>6676 PATRIKA (DCU) (533 KBC)</t>
-  </si>
-  <si>
-    <t>6677 PATRIKA (DCU) (25191 PADDING)</t>
-  </si>
-  <si>
-    <t>7265 PATRIKA (O.C.) (133)</t>
-  </si>
-  <si>
-    <t>7283 PATRIKA {F} (O.C.) (4148)</t>
-  </si>
-  <si>
-    <t>7287 PATRIKA (O.C.) (1522)</t>
-  </si>
-  <si>
-    <t>7288 PATRIKA (O.C.) (1178)</t>
-  </si>
-  <si>
-    <t>7293 PATRIKA (O.C.) (AS-20)</t>
-  </si>
-  <si>
-    <t>7309 PATRIKA (O.C.) (4087)</t>
-  </si>
-  <si>
-    <t>7312 PATRIKA (O.C.) (SBC 7312)</t>
-  </si>
-  <si>
-    <t>7319 PATRIKA (O.C.) (2204)</t>
-  </si>
-  <si>
-    <t>7332 PATRIKA (O.C.) (2482)</t>
-  </si>
-  <si>
-    <t>7342 PATRIKA (O.C.) (12)</t>
-  </si>
-  <si>
-    <t>7344 PATRIKA (O.C.) (INV B.P. RED (11))</t>
-  </si>
-  <si>
-    <t>7345 PATRIKA (O.C.) (INV B.P. GOLDEN (120) 5)</t>
-  </si>
-  <si>
-    <t>7401 PATRIKA (25/252)</t>
-  </si>
-  <si>
-    <t>7402 PATRIKA (25/264-263)</t>
-  </si>
-  <si>
-    <t>7403 PATRIKA (25/363/863)</t>
-  </si>
-  <si>
-    <t>7404 PATRIKA (25/283)</t>
-  </si>
-  <si>
-    <t>7405 PATRIKA (25/273)</t>
-  </si>
-  <si>
-    <t>7406 PATRIKA (25/172)</t>
-  </si>
-  <si>
-    <t>7407 PATRIKA *-* (F) (7145 VP)</t>
-  </si>
-  <si>
-    <t>7408 PATRIKA (DCU) (25895)</t>
-  </si>
-  <si>
-    <t>7409 PATRIKA (2521)</t>
-  </si>
-  <si>
-    <t>7410 PATRIKA (2526)</t>
-  </si>
-  <si>
-    <t>7411 PATRIKA (2535)</t>
-  </si>
-  <si>
-    <t>7412 PATRIKA (84)</t>
-  </si>
-  <si>
-    <t>7413 PATRIKA (2543 INV OFFSET)</t>
-  </si>
-  <si>
-    <t>7414 PATRIKA (1015 GREEN OFFSET)</t>
-  </si>
-  <si>
-    <t>7415 PATRIKA *-* (F) (3162 SBC)</t>
-  </si>
-  <si>
-    <t>7416 PATRIKA (2234)</t>
-  </si>
-  <si>
-    <t>7417 PATRIKA (S-201 INV)</t>
-  </si>
-  <si>
-    <t>7418 PATRIKA *-* (डोरी) (1639)</t>
-  </si>
-  <si>
-    <t>7419 PATRIKA (5121)</t>
-  </si>
-  <si>
-    <t>7420 PATRIKA (720)</t>
-  </si>
-  <si>
-    <t>7421 PATRIKA *-* (F) (25-146)</t>
-  </si>
-  <si>
-    <t>7422 PATRIKA (3702)</t>
-  </si>
-  <si>
-    <t>7423 PATRIKA (254 SBC)</t>
-  </si>
-  <si>
-    <t>7424 PATRIKA *-* (F) (25-047)</t>
-  </si>
-  <si>
-    <t>7425 PATRIKA (2082)</t>
-  </si>
-  <si>
-    <t>7426 PATRIKA (F/G) *-* (4052)</t>
-  </si>
-  <si>
-    <t>7427 PATRIKA (2103)</t>
-  </si>
-  <si>
-    <t>7428 PATRIKA (1223 SBC)</t>
-  </si>
-  <si>
-    <t>7429 PATRIKA (F/G) *-* (1851 MONARCH)</t>
-  </si>
-  <si>
-    <t>7430 PATRIKA (6310 GE)</t>
-  </si>
-  <si>
-    <t>7431 PATRIKA (2532)</t>
-  </si>
-  <si>
-    <t>7432 PATRIKA (1174)</t>
-  </si>
-  <si>
-    <t>7433 PATRIKA (1034)</t>
-  </si>
-  <si>
-    <t>7434 PATRIKA (2204 INV)</t>
-  </si>
-  <si>
-    <t>7435 PATRIKA (06)</t>
-  </si>
-  <si>
-    <t>7436 PATRIKA (303)</t>
-  </si>
-  <si>
-    <t>7437 PATRIKA (25323 INV)</t>
-  </si>
-  <si>
-    <t>7438 PATRIKA (25413)</t>
-  </si>
-  <si>
-    <t>7439 PATRIKA (2597)</t>
-  </si>
-  <si>
-    <t>7440 PATRIKA (25896)</t>
-  </si>
-  <si>
-    <t>7441 PATRIKA *-* (F) (243-C)</t>
-  </si>
-  <si>
-    <t>7442 PATRIKA (1855)</t>
-  </si>
-  <si>
-    <t>7443 PATRIKA (1044 SBC)</t>
-  </si>
-  <si>
-    <t>7444 PATRIKA (2014)</t>
-  </si>
-  <si>
-    <t>7445 PATRIKA (2006)</t>
-  </si>
-  <si>
-    <t>7446 PATRIKA (DCU) (6106)</t>
-  </si>
-  <si>
-    <t>7447 PATRIKA (GOPAL 32)</t>
-  </si>
-  <si>
-    <t>7448 PATRIKA (2005- G)</t>
-  </si>
-  <si>
-    <t>7449 PATRIKA (5180)</t>
-  </si>
-  <si>
-    <t>7450 PATRIKA (DCU) (3753)</t>
-  </si>
-  <si>
-    <t>7451 PATRIKA (273 NEHA)</t>
-  </si>
-  <si>
-    <t>7452 PATRIKA (278-B)</t>
-  </si>
-  <si>
-    <t>7453 PATRIKA (ECO - 61) (NEW ECO 61)</t>
-  </si>
-  <si>
-    <t>7454 PATRIKA (ECO -63) (NEW ECO 63)</t>
+    <t>4251 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4252 PATRIKA</t>
+  </si>
+  <si>
+    <t>4253 PATRIKA</t>
+  </si>
+  <si>
+    <t>4254 PATRIKA (4210)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA - B (DCU)</t>
+  </si>
+  <si>
+    <t>4255 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4256 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4257 PATRIKA</t>
+  </si>
+  <si>
+    <t>4258 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4259 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4260 PATRIKA</t>
+  </si>
+  <si>
+    <t>4261 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4262 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4263 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4264 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4265 PATRIKA</t>
+  </si>
+  <si>
+    <t>4266 PATRIKA</t>
+  </si>
+  <si>
+    <t>4267 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4268 PATRIKA (JC) *-* (M+T)</t>
+  </si>
+  <si>
+    <t>4269 PATRIKA</t>
+  </si>
+  <si>
+    <t>4270 PATRIKA</t>
+  </si>
+  <si>
+    <t>4271 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4272 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4273 PATRIKA</t>
+  </si>
+  <si>
+    <t>4274 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4275 PATRIKA</t>
+  </si>
+  <si>
+    <t>4276 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4277 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4278 PATRIKA</t>
+  </si>
+  <si>
+    <t>4279 PATRIKA</t>
+  </si>
+  <si>
+    <t>4280 PATRIKA</t>
+  </si>
+  <si>
+    <t>4281 PATRIKA</t>
+  </si>
+  <si>
+    <t>4282 PATRIKA</t>
+  </si>
+  <si>
+    <t>4283 PATRIKA - B (YELLOW)</t>
+  </si>
+  <si>
+    <t>4283 PATRIKA (GOLDEN)</t>
+  </si>
+  <si>
+    <t>4284 PATRIKA</t>
+  </si>
+  <si>
+    <t>4285 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>4286 PATRIKA</t>
+  </si>
+  <si>
+    <t>4287 PATRIKA</t>
+  </si>
+  <si>
+    <t>4288 PATRIKA</t>
+  </si>
+  <si>
+    <t>4289 PATRIKA</t>
+  </si>
+  <si>
+    <t>4290 PATRIKA</t>
+  </si>
+  <si>
+    <t>4291 PATRIKA</t>
+  </si>
+  <si>
+    <t>4292 PATRIKA</t>
+  </si>
+  <si>
+    <t>4293 PATRIKA</t>
+  </si>
+  <si>
+    <t>4294 PATRIKA</t>
+  </si>
+  <si>
+    <t>4295 PATRIKA</t>
+  </si>
+  <si>
+    <t>4296 PATRIKA</t>
+  </si>
+  <si>
+    <t>4297 PATRIKA</t>
+  </si>
+  <si>
+    <t>4298 PATRIKA</t>
+  </si>
+  <si>
+    <t>4299 PATRIKA</t>
+  </si>
+  <si>
+    <t>4300 PATRIKA</t>
+  </si>
+  <si>
+    <t>4301 PATRIKA</t>
+  </si>
+  <si>
+    <t>4302 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4303 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4304 PATRIKA</t>
+  </si>
+  <si>
+    <t>4305 PATRIKA</t>
+  </si>
+  <si>
+    <t>4306 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>4307 PATRIKA</t>
+  </si>
+  <si>
+    <t>4308 PATRIKA</t>
+  </si>
+  <si>
+    <t>4309 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4310 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4311 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4312 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4313 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4314 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4315 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>4316 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5051 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5052 PATRIKA</t>
+  </si>
+  <si>
+    <t>5053 PATRIKA</t>
+  </si>
+  <si>
+    <t>5054 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5055 PATRIKA</t>
+  </si>
+  <si>
+    <t>5056 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5057 PATRIKA</t>
+  </si>
+  <si>
+    <t>5058 PATRIKA</t>
+  </si>
+  <si>
+    <t>5059 PATRIKA</t>
+  </si>
+  <si>
+    <t>5060 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5061 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5062 PATRIKA</t>
+  </si>
+  <si>
+    <t>5063 PATRIKA</t>
+  </si>
+  <si>
+    <t>5064 PATRIKA</t>
+  </si>
+  <si>
+    <t>5065 PATRIKA</t>
+  </si>
+  <si>
+    <t>5066 PATRIKA</t>
+  </si>
+  <si>
+    <t>5067 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5068 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5069 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5070 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5071 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5072 PATRIKA</t>
+  </si>
+  <si>
+    <t>5073 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5074 PATRIKA</t>
+  </si>
+  <si>
+    <t>5075 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5076 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5077 PATRIKA</t>
+  </si>
+  <si>
+    <t>5078 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5079 PATRIKA</t>
+  </si>
+  <si>
+    <t>5080 PATRIKA</t>
+  </si>
+  <si>
+    <t>5081 PATRIKA</t>
+  </si>
+  <si>
+    <t>5083 PATRIKA</t>
+  </si>
+  <si>
+    <t>5084 PATRIKA</t>
+  </si>
+  <si>
+    <t>5085 PATRIKA</t>
+  </si>
+  <si>
+    <t>5086 PATRIKA (JC) *-* (M+D)</t>
+  </si>
+  <si>
+    <t>5087 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5088 PATRIKA</t>
+  </si>
+  <si>
+    <t>5089 PATRIKA</t>
+  </si>
+  <si>
+    <t>5090 PATRIKA</t>
+  </si>
+  <si>
+    <t>5091 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5092 PATRIKA</t>
+  </si>
+  <si>
+    <t>5093 PATRIKA</t>
+  </si>
+  <si>
+    <t>5094 PATRIKA</t>
+  </si>
+  <si>
+    <t>5095 PATRIKA</t>
+  </si>
+  <si>
+    <t>5096 PATRIKA</t>
+  </si>
+  <si>
+    <t>5097 PATRIKA</t>
+  </si>
+  <si>
+    <t>5098 PATRIKA *-* (M) (31.12)</t>
+  </si>
+  <si>
+    <t>5099 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5100 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5102 PATRIKA (5021)</t>
+  </si>
+  <si>
+    <t>5103 PATRIKA</t>
+  </si>
+  <si>
+    <t>5104 PATRIKA</t>
+  </si>
+  <si>
+    <t>5105 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5106 PATRIKA</t>
+  </si>
+  <si>
+    <t>5107 PATRIKA</t>
+  </si>
+  <si>
+    <t>5108 PATRIKA</t>
+  </si>
+  <si>
+    <t>5109 PATRIKA</t>
+  </si>
+  <si>
+    <t>5110 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5111 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5112 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5113 PATRIKA</t>
+  </si>
+  <si>
+    <t>5114 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>5115 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5116 PATRIKA</t>
+  </si>
+  <si>
+    <t>5117 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5118 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5501 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5502 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5503 PATRIKA</t>
+  </si>
+  <si>
+    <t>5504 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5505 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5506 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5507 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5508 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5509 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5510 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5511 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5512 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5513 PATRIKA</t>
+  </si>
+  <si>
+    <t>5514 PATRIKA</t>
+  </si>
+  <si>
+    <t>5515 PATRIKA</t>
+  </si>
+  <si>
+    <t>5516 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5517 PATRIKA *-* (M) (Patti Aayegi)</t>
+  </si>
+  <si>
+    <t>5518 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5519 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5520 PATRIKA</t>
+  </si>
+  <si>
+    <t>5521 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5522 PATRIKA</t>
+  </si>
+  <si>
+    <t>5523 PATRIKA</t>
+  </si>
+  <si>
+    <t>5524 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5525 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5526 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5527 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5528 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5529 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5530 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5531 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5532 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5533 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5534 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5535 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5537 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5538 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA-B</t>
+  </si>
+  <si>
+    <t>5539 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5540 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5541 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5542 PATRIKA</t>
+  </si>
+  <si>
+    <t>5543 PATRIKA</t>
+  </si>
+  <si>
+    <t>5544 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5545 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5546 PATRIKA</t>
+  </si>
+  <si>
+    <t>5547 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5548 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5549 PATRIKA</t>
+  </si>
+  <si>
+    <t>5550 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5551 PATRIKA</t>
+  </si>
+  <si>
+    <t>5552 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5553 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5554 PATRIKA *-* (F/G)</t>
+  </si>
+  <si>
+    <t>5555 PATRIKA</t>
+  </si>
+  <si>
+    <t>5556 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5557 PATRIKA</t>
+  </si>
+  <si>
+    <t>5558 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5559 PATRIKA</t>
+  </si>
+  <si>
+    <t>5560 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>5561 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5562 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5563 PATRIKA</t>
+  </si>
+  <si>
+    <t>5564 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5565 PATRIKA</t>
+  </si>
+  <si>
+    <t>5566 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5567 PATRIKA</t>
+  </si>
+  <si>
+    <t>5568 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5569 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5570 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5571 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5572 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5573 PATRIKA</t>
+  </si>
+  <si>
+    <t>5574 PATRIKA</t>
+  </si>
+  <si>
+    <t>5575 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5576 PATRIKA</t>
+  </si>
+  <si>
+    <t>5577 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5578 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5579 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5580 PATRIKA</t>
+  </si>
+  <si>
+    <t>5581 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5582 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5583 PATRIKA</t>
+  </si>
+  <si>
+    <t>5584 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5585 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5586 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5587 PATRIKA</t>
+  </si>
+  <si>
+    <t>5588 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5589 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5590 PATRIKA</t>
+  </si>
+  <si>
+    <t>5591 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5592 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5593 PATRIKA</t>
+  </si>
+  <si>
+    <t>5594 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5595 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5596 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5597 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5599 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5600 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5601 PATRIKA</t>
+  </si>
+  <si>
+    <t>5602 PATRIKA</t>
+  </si>
+  <si>
+    <t>5603 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5604 PATRIKA</t>
+  </si>
+  <si>
+    <t>5605 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5606 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5607 PATRIKA</t>
+  </si>
+  <si>
+    <t>5608 PATRIKA</t>
+  </si>
+  <si>
+    <t>5609 PATRIKA</t>
+  </si>
+  <si>
+    <t>5610 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5611 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5612 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5613 PATRIKA (JC) (DC)</t>
+  </si>
+  <si>
+    <t>5614 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5615 PATRIKA</t>
+  </si>
+  <si>
+    <t>5616 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5618 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5619 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5620 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5621 PATRIKA (JC) *-* (M)</t>
+  </si>
+  <si>
+    <t>5622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>5623 PATRIKA</t>
+  </si>
+  <si>
+    <t>5624 PATRIKA (JC)</t>
+  </si>
+  <si>
+    <t>5625 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5626 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5627 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5628 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5629 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>5630 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6601 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6602 PATRIKA</t>
+  </si>
+  <si>
+    <t>6603 PATRIKA</t>
+  </si>
+  <si>
+    <t>6604 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6605 PATRIKA</t>
+  </si>
+  <si>
+    <t>6606 PATRIKA (*-*) R</t>
+  </si>
+  <si>
+    <t>6607 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6608 PATRIKA</t>
+  </si>
+  <si>
+    <t>6609 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6610 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6611 PATRIKA</t>
+  </si>
+  <si>
+    <t>6612 PATRIKA</t>
+  </si>
+  <si>
+    <t>6613 PATRIKA</t>
+  </si>
+  <si>
+    <t>6614 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6615 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6616 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6617 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6618 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6619 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6620 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6621 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6622 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6623 PATRIKA</t>
+  </si>
+  <si>
+    <t>6624 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6625 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6626 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6627 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6628 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6629 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6630 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6631 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6632 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6633 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6634 PATRIKA</t>
+  </si>
+  <si>
+    <t>6635 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6636 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6637 PATRIKA</t>
+  </si>
+  <si>
+    <t>6638 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6639 PATRIKA</t>
+  </si>
+  <si>
+    <t>6639 PATRIKA (B)</t>
+  </si>
+  <si>
+    <t>6640 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6641 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6642 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6643 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6644 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6645 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6646 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6647 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6648 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6649 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6650 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6651 PATRIKA</t>
+  </si>
+  <si>
+    <t>6652 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6653 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6654 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6655 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6656 PATRIKA (L)</t>
+  </si>
+  <si>
+    <t>6657 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6658 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6659 PATRIKA</t>
+  </si>
+  <si>
+    <t>6660 PATRIKA</t>
+  </si>
+  <si>
+    <t>6661 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6662 PATRIKA</t>
+  </si>
+  <si>
+    <t>6663 PATRIKA</t>
+  </si>
+  <si>
+    <t>6664 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6665 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6666 PATRIKA *-* (M) (DC)</t>
+  </si>
+  <si>
+    <t>6667 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6668 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6669 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA - B (M)</t>
+  </si>
+  <si>
+    <t>6670 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6671 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6672 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6673 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6674 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6675 PATRIKA *-* (M)</t>
+  </si>
+  <si>
+    <t>6676 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>6677 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7265 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7283 PATRIKA {F} (O.C.)</t>
+  </si>
+  <si>
+    <t>7287 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7288 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7293 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7309 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7312 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7319 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7332 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7342 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7344 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7345 PATRIKA (O.C.)</t>
+  </si>
+  <si>
+    <t>7401 PATRIKA</t>
+  </si>
+  <si>
+    <t>7402 PATRIKA</t>
+  </si>
+  <si>
+    <t>7403 PATRIKA</t>
+  </si>
+  <si>
+    <t>7404 PATRIKA</t>
+  </si>
+  <si>
+    <t>7405 PATRIKA</t>
+  </si>
+  <si>
+    <t>7406 PATRIKA</t>
+  </si>
+  <si>
+    <t>7407 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7408 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7409 PATRIKA</t>
+  </si>
+  <si>
+    <t>7410 PATRIKA</t>
+  </si>
+  <si>
+    <t>7411 PATRIKA</t>
+  </si>
+  <si>
+    <t>7412 PATRIKA</t>
+  </si>
+  <si>
+    <t>7413 PATRIKA</t>
+  </si>
+  <si>
+    <t>7414 PATRIKA</t>
+  </si>
+  <si>
+    <t>7415 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7416 PATRIKA</t>
+  </si>
+  <si>
+    <t>7417 PATRIKA</t>
+  </si>
+  <si>
+    <t>7418 PATRIKA *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>7419 PATRIKA</t>
+  </si>
+  <si>
+    <t>7420 PATRIKA</t>
+  </si>
+  <si>
+    <t>7421 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7422 PATRIKA</t>
+  </si>
+  <si>
+    <t>7423 PATRIKA</t>
+  </si>
+  <si>
+    <t>7424 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7425 PATRIKA</t>
+  </si>
+  <si>
+    <t>7426 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7427 PATRIKA</t>
+  </si>
+  <si>
+    <t>7428 PATRIKA</t>
+  </si>
+  <si>
+    <t>7429 PATRIKA (F/G) *-*</t>
+  </si>
+  <si>
+    <t>7430 PATRIKA</t>
+  </si>
+  <si>
+    <t>7431 PATRIKA</t>
+  </si>
+  <si>
+    <t>7432 PATRIKA</t>
+  </si>
+  <si>
+    <t>7433 PATRIKA</t>
+  </si>
+  <si>
+    <t>7434 PATRIKA</t>
+  </si>
+  <si>
+    <t>7435 PATRIKA</t>
+  </si>
+  <si>
+    <t>7436 PATRIKA</t>
+  </si>
+  <si>
+    <t>7437 PATRIKA</t>
+  </si>
+  <si>
+    <t>7438 PATRIKA</t>
+  </si>
+  <si>
+    <t>7439 PATRIKA</t>
+  </si>
+  <si>
+    <t>7440 PATRIKA</t>
+  </si>
+  <si>
+    <t>7441 PATRIKA *-* (F)</t>
+  </si>
+  <si>
+    <t>7442 PATRIKA</t>
+  </si>
+  <si>
+    <t>7443 PATRIKA</t>
+  </si>
+  <si>
+    <t>7444 PATRIKA</t>
+  </si>
+  <si>
+    <t>7445 PATRIKA</t>
+  </si>
+  <si>
+    <t>7446 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7447 PATRIKA</t>
+  </si>
+  <si>
+    <t>7448 PATRIKA</t>
+  </si>
+  <si>
+    <t>7449 PATRIKA</t>
+  </si>
+  <si>
+    <t>7450 PATRIKA (DCU)</t>
+  </si>
+  <si>
+    <t>7451 PATRIKA</t>
+  </si>
+  <si>
+    <t>7452 PATRIKA</t>
+  </si>
+  <si>
+    <t>7453 PATRIKA (ECO - 61)</t>
+  </si>
+  <si>
+    <t>7454 PATRIKA (ECO -63)</t>
   </si>
   <si>
     <t>7604 PATRIKA</t>
   </si>
   <si>
-    <t>9001 CARD (O.C.) (2498 Cream)</t>
+    <t>9001 CARD (O.C.)</t>
   </si>
   <si>
     <t>9221 CARDS - YELLOW</t>
@@ -1793,277 +1793,277 @@
     <t>9227 CARDS (9*5 OFFSET)</t>
   </si>
   <si>
-    <t>9228 CARDS (Y) (ORANGE WITH ONLY FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS - B (DCU) (GOLDEN WITH GANESH JI &amp; FOIL)</t>
-  </si>
-  <si>
-    <t>9229 CARDS (C) (CREAM WITH GANESH JI &amp; FOIL)</t>
+    <t>9228 CARDS (Y)</t>
+  </si>
+  <si>
+    <t>9229 CARDS - B (DCU)</t>
+  </si>
+  <si>
+    <t>9229 CARDS (C)</t>
   </si>
   <si>
     <t>9230 (CARD) 9*5 SCREEN</t>
   </si>
   <si>
-    <t>9231 CARDS (DCU) (RIYAZ 9*5 PINK)</t>
-  </si>
-  <si>
-    <t>9232 CARDS (DCU) (RIYAZ 9*5 CREAM)</t>
-  </si>
-  <si>
-    <t>9233 CARDS (DCU) (RIYAZ 9*5 YELLOW)</t>
-  </si>
-  <si>
-    <t>9234 CARDS (DCU) (RIYAZ 9*4 PINK)</t>
-  </si>
-  <si>
-    <t>9235 CARDS (DCU) (RIYAZ 9*4 CREAM)</t>
-  </si>
-  <si>
-    <t>9236 CARDS (DCU) (RIYAZ 9*4 YELLOW)</t>
-  </si>
-  <si>
-    <t>9237 CARDS (DCU) (DCU 9*4 RED)</t>
-  </si>
-  <si>
-    <t>9238 CARDS (DCU) (9*5 RED DCU)</t>
-  </si>
-  <si>
-    <t>9301 CARDS (4242)</t>
-  </si>
-  <si>
-    <t>9302 CARDS (5076)</t>
-  </si>
-  <si>
-    <t>9303 CARDS (5080 Pink)</t>
-  </si>
-  <si>
-    <t>9304 CARDS (5083 Blue)</t>
-  </si>
-  <si>
-    <t>9305 CARDS (9070) (4701 Nice)</t>
-  </si>
-  <si>
-    <t>9306 CARDS (0543 Nice)</t>
-  </si>
-  <si>
-    <t>9307 CARDS *-* (M) (5243 Nice)</t>
-  </si>
-  <si>
-    <t>9308 CARDS (9852)</t>
-  </si>
-  <si>
-    <t>9309 CARDS *-* (T) (9561 Vp)</t>
-  </si>
-  <si>
-    <t>9310 CARDS (3103)</t>
-  </si>
-  <si>
-    <t>9311 CARDS (3115)</t>
-  </si>
-  <si>
-    <t>9312 CARDS *-* (T) (208 VV)</t>
-  </si>
-  <si>
-    <t>9313 CARDS *-* (T) (216)</t>
-  </si>
-  <si>
-    <t>9314 CARDS (P-1)</t>
-  </si>
-  <si>
-    <t>9315 CARDS (DCU) (P-2)</t>
-  </si>
-  <si>
-    <t>9316 CARDS (DCU) (P-3)</t>
-  </si>
-  <si>
-    <t>9317 CARDS (P-4)</t>
-  </si>
-  <si>
-    <t>9318 CARDS (25905)</t>
-  </si>
-  <si>
-    <t>9319 CARDS (25906)</t>
-  </si>
-  <si>
-    <t>9320 CARDS (S-20)</t>
-  </si>
-  <si>
-    <t>9321 CARDS (22912 GANESH JI)</t>
-  </si>
-  <si>
-    <t>9322 CARDS *-* (M) - DC (22912 COMMON)</t>
-  </si>
-  <si>
-    <t>9323 CARDS (9005 OLD) (9*5 CREAM FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9324 CARDS (9*5 PINK FOIL NEW)</t>
-  </si>
-  <si>
-    <t>9325 CARDS (5229)</t>
-  </si>
-  <si>
-    <t>9326 CARDS (1601)</t>
-  </si>
-  <si>
-    <t>9327 CARDS (25908)</t>
-  </si>
-  <si>
-    <t>9328 CARDS (2543)</t>
-  </si>
-  <si>
-    <t>9329 CARDS (Desgin H/d) (3606)</t>
-  </si>
-  <si>
-    <t>9330 CARDS *-* (T) (9557)</t>
-  </si>
-  <si>
-    <t>9331 CARDS *-*  (T) (9560)</t>
-  </si>
-  <si>
-    <t>9332 CARDS (9847)</t>
-  </si>
-  <si>
-    <t>9333 CARDS (6042)</t>
-  </si>
-  <si>
-    <t>9334 CARDS (10X6 WHITE (2898))</t>
-  </si>
-  <si>
-    <t>9335 CARDS (9003 OLD) (9*5 WHITE)</t>
-  </si>
-  <si>
-    <t>9336 CARDS (2884)</t>
-  </si>
-  <si>
-    <t>9337 CARDS (1635 AP)</t>
-  </si>
-  <si>
-    <t>9338 CARDS (1637 AP)</t>
-  </si>
-  <si>
-    <t>9339 CARDS (5361)</t>
-  </si>
-  <si>
-    <t>9340 CARDS (5658)</t>
-  </si>
-  <si>
-    <t>9341 CARDS (5497)</t>
-  </si>
-  <si>
-    <t>9342 CARDS (2861)</t>
-  </si>
-  <si>
-    <t>9343 CARDS (9*5 WHTE GE HEAVY)</t>
-  </si>
-  <si>
-    <t>9344 CARDS (689)</t>
-  </si>
-  <si>
-    <t>9345 CARDS (358 KALYANI)</t>
-  </si>
-  <si>
-    <t>9346 CARDS (359)</t>
-  </si>
-  <si>
-    <t>9347 CARDS (2853)</t>
-  </si>
-  <si>
-    <t>9348 CARDS *-* (डोरी) (S-124)</t>
-  </si>
-  <si>
-    <t>9349 CARDS (W/o Window) (S-120)</t>
-  </si>
-  <si>
-    <t>9350 CARDS *-* (T) (1632)</t>
-  </si>
-  <si>
-    <t>9351 Card - B (1603 B)</t>
-  </si>
-  <si>
-    <t>9351 CARDS *-* (T) (1603)</t>
-  </si>
-  <si>
-    <t>9352 CARDS *-* (T) (1606 AP)</t>
-  </si>
-  <si>
-    <t>9353 CARDS (1618)</t>
-  </si>
-  <si>
-    <t>9354 CARDS (DCU) (345)</t>
-  </si>
-  <si>
-    <t>9355 CARDS (1624)</t>
-  </si>
-  <si>
-    <t>9356 CARDS (2895/2897)</t>
-  </si>
-  <si>
-    <t>9357 CARDS (2872)</t>
-  </si>
-  <si>
-    <t>9358 CARDS (WHITE PATTA)</t>
-  </si>
-  <si>
-    <t>9359 CARDS (PITCH PATTA)</t>
-  </si>
-  <si>
-    <t>9360 CARDS *-* (M) (GOL ANDA)</t>
-  </si>
-  <si>
-    <t>9361 CARDS (25426)</t>
-  </si>
-  <si>
-    <t>9362 CARDS (363)</t>
-  </si>
-  <si>
-    <t>9363 CARDS *-* (T) (1652)</t>
-  </si>
-  <si>
-    <t>9364 CARDS *-* (T) (1612)</t>
-  </si>
-  <si>
-    <t>9365 CARDS (25429)</t>
-  </si>
-  <si>
-    <t>9366 CARDS (25427 GOLDEN)</t>
-  </si>
-  <si>
-    <t>9367 CARDS (5652)</t>
-  </si>
-  <si>
-    <t>9368 CARDS (9*5 SET 25/26 GOLDEN (25425))</t>
-  </si>
-  <si>
-    <t>9369 CARDS (9*5 SET 25/26 YELLOW (25424))</t>
-  </si>
-  <si>
-    <t>9370 CARDS (9*5 SET 25/26 RED (25423))</t>
-  </si>
-  <si>
-    <t>9371 CARDS (3111 VP)</t>
-  </si>
-  <si>
-    <t>9372 CARDS (9*5 YLW SET (2841))</t>
-  </si>
-  <si>
-    <t>9373 CARDS (1482)</t>
-  </si>
-  <si>
-    <t>9374 CARDS (1485)</t>
-  </si>
-  <si>
-    <t>9375 CARDS (1452 WHITE)</t>
-  </si>
-  <si>
-    <t>9376 CARDS (1529 PRINCE)</t>
-  </si>
-  <si>
-    <t>9377 CARDS (DCU) (9*5 SET GREEN (009))</t>
-  </si>
-  <si>
-    <t>9378 CARDS (2892)</t>
+    <t>9231 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9232 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9233 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9234 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9235 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9236 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9237 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9238 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9301 CARDS</t>
+  </si>
+  <si>
+    <t>9302 CARDS</t>
+  </si>
+  <si>
+    <t>9303 CARDS</t>
+  </si>
+  <si>
+    <t>9304 CARDS</t>
+  </si>
+  <si>
+    <t>9305 CARDS (9070)</t>
+  </si>
+  <si>
+    <t>9306 CARDS</t>
+  </si>
+  <si>
+    <t>9307 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9308 CARDS</t>
+  </si>
+  <si>
+    <t>9309 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9310 CARDS</t>
+  </si>
+  <si>
+    <t>9311 CARDS</t>
+  </si>
+  <si>
+    <t>9312 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9313 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9314 CARDS</t>
+  </si>
+  <si>
+    <t>9315 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9316 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9317 CARDS</t>
+  </si>
+  <si>
+    <t>9318 CARDS</t>
+  </si>
+  <si>
+    <t>9319 CARDS</t>
+  </si>
+  <si>
+    <t>9320 CARDS</t>
+  </si>
+  <si>
+    <t>9321 CARDS</t>
+  </si>
+  <si>
+    <t>9322 CARDS *-* (M) - DC</t>
+  </si>
+  <si>
+    <t>9323 CARDS (9005 OLD)</t>
+  </si>
+  <si>
+    <t>9324 CARDS</t>
+  </si>
+  <si>
+    <t>9325 CARDS</t>
+  </si>
+  <si>
+    <t>9326 CARDS</t>
+  </si>
+  <si>
+    <t>9327 CARDS</t>
+  </si>
+  <si>
+    <t>9328 CARDS</t>
+  </si>
+  <si>
+    <t>9329 CARDS (Desgin H/d)</t>
+  </si>
+  <si>
+    <t>9330 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9331 CARDS *-*  (T)</t>
+  </si>
+  <si>
+    <t>9332 CARDS</t>
+  </si>
+  <si>
+    <t>9333 CARDS</t>
+  </si>
+  <si>
+    <t>9334 CARDS</t>
+  </si>
+  <si>
+    <t>9335 CARDS (9003 OLD)</t>
+  </si>
+  <si>
+    <t>9336 CARDS</t>
+  </si>
+  <si>
+    <t>9337 CARDS</t>
+  </si>
+  <si>
+    <t>9338 CARDS</t>
+  </si>
+  <si>
+    <t>9339 CARDS</t>
+  </si>
+  <si>
+    <t>9340 CARDS</t>
+  </si>
+  <si>
+    <t>9341 CARDS</t>
+  </si>
+  <si>
+    <t>9342 CARDS</t>
+  </si>
+  <si>
+    <t>9343 CARDS</t>
+  </si>
+  <si>
+    <t>9344 CARDS</t>
+  </si>
+  <si>
+    <t>9345 CARDS</t>
+  </si>
+  <si>
+    <t>9346 CARDS</t>
+  </si>
+  <si>
+    <t>9347 CARDS</t>
+  </si>
+  <si>
+    <t>9348 CARDS *-* (डोरी)</t>
+  </si>
+  <si>
+    <t>9349 CARDS (W/o Window)</t>
+  </si>
+  <si>
+    <t>9350 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9351 Card - B</t>
+  </si>
+  <si>
+    <t>9351 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9352 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9353 CARDS</t>
+  </si>
+  <si>
+    <t>9354 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9355 CARDS</t>
+  </si>
+  <si>
+    <t>9356 CARDS</t>
+  </si>
+  <si>
+    <t>9357 CARDS</t>
+  </si>
+  <si>
+    <t>9358 CARDS</t>
+  </si>
+  <si>
+    <t>9359 CARDS</t>
+  </si>
+  <si>
+    <t>9360 CARDS *-* (M)</t>
+  </si>
+  <si>
+    <t>9361 CARDS</t>
+  </si>
+  <si>
+    <t>9362 CARDS</t>
+  </si>
+  <si>
+    <t>9363 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9364 CARDS *-* (T)</t>
+  </si>
+  <si>
+    <t>9365 CARDS</t>
+  </si>
+  <si>
+    <t>9366 CARDS</t>
+  </si>
+  <si>
+    <t>9367 CARDS</t>
+  </si>
+  <si>
+    <t>9368 CARDS</t>
+  </si>
+  <si>
+    <t>9369 CARDS</t>
+  </si>
+  <si>
+    <t>9370 CARDS</t>
+  </si>
+  <si>
+    <t>9371 CARDS</t>
+  </si>
+  <si>
+    <t>9372 CARDS</t>
+  </si>
+  <si>
+    <t>9373 CARDS</t>
+  </si>
+  <si>
+    <t>9374 CARDS</t>
+  </si>
+  <si>
+    <t>9375 CARDS</t>
+  </si>
+  <si>
+    <t>9376 CARDS</t>
+  </si>
+  <si>
+    <t>9377 CARDS (DCU)</t>
+  </si>
+  <si>
+    <t>9378 CARDS</t>
   </si>
   <si>
     <t>9379 CARDS - R</t>
@@ -2096,19 +2096,19 @@
     <t>9388 CARDS (DCU)</t>
   </si>
   <si>
-    <t>9389 CARDS (9147 RJ)</t>
-  </si>
-  <si>
-    <t>9390 CARDS (DCU) (118KBC)</t>
+    <t>9389 CARDS</t>
+  </si>
+  <si>
+    <t>9390 CARDS (DCU)</t>
   </si>
   <si>
     <t>9391 CARDS</t>
   </si>
   <si>
-    <t>9*4 ENVELOPE (SBC) (CHOTA ENVELOPE (60/40 BILL))</t>
-  </si>
-  <si>
-    <t>9*5 ENVELOPE (FOIL) SBC (BADA ENVLP WITH FOIL (60/40 BILL))</t>
+    <t>9*4 ENVELOPE (SBC)</t>
+  </si>
+  <si>
+    <t>9*5 ENVELOPE (FOIL) SBC</t>
   </si>
   <si>
     <t>ACRYLIC NAME PLATE</t>
@@ -2126,7 +2126,7 @@
     <t>DEV SAMPLE SET</t>
   </si>
   <si>
-    <t>FANCY GIFT ENVELOPE-(SR) (SR ENVELOPES)</t>
+    <t>FANCY GIFT ENVELOPE-(SR)</t>
   </si>
   <si>
     <t>FANCY SAMPLE SET</t>
@@ -2147,34 +2147,34 @@
     <t>RIBBON (रिबीन)</t>
   </si>
   <si>
-    <t>RX-01 ENVELOPE (LX01)</t>
-  </si>
-  <si>
-    <t>RX-02 ENVELOPE (LX02)</t>
-  </si>
-  <si>
-    <t>RX-03 ENVELOPE (LX03)</t>
-  </si>
-  <si>
-    <t>RX-04 ENVELOPE (LX04)</t>
-  </si>
-  <si>
-    <t>RX-05 ENVELOPE (LX05)</t>
-  </si>
-  <si>
-    <t>RX-06 ENVELOPE (LX06)</t>
-  </si>
-  <si>
-    <t>RX-07 ENVELOPE (LX07)</t>
-  </si>
-  <si>
-    <t>RX-08 ENVELOPE (LX08)</t>
-  </si>
-  <si>
-    <t>RX-09 ENVELOPE (LX09)</t>
-  </si>
-  <si>
-    <t>गोल गणेश / गोल फ्लावर (GOL GANESH OR GOL FLOWER)</t>
+    <t>RX-01 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-02 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-03 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-04 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-05 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-06 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-07 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-08 ENVELOPE</t>
+  </si>
+  <si>
+    <t>RX-09 ENVELOPE</t>
+  </si>
+  <si>
+    <t>गोल गणेश / गोल फ्लावर</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -2707,7 +2707,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -3353,13 +3353,13 @@
         <v>13</v>
       </c>
       <c r="C42" s="25">
-        <v>1.5</v>
+        <v>109.5</v>
       </c>
       <c r="D42" s="26">
         <v>2.35</v>
       </c>
       <c r="E42" s="27">
-        <v>3.53</v>
+        <v>257.33</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3367,16 +3367,16 @@
         <v>45</v>
       </c>
       <c r="B43" s="24">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43" s="25">
-        <v>26.5</v>
+        <v>96</v>
       </c>
       <c r="D43" s="26">
         <v>2.35</v>
       </c>
       <c r="E43" s="27">
-        <v>62.28</v>
+        <v>225.6</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3469,16 +3469,16 @@
         <v>51</v>
       </c>
       <c r="B49" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C49" s="25">
-        <v>98.5</v>
+        <v>96.5</v>
       </c>
       <c r="D49" s="26">
         <v>1.4</v>
       </c>
       <c r="E49" s="27">
-        <v>137.9</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3839,16 +3839,16 @@
         <v>73</v>
       </c>
       <c r="B71" s="24">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C71" s="25">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D71" s="26">
         <v>1.4</v>
       </c>
       <c r="E71" s="27">
-        <v>270.2</v>
+        <v>264.60000000000002</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3873,16 +3873,16 @@
         <v>75</v>
       </c>
       <c r="B73" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C73" s="25">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="D73" s="26">
         <v>1.4</v>
       </c>
       <c r="E73" s="27">
-        <v>639.79999999999995</v>
+        <v>630</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3890,16 +3890,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="24">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C74" s="25">
-        <v>463.5</v>
+        <v>440.5</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>556.20000000000005</v>
+        <v>528.6</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3956,16 +3956,16 @@
         <v>80</v>
       </c>
       <c r="B78" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C78" s="25">
-        <v>585.5</v>
+        <v>580.5</v>
       </c>
       <c r="D78" s="26">
         <v>1.2</v>
       </c>
       <c r="E78" s="27">
-        <v>702.6</v>
+        <v>696.6</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3973,16 +3973,16 @@
         <v>81</v>
       </c>
       <c r="B79" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C79" s="25">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="D79" s="26">
         <v>1.2</v>
       </c>
       <c r="E79" s="27">
-        <v>796.8</v>
+        <v>784.8</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -4058,16 +4058,16 @@
         <v>86</v>
       </c>
       <c r="B84" s="24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C84" s="25">
-        <v>1817</v>
+        <v>1813</v>
       </c>
       <c r="D84" s="26">
         <v>1.3</v>
       </c>
       <c r="E84" s="27">
-        <v>2362.1</v>
+        <v>2356.9</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4075,16 +4075,16 @@
         <v>87</v>
       </c>
       <c r="B85" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C85" s="25">
-        <v>1603.5</v>
+        <v>1602.5</v>
       </c>
       <c r="D85" s="26">
         <v>1.3</v>
       </c>
       <c r="E85" s="27">
-        <v>2084.5500000000002</v>
+        <v>2083.25</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4143,16 +4143,16 @@
         <v>91</v>
       </c>
       <c r="B89" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C89" s="25">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D89" s="26">
         <v>1.37</v>
       </c>
       <c r="E89" s="27">
-        <v>334.95</v>
+        <v>330.83</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4177,16 +4177,16 @@
         <v>93</v>
       </c>
       <c r="B91" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C91" s="25">
-        <v>170.5</v>
+        <v>160.5</v>
       </c>
       <c r="D91" s="26">
         <v>0.66</v>
       </c>
       <c r="E91" s="27">
-        <v>113.35</v>
+        <v>106.7</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4730,16 +4730,16 @@
         <v>132</v>
       </c>
       <c r="B130" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C130" s="25">
-        <v>39.5</v>
+        <v>38.5</v>
       </c>
       <c r="D130" s="26">
         <v>12.5</v>
       </c>
       <c r="E130" s="27">
-        <v>493.75</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4980,13 +4980,13 @@
         <v>9</v>
       </c>
       <c r="C145" s="25">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="D145" s="26">
         <v>18.5</v>
       </c>
       <c r="E145" s="27">
-        <v>231.25</v>
+        <v>249.75</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -5232,16 +5232,16 @@
         <v>162</v>
       </c>
       <c r="B160" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C160" s="25">
-        <v>10.5</v>
+        <v>8.5</v>
       </c>
       <c r="D160" s="26">
         <v>11.5</v>
       </c>
       <c r="E160" s="27">
-        <v>120.75</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -5872,16 +5872,16 @@
         <v>202</v>
       </c>
       <c r="B200" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C200" s="25">
-        <v>124</v>
+        <v>122.5</v>
       </c>
       <c r="D200" s="26">
         <v>3.4</v>
       </c>
       <c r="E200" s="27">
-        <v>421.6</v>
+        <v>416.5</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5906,16 +5906,16 @@
         <v>204</v>
       </c>
       <c r="B202" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C202" s="25">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D202" s="26">
         <v>2.6</v>
       </c>
       <c r="E202" s="27">
-        <v>88.4</v>
+        <v>83.2</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -6172,16 +6172,16 @@
         <v>220</v>
       </c>
       <c r="B218" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C218" s="25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D218" s="26">
         <v>2.7</v>
       </c>
       <c r="E218" s="27">
-        <v>62.1</v>
+        <v>59.4</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -6291,16 +6291,16 @@
         <v>227</v>
       </c>
       <c r="B225" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C225" s="25">
-        <v>113</v>
+        <v>111.5</v>
       </c>
       <c r="D225" s="26">
         <v>3.96</v>
       </c>
       <c r="E225" s="27">
-        <v>447.13</v>
+        <v>441.19</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -6336,16 +6336,16 @@
         <v>230</v>
       </c>
       <c r="B228" s="24">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C228" s="25">
-        <v>47.5</v>
+        <v>43.5</v>
       </c>
       <c r="D228" s="26">
         <v>3.25</v>
       </c>
       <c r="E228" s="27">
-        <v>154.38</v>
+        <v>141.38</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6501,16 +6501,16 @@
         <v>241</v>
       </c>
       <c r="B239" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C239" s="25">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D239" s="26">
-        <v>5.75</v>
+        <v>5.76</v>
       </c>
       <c r="E239" s="27">
-        <v>11.5</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -6552,16 +6552,16 @@
         <v>244</v>
       </c>
       <c r="B242" s="24">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C242" s="25">
-        <v>30</v>
+        <v>27.5</v>
       </c>
       <c r="D242" s="26">
         <v>3</v>
       </c>
       <c r="E242" s="27">
-        <v>90</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6815,16 +6815,16 @@
         <v>261</v>
       </c>
       <c r="B259" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C259" s="25">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D259" s="26">
         <v>6.12</v>
       </c>
       <c r="E259" s="27">
-        <v>195.9</v>
+        <v>171.41</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -7469,16 +7469,16 @@
         <v>301</v>
       </c>
       <c r="B299" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C299" s="25">
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="D299" s="26">
         <v>4.75</v>
       </c>
       <c r="E299" s="27">
-        <v>97.38</v>
+        <v>83.13</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7798,16 +7798,16 @@
         <v>322</v>
       </c>
       <c r="B320" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C320" s="25">
-        <v>37.5</v>
+        <v>33.5</v>
       </c>
       <c r="D320" s="26">
         <v>6.75</v>
       </c>
       <c r="E320" s="27">
-        <v>253.13</v>
+        <v>226.13</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -7881,16 +7881,16 @@
         <v>327</v>
       </c>
       <c r="B325" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C325" s="25">
-        <v>199</v>
+        <v>193.5</v>
       </c>
       <c r="D325" s="26">
         <v>4.28</v>
       </c>
       <c r="E325" s="27">
-        <v>851.72</v>
+        <v>828.18</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -7994,16 +7994,16 @@
         <v>334</v>
       </c>
       <c r="B332" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C332" s="25">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="D332" s="26">
         <v>9</v>
       </c>
       <c r="E332" s="27">
-        <v>94.5</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -8610,16 +8610,16 @@
         <v>372</v>
       </c>
       <c r="B370" s="24">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C370" s="25">
-        <v>117.95</v>
+        <v>116.95</v>
       </c>
       <c r="D370" s="26">
         <v>4.5</v>
       </c>
       <c r="E370" s="27">
-        <v>530.78</v>
+        <v>526.28</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -9072,16 +9072,16 @@
         <v>400</v>
       </c>
       <c r="B398" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C398" s="25">
-        <v>43</v>
+        <v>39.5</v>
       </c>
       <c r="D398" s="26">
         <v>6.65</v>
       </c>
       <c r="E398" s="27">
-        <v>285.95</v>
+        <v>262.68</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -9089,16 +9089,16 @@
         <v>401</v>
       </c>
       <c r="B399" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C399" s="25">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D399" s="26">
         <v>7</v>
       </c>
       <c r="E399" s="27">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -9955,9 +9955,15 @@
       <c r="B453" s="24">
         <v>1</v>
       </c>
-      <c r="C453" s="28"/>
-      <c r="D453" s="29"/>
-      <c r="E453" s="28"/>
+      <c r="C453" s="25">
+        <v>3</v>
+      </c>
+      <c r="D453" s="26">
+        <v>28.5</v>
+      </c>
+      <c r="E453" s="27">
+        <v>85.5</v>
+      </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454" s="23" t="s">
@@ -10015,16 +10021,16 @@
         <v>459</v>
       </c>
       <c r="B457" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C457" s="25">
-        <v>13.5</v>
+        <v>13</v>
       </c>
       <c r="D457" s="26">
         <v>10.5</v>
       </c>
       <c r="E457" s="27">
-        <v>141.75</v>
+        <v>136.5</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
@@ -10232,16 +10238,16 @@
         <v>472</v>
       </c>
       <c r="B470" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C470" s="25">
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="D470" s="26">
         <v>9.5</v>
       </c>
       <c r="E470" s="27">
-        <v>85.5</v>
+        <v>61.75</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
@@ -11301,16 +11307,16 @@
         <v>537</v>
       </c>
       <c r="B535" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C535" s="25">
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="D535" s="26">
         <v>2.8</v>
       </c>
       <c r="E535" s="27">
-        <v>65.8</v>
+        <v>63</v>
       </c>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.25">
@@ -11590,16 +11596,16 @@
         <v>554</v>
       </c>
       <c r="B552" s="24">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C552" s="25">
-        <v>167.2</v>
+        <v>164.2</v>
       </c>
       <c r="D552" s="26">
         <v>3.9</v>
       </c>
       <c r="E552" s="27">
-        <v>652.08000000000004</v>
+        <v>640.38</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -12054,10 +12060,10 @@
         <v>582</v>
       </c>
       <c r="B580" s="24">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C580" s="25">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D580" s="29"/>
       <c r="E580" s="28"/>
@@ -12080,10 +12086,10 @@
         <v>584</v>
       </c>
       <c r="B582" s="24">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C582" s="25">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D582" s="29"/>
       <c r="E582" s="28"/>
@@ -12093,10 +12099,10 @@
         <v>585</v>
       </c>
       <c r="B583" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C583" s="25">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D583" s="29"/>
       <c r="E583" s="28"/>
@@ -12221,10 +12227,10 @@
         <v>593</v>
       </c>
       <c r="B591" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C591" s="25">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D591" s="29"/>
       <c r="E591" s="28"/>
@@ -12234,10 +12240,10 @@
         <v>594</v>
       </c>
       <c r="B592" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C592" s="25">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D592" s="29"/>
       <c r="E592" s="28"/>
@@ -12247,10 +12253,10 @@
         <v>595</v>
       </c>
       <c r="B593" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C593" s="25">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D593" s="29"/>
       <c r="E593" s="28"/>
@@ -12273,10 +12279,10 @@
         <v>597</v>
       </c>
       <c r="B595" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C595" s="25">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D595" s="29"/>
       <c r="E595" s="28"/>
@@ -12457,16 +12463,16 @@
         <v>609</v>
       </c>
       <c r="B607" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C607" s="25">
-        <v>19.5</v>
+        <v>17.5</v>
       </c>
       <c r="D607" s="26">
         <v>3.5</v>
       </c>
       <c r="E607" s="27">
-        <v>68.25</v>
+        <v>61.25</v>
       </c>
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
@@ -12593,16 +12599,16 @@
         <v>617</v>
       </c>
       <c r="B615" s="24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C615" s="25">
-        <v>44.5</v>
+        <v>42.5</v>
       </c>
       <c r="D615" s="26">
         <v>2.74</v>
       </c>
       <c r="E615" s="27">
-        <v>122.04</v>
+        <v>116.55</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12638,16 +12644,16 @@
         <v>620</v>
       </c>
       <c r="B618" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C618" s="25">
-        <v>41.5</v>
+        <v>39.5</v>
       </c>
       <c r="D618" s="26">
         <v>1.5</v>
       </c>
       <c r="E618" s="27">
-        <v>62.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12655,16 +12661,16 @@
         <v>621</v>
       </c>
       <c r="B619" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C619" s="25">
-        <v>10.5</v>
+        <v>7.5</v>
       </c>
       <c r="D619" s="26">
         <v>1.5</v>
       </c>
       <c r="E619" s="27">
-        <v>15.75</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12751,16 +12757,16 @@
         <v>627</v>
       </c>
       <c r="B625" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C625" s="25">
-        <v>31</v>
+        <v>29.5</v>
       </c>
       <c r="D625" s="26">
         <v>3</v>
       </c>
       <c r="E625" s="27">
-        <v>93</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12785,16 +12791,16 @@
         <v>629</v>
       </c>
       <c r="B627" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C627" s="25">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="D627" s="26">
         <v>5</v>
       </c>
       <c r="E627" s="27">
-        <v>45</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -13321,16 +13327,16 @@
         <v>661</v>
       </c>
       <c r="B659" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C659" s="25">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D659" s="26">
         <v>3.75</v>
       </c>
       <c r="E659" s="27">
-        <v>9.3800000000000008</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.25">
@@ -13372,16 +13378,16 @@
         <v>664</v>
       </c>
       <c r="B662" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C662" s="25">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="D662" s="26">
         <v>5.75</v>
       </c>
       <c r="E662" s="27">
-        <v>23</v>
+        <v>8.6300000000000008</v>
       </c>
     </row>
     <row r="663" spans="1:5" x14ac:dyDescent="0.25">
@@ -13559,16 +13565,16 @@
         <v>675</v>
       </c>
       <c r="B673" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C673" s="25">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D673" s="26">
         <v>4.25</v>
       </c>
       <c r="E673" s="27">
-        <v>72.25</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="674" spans="1:5" x14ac:dyDescent="0.25">
@@ -13729,10 +13735,10 @@
         <v>687</v>
       </c>
       <c r="B685" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C685" s="25">
-        <v>49.5</v>
+        <v>48.5</v>
       </c>
       <c r="D685" s="29"/>
       <c r="E685" s="28"/>
@@ -14112,16 +14118,16 @@
         <v>714</v>
       </c>
       <c r="B712" s="24">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C712" s="25">
-        <v>57.75</v>
+        <v>52.75</v>
       </c>
       <c r="D712" s="26">
         <v>2.5</v>
       </c>
       <c r="E712" s="27">
-        <v>144.38</v>
+        <v>131.88</v>
       </c>
     </row>
     <row r="713" spans="1:5" x14ac:dyDescent="0.25">
@@ -14146,10 +14152,10 @@
         <v>716</v>
       </c>
       <c r="B714" s="24">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C714" s="25">
-        <v>-288</v>
+        <v>-291</v>
       </c>
       <c r="D714" s="29"/>
       <c r="E714" s="28"/>
@@ -14160,11 +14166,11 @@
       </c>
       <c r="B715" s="31"/>
       <c r="C715" s="32">
-        <v>40271.29</v>
+        <v>40262.79</v>
       </c>
       <c r="D715" s="33"/>
       <c r="E715" s="34">
-        <v>109474.43</v>
+        <v>109563.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RAJ 02 JAN @837
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="10215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="9300"/>
   </bookViews>
   <sheets>
     <sheet name="PATRIKA 25-26" sheetId="1" r:id="rId1"/>
@@ -1091,7 +1091,7 @@
     <t>5549 PATRIKA (5261 NICE)</t>
   </si>
   <si>
-    <t>5550 PATRIKA *-* (M) (5424)</t>
+    <t>5550 PATRIKA *-* (M) (08.01) (5424)</t>
   </si>
   <si>
     <t>5551 PATRIKA (5231)</t>
@@ -1382,7 +1382,7 @@
     <t>6617 PATRIKA *-* (M) (3422)</t>
   </si>
   <si>
-    <t>6618 PATRIKA *-* (M) (3423)</t>
+    <t>6618 PATRIKA *-* (M)''Dc''' (3423)</t>
   </si>
   <si>
     <t>6619 PATRIKA *-* (M) (1193)</t>
@@ -1391,7 +1391,7 @@
     <t>6620 PATRIKA *-* (M) (1045 GGN (PADDING))</t>
   </si>
   <si>
-    <t>6621 PATRIKA *-* (M) (7108 (PADDING))</t>
+    <t>6621 PATRIKA *-* (M) (ON ORDER) (7108 (PADDING))</t>
   </si>
   <si>
     <t>6622 PATRIKA *-* (M) (7259 (PADDING))</t>
@@ -1472,7 +1472,7 @@
     <t>6646 PATRIKA *-* (M) (3034)</t>
   </si>
   <si>
-    <t>6647 PATRIKA *-* (M) (25382)</t>
+    <t>6647 PATRIKA *-* (M) (07.01) (25382)</t>
   </si>
   <si>
     <t>6648 PATRIKA *-* (M) (5011 (PADDING))</t>
@@ -1895,7 +1895,7 @@
     <t>9322 CARDS *-* (M) - DC (22912 COMMON)</t>
   </si>
   <si>
-    <t>9323 CARDS (9005 OLD) (9*5 CREAM FOIL NEW)</t>
+    <t>9323 CARDS (9005 OLD) Aagay (9*5 CREAM FOIL NEW)</t>
   </si>
   <si>
     <t>9324 CARDS (9*5 PINK FOIL NEW)</t>
@@ -2832,13 +2832,13 @@
         <v>23</v>
       </c>
       <c r="C11" s="25">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="D11" s="26">
         <v>1.8</v>
       </c>
       <c r="E11" s="27">
-        <v>77.400000000000006</v>
+        <v>257.39999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2883,13 +2883,13 @@
         <v>33</v>
       </c>
       <c r="C14" s="25">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="D14" s="26">
         <v>2</v>
       </c>
       <c r="E14" s="27">
-        <v>156</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2900,13 +2900,13 @@
         <v>23</v>
       </c>
       <c r="C15" s="25">
-        <v>64.5</v>
+        <v>144.5</v>
       </c>
       <c r="D15" s="26">
         <v>2</v>
       </c>
       <c r="E15" s="27">
-        <v>129</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3050,16 +3050,16 @@
         <v>26</v>
       </c>
       <c r="B24" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24" s="25">
-        <v>43.5</v>
+        <v>38.5</v>
       </c>
       <c r="D24" s="26">
         <v>1.8</v>
       </c>
       <c r="E24" s="27">
-        <v>78.3</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3217,13 +3217,13 @@
         <v>7</v>
       </c>
       <c r="C34" s="25">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D34" s="26">
         <v>2.5</v>
       </c>
       <c r="E34" s="27">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3316,16 +3316,16 @@
         <v>42</v>
       </c>
       <c r="B40" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C40" s="25">
-        <v>55.5</v>
+        <v>50.5</v>
       </c>
       <c r="D40" s="26">
         <v>2.14</v>
       </c>
       <c r="E40" s="27">
-        <v>118.77</v>
+        <v>108.07</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3438,13 +3438,13 @@
         <v>16</v>
       </c>
       <c r="C47" s="25">
-        <v>27.5</v>
+        <v>143.5</v>
       </c>
       <c r="D47" s="26">
         <v>1.25</v>
       </c>
       <c r="E47" s="27">
-        <v>34.380000000000003</v>
+        <v>179.38</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,16 +3452,16 @@
         <v>50</v>
       </c>
       <c r="B48" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C48" s="25">
-        <v>0.5</v>
+        <v>98.5</v>
       </c>
       <c r="D48" s="26">
         <v>1.26</v>
       </c>
       <c r="E48" s="27">
-        <v>0.63</v>
+        <v>123.71</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3503,16 +3503,16 @@
         <v>53</v>
       </c>
       <c r="B51" s="24">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C51" s="25">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D51" s="26">
         <v>1.8</v>
       </c>
       <c r="E51" s="27">
-        <v>149.4</v>
+        <v>115.2</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3605,16 +3605,16 @@
         <v>59</v>
       </c>
       <c r="B57" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C57" s="25">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D57" s="26">
         <v>1.9</v>
       </c>
       <c r="E57" s="27">
-        <v>212.8</v>
+        <v>207.1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3656,16 +3656,16 @@
         <v>62</v>
       </c>
       <c r="B60" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C60" s="25">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D60" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E60" s="27">
-        <v>233.1</v>
+        <v>227.55</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3673,16 +3673,16 @@
         <v>63</v>
       </c>
       <c r="B61" s="24">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C61" s="25">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D61" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E61" s="27">
-        <v>215.34</v>
+        <v>204.24</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3722,16 +3722,16 @@
         <v>66</v>
       </c>
       <c r="B64" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C64" s="25">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D64" s="26">
         <v>1.65</v>
       </c>
       <c r="E64" s="27">
-        <v>150.15</v>
+        <v>146.85</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3856,16 +3856,16 @@
         <v>74</v>
       </c>
       <c r="B72" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C72" s="25">
-        <v>326</v>
+        <v>321.5</v>
       </c>
       <c r="D72" s="26">
         <v>1.4</v>
       </c>
       <c r="E72" s="27">
-        <v>456.4</v>
+        <v>450.1</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3890,16 +3890,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C74" s="25">
-        <v>440.5</v>
+        <v>436.5</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>528.6</v>
+        <v>523.79999999999995</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3907,16 +3907,16 @@
         <v>77</v>
       </c>
       <c r="B75" s="24">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C75" s="25">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="D75" s="26">
         <v>1.2</v>
       </c>
       <c r="E75" s="27">
-        <v>589.20000000000005</v>
+        <v>577.20000000000005</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4058,16 +4058,16 @@
         <v>86</v>
       </c>
       <c r="B84" s="24">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C84" s="25">
-        <v>1813</v>
+        <v>1806</v>
       </c>
       <c r="D84" s="26">
         <v>1.3</v>
       </c>
       <c r="E84" s="27">
-        <v>2356.9</v>
+        <v>2347.8000000000002</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4109,16 +4109,16 @@
         <v>89</v>
       </c>
       <c r="B87" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C87" s="25">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="D87" s="26">
         <v>1.7</v>
       </c>
       <c r="E87" s="27">
-        <v>10.199999999999999</v>
+        <v>-3.4</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4143,16 +4143,16 @@
         <v>91</v>
       </c>
       <c r="B89" s="24">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C89" s="25">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="D89" s="26">
         <v>1.37</v>
       </c>
       <c r="E89" s="27">
-        <v>330.83</v>
+        <v>299.26</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4557,10 +4557,10 @@
         <v>119</v>
       </c>
       <c r="B117" s="24">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C117" s="25">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="28"/>
@@ -4573,7 +4573,7 @@
         <v>270</v>
       </c>
       <c r="C118" s="25">
-        <v>-0.3</v>
+        <v>0.12</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="28"/>
@@ -4586,7 +4586,7 @@
         <v>288</v>
       </c>
       <c r="C119" s="25">
-        <v>-0.45</v>
+        <v>0.02</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="28"/>
@@ -4605,10 +4605,10 @@
         <v>123</v>
       </c>
       <c r="B121" s="24">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C121" s="25">
-        <v>-1.84</v>
+        <v>0.39</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="28"/>
@@ -4621,7 +4621,7 @@
         <v>242</v>
       </c>
       <c r="C122" s="25">
-        <v>-2.4300000000000002</v>
+        <v>0.11</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="28"/>
@@ -4696,16 +4696,16 @@
         <v>130</v>
       </c>
       <c r="B128" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C128" s="25">
-        <v>3.5</v>
+        <v>-2.5</v>
       </c>
       <c r="D128" s="26">
         <v>12.5</v>
       </c>
       <c r="E128" s="27">
-        <v>43.75</v>
+        <v>-31.25</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4909,16 +4909,16 @@
         <v>143</v>
       </c>
       <c r="B141" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C141" s="25">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="D141" s="26">
         <v>18.5</v>
       </c>
       <c r="E141" s="27">
-        <v>138.75</v>
+        <v>101.75</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4943,16 +4943,16 @@
         <v>145</v>
       </c>
       <c r="B143" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C143" s="25">
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="D143" s="26">
         <v>18.5</v>
       </c>
       <c r="E143" s="27">
-        <v>397.75</v>
+        <v>370</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4960,16 +4960,16 @@
         <v>146</v>
       </c>
       <c r="B144" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C144" s="25">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="D144" s="26">
         <v>18.5</v>
       </c>
       <c r="E144" s="27">
-        <v>175.75</v>
+        <v>157.25</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -5011,16 +5011,16 @@
         <v>149</v>
       </c>
       <c r="B147" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C147" s="25">
-        <v>7.5</v>
+        <v>0.5</v>
       </c>
       <c r="D147" s="26">
         <v>18.5</v>
       </c>
       <c r="E147" s="27">
-        <v>138.75</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -5028,16 +5028,16 @@
         <v>150</v>
       </c>
       <c r="B148" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C148" s="25">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="D148" s="26">
         <v>18.5</v>
       </c>
       <c r="E148" s="27">
-        <v>129.5</v>
+        <v>83.25</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -5079,16 +5079,16 @@
         <v>153</v>
       </c>
       <c r="B151" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C151" s="25">
-        <v>5.5</v>
+        <v>0.5</v>
       </c>
       <c r="D151" s="26">
         <v>11.5</v>
       </c>
       <c r="E151" s="27">
-        <v>63.25</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -5345,16 +5345,16 @@
         <v>169</v>
       </c>
       <c r="B167" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C167" s="25">
-        <v>172.5</v>
+        <v>168.5</v>
       </c>
       <c r="D167" s="26">
         <v>1.3</v>
       </c>
       <c r="E167" s="27">
-        <v>224.25</v>
+        <v>219.05</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5552,16 +5552,16 @@
         <v>182</v>
       </c>
       <c r="B180" s="24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C180" s="25">
-        <v>52.5</v>
+        <v>45.5</v>
       </c>
       <c r="D180" s="26">
         <v>3.33</v>
       </c>
       <c r="E180" s="27">
-        <v>174.83</v>
+        <v>151.52000000000001</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5642,16 +5642,16 @@
         <v>188</v>
       </c>
       <c r="B186" s="24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C186" s="25">
-        <v>89.5</v>
+        <v>79.5</v>
       </c>
       <c r="D186" s="26">
         <v>2.65</v>
       </c>
       <c r="E186" s="27">
-        <v>237.18</v>
+        <v>210.68</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5708,16 +5708,16 @@
         <v>192</v>
       </c>
       <c r="B190" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C190" s="25">
-        <v>55</v>
+        <v>54.5</v>
       </c>
       <c r="D190" s="26">
         <v>5</v>
       </c>
       <c r="E190" s="27">
-        <v>275</v>
+        <v>272.5</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5906,16 +5906,16 @@
         <v>204</v>
       </c>
       <c r="B202" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C202" s="25">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D202" s="26">
         <v>2.6</v>
       </c>
       <c r="E202" s="27">
-        <v>83.2</v>
+        <v>70.2</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5985,16 +5985,16 @@
         <v>209</v>
       </c>
       <c r="B207" s="24">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C207" s="25">
-        <v>41.5</v>
+        <v>36.5</v>
       </c>
       <c r="D207" s="26">
         <v>3.9</v>
       </c>
       <c r="E207" s="27">
-        <v>161.86000000000001</v>
+        <v>142.36000000000001</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -6002,16 +6002,16 @@
         <v>210</v>
       </c>
       <c r="B208" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C208" s="25">
-        <v>59.5</v>
+        <v>54.5</v>
       </c>
       <c r="D208" s="26">
         <v>4.5</v>
       </c>
       <c r="E208" s="27">
-        <v>267.75</v>
+        <v>245.25</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -6019,16 +6019,16 @@
         <v>211</v>
       </c>
       <c r="B209" s="24">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C209" s="25">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D209" s="26">
         <v>2.7</v>
       </c>
       <c r="E209" s="27">
-        <v>567</v>
+        <v>561.6</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -6036,16 +6036,16 @@
         <v>212</v>
       </c>
       <c r="B210" s="24">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C210" s="25">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D210" s="26">
         <v>2.7</v>
       </c>
       <c r="E210" s="27">
-        <v>415.8</v>
+        <v>394.2</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -6087,16 +6087,16 @@
         <v>215</v>
       </c>
       <c r="B213" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C213" s="25">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D213" s="26">
         <v>3</v>
       </c>
       <c r="E213" s="27">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -6121,16 +6121,16 @@
         <v>217</v>
       </c>
       <c r="B215" s="24">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C215" s="25">
-        <v>129</v>
+        <v>120.5</v>
       </c>
       <c r="D215" s="26">
         <v>3.92</v>
       </c>
       <c r="E215" s="27">
-        <v>505.78</v>
+        <v>472.46</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -6172,16 +6172,16 @@
         <v>220</v>
       </c>
       <c r="B218" s="24">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C218" s="25">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D218" s="26">
         <v>2.7</v>
       </c>
       <c r="E218" s="27">
-        <v>59.4</v>
+        <v>48.6</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -6291,16 +6291,16 @@
         <v>227</v>
       </c>
       <c r="B225" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C225" s="25">
-        <v>111.5</v>
+        <v>106.5</v>
       </c>
       <c r="D225" s="26">
         <v>3.96</v>
       </c>
       <c r="E225" s="27">
-        <v>441.19</v>
+        <v>421.41</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -6336,16 +6336,16 @@
         <v>230</v>
       </c>
       <c r="B228" s="24">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C228" s="25">
-        <v>43.5</v>
+        <v>41</v>
       </c>
       <c r="D228" s="26">
         <v>3.25</v>
       </c>
       <c r="E228" s="27">
-        <v>141.38</v>
+        <v>133.25</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6353,16 +6353,16 @@
         <v>231</v>
       </c>
       <c r="B229" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C229" s="25">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D229" s="26">
         <v>3.25</v>
       </c>
       <c r="E229" s="27">
-        <v>172.25</v>
+        <v>156</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -6484,16 +6484,16 @@
         <v>240</v>
       </c>
       <c r="B238" s="24">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C238" s="25">
-        <v>1.5</v>
+        <v>7.5</v>
       </c>
       <c r="D238" s="26">
         <v>8.25</v>
       </c>
       <c r="E238" s="27">
-        <v>12.38</v>
+        <v>61.88</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -6501,16 +6501,16 @@
         <v>241</v>
       </c>
       <c r="B239" s="24">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C239" s="25">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D239" s="26">
-        <v>5.76</v>
+        <v>5.75</v>
       </c>
       <c r="E239" s="27">
-        <v>2.88</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -6518,16 +6518,16 @@
         <v>242</v>
       </c>
       <c r="B240" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C240" s="25">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D240" s="26">
         <v>4.8</v>
       </c>
       <c r="E240" s="27">
-        <v>288</v>
+        <v>283.2</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6552,16 +6552,16 @@
         <v>244</v>
       </c>
       <c r="B242" s="24">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C242" s="25">
-        <v>17.5</v>
+        <v>20</v>
       </c>
       <c r="D242" s="26">
         <v>3</v>
       </c>
       <c r="E242" s="27">
-        <v>52.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6603,16 +6603,16 @@
         <v>247</v>
       </c>
       <c r="B245" s="24">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C245" s="25">
-        <v>102</v>
+        <v>93.5</v>
       </c>
       <c r="D245" s="26">
         <v>3.9</v>
       </c>
       <c r="E245" s="27">
-        <v>397.8</v>
+        <v>364.65</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6620,16 +6620,16 @@
         <v>248</v>
       </c>
       <c r="B246" s="24">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C246" s="25">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D246" s="26">
         <v>3.9</v>
       </c>
       <c r="E246" s="27">
-        <v>448.5</v>
+        <v>417.3</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6731,16 +6731,16 @@
         <v>255</v>
       </c>
       <c r="B253" s="24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C253" s="25">
-        <v>12.5</v>
+        <v>2.5</v>
       </c>
       <c r="D253" s="26">
         <v>4</v>
       </c>
       <c r="E253" s="27">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6832,16 +6832,16 @@
         <v>262</v>
       </c>
       <c r="B260" s="24">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C260" s="25">
-        <v>339.5</v>
+        <v>337.5</v>
       </c>
       <c r="D260" s="26">
         <v>4.28</v>
       </c>
       <c r="E260" s="27">
-        <v>1453.06</v>
+        <v>1444.5</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6922,16 +6922,16 @@
         <v>268</v>
       </c>
       <c r="B266" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C266" s="25">
-        <v>91.5</v>
+        <v>86.5</v>
       </c>
       <c r="D266" s="26">
         <v>4.5</v>
       </c>
       <c r="E266" s="27">
-        <v>411.75</v>
+        <v>389.25</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -7086,16 +7086,16 @@
         <v>278</v>
       </c>
       <c r="B276" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C276" s="25">
-        <v>178.5</v>
+        <v>177</v>
       </c>
       <c r="D276" s="26">
         <v>4.8600000000000003</v>
       </c>
       <c r="E276" s="27">
-        <v>866.62</v>
+        <v>859.34</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -7114,16 +7114,16 @@
         <v>280</v>
       </c>
       <c r="B278" s="24">
+        <v>21</v>
+      </c>
+      <c r="C278" s="25">
         <v>20</v>
-      </c>
-      <c r="C278" s="25">
-        <v>25</v>
       </c>
       <c r="D278" s="26">
         <v>4.5999999999999996</v>
       </c>
       <c r="E278" s="27">
-        <v>114.95</v>
+        <v>91.96</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -7182,16 +7182,16 @@
         <v>284</v>
       </c>
       <c r="B282" s="24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C282" s="25">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D282" s="26">
         <v>5</v>
       </c>
       <c r="E282" s="27">
-        <v>780</v>
+        <v>755</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -7301,16 +7301,16 @@
         <v>291</v>
       </c>
       <c r="B289" s="24">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C289" s="25">
-        <v>230.5</v>
+        <v>225.5</v>
       </c>
       <c r="D289" s="26">
         <v>4.8899999999999997</v>
       </c>
       <c r="E289" s="27">
-        <v>1126.71</v>
+        <v>1102.27</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7881,16 +7881,16 @@
         <v>327</v>
       </c>
       <c r="B325" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C325" s="25">
-        <v>193.5</v>
+        <v>188.5</v>
       </c>
       <c r="D325" s="26">
         <v>4.28</v>
       </c>
       <c r="E325" s="27">
-        <v>828.18</v>
+        <v>806.78</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -7977,16 +7977,16 @@
         <v>333</v>
       </c>
       <c r="B331" s="24">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C331" s="25">
-        <v>16.5</v>
+        <v>1.5</v>
       </c>
       <c r="D331" s="26">
         <v>9</v>
       </c>
       <c r="E331" s="27">
-        <v>148.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -7994,16 +7994,16 @@
         <v>334</v>
       </c>
       <c r="B332" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C332" s="25">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="D332" s="26">
         <v>9</v>
       </c>
       <c r="E332" s="27">
-        <v>85.5</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -8267,16 +8267,16 @@
         <v>351</v>
       </c>
       <c r="B349" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C349" s="25">
-        <v>47.35</v>
+        <v>46.35</v>
       </c>
       <c r="D349" s="26">
         <v>4.75</v>
       </c>
       <c r="E349" s="27">
-        <v>224.91</v>
+        <v>220.16</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -8327,7 +8327,7 @@
         <v>355</v>
       </c>
       <c r="B353" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C353" s="28"/>
       <c r="D353" s="29"/>
@@ -8389,16 +8389,16 @@
         <v>359</v>
       </c>
       <c r="B357" s="24">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C357" s="25">
-        <v>112.5</v>
+        <v>107.5</v>
       </c>
       <c r="D357" s="26">
         <v>7.76</v>
       </c>
       <c r="E357" s="27">
-        <v>872.7</v>
+        <v>833.91</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -8593,16 +8593,16 @@
         <v>371</v>
       </c>
       <c r="B369" s="24">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C369" s="25">
-        <v>16.5</v>
+        <v>6.5</v>
       </c>
       <c r="D369" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E369" s="27">
-        <v>135.30000000000001</v>
+        <v>53.3</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
@@ -8610,16 +8610,16 @@
         <v>372</v>
       </c>
       <c r="B370" s="24">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C370" s="25">
-        <v>116.95</v>
+        <v>105.95</v>
       </c>
       <c r="D370" s="26">
         <v>4.5</v>
       </c>
       <c r="E370" s="27">
-        <v>526.28</v>
+        <v>476.78</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -8695,16 +8695,16 @@
         <v>377</v>
       </c>
       <c r="B375" s="24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C375" s="25">
-        <v>5.5</v>
+        <v>-4.5</v>
       </c>
       <c r="D375" s="26">
         <v>9.5</v>
       </c>
       <c r="E375" s="27">
-        <v>52.25</v>
+        <v>-42.75</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
@@ -8982,16 +8982,16 @@
         <v>394</v>
       </c>
       <c r="B392" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C392" s="25">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D392" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E392" s="27">
-        <v>85.5</v>
+        <v>42.75</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
@@ -9313,16 +9313,16 @@
         <v>415</v>
       </c>
       <c r="B413" s="24">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C413" s="25">
-        <v>75.5</v>
+        <v>72</v>
       </c>
       <c r="D413" s="26">
         <v>6.17</v>
       </c>
       <c r="E413" s="27">
-        <v>465.48</v>
+        <v>443.9</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
@@ -9851,16 +9851,16 @@
         <v>449</v>
       </c>
       <c r="B447" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C447" s="25">
-        <v>7.5</v>
+        <v>4</v>
       </c>
       <c r="D447" s="26">
         <v>16.3</v>
       </c>
       <c r="E447" s="27">
-        <v>122.25</v>
+        <v>65.2</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -9956,13 +9956,13 @@
         <v>1</v>
       </c>
       <c r="C453" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D453" s="26">
         <v>28.5</v>
       </c>
       <c r="E453" s="27">
-        <v>85.5</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.25">
@@ -10021,16 +10021,16 @@
         <v>459</v>
       </c>
       <c r="B457" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C457" s="25">
-        <v>13</v>
+        <v>12.5</v>
       </c>
       <c r="D457" s="26">
         <v>10.5</v>
       </c>
       <c r="E457" s="27">
-        <v>136.5</v>
+        <v>131.25</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
@@ -10238,16 +10238,16 @@
         <v>472</v>
       </c>
       <c r="B470" s="24">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C470" s="25">
-        <v>6.5</v>
+        <v>2.5</v>
       </c>
       <c r="D470" s="26">
         <v>9.5</v>
       </c>
       <c r="E470" s="27">
-        <v>61.75</v>
+        <v>23.75</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
@@ -10434,16 +10434,16 @@
         <v>484</v>
       </c>
       <c r="B482" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C482" s="25">
-        <v>14</v>
+        <v>11.5</v>
       </c>
       <c r="D482" s="26">
         <v>9.26</v>
       </c>
       <c r="E482" s="27">
-        <v>129.63999999999999</v>
+        <v>106.49</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
@@ -10587,16 +10587,16 @@
         <v>493</v>
       </c>
       <c r="B491" s="24">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C491" s="25">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D491" s="26">
         <v>11.15</v>
       </c>
       <c r="E491" s="27">
-        <v>111.54</v>
+        <v>66.92</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
@@ -11090,16 +11090,16 @@
         <v>524</v>
       </c>
       <c r="B522" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C522" s="25">
-        <v>137.5</v>
+        <v>134.5</v>
       </c>
       <c r="D522" s="26">
         <v>1.4</v>
       </c>
       <c r="E522" s="27">
-        <v>192.5</v>
+        <v>188.3</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.25">
@@ -11107,16 +11107,16 @@
         <v>525</v>
       </c>
       <c r="B523" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C523" s="25">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D523" s="26">
         <v>1.4</v>
       </c>
       <c r="E523" s="27">
-        <v>176.4</v>
+        <v>175</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
@@ -11273,16 +11273,16 @@
         <v>535</v>
       </c>
       <c r="B533" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C533" s="25">
-        <v>36.5</v>
+        <v>32.5</v>
       </c>
       <c r="D533" s="26">
         <v>3.5</v>
       </c>
       <c r="E533" s="27">
-        <v>127.75</v>
+        <v>113.75</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
@@ -11783,16 +11783,16 @@
         <v>565</v>
       </c>
       <c r="B563" s="24">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C563" s="25">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D563" s="26">
         <v>3.5</v>
       </c>
       <c r="E563" s="27">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
@@ -11834,16 +11834,16 @@
         <v>568</v>
       </c>
       <c r="B566" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C566" s="25">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D566" s="26">
         <v>2.14</v>
       </c>
       <c r="E566" s="27">
-        <v>57.78</v>
+        <v>53.5</v>
       </c>
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.25">
@@ -11911,16 +11911,16 @@
         <v>573</v>
       </c>
       <c r="B571" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C571" s="25">
-        <v>15.5</v>
+        <v>14.5</v>
       </c>
       <c r="D571" s="26">
         <v>2.66</v>
       </c>
       <c r="E571" s="27">
-        <v>41.23</v>
+        <v>38.57</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
@@ -12043,16 +12043,16 @@
         <v>581</v>
       </c>
       <c r="B579" s="24">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C579" s="25">
-        <v>342.5</v>
+        <v>335.5</v>
       </c>
       <c r="D579" s="26">
         <v>1.5</v>
       </c>
       <c r="E579" s="27">
-        <v>513.75</v>
+        <v>503.25</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -12112,10 +12112,10 @@
         <v>586</v>
       </c>
       <c r="B584" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C584" s="25">
-        <v>16.399999999999999</v>
+        <v>6.4</v>
       </c>
       <c r="D584" s="29"/>
       <c r="E584" s="28"/>
@@ -12125,16 +12125,16 @@
         <v>587</v>
       </c>
       <c r="B585" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C585" s="25">
-        <v>127.5</v>
+        <v>117.5</v>
       </c>
       <c r="D585" s="26">
         <v>0.87</v>
       </c>
       <c r="E585" s="27">
-        <v>110.93</v>
+        <v>102.23</v>
       </c>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
@@ -12193,16 +12193,16 @@
         <v>591</v>
       </c>
       <c r="B589" s="24">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C589" s="25">
-        <v>309.5</v>
+        <v>307.5</v>
       </c>
       <c r="D589" s="26">
         <v>0.85</v>
       </c>
       <c r="E589" s="27">
-        <v>263.08</v>
+        <v>261.38</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -12463,16 +12463,16 @@
         <v>609</v>
       </c>
       <c r="B607" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C607" s="25">
-        <v>17.5</v>
+        <v>15.5</v>
       </c>
       <c r="D607" s="26">
         <v>3.5</v>
       </c>
       <c r="E607" s="27">
-        <v>61.25</v>
+        <v>54.25</v>
       </c>
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
@@ -12616,16 +12616,16 @@
         <v>618</v>
       </c>
       <c r="B616" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C616" s="25">
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="D616" s="26">
         <v>4</v>
       </c>
       <c r="E616" s="27">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12661,16 +12661,16 @@
         <v>621</v>
       </c>
       <c r="B619" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C619" s="25">
-        <v>7.5</v>
+        <v>0.5</v>
       </c>
       <c r="D619" s="26">
         <v>1.5</v>
       </c>
       <c r="E619" s="27">
-        <v>11.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12678,16 +12678,16 @@
         <v>622</v>
       </c>
       <c r="B620" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C620" s="25">
-        <v>0.75</v>
+        <v>1.75</v>
       </c>
       <c r="D620" s="26">
-        <v>1.51</v>
+        <v>1.5</v>
       </c>
       <c r="E620" s="27">
-        <v>1.1299999999999999</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12706,16 +12706,16 @@
         <v>624</v>
       </c>
       <c r="B622" s="24">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C622" s="25">
-        <v>39.5</v>
+        <v>33</v>
       </c>
       <c r="D622" s="26">
         <v>2.2799999999999998</v>
       </c>
       <c r="E622" s="27">
-        <v>90.06</v>
+        <v>75.239999999999995</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12757,16 +12757,16 @@
         <v>627</v>
       </c>
       <c r="B625" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C625" s="25">
-        <v>29.5</v>
+        <v>28</v>
       </c>
       <c r="D625" s="26">
         <v>3</v>
       </c>
       <c r="E625" s="27">
-        <v>88.5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12893,16 +12893,16 @@
         <v>635</v>
       </c>
       <c r="B633" s="24">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C633" s="25">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D633" s="26">
         <v>1.7</v>
       </c>
       <c r="E633" s="27">
-        <v>640.9</v>
+        <v>632.4</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
@@ -13097,16 +13097,16 @@
         <v>647</v>
       </c>
       <c r="B645" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C645" s="25">
-        <v>21.5</v>
+        <v>18.5</v>
       </c>
       <c r="D645" s="26">
         <v>3.1</v>
       </c>
       <c r="E645" s="27">
-        <v>66.650000000000006</v>
+        <v>57.35</v>
       </c>
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.25">
@@ -13179,13 +13179,13 @@
         <v>11</v>
       </c>
       <c r="C650" s="25">
-        <v>0.5</v>
+        <v>12.5</v>
       </c>
       <c r="D650" s="26">
-        <v>6.76</v>
+        <v>6.75</v>
       </c>
       <c r="E650" s="27">
-        <v>3.38</v>
+        <v>84.38</v>
       </c>
     </row>
     <row r="651" spans="1:5" x14ac:dyDescent="0.25">
@@ -13327,16 +13327,16 @@
         <v>661</v>
       </c>
       <c r="B659" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C659" s="25">
-        <v>1</v>
+        <v>-14</v>
       </c>
       <c r="D659" s="26">
         <v>3.75</v>
       </c>
       <c r="E659" s="27">
-        <v>3.75</v>
+        <v>-52.5</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.25">
@@ -13344,16 +13344,16 @@
         <v>662</v>
       </c>
       <c r="B660" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C660" s="25">
-        <v>11.5</v>
+        <v>1.5</v>
       </c>
       <c r="D660" s="26">
         <v>2.5</v>
       </c>
       <c r="E660" s="27">
-        <v>28.75</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="661" spans="1:5" x14ac:dyDescent="0.25">
@@ -13378,16 +13378,16 @@
         <v>664</v>
       </c>
       <c r="B662" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C662" s="25">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="D662" s="26">
         <v>5.75</v>
       </c>
       <c r="E662" s="27">
-        <v>8.6300000000000008</v>
+        <v>-5.75</v>
       </c>
     </row>
     <row r="663" spans="1:5" x14ac:dyDescent="0.25">
@@ -13395,16 +13395,16 @@
         <v>665</v>
       </c>
       <c r="B663" s="24">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C663" s="25">
-        <v>16.5</v>
+        <v>13.5</v>
       </c>
       <c r="D663" s="26">
         <v>5.8</v>
       </c>
       <c r="E663" s="27">
-        <v>95.7</v>
+        <v>78.3</v>
       </c>
     </row>
     <row r="664" spans="1:5" x14ac:dyDescent="0.25">
@@ -13696,10 +13696,10 @@
         <v>684</v>
       </c>
       <c r="B682" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C682" s="25">
-        <v>69.5</v>
+        <v>64.5</v>
       </c>
       <c r="D682" s="29"/>
       <c r="E682" s="28"/>
@@ -13709,10 +13709,10 @@
         <v>685</v>
       </c>
       <c r="B683" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C683" s="25">
-        <v>113.5</v>
+        <v>108.5</v>
       </c>
       <c r="D683" s="29"/>
       <c r="E683" s="28"/>
@@ -13735,10 +13735,10 @@
         <v>687</v>
       </c>
       <c r="B685" s="24">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C685" s="25">
-        <v>48.5</v>
+        <v>46.5</v>
       </c>
       <c r="D685" s="29"/>
       <c r="E685" s="28"/>
@@ -14166,11 +14166,11 @@
       </c>
       <c r="B715" s="31"/>
       <c r="C715" s="32">
-        <v>40002.25</v>
+        <v>40082.85</v>
       </c>
       <c r="D715" s="33"/>
       <c r="E715" s="34">
-        <v>108764.2</v>
+        <v>107781.34</v>
       </c>
     </row>
   </sheetData>
@@ -14186,6 +14186,6 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nikhil 06 jan @9.13
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -35,7 +35,7 @@
     <t>Stock Group Summary</t>
   </si>
   <si>
-    <t>1-Jul-25 to 5-Jan-26</t>
+    <t>1-Jul-25 to 6-Jan-26</t>
   </si>
   <si>
     <t/>
@@ -416,7 +416,7 @@
     <t>2025- INVITAION (BOX) SAMPLES</t>
   </si>
   <si>
-    <t>2101 PATRIKA (L)</t>
+    <t>2101 PATRIKA (L)-MONDAY</t>
   </si>
   <si>
     <t>2102 PATRIKA *-* (M)</t>
@@ -476,7 +476,7 @@
     <t>2120 PATRIKA (L)</t>
   </si>
   <si>
-    <t>2121 PATRIKA</t>
+    <t>2121 PATRIKA (19.01.26)</t>
   </si>
   <si>
     <t>2122 PATRIKA</t>
@@ -1784,7 +1784,7 @@
     <t>9224 CARDS - RED</t>
   </si>
   <si>
-    <t>9225 CARDS - YELLOW</t>
+    <t>9225 CARDS - YELLOW (AVLBL)</t>
   </si>
   <si>
     <t>9226 CARDS - GOLDEN</t>
@@ -2829,16 +2829,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="25">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D11" s="26">
         <v>1.8</v>
       </c>
       <c r="E11" s="27">
-        <v>237.6</v>
+        <v>228.6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2846,16 +2846,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="25">
-        <v>202.5</v>
+        <v>199.5</v>
       </c>
       <c r="D12" s="26">
         <v>1.95</v>
       </c>
       <c r="E12" s="27">
-        <v>394.88</v>
+        <v>389.03</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2880,16 +2880,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="24">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C14" s="25">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D14" s="26">
         <v>2</v>
       </c>
       <c r="E14" s="27">
-        <v>274</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2897,16 +2897,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="25">
-        <v>128.5</v>
+        <v>126</v>
       </c>
       <c r="D15" s="26">
         <v>2</v>
       </c>
       <c r="E15" s="27">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3118,16 +3118,16 @@
         <v>30</v>
       </c>
       <c r="B28" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C28" s="25">
-        <v>88.5</v>
+        <v>87.5</v>
       </c>
       <c r="D28" s="26">
         <v>2</v>
       </c>
       <c r="E28" s="27">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3138,13 +3138,13 @@
         <v>8</v>
       </c>
       <c r="C29" s="25">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D29" s="26">
         <v>2.6</v>
       </c>
       <c r="E29" s="27">
-        <v>143</v>
+        <v>166.4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3169,16 +3169,16 @@
         <v>33</v>
       </c>
       <c r="B31" s="24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C31" s="25">
-        <v>50.5</v>
+        <v>46.5</v>
       </c>
       <c r="D31" s="26">
         <v>2.85</v>
       </c>
       <c r="E31" s="27">
-        <v>143.93</v>
+        <v>132.53</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3350,16 +3350,16 @@
         <v>44</v>
       </c>
       <c r="B42" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C42" s="25">
-        <v>107.5</v>
+        <v>106.5</v>
       </c>
       <c r="D42" s="26">
         <v>2.35</v>
       </c>
       <c r="E42" s="27">
-        <v>252.63</v>
+        <v>250.28</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3367,16 +3367,16 @@
         <v>45</v>
       </c>
       <c r="B43" s="24">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C43" s="25">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D43" s="26">
         <v>2.35</v>
       </c>
       <c r="E43" s="27">
-        <v>192.7</v>
+        <v>180.95</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3384,16 +3384,16 @@
         <v>46</v>
       </c>
       <c r="B44" s="24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44" s="25">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D44" s="26">
         <v>2.66</v>
       </c>
       <c r="E44" s="27">
-        <v>109.06</v>
+        <v>135.66</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3401,16 +3401,16 @@
         <v>47</v>
       </c>
       <c r="B45" s="24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45" s="25">
-        <v>26.5</v>
+        <v>36.5</v>
       </c>
       <c r="D45" s="26">
         <v>2.66</v>
       </c>
       <c r="E45" s="27">
-        <v>70.489999999999995</v>
+        <v>97.09</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3438,13 +3438,13 @@
         <v>20</v>
       </c>
       <c r="C47" s="25">
-        <v>221.5</v>
+        <v>181.5</v>
       </c>
       <c r="D47" s="26">
         <v>1.25</v>
       </c>
       <c r="E47" s="27">
-        <v>276.88</v>
+        <v>226.88</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3455,13 +3455,13 @@
         <v>27</v>
       </c>
       <c r="C48" s="25">
-        <v>84.5</v>
+        <v>124.5</v>
       </c>
       <c r="D48" s="26">
         <v>1.26</v>
       </c>
       <c r="E48" s="27">
-        <v>106.11</v>
+        <v>156.25</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3503,16 +3503,16 @@
         <v>53</v>
       </c>
       <c r="B51" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C51" s="25">
-        <v>52</v>
+        <v>50.5</v>
       </c>
       <c r="D51" s="26">
         <v>1.8</v>
       </c>
       <c r="E51" s="27">
-        <v>93.6</v>
+        <v>90.9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3520,16 +3520,16 @@
         <v>54</v>
       </c>
       <c r="B52" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C52" s="25">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D52" s="26">
         <v>2.5</v>
       </c>
       <c r="E52" s="27">
-        <v>277.5</v>
+        <v>257.5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3537,16 +3537,16 @@
         <v>55</v>
       </c>
       <c r="B53" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C53" s="25">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D53" s="26">
         <v>2.5</v>
       </c>
       <c r="E53" s="27">
-        <v>220</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3656,16 +3656,16 @@
         <v>62</v>
       </c>
       <c r="B60" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C60" s="25">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D60" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E60" s="27">
-        <v>215.34</v>
+        <v>209.79</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3722,16 +3722,16 @@
         <v>66</v>
       </c>
       <c r="B64" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C64" s="25">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D64" s="26">
         <v>1.65</v>
       </c>
       <c r="E64" s="27">
-        <v>138.6</v>
+        <v>123.75</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3771,16 +3771,16 @@
         <v>69</v>
       </c>
       <c r="B67" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C67" s="25">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D67" s="26">
         <v>1.65</v>
       </c>
       <c r="E67" s="27">
-        <v>90.75</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3788,17 +3788,11 @@
         <v>70</v>
       </c>
       <c r="B68" s="24">
-        <v>20</v>
-      </c>
-      <c r="C68" s="25">
-        <v>3</v>
-      </c>
-      <c r="D68" s="26">
-        <v>1.65</v>
-      </c>
-      <c r="E68" s="27">
-        <v>4.95</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C68" s="28"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="28"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="23" t="s">
@@ -3822,16 +3816,16 @@
         <v>72</v>
       </c>
       <c r="B70" s="24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C70" s="25">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D70" s="26">
         <v>1.4</v>
       </c>
       <c r="E70" s="27">
-        <v>236.6</v>
+        <v>229.6</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3839,16 +3833,16 @@
         <v>73</v>
       </c>
       <c r="B71" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C71" s="25">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D71" s="26">
         <v>1.4</v>
       </c>
       <c r="E71" s="27">
-        <v>205.8</v>
+        <v>198.8</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3890,16 +3884,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="24">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C74" s="25">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>501.6</v>
+        <v>498</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3907,16 +3901,16 @@
         <v>77</v>
       </c>
       <c r="B75" s="24">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C75" s="25">
-        <v>441</v>
+        <v>333</v>
       </c>
       <c r="D75" s="26">
         <v>1.2</v>
       </c>
       <c r="E75" s="27">
-        <v>529.20000000000005</v>
+        <v>399.6</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3924,16 +3918,16 @@
         <v>78</v>
       </c>
       <c r="B76" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C76" s="25">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D76" s="26">
         <v>1.2</v>
       </c>
       <c r="E76" s="27">
-        <v>628.79999999999995</v>
+        <v>627.6</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3956,16 +3950,16 @@
         <v>80</v>
       </c>
       <c r="B78" s="24">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C78" s="25">
-        <v>556.5</v>
+        <v>502.5</v>
       </c>
       <c r="D78" s="26">
         <v>1.2</v>
       </c>
       <c r="E78" s="27">
-        <v>667.8</v>
+        <v>603</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3976,13 +3970,13 @@
         <v>11</v>
       </c>
       <c r="C79" s="25">
-        <v>644</v>
+        <v>620</v>
       </c>
       <c r="D79" s="26">
         <v>1.2</v>
       </c>
       <c r="E79" s="27">
-        <v>772.8</v>
+        <v>744</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3993,13 +3987,13 @@
         <v>11</v>
       </c>
       <c r="C80" s="25">
-        <v>617</v>
+        <v>593</v>
       </c>
       <c r="D80" s="26">
         <v>1.2</v>
       </c>
       <c r="E80" s="27">
-        <v>740.4</v>
+        <v>711.6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -4007,16 +4001,16 @@
         <v>83</v>
       </c>
       <c r="B81" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C81" s="25">
-        <v>640</v>
+        <v>606</v>
       </c>
       <c r="D81" s="26">
         <v>1.2</v>
       </c>
       <c r="E81" s="27">
-        <v>768</v>
+        <v>727.2</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -4092,16 +4086,16 @@
         <v>88</v>
       </c>
       <c r="B86" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C86" s="25">
-        <v>732</v>
+        <v>712</v>
       </c>
       <c r="D86" s="26">
         <v>1.7</v>
       </c>
       <c r="E86" s="27">
-        <v>1244.4000000000001</v>
+        <v>1210.4000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4109,16 +4103,16 @@
         <v>89</v>
       </c>
       <c r="B87" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C87" s="25">
-        <v>1000</v>
+        <v>980</v>
       </c>
       <c r="D87" s="26">
         <v>1.7</v>
       </c>
       <c r="E87" s="27">
-        <v>1700</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4177,16 +4171,16 @@
         <v>93</v>
       </c>
       <c r="B91" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C91" s="25">
-        <v>160.5</v>
+        <v>148.5</v>
       </c>
       <c r="D91" s="26">
         <v>0.66</v>
       </c>
       <c r="E91" s="27">
-        <v>106.7</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4241,16 +4235,16 @@
         <v>97</v>
       </c>
       <c r="B95" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C95" s="25">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="D95" s="26">
         <v>0.73</v>
       </c>
       <c r="E95" s="27">
-        <v>96.28</v>
+        <v>59.53</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4258,16 +4252,16 @@
         <v>98</v>
       </c>
       <c r="B96" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C96" s="25">
-        <v>359</v>
+        <v>309</v>
       </c>
       <c r="D96" s="26">
         <v>0.81</v>
       </c>
       <c r="E96" s="27">
-        <v>290.91000000000003</v>
+        <v>250.4</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -4275,16 +4269,16 @@
         <v>99</v>
       </c>
       <c r="B97" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C97" s="25">
-        <v>142.5</v>
+        <v>132.5</v>
       </c>
       <c r="D97" s="26">
         <v>0.73</v>
       </c>
       <c r="E97" s="27">
-        <v>104.65</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -4452,10 +4446,10 @@
         <v>112</v>
       </c>
       <c r="B110" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C110" s="25">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="28"/>
@@ -4593,10 +4587,10 @@
         <v>123</v>
       </c>
       <c r="B121" s="24">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C121" s="25">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="28"/>
@@ -4684,16 +4678,16 @@
         <v>130</v>
       </c>
       <c r="B128" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C128" s="25">
-        <v>2.5</v>
+        <v>-8.5</v>
       </c>
       <c r="D128" s="26">
         <v>12.5</v>
       </c>
       <c r="E128" s="27">
-        <v>31.25</v>
+        <v>-106.25</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4820,16 +4814,16 @@
         <v>138</v>
       </c>
       <c r="B136" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C136" s="25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D136" s="26">
         <v>12.89</v>
       </c>
       <c r="E136" s="27">
-        <v>77.31</v>
+        <v>51.54</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4837,16 +4831,16 @@
         <v>139</v>
       </c>
       <c r="B137" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C137" s="25">
-        <v>15.5</v>
+        <v>14.5</v>
       </c>
       <c r="D137" s="26">
         <v>12.5</v>
       </c>
       <c r="E137" s="27">
-        <v>193.75</v>
+        <v>181.25</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -5022,16 +5016,16 @@
         <v>150</v>
       </c>
       <c r="B148" s="24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C148" s="25">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="D148" s="26">
         <v>18.5</v>
       </c>
       <c r="E148" s="27">
-        <v>9.25</v>
+        <v>-9.25</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -5039,16 +5033,16 @@
         <v>151</v>
       </c>
       <c r="B149" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C149" s="25">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D149" s="26">
         <v>18.5</v>
       </c>
       <c r="E149" s="27">
-        <v>222</v>
+        <v>185</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -5226,16 +5220,16 @@
         <v>162</v>
       </c>
       <c r="B160" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C160" s="25">
-        <v>10.5</v>
+        <v>8.5</v>
       </c>
       <c r="D160" s="26">
         <v>11.5</v>
       </c>
       <c r="E160" s="27">
-        <v>120.75</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -5243,16 +5237,16 @@
         <v>163</v>
       </c>
       <c r="B161" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C161" s="25">
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="D161" s="26">
         <v>11.5</v>
       </c>
       <c r="E161" s="27">
-        <v>92</v>
+        <v>17.25</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5418,16 +5412,16 @@
         <v>174</v>
       </c>
       <c r="B172" s="24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C172" s="25">
-        <v>9.9499999999999993</v>
+        <v>19.95</v>
       </c>
       <c r="D172" s="26">
         <v>3.25</v>
       </c>
       <c r="E172" s="27">
-        <v>32.340000000000003</v>
+        <v>64.84</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -5435,16 +5429,16 @@
         <v>175</v>
       </c>
       <c r="B173" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C173" s="25">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D173" s="26">
         <v>2.7</v>
       </c>
       <c r="E173" s="27">
-        <v>229.5</v>
+        <v>221.4</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5636,16 +5630,16 @@
         <v>188</v>
       </c>
       <c r="B186" s="24">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C186" s="25">
-        <v>79.5</v>
+        <v>73</v>
       </c>
       <c r="D186" s="26">
         <v>2.65</v>
       </c>
       <c r="E186" s="27">
-        <v>210.68</v>
+        <v>193.45</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5787,16 +5781,16 @@
         <v>197</v>
       </c>
       <c r="B195" s="24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C195" s="25">
-        <v>85.5</v>
+        <v>82</v>
       </c>
       <c r="D195" s="26">
         <v>4.5</v>
       </c>
       <c r="E195" s="27">
-        <v>384.75</v>
+        <v>369</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5917,16 +5911,16 @@
         <v>205</v>
       </c>
       <c r="B203" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C203" s="25">
-        <v>32</v>
+        <v>30.5</v>
       </c>
       <c r="D203" s="26">
         <v>2.6</v>
       </c>
       <c r="E203" s="27">
-        <v>83.2</v>
+        <v>79.3</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5936,9 +5930,15 @@
       <c r="B204" s="24">
         <v>2</v>
       </c>
-      <c r="C204" s="28"/>
-      <c r="D204" s="29"/>
-      <c r="E204" s="28"/>
+      <c r="C204" s="25">
+        <v>50</v>
+      </c>
+      <c r="D204" s="26">
+        <v>2.6</v>
+      </c>
+      <c r="E204" s="27">
+        <v>130</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="23" t="s">
@@ -5979,16 +5979,16 @@
         <v>209</v>
       </c>
       <c r="B207" s="24">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C207" s="25">
-        <v>33.5</v>
+        <v>34.5</v>
       </c>
       <c r="D207" s="26">
         <v>3.9</v>
       </c>
       <c r="E207" s="27">
-        <v>130.66</v>
+        <v>134.56</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -6013,16 +6013,16 @@
         <v>211</v>
       </c>
       <c r="B209" s="24">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C209" s="25">
-        <v>205</v>
+        <v>200.5</v>
       </c>
       <c r="D209" s="26">
         <v>2.7</v>
       </c>
       <c r="E209" s="27">
-        <v>553.5</v>
+        <v>541.35</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -6033,13 +6033,13 @@
         <v>48</v>
       </c>
       <c r="C210" s="25">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D210" s="26">
         <v>2.7</v>
       </c>
       <c r="E210" s="27">
-        <v>378</v>
+        <v>394.2</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -6115,16 +6115,16 @@
         <v>217</v>
       </c>
       <c r="B215" s="24">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C215" s="25">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D215" s="26">
         <v>3.92</v>
       </c>
       <c r="E215" s="27">
-        <v>439.13</v>
+        <v>415.61</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -6132,16 +6132,16 @@
         <v>218</v>
       </c>
       <c r="B216" s="24">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C216" s="25">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D216" s="26">
         <v>3.25</v>
       </c>
       <c r="E216" s="27">
-        <v>399.75</v>
+        <v>396.5</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -6183,16 +6183,16 @@
         <v>221</v>
       </c>
       <c r="B219" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C219" s="25">
-        <v>49.72</v>
+        <v>48.72</v>
       </c>
       <c r="D219" s="26">
         <v>3.16</v>
       </c>
       <c r="E219" s="27">
-        <v>157.12</v>
+        <v>153.96</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -6203,13 +6203,13 @@
         <v>21</v>
       </c>
       <c r="C220" s="25">
-        <v>74.5</v>
+        <v>76.5</v>
       </c>
       <c r="D220" s="26">
         <v>2.66</v>
       </c>
       <c r="E220" s="27">
-        <v>198.17</v>
+        <v>203.49</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -6234,16 +6234,16 @@
         <v>224</v>
       </c>
       <c r="B222" s="24">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C222" s="25">
-        <v>115.5</v>
+        <v>112</v>
       </c>
       <c r="D222" s="26">
         <v>4</v>
       </c>
       <c r="E222" s="27">
-        <v>462</v>
+        <v>448</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -6330,16 +6330,16 @@
         <v>230</v>
       </c>
       <c r="B228" s="24">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C228" s="25">
-        <v>31</v>
+        <v>24.88</v>
       </c>
       <c r="D228" s="26">
         <v>3.25</v>
       </c>
       <c r="E228" s="27">
-        <v>100.75</v>
+        <v>80.86</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6347,16 +6347,16 @@
         <v>231</v>
       </c>
       <c r="B229" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C229" s="25">
-        <v>39</v>
+        <v>37.5</v>
       </c>
       <c r="D229" s="26">
         <v>3.25</v>
       </c>
       <c r="E229" s="27">
-        <v>126.75</v>
+        <v>121.88</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -6495,16 +6495,16 @@
         <v>241</v>
       </c>
       <c r="B239" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C239" s="25">
-        <v>15.5</v>
+        <v>14.5</v>
       </c>
       <c r="D239" s="26">
         <v>5.75</v>
       </c>
       <c r="E239" s="27">
-        <v>89.13</v>
+        <v>83.38</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -6529,16 +6529,16 @@
         <v>243</v>
       </c>
       <c r="B241" s="24">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C241" s="25">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D241" s="26">
         <v>6.3</v>
       </c>
       <c r="E241" s="27">
-        <v>144.9</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6546,16 +6546,16 @@
         <v>244</v>
       </c>
       <c r="B242" s="24">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C242" s="25">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D242" s="26">
         <v>3</v>
       </c>
       <c r="E242" s="27">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6580,16 +6580,16 @@
         <v>246</v>
       </c>
       <c r="B244" s="24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C244" s="25">
-        <v>40.5</v>
+        <v>50.5</v>
       </c>
       <c r="D244" s="26">
         <v>3.8</v>
       </c>
       <c r="E244" s="27">
-        <v>153.9</v>
+        <v>191.9</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6617,13 +6617,13 @@
         <v>55</v>
       </c>
       <c r="C246" s="25">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D246" s="26">
         <v>3.9</v>
       </c>
       <c r="E246" s="27">
-        <v>362.7</v>
+        <v>393.9</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6725,11 +6725,17 @@
         <v>255</v>
       </c>
       <c r="B253" s="24">
-        <v>9</v>
-      </c>
-      <c r="C253" s="28"/>
-      <c r="D253" s="29"/>
-      <c r="E253" s="28"/>
+        <v>8</v>
+      </c>
+      <c r="C253" s="25">
+        <v>10</v>
+      </c>
+      <c r="D253" s="26">
+        <v>4</v>
+      </c>
+      <c r="E253" s="27">
+        <v>40</v>
+      </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="23" t="s">
@@ -6803,16 +6809,16 @@
         <v>261</v>
       </c>
       <c r="B259" s="24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C259" s="25">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D259" s="26">
         <v>6.12</v>
       </c>
       <c r="E259" s="27">
-        <v>116.32</v>
+        <v>122.44</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6820,16 +6826,16 @@
         <v>262</v>
       </c>
       <c r="B260" s="24">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C260" s="25">
-        <v>307</v>
+        <v>314.5</v>
       </c>
       <c r="D260" s="26">
         <v>4.28</v>
       </c>
       <c r="E260" s="27">
-        <v>1313.96</v>
+        <v>1346.06</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6882,16 +6888,16 @@
         <v>266</v>
       </c>
       <c r="B264" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C264" s="25">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D264" s="26">
         <v>3.1</v>
       </c>
       <c r="E264" s="27">
-        <v>136.4</v>
+        <v>130.19999999999999</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6913,13 +6919,13 @@
         <v>18</v>
       </c>
       <c r="C266" s="25">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D266" s="26">
         <v>4.5</v>
       </c>
       <c r="E266" s="27">
-        <v>279</v>
+        <v>315</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6978,16 +6984,16 @@
         <v>272</v>
       </c>
       <c r="B270" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C270" s="25">
-        <v>114.5</v>
+        <v>110.5</v>
       </c>
       <c r="D270" s="26">
         <v>4.3899999999999997</v>
       </c>
       <c r="E270" s="27">
-        <v>502.64</v>
+        <v>485.08</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -7040,16 +7046,16 @@
         <v>276</v>
       </c>
       <c r="B274" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C274" s="25">
-        <v>40.5</v>
+        <v>38.5</v>
       </c>
       <c r="D274" s="26">
         <v>6.5</v>
       </c>
       <c r="E274" s="27">
-        <v>263.25</v>
+        <v>250.25</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -7170,16 +7176,16 @@
         <v>284</v>
       </c>
       <c r="B282" s="24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C282" s="25">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D282" s="26">
         <v>5</v>
       </c>
       <c r="E282" s="27">
-        <v>755</v>
+        <v>750</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -7187,16 +7193,16 @@
         <v>285</v>
       </c>
       <c r="B283" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C283" s="25">
-        <v>47</v>
+        <v>45.5</v>
       </c>
       <c r="D283" s="26">
         <v>6</v>
       </c>
       <c r="E283" s="27">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -7255,16 +7261,16 @@
         <v>289</v>
       </c>
       <c r="B287" s="24">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C287" s="25">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D287" s="26">
         <v>4.5</v>
       </c>
       <c r="E287" s="27">
-        <v>616.5</v>
+        <v>661.5</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -7323,16 +7329,16 @@
         <v>293</v>
       </c>
       <c r="B291" s="24">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C291" s="25">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D291" s="26">
         <v>3.15</v>
       </c>
       <c r="E291" s="27">
-        <v>192.15</v>
+        <v>223.65</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7340,16 +7346,16 @@
         <v>294</v>
       </c>
       <c r="B292" s="24">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C292" s="25">
-        <v>240</v>
+        <v>237.5</v>
       </c>
       <c r="D292" s="26">
         <v>6.01</v>
       </c>
       <c r="E292" s="27">
-        <v>1443.56</v>
+        <v>1428.52</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -7374,16 +7380,16 @@
         <v>296</v>
       </c>
       <c r="B294" s="24">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C294" s="25">
-        <v>305.5</v>
+        <v>315.5</v>
       </c>
       <c r="D294" s="26">
         <v>4.2699999999999996</v>
       </c>
       <c r="E294" s="27">
-        <v>1303.96</v>
+        <v>1346.65</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -7491,16 +7497,16 @@
         <v>303</v>
       </c>
       <c r="B301" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C301" s="25">
-        <v>99</v>
+        <v>96.5</v>
       </c>
       <c r="D301" s="26">
         <v>5.13</v>
       </c>
       <c r="E301" s="27">
-        <v>507.87</v>
+        <v>495.05</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7617,16 +7623,16 @@
         <v>311</v>
       </c>
       <c r="B309" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C309" s="25">
-        <v>21.35</v>
+        <v>20.350000000000001</v>
       </c>
       <c r="D309" s="26">
         <v>9.4499999999999993</v>
       </c>
       <c r="E309" s="27">
-        <v>201.76</v>
+        <v>192.31</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -7786,16 +7792,16 @@
         <v>322</v>
       </c>
       <c r="B320" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C320" s="25">
-        <v>33.5</v>
+        <v>32.5</v>
       </c>
       <c r="D320" s="26">
         <v>6.75</v>
       </c>
       <c r="E320" s="27">
-        <v>226.13</v>
+        <v>219.38</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -7920,16 +7926,16 @@
         <v>330</v>
       </c>
       <c r="B328" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C328" s="25">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D328" s="26">
         <v>7.97</v>
       </c>
       <c r="E328" s="27">
-        <v>239.14</v>
+        <v>231.17</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -7968,13 +7974,13 @@
         <v>35</v>
       </c>
       <c r="C331" s="25">
-        <v>1.5</v>
+        <v>16.5</v>
       </c>
       <c r="D331" s="26">
         <v>9</v>
       </c>
       <c r="E331" s="27">
-        <v>13.5</v>
+        <v>148.5</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -7982,16 +7988,16 @@
         <v>334</v>
       </c>
       <c r="B332" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C332" s="25">
-        <v>8.5</v>
+        <v>6</v>
       </c>
       <c r="D332" s="26">
         <v>9</v>
       </c>
       <c r="E332" s="27">
-        <v>76.5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7999,16 +8005,16 @@
         <v>335</v>
       </c>
       <c r="B333" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C333" s="25">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D333" s="26">
         <v>9</v>
       </c>
       <c r="E333" s="27">
-        <v>459</v>
+        <v>441</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -8044,16 +8050,16 @@
         <v>338</v>
       </c>
       <c r="B336" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C336" s="25">
-        <v>15.5</v>
+        <v>13.5</v>
       </c>
       <c r="D336" s="26">
         <v>9</v>
       </c>
       <c r="E336" s="27">
-        <v>139.5</v>
+        <v>121.5</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -8153,16 +8159,16 @@
         <v>345</v>
       </c>
       <c r="B343" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C343" s="25">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="D343" s="26">
         <v>8.6999999999999993</v>
       </c>
       <c r="E343" s="27">
-        <v>108.75</v>
+        <v>100.05</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -8266,16 +8272,16 @@
         <v>352</v>
       </c>
       <c r="B350" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C350" s="25">
-        <v>-1.5</v>
+        <v>-5</v>
       </c>
       <c r="D350" s="26">
         <v>9.1999999999999993</v>
       </c>
       <c r="E350" s="27">
-        <v>-13.8</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -8383,16 +8389,16 @@
         <v>359</v>
       </c>
       <c r="B357" s="24">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C357" s="25">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D357" s="26">
         <v>7.76</v>
       </c>
       <c r="E357" s="27">
-        <v>845.55</v>
+        <v>799</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -8519,16 +8525,16 @@
         <v>367</v>
       </c>
       <c r="B365" s="24">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C365" s="25">
-        <v>197.5</v>
+        <v>196</v>
       </c>
       <c r="D365" s="26">
         <v>6.6</v>
       </c>
       <c r="E365" s="27">
-        <v>1303.5</v>
+        <v>1293.5999999999999</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -8587,16 +8593,16 @@
         <v>371</v>
       </c>
       <c r="B369" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C369" s="25">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="D369" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E369" s="27">
-        <v>53.3</v>
+        <v>45.1</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
@@ -8604,16 +8610,16 @@
         <v>372</v>
       </c>
       <c r="B370" s="24">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C370" s="25">
-        <v>93.95</v>
+        <v>84.45</v>
       </c>
       <c r="D370" s="26">
         <v>4.5</v>
       </c>
       <c r="E370" s="27">
-        <v>422.78</v>
+        <v>380.03</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -8876,16 +8882,16 @@
         <v>388</v>
       </c>
       <c r="B386" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C386" s="25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D386" s="26">
         <v>5.7</v>
       </c>
       <c r="E386" s="27">
-        <v>136.80000000000001</v>
+        <v>131.1</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -8976,16 +8982,16 @@
         <v>394</v>
       </c>
       <c r="B392" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C392" s="25">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D392" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E392" s="27">
-        <v>12.83</v>
+        <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
@@ -9066,16 +9072,16 @@
         <v>400</v>
       </c>
       <c r="B398" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C398" s="25">
-        <v>39.5</v>
+        <v>38</v>
       </c>
       <c r="D398" s="26">
         <v>6.65</v>
       </c>
       <c r="E398" s="27">
-        <v>262.68</v>
+        <v>252.7</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -9083,16 +9089,16 @@
         <v>401</v>
       </c>
       <c r="B399" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C399" s="25">
-        <v>23</v>
+        <v>20.5</v>
       </c>
       <c r="D399" s="26">
         <v>7</v>
       </c>
       <c r="E399" s="27">
-        <v>161</v>
+        <v>143.5</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -9226,16 +9232,16 @@
         <v>410</v>
       </c>
       <c r="B408" s="24">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C408" s="25">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D408" s="26">
         <v>5.2</v>
       </c>
       <c r="E408" s="27">
-        <v>613.6</v>
+        <v>546</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
@@ -9275,16 +9281,16 @@
         <v>413</v>
       </c>
       <c r="B411" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C411" s="25">
-        <v>56.5</v>
+        <v>54.5</v>
       </c>
       <c r="D411" s="26">
         <v>5.3</v>
       </c>
       <c r="E411" s="27">
-        <v>299.45</v>
+        <v>288.85000000000002</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
@@ -9307,16 +9313,16 @@
         <v>415</v>
       </c>
       <c r="B413" s="24">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C413" s="25">
-        <v>68.5</v>
+        <v>67.5</v>
       </c>
       <c r="D413" s="26">
         <v>6.17</v>
       </c>
       <c r="E413" s="27">
-        <v>422.32</v>
+        <v>416.16</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
@@ -9487,16 +9493,16 @@
         <v>427</v>
       </c>
       <c r="B425" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C425" s="25">
-        <v>34.5</v>
+        <v>33.5</v>
       </c>
       <c r="D425" s="26">
         <v>5</v>
       </c>
       <c r="E425" s="27">
-        <v>172.5</v>
+        <v>167.5</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9777,33 +9783,27 @@
         <v>445</v>
       </c>
       <c r="B443" s="24">
-        <v>2</v>
-      </c>
-      <c r="C443" s="25">
-        <v>7</v>
-      </c>
-      <c r="D443" s="26">
-        <v>9</v>
-      </c>
-      <c r="E443" s="27">
-        <v>63</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C443" s="28"/>
+      <c r="D443" s="29"/>
+      <c r="E443" s="28"/>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" s="23" t="s">
         <v>446</v>
       </c>
       <c r="B444" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C444" s="25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D444" s="26">
         <v>9</v>
       </c>
       <c r="E444" s="27">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
@@ -9811,16 +9811,16 @@
         <v>447</v>
       </c>
       <c r="B445" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C445" s="25">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D445" s="26">
         <v>10.5</v>
       </c>
       <c r="E445" s="27">
-        <v>157.5</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
@@ -9845,16 +9845,16 @@
         <v>449</v>
       </c>
       <c r="B447" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C447" s="25">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="D447" s="26">
         <v>16.3</v>
       </c>
       <c r="E447" s="27">
-        <v>65.2</v>
+        <v>8.15</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -9879,16 +9879,16 @@
         <v>451</v>
       </c>
       <c r="B449" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C449" s="25">
-        <v>14.5</v>
+        <v>13</v>
       </c>
       <c r="D449" s="26">
         <v>9.75</v>
       </c>
       <c r="E449" s="27">
-        <v>141.38</v>
+        <v>126.75</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
@@ -10060,16 +10060,16 @@
         <v>462</v>
       </c>
       <c r="B460" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C460" s="25">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="D460" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E460" s="27">
-        <v>226.58</v>
+        <v>222.3</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
@@ -10226,17 +10226,11 @@
         <v>472</v>
       </c>
       <c r="B470" s="24">
-        <v>36</v>
-      </c>
-      <c r="C470" s="25">
-        <v>2</v>
-      </c>
-      <c r="D470" s="26">
-        <v>9.5</v>
-      </c>
-      <c r="E470" s="27">
-        <v>19</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C470" s="28"/>
+      <c r="D470" s="29"/>
+      <c r="E470" s="28"/>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" s="23" t="s">
@@ -10294,16 +10288,16 @@
         <v>476</v>
       </c>
       <c r="B474" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C474" s="25">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="D474" s="26">
         <v>10</v>
       </c>
       <c r="E474" s="27">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.25">
@@ -10428,16 +10422,16 @@
         <v>484</v>
       </c>
       <c r="B482" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C482" s="25">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D482" s="26">
         <v>9.26</v>
       </c>
       <c r="E482" s="27">
-        <v>129.63999999999999</v>
+        <v>92.6</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
@@ -10564,17 +10558,11 @@
         <v>492</v>
       </c>
       <c r="B490" s="24">
-        <v>2</v>
-      </c>
-      <c r="C490" s="25">
         <v>3</v>
       </c>
-      <c r="D490" s="26">
-        <v>10.5</v>
-      </c>
-      <c r="E490" s="27">
-        <v>31.5</v>
-      </c>
+      <c r="C490" s="28"/>
+      <c r="D490" s="29"/>
+      <c r="E490" s="28"/>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A491" s="23" t="s">
@@ -10649,16 +10637,16 @@
         <v>497</v>
       </c>
       <c r="B495" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C495" s="25">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="D495" s="26">
         <v>9</v>
       </c>
       <c r="E495" s="27">
-        <v>184.5</v>
+        <v>171</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -10907,9 +10895,15 @@
       <c r="B511" s="24">
         <v>1</v>
       </c>
-      <c r="C511" s="28"/>
-      <c r="D511" s="29"/>
-      <c r="E511" s="28"/>
+      <c r="C511" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D511" s="26">
+        <v>55</v>
+      </c>
+      <c r="E511" s="27">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A512" s="23" t="s">
@@ -11584,16 +11578,16 @@
         <v>554</v>
       </c>
       <c r="B552" s="24">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C552" s="25">
-        <v>138.69999999999999</v>
+        <v>136.69999999999999</v>
       </c>
       <c r="D552" s="26">
         <v>3.9</v>
       </c>
       <c r="E552" s="27">
-        <v>540.92999999999995</v>
+        <v>533.13</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -11720,16 +11714,16 @@
         <v>562</v>
       </c>
       <c r="B560" s="24">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C560" s="25">
-        <v>93.75</v>
+        <v>90.75</v>
       </c>
       <c r="D560" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E560" s="27">
-        <v>215.63</v>
+        <v>208.73</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
@@ -11899,16 +11893,16 @@
         <v>573</v>
       </c>
       <c r="B571" s="24">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C571" s="25">
-        <v>4.5</v>
+        <v>14.5</v>
       </c>
       <c r="D571" s="26">
         <v>2.66</v>
       </c>
       <c r="E571" s="27">
-        <v>11.97</v>
+        <v>38.57</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
@@ -11987,13 +11981,13 @@
         <v>3</v>
       </c>
       <c r="C576" s="25">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D576" s="26">
         <v>1.2</v>
       </c>
       <c r="E576" s="27">
-        <v>40.799999999999997</v>
+        <v>31.2</v>
       </c>
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.25">
@@ -12004,13 +11998,13 @@
         <v>5</v>
       </c>
       <c r="C577" s="25">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D577" s="26">
         <v>1.2</v>
       </c>
       <c r="E577" s="27">
-        <v>33.6</v>
+        <v>26.4</v>
       </c>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
@@ -12031,16 +12025,16 @@
         <v>581</v>
       </c>
       <c r="B579" s="24">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C579" s="25">
-        <v>332.5</v>
+        <v>331.5</v>
       </c>
       <c r="D579" s="26">
         <v>1.5</v>
       </c>
       <c r="E579" s="27">
-        <v>498.75</v>
+        <v>497.25</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -12048,10 +12042,10 @@
         <v>582</v>
       </c>
       <c r="B580" s="24">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C580" s="25">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D580" s="29"/>
       <c r="E580" s="28"/>
@@ -12074,10 +12068,10 @@
         <v>584</v>
       </c>
       <c r="B582" s="24">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C582" s="25">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D582" s="29"/>
       <c r="E582" s="28"/>
@@ -12087,10 +12081,10 @@
         <v>585</v>
       </c>
       <c r="B583" s="24">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C583" s="25">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D583" s="29"/>
       <c r="E583" s="28"/>
@@ -12100,10 +12094,10 @@
         <v>586</v>
       </c>
       <c r="B584" s="24">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C584" s="25">
-        <v>4.4000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="D584" s="29"/>
       <c r="E584" s="28"/>
@@ -12113,16 +12107,16 @@
         <v>587</v>
       </c>
       <c r="B585" s="24">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C585" s="25">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D585" s="26">
         <v>0.87</v>
       </c>
       <c r="E585" s="27">
-        <v>73.95</v>
+        <v>72.209999999999994</v>
       </c>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
@@ -12147,16 +12141,16 @@
         <v>589</v>
       </c>
       <c r="B587" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C587" s="25">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D587" s="26">
         <v>0.85</v>
       </c>
       <c r="E587" s="27">
-        <v>277.95</v>
+        <v>277.10000000000002</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
@@ -12181,16 +12175,16 @@
         <v>591</v>
       </c>
       <c r="B589" s="24">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C589" s="25">
-        <v>298.5</v>
+        <v>296</v>
       </c>
       <c r="D589" s="26">
         <v>0.85</v>
       </c>
       <c r="E589" s="27">
-        <v>253.73</v>
+        <v>251.6</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -12244,7 +12238,7 @@
         <v>17</v>
       </c>
       <c r="C593" s="25">
-        <v>164</v>
+        <v>2</v>
       </c>
       <c r="D593" s="29"/>
       <c r="E593" s="28"/>
@@ -12536,16 +12530,16 @@
         <v>614</v>
       </c>
       <c r="B612" s="24">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C612" s="25">
-        <v>22.5</v>
+        <v>14.5</v>
       </c>
       <c r="D612" s="26">
         <v>2.78</v>
       </c>
       <c r="E612" s="27">
-        <v>62.62</v>
+        <v>40.36</v>
       </c>
     </row>
     <row r="613" spans="1:5" x14ac:dyDescent="0.25">
@@ -12587,16 +12581,16 @@
         <v>617</v>
       </c>
       <c r="B615" s="24">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C615" s="25">
-        <v>42.5</v>
+        <v>38.5</v>
       </c>
       <c r="D615" s="26">
         <v>2.74</v>
       </c>
       <c r="E615" s="27">
-        <v>116.55</v>
+        <v>105.58</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12802,33 +12796,27 @@
         <v>630</v>
       </c>
       <c r="B628" s="24">
-        <v>8</v>
-      </c>
-      <c r="C628" s="25">
-        <v>1.5</v>
-      </c>
-      <c r="D628" s="26">
-        <v>3.5</v>
-      </c>
-      <c r="E628" s="27">
-        <v>5.25</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C628" s="28"/>
+      <c r="D628" s="29"/>
+      <c r="E628" s="28"/>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A629" s="23" t="s">
         <v>631</v>
       </c>
       <c r="B629" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C629" s="25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D629" s="26">
         <v>3.5</v>
       </c>
       <c r="E629" s="27">
-        <v>87.5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -12870,16 +12858,16 @@
         <v>634</v>
       </c>
       <c r="B632" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C632" s="25">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D632" s="26">
         <v>3.1</v>
       </c>
       <c r="E632" s="27">
-        <v>220.1</v>
+        <v>210.8</v>
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
@@ -12887,16 +12875,16 @@
         <v>635</v>
       </c>
       <c r="B633" s="24">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C633" s="25">
-        <v>344.5</v>
+        <v>334.5</v>
       </c>
       <c r="D633" s="26">
         <v>1.7</v>
       </c>
       <c r="E633" s="27">
-        <v>585.65</v>
+        <v>568.65</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
@@ -13006,16 +12994,16 @@
         <v>642</v>
       </c>
       <c r="B640" s="24">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C640" s="25">
-        <v>77.8</v>
+        <v>75.3</v>
       </c>
       <c r="D640" s="26">
         <v>2.85</v>
       </c>
       <c r="E640" s="27">
-        <v>221.73</v>
+        <v>214.61</v>
       </c>
     </row>
     <row r="641" spans="1:5" x14ac:dyDescent="0.25">
@@ -13236,16 +13224,16 @@
         <v>656</v>
       </c>
       <c r="B654" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C654" s="25">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="D654" s="26">
         <v>5.5</v>
       </c>
       <c r="E654" s="27">
-        <v>41.25</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="655" spans="1:5" x14ac:dyDescent="0.25">
@@ -13253,16 +13241,16 @@
         <v>657</v>
       </c>
       <c r="B655" s="24">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C655" s="25">
-        <v>94.5</v>
+        <v>88.5</v>
       </c>
       <c r="D655" s="26">
         <v>3.1</v>
       </c>
       <c r="E655" s="27">
-        <v>292.95</v>
+        <v>274.35000000000002</v>
       </c>
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.25">
@@ -13304,16 +13292,16 @@
         <v>660</v>
       </c>
       <c r="B658" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C658" s="25">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D658" s="26">
         <v>4.25</v>
       </c>
       <c r="E658" s="27">
-        <v>25.5</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="659" spans="1:5" x14ac:dyDescent="0.25">
@@ -13338,16 +13326,16 @@
         <v>662</v>
       </c>
       <c r="B660" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C660" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D660" s="26">
         <v>2.5</v>
       </c>
       <c r="E660" s="27">
-        <v>12.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="661" spans="1:5" x14ac:dyDescent="0.25">
@@ -13423,16 +13411,16 @@
         <v>667</v>
       </c>
       <c r="B665" s="24">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C665" s="25">
-        <v>45.5</v>
+        <v>44.5</v>
       </c>
       <c r="D665" s="26">
         <v>2.25</v>
       </c>
       <c r="E665" s="27">
-        <v>102.38</v>
+        <v>100.13</v>
       </c>
     </row>
     <row r="666" spans="1:5" x14ac:dyDescent="0.25">
@@ -13664,10 +13652,10 @@
         <v>682</v>
       </c>
       <c r="B680" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C680" s="25">
-        <v>11.69</v>
+        <v>7.69</v>
       </c>
       <c r="D680" s="29"/>
       <c r="E680" s="28"/>
@@ -13677,10 +13665,10 @@
         <v>683</v>
       </c>
       <c r="B681" s="24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C681" s="25">
-        <v>22</v>
+        <v>16.5</v>
       </c>
       <c r="D681" s="29"/>
       <c r="E681" s="28"/>
@@ -13690,10 +13678,10 @@
         <v>684</v>
       </c>
       <c r="B682" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C682" s="25">
-        <v>63.5</v>
+        <v>62.5</v>
       </c>
       <c r="D682" s="29"/>
       <c r="E682" s="28"/>
@@ -13703,10 +13691,10 @@
         <v>685</v>
       </c>
       <c r="B683" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C683" s="25">
-        <v>106.5</v>
+        <v>105.5</v>
       </c>
       <c r="D683" s="29"/>
       <c r="E683" s="28"/>
@@ -13716,10 +13704,10 @@
         <v>686</v>
       </c>
       <c r="B684" s="24">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C684" s="25">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D684" s="29"/>
       <c r="E684" s="28"/>
@@ -13729,10 +13717,10 @@
         <v>687</v>
       </c>
       <c r="B685" s="24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C685" s="25">
-        <v>44.5</v>
+        <v>41</v>
       </c>
       <c r="D685" s="29"/>
       <c r="E685" s="28"/>
@@ -13742,10 +13730,10 @@
         <v>688</v>
       </c>
       <c r="B686" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C686" s="25">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D686" s="29"/>
       <c r="E686" s="28"/>
@@ -13764,16 +13752,16 @@
         <v>690</v>
       </c>
       <c r="B688" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C688" s="25">
-        <v>73.5</v>
+        <v>68.5</v>
       </c>
       <c r="D688" s="26">
         <v>2.9</v>
       </c>
       <c r="E688" s="27">
-        <v>213</v>
+        <v>198.51</v>
       </c>
     </row>
     <row r="689" spans="1:5" x14ac:dyDescent="0.25">
@@ -13950,10 +13938,10 @@
         <v>704</v>
       </c>
       <c r="B702" s="24">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C702" s="25">
-        <v>-0.68</v>
+        <v>-0.73</v>
       </c>
       <c r="D702" s="29"/>
       <c r="E702" s="28"/>
@@ -14027,16 +14015,16 @@
         <v>709</v>
       </c>
       <c r="B707" s="24">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C707" s="25">
-        <v>55.25</v>
+        <v>50.25</v>
       </c>
       <c r="D707" s="26">
         <v>2.5</v>
       </c>
       <c r="E707" s="27">
-        <v>138.13</v>
+        <v>125.63</v>
       </c>
     </row>
     <row r="708" spans="1:5" x14ac:dyDescent="0.25">
@@ -14061,16 +14049,16 @@
         <v>711</v>
       </c>
       <c r="B709" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C709" s="25">
-        <v>36.25</v>
+        <v>34.25</v>
       </c>
       <c r="D709" s="26">
         <v>2.5</v>
       </c>
       <c r="E709" s="27">
-        <v>90.63</v>
+        <v>85.63</v>
       </c>
     </row>
     <row r="710" spans="1:5" x14ac:dyDescent="0.25">
@@ -14129,16 +14117,16 @@
         <v>715</v>
       </c>
       <c r="B713" s="24">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C713" s="25">
-        <v>37.25</v>
+        <v>32.25</v>
       </c>
       <c r="D713" s="26">
         <v>2.5</v>
       </c>
       <c r="E713" s="27">
-        <v>93.13</v>
+        <v>80.63</v>
       </c>
     </row>
     <row r="714" spans="1:5" x14ac:dyDescent="0.25">
@@ -14146,10 +14134,10 @@
         <v>716</v>
       </c>
       <c r="B714" s="24">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C714" s="25">
-        <v>-320</v>
+        <v>-322</v>
       </c>
       <c r="D714" s="29"/>
       <c r="E714" s="28"/>
@@ -14160,11 +14148,11 @@
       </c>
       <c r="B715" s="31"/>
       <c r="C715" s="32">
-        <v>41005.93</v>
+        <v>40239.24</v>
       </c>
       <c r="D715" s="33"/>
       <c r="E715" s="34">
-        <v>107927.33</v>
+        <v>106585.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nikhil 13 jan @9.09
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -515,7 +515,7 @@
     <t>2133 PATRIKA</t>
   </si>
   <si>
-    <t>2134 PATRIKA *-* (M)-Aagya</t>
+    <t>2134 PATRIKA *-* (M)</t>
   </si>
   <si>
     <t>2135 PATRIKA *-* (M)</t>
@@ -2841,16 +2841,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="25">
-        <v>110.5</v>
+        <v>108</v>
       </c>
       <c r="D11" s="26">
         <v>1.8</v>
       </c>
       <c r="E11" s="27">
-        <v>198.9</v>
+        <v>194.4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2909,16 +2909,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="25">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="26">
         <v>2</v>
       </c>
       <c r="E15" s="27">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2994,16 +2994,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="25">
-        <v>-170</v>
+        <v>-176</v>
       </c>
       <c r="D20" s="26">
         <v>0.75</v>
       </c>
       <c r="E20" s="27">
-        <v>-127.5</v>
+        <v>-132</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3028,16 +3028,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="25">
-        <v>94.5</v>
+        <v>92.5</v>
       </c>
       <c r="D22" s="26">
         <v>1.8</v>
       </c>
       <c r="E22" s="27">
-        <v>170.1</v>
+        <v>166.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3079,16 +3079,16 @@
         <v>27</v>
       </c>
       <c r="B25" s="24">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C25" s="25">
-        <v>68.5</v>
+        <v>66</v>
       </c>
       <c r="D25" s="26">
         <v>1.65</v>
       </c>
       <c r="E25" s="27">
-        <v>113.03</v>
+        <v>108.9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3181,16 +3181,16 @@
         <v>33</v>
       </c>
       <c r="B31" s="24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C31" s="25">
-        <v>30.5</v>
+        <v>27</v>
       </c>
       <c r="D31" s="26">
         <v>2.85</v>
       </c>
       <c r="E31" s="27">
-        <v>86.93</v>
+        <v>76.95</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3260,16 +3260,16 @@
         <v>38</v>
       </c>
       <c r="B36" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C36" s="25">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D36" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E36" s="27">
-        <v>236.9</v>
+        <v>227.7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3328,16 +3328,16 @@
         <v>42</v>
       </c>
       <c r="B40" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C40" s="25">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="26">
         <v>2.14</v>
       </c>
       <c r="E40" s="27">
-        <v>92.02</v>
+        <v>89.88</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3345,33 +3345,27 @@
         <v>43</v>
       </c>
       <c r="B41" s="24">
-        <v>17</v>
-      </c>
-      <c r="C41" s="25">
-        <v>15</v>
-      </c>
-      <c r="D41" s="26">
-        <v>2.14</v>
-      </c>
-      <c r="E41" s="27">
-        <v>32.1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="28"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B42" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C42" s="25">
-        <v>105.5</v>
+        <v>104.5</v>
       </c>
       <c r="D42" s="26">
         <v>2.42</v>
       </c>
       <c r="E42" s="27">
-        <v>255.64</v>
+        <v>253.22</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3379,16 +3373,16 @@
         <v>45</v>
       </c>
       <c r="B43" s="24">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C43" s="25">
-        <v>46.5</v>
+        <v>42.5</v>
       </c>
       <c r="D43" s="26">
         <v>2.39</v>
       </c>
       <c r="E43" s="27">
-        <v>110.92</v>
+        <v>101.38</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3413,16 +3407,16 @@
         <v>47</v>
       </c>
       <c r="B45" s="24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C45" s="25">
-        <v>26.5</v>
+        <v>25.5</v>
       </c>
       <c r="D45" s="26">
         <v>2.66</v>
       </c>
       <c r="E45" s="27">
-        <v>70.489999999999995</v>
+        <v>67.83</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3447,16 +3441,16 @@
         <v>49</v>
       </c>
       <c r="B47" s="24">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C47" s="25">
-        <v>155.5</v>
+        <v>135.5</v>
       </c>
       <c r="D47" s="26">
         <v>1.25</v>
       </c>
       <c r="E47" s="27">
-        <v>194.38</v>
+        <v>169.38</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3464,16 +3458,16 @@
         <v>50</v>
       </c>
       <c r="B48" s="24">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C48" s="25">
-        <v>90.5</v>
+        <v>68.5</v>
       </c>
       <c r="D48" s="26">
         <v>1.26</v>
       </c>
       <c r="E48" s="27">
-        <v>113.58</v>
+        <v>85.97</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3481,16 +3475,16 @@
         <v>51</v>
       </c>
       <c r="B49" s="24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C49" s="25">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D49" s="26">
         <v>1.4</v>
       </c>
       <c r="E49" s="27">
-        <v>95.2</v>
+        <v>88.2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3498,16 +3492,16 @@
         <v>52</v>
       </c>
       <c r="B50" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C50" s="25">
-        <v>129.5</v>
+        <v>127.5</v>
       </c>
       <c r="D50" s="26">
         <v>1.4</v>
       </c>
       <c r="E50" s="27">
-        <v>181.3</v>
+        <v>178.5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3515,16 +3509,16 @@
         <v>53</v>
       </c>
       <c r="B51" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C51" s="25">
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="D51" s="26">
         <v>1.8</v>
       </c>
       <c r="E51" s="27">
-        <v>20.7</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3549,16 +3543,16 @@
         <v>55</v>
       </c>
       <c r="B53" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C53" s="25">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D53" s="26">
         <v>2.5</v>
       </c>
       <c r="E53" s="27">
-        <v>207.5</v>
+        <v>202.5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3583,16 +3577,16 @@
         <v>57</v>
       </c>
       <c r="B55" s="24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C55" s="25">
-        <v>21.75</v>
+        <v>16.25</v>
       </c>
       <c r="D55" s="26">
         <v>2.75</v>
       </c>
       <c r="E55" s="27">
-        <v>59.81</v>
+        <v>44.69</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3600,16 +3594,16 @@
         <v>58</v>
       </c>
       <c r="B56" s="24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C56" s="25">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D56" s="26">
         <v>1.8</v>
       </c>
       <c r="E56" s="27">
-        <v>235.8</v>
+        <v>219.6</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3668,16 +3662,16 @@
         <v>62</v>
       </c>
       <c r="B60" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C60" s="25">
-        <v>164</v>
+        <v>161.5</v>
       </c>
       <c r="D60" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E60" s="27">
-        <v>182.04</v>
+        <v>179.27</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3685,16 +3679,16 @@
         <v>63</v>
       </c>
       <c r="B61" s="24">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C61" s="25">
-        <v>136.5</v>
+        <v>134</v>
       </c>
       <c r="D61" s="26">
         <v>1.1100000000000001</v>
       </c>
       <c r="E61" s="27">
-        <v>151.52000000000001</v>
+        <v>148.74</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3881,16 +3875,16 @@
         <v>75</v>
       </c>
       <c r="B73" s="24">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C73" s="25">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="D73" s="26">
         <v>1.4</v>
       </c>
       <c r="E73" s="27">
-        <v>1068.2</v>
+        <v>1054.2</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3898,16 +3892,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="24">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C74" s="25">
-        <v>653.5</v>
+        <v>623.5</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>784.2</v>
+        <v>748.2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3932,31 +3926,33 @@
         <v>78</v>
       </c>
       <c r="B76" s="24">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C76" s="25">
-        <v>759.5</v>
+        <v>733.5</v>
       </c>
       <c r="D76" s="26">
         <v>1.2</v>
       </c>
       <c r="E76" s="27">
-        <v>911.4</v>
+        <v>880.2</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B77" s="24"/>
+      <c r="B77" s="24">
+        <v>1</v>
+      </c>
       <c r="C77" s="25">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D77" s="26">
         <v>1.2</v>
       </c>
       <c r="E77" s="27">
-        <v>72</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3964,16 +3960,16 @@
         <v>80</v>
       </c>
       <c r="B78" s="24">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C78" s="25">
-        <v>706</v>
+        <v>670</v>
       </c>
       <c r="D78" s="26">
         <v>1.2</v>
       </c>
       <c r="E78" s="27">
-        <v>847.2</v>
+        <v>804</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3981,16 +3977,16 @@
         <v>81</v>
       </c>
       <c r="B79" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C79" s="25">
-        <v>886</v>
+        <v>856</v>
       </c>
       <c r="D79" s="26">
         <v>1.2</v>
       </c>
       <c r="E79" s="27">
-        <v>1063.2</v>
+        <v>1027.2</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3998,16 +3994,16 @@
         <v>82</v>
       </c>
       <c r="B80" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C80" s="25">
-        <v>863</v>
+        <v>833</v>
       </c>
       <c r="D80" s="26">
         <v>1.2</v>
       </c>
       <c r="E80" s="27">
-        <v>1035.5999999999999</v>
+        <v>999.6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -4032,16 +4028,16 @@
         <v>84</v>
       </c>
       <c r="B82" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C82" s="25">
-        <v>904</v>
+        <v>874</v>
       </c>
       <c r="D82" s="26">
         <v>1.2</v>
       </c>
       <c r="E82" s="27">
-        <v>1084.8</v>
+        <v>1048.8</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4049,16 +4045,16 @@
         <v>85</v>
       </c>
       <c r="B83" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C83" s="25">
-        <v>916</v>
+        <v>886</v>
       </c>
       <c r="D83" s="26">
         <v>1.2</v>
       </c>
       <c r="E83" s="27">
-        <v>1099.2</v>
+        <v>1063.2</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4151,16 +4147,16 @@
         <v>91</v>
       </c>
       <c r="B89" s="24">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C89" s="25">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D89" s="26">
         <v>1.37</v>
       </c>
       <c r="E89" s="27">
-        <v>251.21</v>
+        <v>248.46</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4202,16 +4198,16 @@
         <v>94</v>
       </c>
       <c r="B92" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C92" s="25">
-        <v>325</v>
+        <v>295</v>
       </c>
       <c r="D92" s="26">
         <v>1.62</v>
       </c>
       <c r="E92" s="27">
-        <v>527.12</v>
+        <v>478.47</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4266,16 +4262,16 @@
         <v>98</v>
       </c>
       <c r="B96" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C96" s="25">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D96" s="26">
         <v>0.81</v>
       </c>
       <c r="E96" s="27">
-        <v>239.05</v>
+        <v>236.62</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -4283,16 +4279,16 @@
         <v>99</v>
       </c>
       <c r="B97" s="24">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C97" s="25">
-        <v>97.5</v>
+        <v>90.5</v>
       </c>
       <c r="D97" s="26">
         <v>0.73</v>
       </c>
       <c r="E97" s="27">
-        <v>71.599999999999994</v>
+        <v>66.459999999999994</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -4374,16 +4370,16 @@
         <v>106</v>
       </c>
       <c r="B104" s="24">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C104" s="25">
-        <v>513</v>
+        <v>403</v>
       </c>
       <c r="D104" s="26">
         <v>2.5</v>
       </c>
       <c r="E104" s="27">
-        <v>1282.5</v>
+        <v>1007.5</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -4391,16 +4387,16 @@
         <v>107</v>
       </c>
       <c r="B105" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C105" s="25">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="D105" s="26">
         <v>2.5</v>
       </c>
       <c r="E105" s="27">
-        <v>1250</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4408,16 +4404,16 @@
         <v>108</v>
       </c>
       <c r="B106" s="24">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C106" s="25">
-        <v>512</v>
+        <v>402</v>
       </c>
       <c r="D106" s="26">
         <v>2.5</v>
       </c>
       <c r="E106" s="27">
-        <v>1280</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4425,16 +4421,16 @@
         <v>109</v>
       </c>
       <c r="B107" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C107" s="25">
-        <v>500</v>
+        <v>480</v>
       </c>
       <c r="D107" s="26">
         <v>2.5</v>
       </c>
       <c r="E107" s="27">
-        <v>1250</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4442,16 +4438,16 @@
         <v>110</v>
       </c>
       <c r="B108" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C108" s="25">
-        <v>508</v>
+        <v>458</v>
       </c>
       <c r="D108" s="26">
         <v>2.5</v>
       </c>
       <c r="E108" s="27">
-        <v>1270</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4472,10 +4468,10 @@
         <v>112</v>
       </c>
       <c r="B110" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C110" s="25">
-        <v>443.5</v>
+        <v>413.5</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="28"/>
@@ -4498,10 +4494,10 @@
         <v>114</v>
       </c>
       <c r="B112" s="24">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C112" s="25">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="28"/>
@@ -4511,10 +4507,10 @@
         <v>115</v>
       </c>
       <c r="B113" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C113" s="25">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="28"/>
@@ -4524,10 +4520,10 @@
         <v>116</v>
       </c>
       <c r="B114" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C114" s="25">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="28"/>
@@ -4591,10 +4587,10 @@
         <v>121</v>
       </c>
       <c r="B119" s="24">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C119" s="25">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="28"/>
@@ -4613,10 +4609,10 @@
         <v>123</v>
       </c>
       <c r="B121" s="24">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C121" s="25">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="28"/>
@@ -4707,13 +4703,13 @@
         <v>27</v>
       </c>
       <c r="C128" s="25">
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
       <c r="D128" s="26">
         <v>12.5</v>
       </c>
       <c r="E128" s="27">
-        <v>256.25</v>
+        <v>243.75</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4738,16 +4734,16 @@
         <v>132</v>
       </c>
       <c r="B130" s="24">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C130" s="25">
-        <v>27.5</v>
+        <v>26.5</v>
       </c>
       <c r="D130" s="26">
         <v>12.5</v>
       </c>
       <c r="E130" s="27">
-        <v>343.75</v>
+        <v>331.25</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4840,16 +4836,16 @@
         <v>138</v>
       </c>
       <c r="B136" s="24">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C136" s="25">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D136" s="26">
         <v>12.83</v>
       </c>
       <c r="E136" s="27">
-        <v>179.67</v>
+        <v>128.34</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4923,16 +4919,16 @@
         <v>143</v>
       </c>
       <c r="B141" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C141" s="25">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="D141" s="26">
         <v>18.5</v>
       </c>
       <c r="E141" s="27">
-        <v>64.75</v>
+        <v>27.75</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,16 +4970,16 @@
         <v>146</v>
       </c>
       <c r="B144" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C144" s="25">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="D144" s="26">
         <v>18.5</v>
       </c>
       <c r="E144" s="27">
-        <v>64.75</v>
+        <v>27.75</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -5246,16 +5242,16 @@
         <v>162</v>
       </c>
       <c r="B160" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C160" s="25">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="D160" s="26">
         <v>11.5</v>
       </c>
       <c r="E160" s="27">
-        <v>120.75</v>
+        <v>109.25</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -5263,16 +5259,16 @@
         <v>163</v>
       </c>
       <c r="B161" s="24">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C161" s="25">
-        <v>-10</v>
+        <v>7.5</v>
       </c>
       <c r="D161" s="26">
         <v>11.5</v>
       </c>
       <c r="E161" s="27">
-        <v>-115</v>
+        <v>86.25</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5807,16 +5803,16 @@
         <v>197</v>
       </c>
       <c r="B195" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C195" s="25">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D195" s="26">
         <v>4.5</v>
       </c>
       <c r="E195" s="27">
-        <v>355.5</v>
+        <v>351</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5852,16 +5848,16 @@
         <v>200</v>
       </c>
       <c r="B198" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C198" s="25">
-        <v>71.5</v>
+        <v>69.5</v>
       </c>
       <c r="D198" s="26">
         <v>4.5</v>
       </c>
       <c r="E198" s="27">
-        <v>321.75</v>
+        <v>312.75</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5886,16 +5882,16 @@
         <v>202</v>
       </c>
       <c r="B200" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C200" s="25">
-        <v>107.5</v>
+        <v>104</v>
       </c>
       <c r="D200" s="26">
         <v>3.4</v>
       </c>
       <c r="E200" s="27">
-        <v>365.5</v>
+        <v>353.6</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5954,16 +5950,16 @@
         <v>206</v>
       </c>
       <c r="B204" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C204" s="25">
-        <v>42.5</v>
+        <v>39.5</v>
       </c>
       <c r="D204" s="26">
         <v>2.6</v>
       </c>
       <c r="E204" s="27">
-        <v>110.5</v>
+        <v>102.7</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -6005,16 +6001,16 @@
         <v>209</v>
       </c>
       <c r="B207" s="24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C207" s="25">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D207" s="26">
         <v>3.9</v>
       </c>
       <c r="E207" s="27">
-        <v>66.28</v>
+        <v>50.68</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -6039,16 +6035,16 @@
         <v>211</v>
       </c>
       <c r="B209" s="24">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C209" s="25">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D209" s="26">
         <v>2.7</v>
       </c>
       <c r="E209" s="27">
-        <v>434.7</v>
+        <v>407.7</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -6158,16 +6154,16 @@
         <v>218</v>
       </c>
       <c r="B216" s="24">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C216" s="25">
-        <v>85.5</v>
+        <v>83.5</v>
       </c>
       <c r="D216" s="26">
         <v>3.25</v>
       </c>
       <c r="E216" s="27">
-        <v>277.88</v>
+        <v>271.38</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -6226,16 +6222,16 @@
         <v>222</v>
       </c>
       <c r="B220" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C220" s="25">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D220" s="26">
         <v>2.66</v>
       </c>
       <c r="E220" s="27">
-        <v>135.66</v>
+        <v>127.68</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -6328,16 +6324,16 @@
         <v>228</v>
       </c>
       <c r="B226" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C226" s="25">
-        <v>56.5</v>
+        <v>53.5</v>
       </c>
       <c r="D226" s="26">
         <v>3.5</v>
       </c>
       <c r="E226" s="27">
-        <v>197.75</v>
+        <v>187.25</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6373,16 +6369,16 @@
         <v>231</v>
       </c>
       <c r="B229" s="24">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C229" s="25">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D229" s="26">
         <v>3.25</v>
       </c>
       <c r="E229" s="27">
-        <v>279.5</v>
+        <v>266.5</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -6538,16 +6534,16 @@
         <v>242</v>
       </c>
       <c r="B240" s="24">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C240" s="25">
-        <v>50.5</v>
+        <v>47.5</v>
       </c>
       <c r="D240" s="26">
         <v>4.8</v>
       </c>
       <c r="E240" s="27">
-        <v>242.4</v>
+        <v>228</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6555,16 +6551,16 @@
         <v>243</v>
       </c>
       <c r="B241" s="24">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C241" s="25">
-        <v>37.5</v>
+        <v>17.5</v>
       </c>
       <c r="D241" s="26">
         <v>6.3</v>
       </c>
       <c r="E241" s="27">
-        <v>236.25</v>
+        <v>110.25</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6589,16 +6585,16 @@
         <v>245</v>
       </c>
       <c r="B243" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C243" s="25">
-        <v>60</v>
+        <v>59.68</v>
       </c>
       <c r="D243" s="26">
         <v>3</v>
       </c>
       <c r="E243" s="27">
-        <v>180</v>
+        <v>179.04</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6623,16 +6619,16 @@
         <v>247</v>
       </c>
       <c r="B245" s="24">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C245" s="25">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D245" s="26">
         <v>3.9</v>
       </c>
       <c r="E245" s="27">
-        <v>257.39999999999998</v>
+        <v>249.6</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6640,16 +6636,16 @@
         <v>248</v>
       </c>
       <c r="B246" s="24">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C246" s="25">
-        <v>36.5</v>
+        <v>32.5</v>
       </c>
       <c r="D246" s="26">
         <v>3.9</v>
       </c>
       <c r="E246" s="27">
-        <v>142.35</v>
+        <v>126.75</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6700,16 +6696,16 @@
         <v>252</v>
       </c>
       <c r="B250" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C250" s="25">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D250" s="26">
         <v>3.5</v>
       </c>
       <c r="E250" s="27">
-        <v>399</v>
+        <v>388.5</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6734,16 +6730,16 @@
         <v>254</v>
       </c>
       <c r="B252" s="24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C252" s="25">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D252" s="26">
         <v>3.5</v>
       </c>
       <c r="E252" s="27">
-        <v>283.5</v>
+        <v>269.5</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6852,16 +6848,16 @@
         <v>262</v>
       </c>
       <c r="B260" s="24">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C260" s="25">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D260" s="26">
         <v>4.28</v>
       </c>
       <c r="E260" s="27">
-        <v>1134.2</v>
+        <v>1104.24</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6914,16 +6910,16 @@
         <v>266</v>
       </c>
       <c r="B264" s="24">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C264" s="25">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D264" s="26">
         <v>3.1</v>
       </c>
       <c r="E264" s="27">
-        <v>266.60000000000002</v>
+        <v>232.5</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6976,16 +6972,16 @@
         <v>270</v>
       </c>
       <c r="B268" s="24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C268" s="25">
-        <v>124.87</v>
+        <v>121.87</v>
       </c>
       <c r="D268" s="26">
         <v>4.25</v>
       </c>
       <c r="E268" s="27">
-        <v>530.70000000000005</v>
+        <v>517.95000000000005</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -7089,16 +7085,16 @@
         <v>277</v>
       </c>
       <c r="B275" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C275" s="25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D275" s="26">
         <v>5.23</v>
       </c>
       <c r="E275" s="27">
-        <v>20.92</v>
+        <v>10.46</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -7134,16 +7130,16 @@
         <v>280</v>
       </c>
       <c r="B278" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C278" s="25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D278" s="26">
         <v>4.5999999999999996</v>
       </c>
       <c r="E278" s="27">
-        <v>18.39</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -7202,16 +7198,16 @@
         <v>284</v>
       </c>
       <c r="B282" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C282" s="25">
-        <v>147.5</v>
+        <v>146.5</v>
       </c>
       <c r="D282" s="26">
         <v>5</v>
       </c>
       <c r="E282" s="27">
-        <v>737.5</v>
+        <v>732.5</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -7236,16 +7232,16 @@
         <v>286</v>
       </c>
       <c r="B284" s="24">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C284" s="25">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D284" s="26">
         <v>5.75</v>
       </c>
       <c r="E284" s="27">
-        <v>74.81</v>
+        <v>46.03</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -7256,13 +7252,13 @@
         <v>10</v>
       </c>
       <c r="C285" s="25">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D285" s="26">
-        <v>4.63</v>
+        <v>4.66</v>
       </c>
       <c r="E285" s="27">
-        <v>115.63</v>
+        <v>302.88</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -7287,16 +7283,16 @@
         <v>289</v>
       </c>
       <c r="B287" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C287" s="25">
-        <v>132.5</v>
+        <v>131</v>
       </c>
       <c r="D287" s="26">
         <v>4.5</v>
       </c>
       <c r="E287" s="27">
-        <v>596.25</v>
+        <v>589.5</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -7304,16 +7300,16 @@
         <v>290</v>
       </c>
       <c r="B288" s="24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C288" s="25">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="D288" s="26">
         <v>3.8</v>
       </c>
       <c r="E288" s="27">
-        <v>102.6</v>
+        <v>96.9</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -7321,16 +7317,16 @@
         <v>291</v>
       </c>
       <c r="B289" s="24">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C289" s="25">
-        <v>206.5</v>
+        <v>205.5</v>
       </c>
       <c r="D289" s="26">
         <v>4.8899999999999997</v>
       </c>
       <c r="E289" s="27">
-        <v>1009.4</v>
+        <v>1004.51</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7372,16 +7368,16 @@
         <v>294</v>
       </c>
       <c r="B292" s="24">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C292" s="25">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D292" s="26">
-        <v>6.09</v>
+        <v>6.1</v>
       </c>
       <c r="E292" s="27">
-        <v>1078.17</v>
+        <v>1012.04</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -7440,16 +7436,16 @@
         <v>298</v>
       </c>
       <c r="B296" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C296" s="25">
-        <v>14.5</v>
+        <v>12</v>
       </c>
       <c r="D296" s="26">
         <v>5.43</v>
       </c>
       <c r="E296" s="27">
-        <v>78.760000000000005</v>
+        <v>65.180000000000007</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -7602,16 +7598,16 @@
         <v>308</v>
       </c>
       <c r="B306" s="24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C306" s="25">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D306" s="26">
         <v>7.75</v>
       </c>
       <c r="E306" s="27">
-        <v>100.75</v>
+        <v>85.25</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -7694,16 +7690,16 @@
         <v>314</v>
       </c>
       <c r="B312" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C312" s="25">
-        <v>12.5</v>
+        <v>7.5</v>
       </c>
       <c r="D312" s="26">
         <v>8.1</v>
       </c>
       <c r="E312" s="27">
-        <v>101.25</v>
+        <v>60.75</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -7905,16 +7901,16 @@
         <v>327</v>
       </c>
       <c r="B325" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C325" s="25">
-        <v>178.5</v>
+        <v>173.5</v>
       </c>
       <c r="D325" s="26">
         <v>4.28</v>
       </c>
       <c r="E325" s="27">
-        <v>763.98</v>
+        <v>742.58</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -8035,16 +8031,16 @@
         <v>335</v>
       </c>
       <c r="B333" s="24">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C333" s="25">
-        <v>42.5</v>
+        <v>34.5</v>
       </c>
       <c r="D333" s="26">
         <v>9</v>
       </c>
       <c r="E333" s="27">
-        <v>382.5</v>
+        <v>310.5</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -8063,16 +8059,16 @@
         <v>337</v>
       </c>
       <c r="B335" s="24">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C335" s="25">
-        <v>19</v>
+        <v>16.5</v>
       </c>
       <c r="D335" s="26">
         <v>9</v>
       </c>
       <c r="E335" s="27">
-        <v>171</v>
+        <v>148.5</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -8274,16 +8270,16 @@
         <v>350</v>
       </c>
       <c r="B348" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C348" s="25">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="D348" s="26">
         <v>7.36</v>
       </c>
       <c r="E348" s="27">
-        <v>55.2</v>
+        <v>33.119999999999997</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -8308,16 +8304,16 @@
         <v>352</v>
       </c>
       <c r="B350" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C350" s="25">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D350" s="26">
         <v>9.1999999999999993</v>
       </c>
       <c r="E350" s="27">
-        <v>119.6</v>
+        <v>92</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -8374,16 +8370,16 @@
         <v>356</v>
       </c>
       <c r="B354" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C354" s="25">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D354" s="26">
         <v>6.64</v>
       </c>
       <c r="E354" s="27">
-        <v>298.86</v>
+        <v>292.22000000000003</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -8442,16 +8438,16 @@
         <v>360</v>
       </c>
       <c r="B358" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C358" s="25">
-        <v>44.5</v>
+        <v>44</v>
       </c>
       <c r="D358" s="26">
         <v>7.13</v>
       </c>
       <c r="E358" s="27">
-        <v>317.29000000000002</v>
+        <v>313.72000000000003</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
@@ -8476,16 +8472,16 @@
         <v>362</v>
       </c>
       <c r="B360" s="24">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C360" s="25">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D360" s="26">
         <v>5.94</v>
       </c>
       <c r="E360" s="27">
-        <v>219.78</v>
+        <v>243.54</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -8527,16 +8523,16 @@
         <v>365</v>
       </c>
       <c r="B363" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C363" s="25">
-        <v>45.5</v>
+        <v>43.5</v>
       </c>
       <c r="D363" s="26">
         <v>7.13</v>
       </c>
       <c r="E363" s="27">
-        <v>324.42</v>
+        <v>310.16000000000003</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -8544,16 +8540,16 @@
         <v>366</v>
       </c>
       <c r="B364" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C364" s="25">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D364" s="26">
         <v>7</v>
       </c>
       <c r="E364" s="27">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
@@ -8561,16 +8557,16 @@
         <v>367</v>
       </c>
       <c r="B365" s="24">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C365" s="25">
-        <v>186.5</v>
+        <v>185</v>
       </c>
       <c r="D365" s="26">
         <v>6.6</v>
       </c>
       <c r="E365" s="27">
-        <v>1230.9000000000001</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -8612,16 +8608,16 @@
         <v>370</v>
       </c>
       <c r="B368" s="24">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C368" s="25">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="D368" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E368" s="27">
-        <v>28.7</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -8629,16 +8625,16 @@
         <v>371</v>
       </c>
       <c r="B369" s="24">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C369" s="25">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D369" s="26">
         <v>8.1999999999999993</v>
       </c>
       <c r="E369" s="27">
-        <v>246</v>
+        <v>164</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
@@ -8646,16 +8642,16 @@
         <v>372</v>
       </c>
       <c r="B370" s="24">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C370" s="25">
-        <v>56.45</v>
+        <v>52.45</v>
       </c>
       <c r="D370" s="26">
         <v>4.5</v>
       </c>
       <c r="E370" s="27">
-        <v>254.03</v>
+        <v>236.03</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -8663,16 +8659,16 @@
         <v>373</v>
       </c>
       <c r="B371" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C371" s="25">
-        <v>36</v>
+        <v>28.5</v>
       </c>
       <c r="D371" s="26">
         <v>8.08</v>
       </c>
       <c r="E371" s="27">
-        <v>290.88</v>
+        <v>230.28</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -8714,16 +8710,16 @@
         <v>376</v>
       </c>
       <c r="B374" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C374" s="25">
-        <v>50.5</v>
+        <v>49</v>
       </c>
       <c r="D374" s="26">
         <v>7</v>
       </c>
       <c r="E374" s="27">
-        <v>353.5</v>
+        <v>343</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
@@ -9035,16 +9031,16 @@
         <v>395</v>
       </c>
       <c r="B393" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C393" s="25">
-        <v>22.5</v>
+        <v>20.5</v>
       </c>
       <c r="D393" s="26">
         <v>6.65</v>
       </c>
       <c r="E393" s="27">
-        <v>149.63</v>
+        <v>136.33000000000001</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
@@ -9108,16 +9104,16 @@
         <v>400</v>
       </c>
       <c r="B398" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C398" s="25">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D398" s="26">
         <v>6.65</v>
       </c>
       <c r="E398" s="27">
-        <v>252.7</v>
+        <v>239.4</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -9258,16 +9254,16 @@
         <v>410</v>
       </c>
       <c r="B408" s="24">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C408" s="25">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D408" s="26">
         <v>5.2</v>
       </c>
       <c r="E408" s="27">
-        <v>436.8</v>
+        <v>358.8</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
@@ -9275,16 +9271,16 @@
         <v>411</v>
       </c>
       <c r="B409" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C409" s="25">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D409" s="26">
         <v>8</v>
       </c>
       <c r="E409" s="27">
-        <v>152</v>
+        <v>120</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
@@ -9307,16 +9303,16 @@
         <v>413</v>
       </c>
       <c r="B411" s="24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C411" s="25">
-        <v>46.5</v>
+        <v>45.5</v>
       </c>
       <c r="D411" s="26">
         <v>5.3</v>
       </c>
       <c r="E411" s="27">
-        <v>246.45</v>
+        <v>241.15</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
@@ -9384,16 +9380,16 @@
         <v>418</v>
       </c>
       <c r="B416" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C416" s="25">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D416" s="26">
         <v>6.46</v>
       </c>
       <c r="E416" s="27">
-        <v>16.149999999999999</v>
+        <v>12.92</v>
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.25">
@@ -9726,16 +9722,16 @@
         <v>440</v>
       </c>
       <c r="B438" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C438" s="25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D438" s="26">
         <v>9.75</v>
       </c>
       <c r="E438" s="27">
-        <v>68.25</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
@@ -10020,16 +10016,16 @@
         <v>458</v>
       </c>
       <c r="B456" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C456" s="25">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D456" s="26">
         <v>14</v>
       </c>
       <c r="E456" s="27">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
@@ -10037,16 +10033,16 @@
         <v>459</v>
       </c>
       <c r="B457" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C457" s="25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D457" s="26">
         <v>10.5</v>
       </c>
       <c r="E457" s="27">
-        <v>73.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
@@ -10105,16 +10101,16 @@
         <v>463</v>
       </c>
       <c r="B461" s="24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C461" s="25">
-        <v>20.16</v>
+        <v>17.66</v>
       </c>
       <c r="D461" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E461" s="27">
-        <v>172.37</v>
+        <v>150.99</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.25">
@@ -10203,16 +10199,16 @@
         <v>469</v>
       </c>
       <c r="B467" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C467" s="25">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D467" s="26">
         <v>11.2</v>
       </c>
       <c r="E467" s="27">
-        <v>179.2</v>
+        <v>145.6</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.25">
@@ -10237,16 +10233,16 @@
         <v>471</v>
       </c>
       <c r="B469" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C469" s="25">
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="D469" s="26">
         <v>10</v>
       </c>
       <c r="E469" s="27">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
@@ -10254,11 +10250,17 @@
         <v>472</v>
       </c>
       <c r="B470" s="24">
-        <v>43</v>
-      </c>
-      <c r="C470" s="28"/>
-      <c r="D470" s="29"/>
-      <c r="E470" s="28"/>
+        <v>45</v>
+      </c>
+      <c r="C470" s="25">
+        <v>6.88</v>
+      </c>
+      <c r="D470" s="26">
+        <v>9.5</v>
+      </c>
+      <c r="E470" s="27">
+        <v>65.36</v>
+      </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" s="23" t="s">
@@ -10461,16 +10463,16 @@
         <v>485</v>
       </c>
       <c r="B483" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C483" s="25">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="D483" s="26">
         <v>10.199999999999999</v>
       </c>
       <c r="E483" s="27">
-        <v>86.7</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">
@@ -10495,16 +10497,16 @@
         <v>487</v>
       </c>
       <c r="B485" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C485" s="25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D485" s="26">
         <v>9.26</v>
       </c>
       <c r="E485" s="27">
-        <v>37.04</v>
+        <v>18.52</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
@@ -10659,16 +10661,16 @@
         <v>497</v>
       </c>
       <c r="B495" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C495" s="25">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="D495" s="26">
         <v>9</v>
       </c>
       <c r="E495" s="27">
-        <v>130.5</v>
+        <v>112.5</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -11179,16 +11181,16 @@
         <v>529</v>
       </c>
       <c r="B527" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C527" s="25">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D527" s="26">
         <v>2.1</v>
       </c>
       <c r="E527" s="27">
-        <v>130.19999999999999</v>
+        <v>123.9</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
@@ -11549,16 +11551,16 @@
         <v>551</v>
       </c>
       <c r="B549" s="24">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C549" s="25">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D549" s="26">
         <v>9.5</v>
       </c>
       <c r="E549" s="27">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
@@ -11600,16 +11602,16 @@
         <v>554</v>
       </c>
       <c r="B552" s="24">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C552" s="25">
-        <v>123.2</v>
+        <v>104.2</v>
       </c>
       <c r="D552" s="26">
         <v>3.9</v>
       </c>
       <c r="E552" s="27">
-        <v>480.48</v>
+        <v>406.38</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -11685,16 +11687,16 @@
         <v>559</v>
       </c>
       <c r="B557" s="24">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C557" s="25">
-        <v>10.5</v>
+        <v>8.5</v>
       </c>
       <c r="D557" s="26">
         <v>3.6</v>
       </c>
       <c r="E557" s="27">
-        <v>37.799999999999997</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.25">
@@ -11787,16 +11789,16 @@
         <v>565</v>
       </c>
       <c r="B563" s="24">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C563" s="25">
-        <v>53.5</v>
+        <v>51.5</v>
       </c>
       <c r="D563" s="26">
         <v>3.5</v>
       </c>
       <c r="E563" s="27">
-        <v>187.25</v>
+        <v>180.25</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
@@ -12083,10 +12085,10 @@
         <v>583</v>
       </c>
       <c r="B581" s="24">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C581" s="25">
-        <v>340.5</v>
+        <v>338.5</v>
       </c>
       <c r="D581" s="29"/>
       <c r="E581" s="28"/>
@@ -12096,10 +12098,10 @@
         <v>584</v>
       </c>
       <c r="B582" s="24">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C582" s="25">
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="D582" s="29"/>
       <c r="E582" s="28"/>
@@ -12125,7 +12127,7 @@
         <v>41</v>
       </c>
       <c r="C584" s="25">
-        <v>-13.6</v>
+        <v>65</v>
       </c>
       <c r="D584" s="29"/>
       <c r="E584" s="28"/>
@@ -12152,16 +12154,16 @@
         <v>588</v>
       </c>
       <c r="B586" s="24">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C586" s="25">
-        <v>1040</v>
+        <v>1007</v>
       </c>
       <c r="D586" s="26">
         <v>0.57999999999999996</v>
       </c>
       <c r="E586" s="27">
-        <v>603.20000000000005</v>
+        <v>584.05999999999995</v>
       </c>
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
@@ -12169,16 +12171,16 @@
         <v>589</v>
       </c>
       <c r="B587" s="24">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C587" s="25">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D587" s="26">
         <v>0.85</v>
       </c>
       <c r="E587" s="27">
-        <v>261.8</v>
+        <v>252.45</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
@@ -12203,16 +12205,16 @@
         <v>591</v>
       </c>
       <c r="B589" s="24">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C589" s="25">
-        <v>1004.5</v>
+        <v>978.5</v>
       </c>
       <c r="D589" s="26">
         <v>0.85</v>
       </c>
       <c r="E589" s="27">
-        <v>853.83</v>
+        <v>831.73</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -12237,10 +12239,10 @@
         <v>593</v>
       </c>
       <c r="B591" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C591" s="25">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D591" s="29"/>
       <c r="E591" s="28"/>
@@ -12592,16 +12594,16 @@
         <v>616</v>
       </c>
       <c r="B614" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C614" s="25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D614" s="26">
         <v>6.5</v>
       </c>
       <c r="E614" s="27">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12626,16 +12628,16 @@
         <v>618</v>
       </c>
       <c r="B616" s="24">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C616" s="25">
-        <v>10.5</v>
+        <v>5.5</v>
       </c>
       <c r="D616" s="26">
         <v>2.78</v>
       </c>
       <c r="E616" s="27">
-        <v>29.22</v>
+        <v>15.31</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12677,16 +12679,16 @@
         <v>621</v>
       </c>
       <c r="B619" s="24">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C619" s="25">
-        <v>29.5</v>
+        <v>19.5</v>
       </c>
       <c r="D619" s="26">
         <v>2.74</v>
       </c>
       <c r="E619" s="27">
-        <v>80.900000000000006</v>
+        <v>53.48</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12694,16 +12696,16 @@
         <v>622</v>
       </c>
       <c r="B620" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C620" s="25">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D620" s="26">
         <v>4</v>
       </c>
       <c r="E620" s="27">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12711,16 +12713,16 @@
         <v>623</v>
       </c>
       <c r="B621" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C621" s="25">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D621" s="26">
         <v>4</v>
       </c>
       <c r="E621" s="27">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12728,16 +12730,16 @@
         <v>624</v>
       </c>
       <c r="B622" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C622" s="25">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="D622" s="26">
         <v>1.5</v>
       </c>
       <c r="E622" s="27">
-        <v>51.75</v>
+        <v>48.75</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12779,16 +12781,16 @@
         <v>627</v>
       </c>
       <c r="B625" s="24">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C625" s="25">
-        <v>143.5</v>
+        <v>133.5</v>
       </c>
       <c r="D625" s="26">
         <v>2.2799999999999998</v>
       </c>
       <c r="E625" s="27">
-        <v>327.18</v>
+        <v>304.38</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12796,16 +12798,16 @@
         <v>628</v>
       </c>
       <c r="B626" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C626" s="25">
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
       <c r="D626" s="26">
         <v>2.2799999999999998</v>
       </c>
       <c r="E626" s="27">
-        <v>49.02</v>
+        <v>46.74</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -12881,16 +12883,16 @@
         <v>633</v>
       </c>
       <c r="B631" s="24">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C631" s="25">
-        <v>21.5</v>
+        <v>10.5</v>
       </c>
       <c r="D631" s="26">
         <v>5</v>
       </c>
       <c r="E631" s="27">
-        <v>107.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
@@ -12966,16 +12968,16 @@
         <v>638</v>
       </c>
       <c r="B636" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C636" s="25">
-        <v>64.5</v>
+        <v>64</v>
       </c>
       <c r="D636" s="26">
         <v>3.1</v>
       </c>
       <c r="E636" s="27">
-        <v>199.95</v>
+        <v>198.4</v>
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.25">
@@ -12983,16 +12985,16 @@
         <v>639</v>
       </c>
       <c r="B637" s="24">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C637" s="25">
-        <v>295.5</v>
+        <v>293</v>
       </c>
       <c r="D637" s="26">
         <v>1.7</v>
       </c>
       <c r="E637" s="27">
-        <v>502.35</v>
+        <v>498.1</v>
       </c>
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.25">
@@ -13017,16 +13019,16 @@
         <v>641</v>
       </c>
       <c r="B639" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C639" s="25">
-        <v>12</v>
+        <v>10.5</v>
       </c>
       <c r="D639" s="26">
         <v>3.5</v>
       </c>
       <c r="E639" s="27">
-        <v>42</v>
+        <v>36.75</v>
       </c>
     </row>
     <row r="640" spans="1:5" x14ac:dyDescent="0.25">
@@ -13068,16 +13070,16 @@
         <v>644</v>
       </c>
       <c r="B642" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C642" s="25">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D642" s="26">
         <v>8.75</v>
       </c>
       <c r="E642" s="27">
-        <v>87.5</v>
+        <v>78.75</v>
       </c>
     </row>
     <row r="643" spans="1:5" x14ac:dyDescent="0.25">
@@ -13102,16 +13104,16 @@
         <v>646</v>
       </c>
       <c r="B644" s="24">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C644" s="25">
-        <v>31.8</v>
+        <v>8.61</v>
       </c>
       <c r="D644" s="26">
         <v>2.85</v>
       </c>
       <c r="E644" s="27">
-        <v>90.63</v>
+        <v>24.54</v>
       </c>
     </row>
     <row r="645" spans="1:5" x14ac:dyDescent="0.25">
@@ -13187,16 +13189,16 @@
         <v>651</v>
       </c>
       <c r="B649" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C649" s="25">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="D649" s="26">
         <v>3.1</v>
       </c>
       <c r="E649" s="27">
-        <v>13.95</v>
+        <v>10.85</v>
       </c>
     </row>
     <row r="650" spans="1:5" x14ac:dyDescent="0.25">
@@ -13238,16 +13240,16 @@
         <v>654</v>
       </c>
       <c r="B652" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C652" s="25">
-        <v>7.5</v>
+        <v>2.5</v>
       </c>
       <c r="D652" s="26">
         <v>4.8</v>
       </c>
       <c r="E652" s="27">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="653" spans="1:5" x14ac:dyDescent="0.25">
@@ -13349,16 +13351,16 @@
         <v>661</v>
       </c>
       <c r="B659" s="24">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C659" s="25">
-        <v>25.5</v>
+        <v>23.5</v>
       </c>
       <c r="D659" s="26">
         <v>3.1</v>
       </c>
       <c r="E659" s="27">
-        <v>79.05</v>
+        <v>72.849999999999994</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.25">
@@ -13383,11 +13385,17 @@
         <v>663</v>
       </c>
       <c r="B661" s="24">
-        <v>23</v>
-      </c>
-      <c r="C661" s="28"/>
-      <c r="D661" s="29"/>
-      <c r="E661" s="28"/>
+        <v>24</v>
+      </c>
+      <c r="C661" s="25">
+        <v>-1</v>
+      </c>
+      <c r="D661" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="E661" s="27">
+        <v>-3.5</v>
+      </c>
     </row>
     <row r="662" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A662" s="23" t="s">
@@ -13496,16 +13504,16 @@
         <v>670</v>
       </c>
       <c r="B668" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C668" s="25">
-        <v>46.5</v>
+        <v>36.5</v>
       </c>
       <c r="D668" s="26">
         <v>2.25</v>
       </c>
       <c r="E668" s="27">
-        <v>104.63</v>
+        <v>82.13</v>
       </c>
     </row>
     <row r="669" spans="1:5" x14ac:dyDescent="0.25">
@@ -13513,16 +13521,16 @@
         <v>671</v>
       </c>
       <c r="B669" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C669" s="25">
-        <v>40.5</v>
+        <v>37.5</v>
       </c>
       <c r="D669" s="26">
         <v>2.25</v>
       </c>
       <c r="E669" s="27">
-        <v>91.13</v>
+        <v>84.38</v>
       </c>
     </row>
     <row r="670" spans="1:5" x14ac:dyDescent="0.25">
@@ -13581,16 +13589,16 @@
         <v>675</v>
       </c>
       <c r="B673" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C673" s="25">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D673" s="26">
         <v>2.75</v>
       </c>
       <c r="E673" s="27">
-        <v>123.75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="674" spans="1:5" x14ac:dyDescent="0.25">
@@ -13598,16 +13606,16 @@
         <v>676</v>
       </c>
       <c r="B674" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C674" s="25">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="D674" s="26">
         <v>4</v>
       </c>
       <c r="E674" s="27">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="675" spans="1:5" x14ac:dyDescent="0.25">
@@ -13649,16 +13657,16 @@
         <v>679</v>
       </c>
       <c r="B677" s="24">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C677" s="25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D677" s="26">
         <v>4.25</v>
       </c>
       <c r="E677" s="27">
-        <v>51</v>
+        <v>46.75</v>
       </c>
     </row>
     <row r="678" spans="1:5" x14ac:dyDescent="0.25">
@@ -13754,10 +13762,10 @@
         <v>686</v>
       </c>
       <c r="B684" s="24">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C684" s="25">
-        <v>2.69</v>
+        <v>5.69</v>
       </c>
       <c r="D684" s="29"/>
       <c r="E684" s="28"/>
@@ -13806,10 +13814,10 @@
         <v>690</v>
       </c>
       <c r="B688" s="24">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C688" s="25">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D688" s="29"/>
       <c r="E688" s="28"/>
@@ -13819,10 +13827,10 @@
         <v>691</v>
       </c>
       <c r="B689" s="24">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C689" s="25">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D689" s="29"/>
       <c r="E689" s="28"/>
@@ -13854,16 +13862,16 @@
         <v>694</v>
       </c>
       <c r="B692" s="24">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C692" s="25">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D692" s="26">
         <v>2.9</v>
       </c>
       <c r="E692" s="27">
-        <v>55.06</v>
+        <v>11.59</v>
       </c>
     </row>
     <row r="693" spans="1:5" x14ac:dyDescent="0.25">
@@ -14070,10 +14078,10 @@
         <v>710</v>
       </c>
       <c r="B708" s="24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C708" s="25">
-        <v>-75.650000000000006</v>
+        <v>-76.650000000000006</v>
       </c>
       <c r="D708" s="29"/>
       <c r="E708" s="28"/>
@@ -14117,16 +14125,16 @@
         <v>713</v>
       </c>
       <c r="B711" s="24">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C711" s="25">
-        <v>35.25</v>
+        <v>32.25</v>
       </c>
       <c r="D711" s="26">
         <v>2.5</v>
       </c>
       <c r="E711" s="27">
-        <v>88.13</v>
+        <v>80.63</v>
       </c>
     </row>
     <row r="712" spans="1:5" x14ac:dyDescent="0.25">
@@ -14151,16 +14159,16 @@
         <v>715</v>
       </c>
       <c r="B713" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C713" s="25">
-        <v>19.25</v>
+        <v>16.25</v>
       </c>
       <c r="D713" s="26">
         <v>2.5</v>
       </c>
       <c r="E713" s="27">
-        <v>48.13</v>
+        <v>40.630000000000003</v>
       </c>
     </row>
     <row r="714" spans="1:5" x14ac:dyDescent="0.25">
@@ -14168,16 +14176,16 @@
         <v>716</v>
       </c>
       <c r="B714" s="24">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C714" s="25">
-        <v>8.25</v>
+        <v>5.25</v>
       </c>
       <c r="D714" s="26">
         <v>2.5</v>
       </c>
       <c r="E714" s="27">
-        <v>20.63</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="715" spans="1:5" x14ac:dyDescent="0.25">
@@ -14185,16 +14193,16 @@
         <v>717</v>
       </c>
       <c r="B715" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C715" s="25">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="D715" s="26">
         <v>2.5</v>
       </c>
       <c r="E715" s="27">
-        <v>13.75</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="716" spans="1:5" x14ac:dyDescent="0.25">
@@ -14219,16 +14227,16 @@
         <v>719</v>
       </c>
       <c r="B717" s="24">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C717" s="25">
-        <v>16.75</v>
+        <v>13.75</v>
       </c>
       <c r="D717" s="26">
         <v>2.5</v>
       </c>
       <c r="E717" s="27">
-        <v>41.88</v>
+        <v>34.380000000000003</v>
       </c>
     </row>
     <row r="718" spans="1:5" x14ac:dyDescent="0.25">
@@ -14236,10 +14244,10 @@
         <v>720</v>
       </c>
       <c r="B718" s="24">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C718" s="25">
-        <v>-335.5</v>
+        <v>-356.5</v>
       </c>
       <c r="D718" s="29"/>
       <c r="E718" s="28"/>
@@ -14250,11 +14258,11 @@
       </c>
       <c r="B719" s="31"/>
       <c r="C719" s="32">
-        <v>48500.39</v>
+        <v>47356.37</v>
       </c>
       <c r="D719" s="33"/>
       <c r="E719" s="34">
-        <v>117622.2</v>
+        <v>114705.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apurva 10 feb 12:36
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -35,7 +35,7 @@
     <t>Stock Group Summary</t>
   </si>
   <si>
-    <t>1-Jul-25 to 9-Feb-26</t>
+    <t>1-Jul-25 to 10-Feb-26</t>
   </si>
   <si>
     <t/>
@@ -1292,7 +1292,7 @@
     <t>5616 PATRIKA (DCU) (7069)</t>
   </si>
   <si>
-    <t>5617 PATRIKA *-* (M) (7067)</t>
+    <t>5617 PATRIKA *-* (M) PUCHNA HAI (7067)</t>
   </si>
   <si>
     <t>5618 PATRIKA (JC) *-* (M) (S-52)</t>
@@ -3941,16 +3941,16 @@
         <v>77</v>
       </c>
       <c r="B75" s="24">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C75" s="25">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D75" s="26">
         <v>1.2</v>
       </c>
       <c r="E75" s="27">
-        <v>219.6</v>
+        <v>214.8</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4213,16 +4213,16 @@
         <v>93</v>
       </c>
       <c r="B91" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C91" s="25">
-        <v>8.5</v>
+        <v>-10</v>
       </c>
       <c r="D91" s="26">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="E91" s="27">
-        <v>5.65</v>
+        <v>-6.65</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -6412,16 +6412,16 @@
         <v>232</v>
       </c>
       <c r="B230" s="24">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C230" s="25">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D230" s="26">
         <v>3.25</v>
       </c>
       <c r="E230" s="27">
-        <v>195</v>
+        <v>191.75</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6887,16 +6887,16 @@
         <v>263</v>
       </c>
       <c r="B261" s="24">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C261" s="25">
-        <v>100.5</v>
+        <v>99</v>
       </c>
       <c r="D261" s="26">
         <v>4.28</v>
       </c>
       <c r="E261" s="27">
-        <v>430.14</v>
+        <v>423.72</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -8601,16 +8601,16 @@
         <v>369</v>
       </c>
       <c r="B367" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C367" s="25">
-        <v>29.5</v>
+        <v>27.5</v>
       </c>
       <c r="D367" s="26">
         <v>7.55</v>
       </c>
       <c r="E367" s="27">
-        <v>222.61</v>
+        <v>207.51</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
@@ -8669,16 +8669,16 @@
         <v>373</v>
       </c>
       <c r="B371" s="24">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C371" s="25">
-        <v>45.33</v>
+        <v>90.33</v>
       </c>
       <c r="D371" s="26">
         <v>4.5</v>
       </c>
       <c r="E371" s="27">
-        <v>203.99</v>
+        <v>406.49</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -9058,16 +9058,16 @@
         <v>396</v>
       </c>
       <c r="B394" s="24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C394" s="25">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="D394" s="26">
         <v>6.65</v>
       </c>
       <c r="E394" s="27">
-        <v>96.43</v>
+        <v>83.13</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
@@ -9281,16 +9281,16 @@
         <v>411</v>
       </c>
       <c r="B409" s="24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C409" s="25">
-        <v>68.5</v>
+        <v>66.5</v>
       </c>
       <c r="D409" s="26">
         <v>5.2</v>
       </c>
       <c r="E409" s="27">
-        <v>356.2</v>
+        <v>345.8</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
@@ -10346,16 +10346,16 @@
         <v>478</v>
       </c>
       <c r="B476" s="24">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C476" s="25">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="D476" s="26">
         <v>10.32</v>
       </c>
       <c r="E476" s="27">
-        <v>108.37</v>
+        <v>98.05</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -10565,16 +10565,16 @@
         <v>491</v>
       </c>
       <c r="B489" s="24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C489" s="25">
-        <v>8.5</v>
+        <v>3.5</v>
       </c>
       <c r="D489" s="26">
         <v>26</v>
       </c>
       <c r="E489" s="27">
-        <v>221</v>
+        <v>91</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.25">
@@ -11610,13 +11610,13 @@
         <v>136</v>
       </c>
       <c r="C553" s="25">
-        <v>5.7</v>
+        <v>105.7</v>
       </c>
       <c r="D553" s="26">
         <v>3.9</v>
       </c>
       <c r="E553" s="27">
-        <v>22.23</v>
+        <v>412.23</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -12176,16 +12176,16 @@
         <v>590</v>
       </c>
       <c r="B588" s="24">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C588" s="25">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D588" s="26">
         <v>0.87</v>
       </c>
       <c r="E588" s="27">
-        <v>184.44</v>
+        <v>182.7</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
@@ -12193,16 +12193,16 @@
         <v>591</v>
       </c>
       <c r="B589" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C589" s="25">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D589" s="26">
         <v>0.57999999999999996</v>
       </c>
       <c r="E589" s="27">
-        <v>481.98</v>
+        <v>480.82</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -12210,16 +12210,16 @@
         <v>592</v>
       </c>
       <c r="B590" s="24">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C590" s="25">
-        <v>794</v>
+        <v>784</v>
       </c>
       <c r="D590" s="26">
         <v>0.85</v>
       </c>
       <c r="E590" s="27">
-        <v>674.9</v>
+        <v>666.4</v>
       </c>
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
@@ -12238,16 +12238,16 @@
         <v>594</v>
       </c>
       <c r="B592" s="24">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C592" s="25">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D592" s="26">
         <v>0.85</v>
       </c>
       <c r="E592" s="27">
-        <v>194.65</v>
+        <v>186.15</v>
       </c>
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.25">
@@ -13300,16 +13300,16 @@
         <v>660</v>
       </c>
       <c r="B658" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C658" s="25">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="D658" s="26">
         <v>4.8</v>
       </c>
       <c r="E658" s="27">
-        <v>69.599999999999994</v>
+        <v>60</v>
       </c>
     </row>
     <row r="659" spans="1:5" x14ac:dyDescent="0.25">
@@ -13728,13 +13728,13 @@
         <v>21</v>
       </c>
       <c r="C683" s="25">
-        <v>2.5</v>
+        <v>22.5</v>
       </c>
       <c r="D683" s="26">
         <v>4.25</v>
       </c>
       <c r="E683" s="27">
-        <v>10.63</v>
+        <v>95.63</v>
       </c>
     </row>
     <row r="684" spans="1:5" x14ac:dyDescent="0.25">
@@ -13762,13 +13762,13 @@
         <v>17</v>
       </c>
       <c r="C685" s="25">
-        <v>19</v>
+        <v>38.5</v>
       </c>
       <c r="D685" s="26">
         <v>5</v>
       </c>
       <c r="E685" s="27">
-        <v>95</v>
+        <v>192.5</v>
       </c>
     </row>
     <row r="686" spans="1:5" x14ac:dyDescent="0.25">
@@ -13843,10 +13843,10 @@
         <v>693</v>
       </c>
       <c r="B691" s="24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C691" s="25">
-        <v>13.5</v>
+        <v>11.5</v>
       </c>
       <c r="D691" s="29"/>
       <c r="E691" s="28"/>
@@ -14370,11 +14370,11 @@
       </c>
       <c r="B729" s="31"/>
       <c r="C729" s="32">
-        <v>40553.120000000003</v>
+        <v>40672.620000000003</v>
       </c>
       <c r="D729" s="33"/>
       <c r="E729" s="34">
-        <v>101903.09</v>
+        <v>102442.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apurva 10 feb 3:16
</commit_message>
<xml_diff>
--- a/data/website stock.xlsx
+++ b/data/website stock.xlsx
@@ -3284,16 +3284,16 @@
         <v>38</v>
       </c>
       <c r="B36" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C36" s="25">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D36" s="26">
         <v>2.2999999999999998</v>
       </c>
       <c r="E36" s="27">
-        <v>163.30000000000001</v>
+        <v>158.69999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3318,16 +3318,16 @@
         <v>40</v>
       </c>
       <c r="B38" s="24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" s="25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" s="26">
         <v>2.76</v>
       </c>
       <c r="E38" s="27">
-        <v>35.880000000000003</v>
+        <v>33.119999999999997</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3924,16 +3924,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="24">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C74" s="25">
-        <v>321.5</v>
+        <v>319.5</v>
       </c>
       <c r="D74" s="26">
         <v>1.2</v>
       </c>
       <c r="E74" s="27">
-        <v>385.8</v>
+        <v>383.4</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4111,16 +4111,16 @@
         <v>87</v>
       </c>
       <c r="B85" s="24">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C85" s="25">
-        <v>1464.5</v>
+        <v>1454.5</v>
       </c>
       <c r="D85" s="26">
         <v>1.3</v>
       </c>
       <c r="E85" s="27">
-        <v>1903.85</v>
+        <v>1890.85</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4145,16 +4145,16 @@
         <v>89</v>
       </c>
       <c r="B87" s="24">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C87" s="25">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="D87" s="26">
         <v>1.7</v>
       </c>
       <c r="E87" s="27">
-        <v>1470.5</v>
+        <v>1463.7</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4196,16 +4196,16 @@
         <v>92</v>
       </c>
       <c r="B90" s="24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C90" s="25">
-        <v>431.7</v>
+        <v>427.7</v>
       </c>
       <c r="D90" s="26">
         <v>1.28</v>
       </c>
       <c r="E90" s="27">
-        <v>553.74</v>
+        <v>548.61</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -4247,11 +4247,17 @@
         <v>95</v>
       </c>
       <c r="B93" s="24">
-        <v>19</v>
-      </c>
-      <c r="C93" s="28"/>
-      <c r="D93" s="29"/>
-      <c r="E93" s="28"/>
+        <v>20</v>
+      </c>
+      <c r="C93" s="25">
+        <v>-3</v>
+      </c>
+      <c r="D93" s="26">
+        <v>2.76</v>
+      </c>
+      <c r="E93" s="27">
+        <v>-8.2799999999999994</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
@@ -4637,10 +4643,10 @@
         <v>123</v>
       </c>
       <c r="B121" s="24">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C121" s="25">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="28"/>
@@ -4981,16 +4987,16 @@
         <v>145</v>
       </c>
       <c r="B143" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C143" s="25">
-        <v>14.27</v>
+        <v>12.77</v>
       </c>
       <c r="D143" s="26">
         <v>18.5</v>
       </c>
       <c r="E143" s="27">
-        <v>264</v>
+        <v>236.25</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -5846,16 +5852,16 @@
         <v>198</v>
       </c>
       <c r="B196" s="24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C196" s="25">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D196" s="26">
         <v>4.5</v>
       </c>
       <c r="E196" s="27">
-        <v>265.5</v>
+        <v>261</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -6095,16 +6101,16 @@
         <v>213</v>
       </c>
       <c r="B211" s="24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C211" s="25">
-        <v>139.5</v>
+        <v>138.5</v>
       </c>
       <c r="D211" s="26">
         <v>2.7</v>
       </c>
       <c r="E211" s="27">
-        <v>376.65</v>
+        <v>373.95</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -6197,16 +6203,16 @@
         <v>219</v>
       </c>
       <c r="B217" s="24">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C217" s="25">
-        <v>125.25</v>
+        <v>122.75</v>
       </c>
       <c r="D217" s="26">
         <v>3.25</v>
       </c>
       <c r="E217" s="27">
-        <v>407.06</v>
+        <v>398.94</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -6656,16 +6662,16 @@
         <v>248</v>
       </c>
       <c r="B246" s="24">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C246" s="25">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D246" s="26">
         <v>3.9</v>
       </c>
       <c r="E246" s="27">
-        <v>468</v>
+        <v>460.2</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6887,16 +6893,16 @@
         <v>263</v>
       </c>
       <c r="B261" s="24">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C261" s="25">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D261" s="26">
         <v>4.28</v>
       </c>
       <c r="E261" s="27">
-        <v>423.72</v>
+        <v>385.2</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -7350,16 +7356,16 @@
         <v>292</v>
       </c>
       <c r="B290" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C290" s="25">
-        <v>118.5</v>
+        <v>117.5</v>
       </c>
       <c r="D290" s="26">
         <v>4.8899999999999997</v>
       </c>
       <c r="E290" s="27">
-        <v>579.23</v>
+        <v>574.34</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -7401,16 +7407,16 @@
         <v>295</v>
       </c>
       <c r="B293" s="24">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C293" s="25">
-        <v>186.5</v>
+        <v>184.5</v>
       </c>
       <c r="D293" s="26">
         <v>6.09</v>
       </c>
       <c r="E293" s="27">
-        <v>1135.58</v>
+        <v>1123.55</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -7680,16 +7686,16 @@
         <v>312</v>
       </c>
       <c r="B310" s="24">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C310" s="25">
-        <v>19.45</v>
+        <v>16.95</v>
       </c>
       <c r="D310" s="26">
         <v>9.4499999999999993</v>
       </c>
       <c r="E310" s="27">
-        <v>183.8</v>
+        <v>160.18</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -7932,16 +7938,16 @@
         <v>328</v>
       </c>
       <c r="B326" s="24">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C326" s="25">
-        <v>139.91</v>
+        <v>138.41</v>
       </c>
       <c r="D326" s="26">
         <v>4.28</v>
       </c>
       <c r="E326" s="27">
-        <v>598.80999999999995</v>
+        <v>592.39</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
@@ -8337,16 +8343,16 @@
         <v>353</v>
       </c>
       <c r="B351" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C351" s="25">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D351" s="26">
         <v>9.1999999999999993</v>
       </c>
       <c r="E351" s="27">
-        <v>211.6</v>
+        <v>193.2</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
@@ -8601,16 +8607,16 @@
         <v>369</v>
       </c>
       <c r="B367" s="24">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C367" s="25">
-        <v>27.5</v>
+        <v>29.5</v>
       </c>
       <c r="D367" s="26">
         <v>7.55</v>
       </c>
       <c r="E367" s="27">
-        <v>207.51</v>
+        <v>222.61</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
@@ -9041,16 +9047,16 @@
         <v>395</v>
       </c>
       <c r="B393" s="24">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C393" s="25">
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="D393" s="26">
         <v>8.5500000000000007</v>
       </c>
       <c r="E393" s="27">
-        <v>98.33</v>
+        <v>81.23</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
@@ -9103,16 +9109,16 @@
         <v>399</v>
       </c>
       <c r="B397" s="24">
+        <v>4</v>
+      </c>
+      <c r="C397" s="25">
         <v>3</v>
-      </c>
-      <c r="C397" s="25">
-        <v>5</v>
       </c>
       <c r="D397" s="26">
         <v>6.4</v>
       </c>
       <c r="E397" s="27">
-        <v>32</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -9281,16 +9287,16 @@
         <v>411</v>
       </c>
       <c r="B409" s="24">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C409" s="25">
-        <v>66.5</v>
+        <v>65.5</v>
       </c>
       <c r="D409" s="26">
         <v>5.2</v>
       </c>
       <c r="E409" s="27">
-        <v>345.8</v>
+        <v>340.6</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
@@ -9364,16 +9370,16 @@
         <v>416</v>
       </c>
       <c r="B414" s="24">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C414" s="25">
-        <v>45.5</v>
+        <v>44.5</v>
       </c>
       <c r="D414" s="26">
         <v>6.19</v>
       </c>
       <c r="E414" s="27">
-        <v>281.77999999999997</v>
+        <v>275.58999999999997</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
@@ -11284,16 +11290,16 @@
         <v>536</v>
       </c>
       <c r="B534" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C534" s="25">
-        <v>21.5</v>
+        <v>18.5</v>
       </c>
       <c r="D534" s="26">
         <v>3.5</v>
       </c>
       <c r="E534" s="27">
-        <v>75.25</v>
+        <v>64.75</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -12179,13 +12185,13 @@
         <v>80</v>
       </c>
       <c r="C588" s="25">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D588" s="26">
         <v>0.87</v>
       </c>
       <c r="E588" s="27">
-        <v>182.7</v>
+        <v>181.83</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
@@ -12193,16 +12199,16 @@
         <v>591</v>
       </c>
       <c r="B589" s="24">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C589" s="25">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D589" s="26">
         <v>0.57999999999999996</v>
       </c>
       <c r="E589" s="27">
-        <v>480.82</v>
+        <v>479.66</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -12644,16 +12650,16 @@
         <v>620</v>
       </c>
       <c r="B618" s="24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C618" s="25">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="D618" s="26">
         <v>5.75</v>
       </c>
       <c r="E618" s="27">
-        <v>112.13</v>
+        <v>106.38</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12712,16 +12718,16 @@
         <v>624</v>
       </c>
       <c r="B622" s="24">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C622" s="25">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D622" s="26">
         <v>2.77</v>
       </c>
       <c r="E622" s="27">
-        <v>152.47999999999999</v>
+        <v>149.71</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12780,16 +12786,16 @@
         <v>628</v>
       </c>
       <c r="B626" s="24">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C626" s="25">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="D626" s="26">
         <v>4</v>
       </c>
       <c r="E626" s="27">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -13830,10 +13836,10 @@
         <v>692</v>
       </c>
       <c r="B690" s="24">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C690" s="25">
-        <v>79.34</v>
+        <v>77.84</v>
       </c>
       <c r="D690" s="29"/>
       <c r="E690" s="28"/>
@@ -14149,10 +14155,10 @@
         <v>717</v>
       </c>
       <c r="B715" s="24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C715" s="25">
-        <v>-0.76</v>
+        <v>-0.77</v>
       </c>
       <c r="D715" s="29"/>
       <c r="E715" s="28"/>
@@ -14370,11 +14376,11 @@
       </c>
       <c r="B729" s="31"/>
       <c r="C729" s="32">
-        <v>40672.620000000003</v>
+        <v>40606.089999999997</v>
       </c>
       <c r="D729" s="33"/>
       <c r="E729" s="34">
-        <v>102442.7</v>
+        <v>102193.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>